<commit_message>
unknown changes on my branch preventing pull
Apologies, Unsure what changes I made, but must have been something. Includes all recent changes of Simon's
</commit_message>
<xml_diff>
--- a/rdf/skosplay-scma-2.xlsx
+++ b/rdf/skosplay-scma-2.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mrwong\OneDrive - Federation University Australia\Documents\GitHub\def-au-scma\rdf\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://federationuniversity-my.sharepoint.com/personal/mr_wong_federation_edu_au/Documents/Documents/GitHub/def-au-scma/rdf/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E832E1B1-BB36-47D1-A82B-188A55C4FE86}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="10" documentId="13_ncr:1_{280EA38A-AAE3-4033-A57D-27CDA991092C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{ECF0682E-58CF-4885-B5DB-FBE57AEC8FD8}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="24240" windowHeight="13140" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="24240" windowHeight="13140" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="SCMA-2011" sheetId="2" r:id="rId1"/>
@@ -4709,8 +4709,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:L466"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="D7" sqref="D7"/>
+    <sheetView topLeftCell="A10" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="C24" sqref="C24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4976,7 +4976,7 @@
       <c r="A14" s="1" t="s">
         <v>645</v>
       </c>
-      <c r="B14" s="38" t="s">
+      <c r="B14" s="26" t="s">
         <v>636</v>
       </c>
       <c r="C14" s="4"/>
@@ -5303,7 +5303,7 @@
       <c r="D28" s="31" t="s">
         <v>659</v>
       </c>
-      <c r="E28" t="s">
+      <c r="E28" s="26" t="s">
         <v>1073</v>
       </c>
       <c r="F28" s="12"/>
@@ -12740,7 +12740,7 @@
   <hyperlinks>
     <hyperlink ref="C2" r:id="rId1" xr:uid="{97D0FE00-0703-48CF-A3AC-F8C02E75A146}"/>
     <hyperlink ref="C3" r:id="rId2" display="http://registry.it.csiro.au/sandbox/soil/scma/" xr:uid="{BB921B57-84FB-4D0B-B401-C316ED0CBD5E}"/>
-    <hyperlink ref="B1" r:id="rId3" display="http://registry.it.csiro.au/sandbox/soil/scma" xr:uid="{E5A211B5-32F4-4D0B-A082-A3D428E2FB08}"/>
+    <hyperlink ref="B1" r:id="rId3" xr:uid="{E5A211B5-32F4-4D0B-A082-A3D428E2FB08}"/>
     <hyperlink ref="H101" r:id="rId4" xr:uid="{EEBDE4B1-0DD6-4612-88C0-B735090E9501}"/>
     <hyperlink ref="C5" r:id="rId5" xr:uid="{E133B0A9-2102-4B70-B4D3-0F005238F1C8}"/>
     <hyperlink ref="H23" r:id="rId6" xr:uid="{C2FF9382-F0D3-4DDB-B13B-B680CE4F0723}"/>
@@ -12870,10 +12870,12 @@
     <hyperlink ref="E25" r:id="rId130" xr:uid="{99A72291-0FF9-459A-85D7-36F2B3051B7B}"/>
     <hyperlink ref="B16" r:id="rId131" display="http://registry.it.csiro.au/sandbox/soil/scma" xr:uid="{7F51B6B3-1B6F-4778-BCFF-9D0D8B93E835}"/>
     <hyperlink ref="E52" r:id="rId132" xr:uid="{0B886457-8AB9-4712-BE77-451FB95C6F9F}"/>
+    <hyperlink ref="E28" r:id="rId133" xr:uid="{9B1B8DB9-DF2A-4D3C-8C85-2322F1EA4B4E}"/>
+    <hyperlink ref="B14" r:id="rId134" xr:uid="{0B261E0C-9123-4445-954A-9D8C9B658D44}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId133"/>
-  <legacyDrawing r:id="rId134"/>
+  <pageSetup orientation="portrait" r:id="rId135"/>
+  <legacyDrawing r:id="rId136"/>
 </worksheet>
 </file>
 
@@ -12881,8 +12883,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4A25E589-C762-47F7-A5B5-46A66BE90C97}">
   <dimension ref="A1:L461"/>
   <sheetViews>
-    <sheetView topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="E23" sqref="E23"/>
+    <sheetView tabSelected="1" topLeftCell="D193" workbookViewId="0">
+      <selection activeCell="H189" sqref="H189"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -13474,7 +13476,7 @@
       <c r="I27" s="32"/>
       <c r="J27" s="32"/>
       <c r="K27" s="32"/>
-      <c r="L27" s="27" t="s">
+      <c r="L27" s="26" t="s">
         <v>1069</v>
       </c>
     </row>
@@ -17882,7 +17884,7 @@
       <c r="G181" s="19" t="s">
         <v>95</v>
       </c>
-      <c r="H181" s="27" t="s">
+      <c r="H181" s="26" t="s">
         <v>545</v>
       </c>
       <c r="I181" s="31" t="s">
@@ -18054,7 +18056,7 @@
       <c r="G187" s="19" t="s">
         <v>95</v>
       </c>
-      <c r="H187" s="27" t="s">
+      <c r="H187" s="26" t="s">
         <v>553</v>
       </c>
       <c r="I187" s="32" t="s">
@@ -18114,7 +18116,7 @@
       <c r="G189" s="19" t="s">
         <v>95</v>
       </c>
-      <c r="H189" s="27" t="s">
+      <c r="H189" s="26" t="s">
         <v>557</v>
       </c>
       <c r="I189" s="32" t="s">
@@ -20404,17 +20406,24 @@
     <hyperlink ref="H25" r:id="rId126" xr:uid="{4EE159A3-7A1E-4BC7-8995-C198701C450A}"/>
     <hyperlink ref="B15" r:id="rId127" display="http://registry.it.csiro.au/sandbox/soil/scma" xr:uid="{0752AF16-E9C0-4D0F-9949-1FCC5DC37060}"/>
     <hyperlink ref="L22" r:id="rId128" xr:uid="{874440BF-61E1-45FF-A38A-42FECFC40089}"/>
+    <hyperlink ref="L27" r:id="rId129" xr:uid="{25A8B64A-BE90-40D0-8502-828D5F39398F}"/>
+    <hyperlink ref="H181" r:id="rId130" xr:uid="{6D993A81-16D3-40C7-8F81-833913097AA8}"/>
+    <hyperlink ref="H187" r:id="rId131" xr:uid="{56A43D80-5339-4B76-9391-49A025D9212B}"/>
+    <hyperlink ref="H189" r:id="rId132" xr:uid="{6315BB13-4B74-464B-9553-A415FD28F07F}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId129"/>
-  <legacyDrawing r:id="rId130"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId133"/>
+  <legacyDrawing r:id="rId134"/>
 </worksheet>
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
@@ -20629,19 +20638,15 @@
 </file>
 
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{AAE62FC3-7D3B-4886-B53E-C881811D2384}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{008ABE91-8C92-4516-916D-4DC325FB5C89}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
@@ -20666,9 +20671,10 @@
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{008ABE91-8C92-4516-916D-4DC325FB5C89}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{AAE62FC3-7D3B-4886-B53E-C881811D2384}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
back matter added to skos:related(separator=",") in 2011 version
</commit_message>
<xml_diff>
--- a/rdf/skosplay-scma-2.xlsx
+++ b/rdf/skosplay-scma-2.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://federationuniversity-my.sharepoint.com/personal/mr_wong_federation_edu_au/Documents/Documents/GitHub/def-au-scma/rdf/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="108" documentId="13_ncr:1_{280EA38A-AAE3-4033-A57D-27CDA991092C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{E8A11F39-ACFB-4257-99DF-725D20F55020}"/>
+  <xr:revisionPtr revIDLastSave="115" documentId="13_ncr:1_{280EA38A-AAE3-4033-A57D-27CDA991092C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{D711240B-6556-4268-AD2D-63F73FFC9EB8}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="24240" windowHeight="13140" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="6135" yWindow="-120" windowWidth="18000" windowHeight="9360" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="SCMA-2011" sheetId="2" r:id="rId1"/>
@@ -103,7 +103,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4115" uniqueCount="1348">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4359" uniqueCount="1349">
   <si>
     <t>ConceptScheme URI</t>
   </si>
@@ -4194,6 +4194,9 @@
   </si>
   <si>
     <t>Australian soil and land survey handbooks ; v. 3.</t>
+  </si>
+  <si>
+    <t>https://raw.githack.com/ANZSoilData/def-au-scma/master/html/90backmatter/91results01.html, https://raw.githack.com/ANZSoilData/def-au-scma/master/html/90backmatter/92accuracyandprecision02.html, https://raw.githack.com/ANZSoilData/def-au-scma/master/html/90backmatter/93acids03.html, https://raw.githack.com/ANZSoilData/def-au-scma/master/html/90backmatter/94atomicweights04.html, https://raw.githack.com/ANZSoilData/def-au-scma/master/html/90backmatter/95Unitsr05.html</t>
   </si>
 </sst>
 </file>
@@ -4868,8 +4871,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:M477"/>
   <sheetViews>
-    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="E13" sqref="E13"/>
+    <sheetView tabSelected="1" topLeftCell="I24" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="K33" sqref="K33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5559,7 +5562,9 @@
       </c>
       <c r="I34" s="55"/>
       <c r="J34" s="32"/>
-      <c r="K34" s="32"/>
+      <c r="K34" s="32" t="s">
+        <v>1348</v>
+      </c>
       <c r="L34" s="29" t="s">
         <v>1327</v>
       </c>
@@ -5592,7 +5597,9 @@
       </c>
       <c r="I35" s="55"/>
       <c r="J35" s="32"/>
-      <c r="K35" s="32"/>
+      <c r="K35" s="32" t="s">
+        <v>1348</v>
+      </c>
       <c r="L35" s="29" t="s">
         <v>1327</v>
       </c>
@@ -5625,7 +5632,9 @@
       </c>
       <c r="I36" s="55"/>
       <c r="J36" s="32"/>
-      <c r="K36" s="32"/>
+      <c r="K36" s="32" t="s">
+        <v>1348</v>
+      </c>
       <c r="L36" s="29" t="s">
         <v>1327</v>
       </c>
@@ -5658,7 +5667,9 @@
       </c>
       <c r="I37" s="55"/>
       <c r="J37" s="32"/>
-      <c r="K37" s="32"/>
+      <c r="K37" s="32" t="s">
+        <v>1348</v>
+      </c>
       <c r="L37" s="29" t="s">
         <v>1327</v>
       </c>
@@ -5691,7 +5702,9 @@
       </c>
       <c r="I38" s="55"/>
       <c r="J38" s="32"/>
-      <c r="K38" s="32"/>
+      <c r="K38" s="32" t="s">
+        <v>1348</v>
+      </c>
       <c r="L38" s="29" t="s">
         <v>1327</v>
       </c>
@@ -5722,7 +5735,9 @@
       </c>
       <c r="I39" s="55"/>
       <c r="J39" s="32"/>
-      <c r="K39" s="32"/>
+      <c r="K39" s="32" t="s">
+        <v>1348</v>
+      </c>
       <c r="L39" s="29" t="s">
         <v>1327</v>
       </c>
@@ -5755,7 +5770,9 @@
       </c>
       <c r="I40" s="55"/>
       <c r="J40" s="32"/>
-      <c r="K40" s="32"/>
+      <c r="K40" s="32" t="s">
+        <v>1348</v>
+      </c>
       <c r="L40" s="29" t="s">
         <v>1327</v>
       </c>
@@ -5788,7 +5805,9 @@
       </c>
       <c r="I41" s="55"/>
       <c r="J41" s="32"/>
-      <c r="K41" s="32"/>
+      <c r="K41" s="32" t="s">
+        <v>1348</v>
+      </c>
       <c r="L41" s="29" t="s">
         <v>1327</v>
       </c>
@@ -5821,7 +5840,9 @@
       </c>
       <c r="I42" s="55"/>
       <c r="J42" s="32"/>
-      <c r="K42" s="32"/>
+      <c r="K42" s="32" t="s">
+        <v>1348</v>
+      </c>
       <c r="L42" s="29" t="s">
         <v>1327</v>
       </c>
@@ -5854,7 +5875,9 @@
       </c>
       <c r="I43" s="55"/>
       <c r="J43" s="32"/>
-      <c r="K43" s="32"/>
+      <c r="K43" s="32" t="s">
+        <v>1348</v>
+      </c>
       <c r="L43" s="29" t="s">
         <v>1327</v>
       </c>
@@ -5885,7 +5908,9 @@
       </c>
       <c r="I44" s="55"/>
       <c r="J44" s="32"/>
-      <c r="K44" s="32"/>
+      <c r="K44" s="32" t="s">
+        <v>1348</v>
+      </c>
       <c r="L44" s="29" t="s">
         <v>1327</v>
       </c>
@@ -5918,7 +5943,9 @@
       </c>
       <c r="I45" s="55"/>
       <c r="J45" s="32"/>
-      <c r="K45" s="32"/>
+      <c r="K45" s="32" t="s">
+        <v>1348</v>
+      </c>
       <c r="L45" s="29" t="s">
         <v>1327</v>
       </c>
@@ -5951,7 +5978,9 @@
       </c>
       <c r="I46" s="55"/>
       <c r="J46" s="32"/>
-      <c r="K46" s="32"/>
+      <c r="K46" s="32" t="s">
+        <v>1348</v>
+      </c>
       <c r="L46" s="29" t="s">
         <v>1327</v>
       </c>
@@ -5984,7 +6013,9 @@
       </c>
       <c r="I47" s="55"/>
       <c r="J47" s="32"/>
-      <c r="K47" s="32"/>
+      <c r="K47" s="32" t="s">
+        <v>1348</v>
+      </c>
       <c r="L47" s="29" t="s">
         <v>1327</v>
       </c>
@@ -6017,7 +6048,9 @@
       </c>
       <c r="I48" s="55"/>
       <c r="J48" s="32"/>
-      <c r="K48" s="32"/>
+      <c r="K48" s="32" t="s">
+        <v>1348</v>
+      </c>
       <c r="L48" s="29" t="s">
         <v>1327</v>
       </c>
@@ -6050,7 +6083,9 @@
       </c>
       <c r="I49" s="55"/>
       <c r="J49" s="32"/>
-      <c r="K49" s="32"/>
+      <c r="K49" s="32" t="s">
+        <v>1348</v>
+      </c>
       <c r="L49" s="29" t="s">
         <v>1327</v>
       </c>
@@ -6083,7 +6118,9 @@
       </c>
       <c r="I50" s="55"/>
       <c r="J50" s="32"/>
-      <c r="K50" s="32"/>
+      <c r="K50" s="32" t="s">
+        <v>1348</v>
+      </c>
       <c r="L50" s="29" t="s">
         <v>1327</v>
       </c>
@@ -6116,7 +6153,9 @@
       </c>
       <c r="I51" s="55"/>
       <c r="J51" s="32"/>
-      <c r="K51" s="32"/>
+      <c r="K51" s="32" t="s">
+        <v>1348</v>
+      </c>
       <c r="L51" s="29" t="s">
         <v>1327</v>
       </c>
@@ -6149,7 +6188,9 @@
       </c>
       <c r="I52" s="55"/>
       <c r="J52" s="32"/>
-      <c r="K52" s="32"/>
+      <c r="K52" s="32" t="s">
+        <v>1348</v>
+      </c>
       <c r="L52" s="29" t="s">
         <v>1327</v>
       </c>
@@ -6182,7 +6223,9 @@
       </c>
       <c r="I53" s="55"/>
       <c r="J53" s="32"/>
-      <c r="K53" s="32"/>
+      <c r="K53" s="32" t="s">
+        <v>1348</v>
+      </c>
       <c r="L53" s="29" t="s">
         <v>1327</v>
       </c>
@@ -6215,7 +6258,9 @@
       </c>
       <c r="I54" s="55"/>
       <c r="J54" s="32"/>
-      <c r="K54" s="32"/>
+      <c r="K54" s="32" t="s">
+        <v>1348</v>
+      </c>
       <c r="L54" s="29" t="s">
         <v>1327</v>
       </c>
@@ -6248,7 +6293,9 @@
       </c>
       <c r="I55" s="55"/>
       <c r="J55" s="32"/>
-      <c r="K55" s="32"/>
+      <c r="K55" s="32" t="s">
+        <v>1348</v>
+      </c>
       <c r="L55" s="29" t="s">
         <v>1327</v>
       </c>
@@ -6281,7 +6328,9 @@
       </c>
       <c r="I56" s="55"/>
       <c r="J56" s="32"/>
-      <c r="K56" s="32"/>
+      <c r="K56" s="32" t="s">
+        <v>1348</v>
+      </c>
       <c r="L56" s="29" t="s">
         <v>1327</v>
       </c>
@@ -6314,7 +6363,9 @@
       </c>
       <c r="I57" s="55"/>
       <c r="J57" s="32"/>
-      <c r="K57" s="32"/>
+      <c r="K57" s="32" t="s">
+        <v>1348</v>
+      </c>
       <c r="L57" s="29" t="s">
         <v>1327</v>
       </c>
@@ -6347,7 +6398,9 @@
       </c>
       <c r="I58" s="55"/>
       <c r="J58" s="32"/>
-      <c r="K58" s="32"/>
+      <c r="K58" s="32" t="s">
+        <v>1348</v>
+      </c>
       <c r="L58" s="29" t="s">
         <v>1327</v>
       </c>
@@ -6380,7 +6433,9 @@
       </c>
       <c r="I59" s="55"/>
       <c r="J59" s="32"/>
-      <c r="K59" s="32"/>
+      <c r="K59" s="32" t="s">
+        <v>1348</v>
+      </c>
       <c r="L59" s="29" t="s">
         <v>1327</v>
       </c>
@@ -6413,7 +6468,9 @@
       </c>
       <c r="I60" s="55"/>
       <c r="J60" s="32"/>
-      <c r="K60" s="32"/>
+      <c r="K60" s="32" t="s">
+        <v>1348</v>
+      </c>
       <c r="L60" s="29" t="s">
         <v>1327</v>
       </c>
@@ -6444,7 +6501,9 @@
       </c>
       <c r="I61" s="55"/>
       <c r="J61" s="32"/>
-      <c r="K61" s="32"/>
+      <c r="K61" s="32" t="s">
+        <v>1348</v>
+      </c>
       <c r="L61" s="29" t="s">
         <v>1327</v>
       </c>
@@ -6477,7 +6536,9 @@
       </c>
       <c r="I62" s="55"/>
       <c r="J62" s="32"/>
-      <c r="K62" s="32"/>
+      <c r="K62" s="32" t="s">
+        <v>1348</v>
+      </c>
       <c r="L62" s="29" t="s">
         <v>1327</v>
       </c>
@@ -6514,7 +6575,9 @@
         <v>823</v>
       </c>
       <c r="J63" s="32"/>
-      <c r="K63" s="32"/>
+      <c r="K63" s="32" t="s">
+        <v>1348</v>
+      </c>
       <c r="L63" s="29" t="s">
         <v>1327</v>
       </c>
@@ -6551,7 +6614,9 @@
         <v>823</v>
       </c>
       <c r="J64" s="32"/>
-      <c r="K64" s="32"/>
+      <c r="K64" s="32" t="s">
+        <v>1348</v>
+      </c>
       <c r="L64" s="29" t="s">
         <v>1327</v>
       </c>
@@ -6584,7 +6649,9 @@
       </c>
       <c r="I65" s="55"/>
       <c r="J65" s="32"/>
-      <c r="K65" s="32"/>
+      <c r="K65" s="32" t="s">
+        <v>1348</v>
+      </c>
       <c r="L65" s="29" t="s">
         <v>1327</v>
       </c>
@@ -6617,7 +6684,9 @@
       </c>
       <c r="I66" s="55"/>
       <c r="J66" s="32"/>
-      <c r="K66" s="32"/>
+      <c r="K66" s="32" t="s">
+        <v>1348</v>
+      </c>
       <c r="L66" s="29" t="s">
         <v>1327</v>
       </c>
@@ -6650,7 +6719,9 @@
       </c>
       <c r="I67" s="55"/>
       <c r="J67" s="32"/>
-      <c r="K67" s="32"/>
+      <c r="K67" s="32" t="s">
+        <v>1348</v>
+      </c>
       <c r="L67" s="29" t="s">
         <v>1327</v>
       </c>
@@ -6681,7 +6752,9 @@
       </c>
       <c r="I68" s="55"/>
       <c r="J68" s="32"/>
-      <c r="K68" s="32"/>
+      <c r="K68" s="32" t="s">
+        <v>1348</v>
+      </c>
       <c r="L68" s="29" t="s">
         <v>1327</v>
       </c>
@@ -6714,7 +6787,9 @@
       </c>
       <c r="I69" s="55"/>
       <c r="J69" s="32"/>
-      <c r="K69" s="32"/>
+      <c r="K69" s="32" t="s">
+        <v>1348</v>
+      </c>
       <c r="L69" s="29" t="s">
         <v>1327</v>
       </c>
@@ -6747,7 +6822,9 @@
       </c>
       <c r="I70" s="55"/>
       <c r="J70" s="32"/>
-      <c r="K70" s="32"/>
+      <c r="K70" s="32" t="s">
+        <v>1348</v>
+      </c>
       <c r="L70" s="29" t="s">
         <v>1327</v>
       </c>
@@ -6780,7 +6857,9 @@
       </c>
       <c r="I71" s="55"/>
       <c r="J71" s="32"/>
-      <c r="K71" s="32"/>
+      <c r="K71" s="32" t="s">
+        <v>1348</v>
+      </c>
       <c r="L71" s="29" t="s">
         <v>1327</v>
       </c>
@@ -6815,7 +6894,9 @@
       </c>
       <c r="I72" s="55"/>
       <c r="J72" s="32"/>
-      <c r="K72" s="32"/>
+      <c r="K72" s="32" t="s">
+        <v>1348</v>
+      </c>
       <c r="L72" s="29" t="s">
         <v>1327</v>
       </c>
@@ -6850,7 +6931,9 @@
       </c>
       <c r="I73" s="55"/>
       <c r="J73" s="32"/>
-      <c r="K73" s="32"/>
+      <c r="K73" s="32" t="s">
+        <v>1348</v>
+      </c>
       <c r="L73" s="29" t="s">
         <v>1327</v>
       </c>
@@ -6883,7 +6966,9 @@
       </c>
       <c r="I74" s="55"/>
       <c r="J74" s="32"/>
-      <c r="K74" s="32"/>
+      <c r="K74" s="32" t="s">
+        <v>1348</v>
+      </c>
       <c r="L74" s="29" t="s">
         <v>1327</v>
       </c>
@@ -6916,7 +7001,9 @@
       </c>
       <c r="I75" s="55"/>
       <c r="J75" s="32"/>
-      <c r="K75" s="32"/>
+      <c r="K75" s="32" t="s">
+        <v>1348</v>
+      </c>
       <c r="L75" s="29" t="s">
         <v>1327</v>
       </c>
@@ -6951,7 +7038,9 @@
       </c>
       <c r="I76" s="55"/>
       <c r="J76" s="32"/>
-      <c r="K76" s="32"/>
+      <c r="K76" s="32" t="s">
+        <v>1348</v>
+      </c>
       <c r="L76" s="29" t="s">
         <v>1327</v>
       </c>
@@ -6986,7 +7075,9 @@
       </c>
       <c r="I77" s="55"/>
       <c r="J77" s="32"/>
-      <c r="K77" s="32"/>
+      <c r="K77" s="32" t="s">
+        <v>1348</v>
+      </c>
       <c r="L77" s="29" t="s">
         <v>1327</v>
       </c>
@@ -7019,7 +7110,9 @@
       </c>
       <c r="I78" s="55"/>
       <c r="J78" s="32"/>
-      <c r="K78" s="32"/>
+      <c r="K78" s="32" t="s">
+        <v>1348</v>
+      </c>
       <c r="L78" s="29" t="s">
         <v>1327</v>
       </c>
@@ -7052,7 +7145,9 @@
       </c>
       <c r="I79" s="55"/>
       <c r="J79" s="32"/>
-      <c r="K79" s="32"/>
+      <c r="K79" s="32" t="s">
+        <v>1348</v>
+      </c>
       <c r="L79" s="29" t="s">
         <v>1327</v>
       </c>
@@ -7085,7 +7180,9 @@
       </c>
       <c r="I80" s="55"/>
       <c r="J80" s="32"/>
-      <c r="K80" s="32"/>
+      <c r="K80" s="32" t="s">
+        <v>1348</v>
+      </c>
       <c r="L80" s="29" t="s">
         <v>1327</v>
       </c>
@@ -7118,7 +7215,9 @@
       </c>
       <c r="I81" s="55"/>
       <c r="J81" s="32"/>
-      <c r="K81" s="32"/>
+      <c r="K81" s="32" t="s">
+        <v>1348</v>
+      </c>
       <c r="L81" s="29" t="s">
         <v>1327</v>
       </c>
@@ -7151,7 +7250,9 @@
       </c>
       <c r="I82" s="55"/>
       <c r="J82" s="32"/>
-      <c r="K82" s="32"/>
+      <c r="K82" s="32" t="s">
+        <v>1348</v>
+      </c>
       <c r="L82" s="29" t="s">
         <v>1327</v>
       </c>
@@ -7182,7 +7283,9 @@
       </c>
       <c r="I83" s="55"/>
       <c r="J83" s="32"/>
-      <c r="K83" s="32"/>
+      <c r="K83" s="32" t="s">
+        <v>1348</v>
+      </c>
       <c r="L83" s="29" t="s">
         <v>1327</v>
       </c>
@@ -7215,7 +7318,9 @@
       </c>
       <c r="I84" s="55"/>
       <c r="J84" s="32"/>
-      <c r="K84" s="32"/>
+      <c r="K84" s="32" t="s">
+        <v>1348</v>
+      </c>
       <c r="L84" s="29" t="s">
         <v>1327</v>
       </c>
@@ -7252,7 +7357,9 @@
         <v>846</v>
       </c>
       <c r="J85" s="32"/>
-      <c r="K85" s="32"/>
+      <c r="K85" s="32" t="s">
+        <v>1348</v>
+      </c>
       <c r="L85" s="29" t="s">
         <v>1327</v>
       </c>
@@ -7289,7 +7396,9 @@
         <v>846</v>
       </c>
       <c r="J86" s="32"/>
-      <c r="K86" s="32"/>
+      <c r="K86" s="32" t="s">
+        <v>1348</v>
+      </c>
       <c r="L86" s="29" t="s">
         <v>1327</v>
       </c>
@@ -7322,7 +7431,9 @@
       </c>
       <c r="I87" s="55"/>
       <c r="J87" s="32"/>
-      <c r="K87" s="32"/>
+      <c r="K87" s="32" t="s">
+        <v>1348</v>
+      </c>
       <c r="L87" s="29" t="s">
         <v>1327</v>
       </c>
@@ -7355,7 +7466,9 @@
       </c>
       <c r="I88" s="55"/>
       <c r="J88" s="32"/>
-      <c r="K88" s="32"/>
+      <c r="K88" s="32" t="s">
+        <v>1348</v>
+      </c>
       <c r="L88" s="29" t="s">
         <v>1327</v>
       </c>
@@ -7388,7 +7501,9 @@
       </c>
       <c r="I89" s="55"/>
       <c r="J89" s="32"/>
-      <c r="K89" s="32"/>
+      <c r="K89" s="32" t="s">
+        <v>1348</v>
+      </c>
       <c r="L89" s="29" t="s">
         <v>1327</v>
       </c>
@@ -7421,7 +7536,9 @@
       </c>
       <c r="I90" s="55"/>
       <c r="J90" s="32"/>
-      <c r="K90" s="32"/>
+      <c r="K90" s="32" t="s">
+        <v>1348</v>
+      </c>
       <c r="L90" s="29" t="s">
         <v>1327</v>
       </c>
@@ -7456,7 +7573,9 @@
       </c>
       <c r="I91" s="55"/>
       <c r="J91" s="32"/>
-      <c r="K91" s="32"/>
+      <c r="K91" s="32" t="s">
+        <v>1348</v>
+      </c>
       <c r="L91" s="29" t="s">
         <v>1327</v>
       </c>
@@ -7491,7 +7610,9 @@
       </c>
       <c r="I92" s="55"/>
       <c r="J92" s="32"/>
-      <c r="K92" s="32"/>
+      <c r="K92" s="32" t="s">
+        <v>1348</v>
+      </c>
       <c r="L92" s="29" t="s">
         <v>1327</v>
       </c>
@@ -7524,7 +7645,9 @@
       </c>
       <c r="I93" s="55"/>
       <c r="J93" s="32"/>
-      <c r="K93" s="32"/>
+      <c r="K93" s="32" t="s">
+        <v>1348</v>
+      </c>
       <c r="L93" s="29" t="s">
         <v>1327</v>
       </c>
@@ -7561,7 +7684,9 @@
         <v>856</v>
       </c>
       <c r="J94" s="32"/>
-      <c r="K94" s="32"/>
+      <c r="K94" s="32" t="s">
+        <v>1348</v>
+      </c>
       <c r="L94" s="29" t="s">
         <v>1327</v>
       </c>
@@ -7598,7 +7723,9 @@
         <v>856</v>
       </c>
       <c r="J95" s="32"/>
-      <c r="K95" s="32"/>
+      <c r="K95" s="32" t="s">
+        <v>1348</v>
+      </c>
       <c r="L95" s="29" t="s">
         <v>1327</v>
       </c>
@@ -7633,7 +7760,9 @@
       </c>
       <c r="I96" s="55"/>
       <c r="J96" s="32"/>
-      <c r="K96" s="32"/>
+      <c r="K96" s="32" t="s">
+        <v>1348</v>
+      </c>
       <c r="L96" s="29" t="s">
         <v>1327</v>
       </c>
@@ -7666,7 +7795,9 @@
       </c>
       <c r="I97" s="55"/>
       <c r="J97" s="32"/>
-      <c r="K97" s="32"/>
+      <c r="K97" s="32" t="s">
+        <v>1348</v>
+      </c>
       <c r="L97" s="29" t="s">
         <v>1327</v>
       </c>
@@ -7701,7 +7832,9 @@
       </c>
       <c r="I98" s="55"/>
       <c r="J98" s="32"/>
-      <c r="K98" s="32"/>
+      <c r="K98" s="32" t="s">
+        <v>1348</v>
+      </c>
       <c r="L98" s="29" t="s">
         <v>1327</v>
       </c>
@@ -7736,7 +7869,9 @@
       </c>
       <c r="I99" s="55"/>
       <c r="J99" s="32"/>
-      <c r="K99" s="32"/>
+      <c r="K99" s="32" t="s">
+        <v>1348</v>
+      </c>
       <c r="L99" s="29" t="s">
         <v>1327</v>
       </c>
@@ -7771,7 +7906,9 @@
       </c>
       <c r="I100" s="55"/>
       <c r="J100" s="32"/>
-      <c r="K100" s="32"/>
+      <c r="K100" s="32" t="s">
+        <v>1348</v>
+      </c>
       <c r="L100" s="29" t="s">
         <v>1327</v>
       </c>
@@ -7806,7 +7943,9 @@
       </c>
       <c r="I101" s="55"/>
       <c r="J101" s="32"/>
-      <c r="K101" s="32"/>
+      <c r="K101" s="32" t="s">
+        <v>1348</v>
+      </c>
       <c r="L101" s="29" t="s">
         <v>1327</v>
       </c>
@@ -7841,7 +7980,9 @@
       </c>
       <c r="I102" s="55"/>
       <c r="J102" s="32"/>
-      <c r="K102" s="32"/>
+      <c r="K102" s="32" t="s">
+        <v>1348</v>
+      </c>
       <c r="L102" s="29" t="s">
         <v>1327</v>
       </c>
@@ -7876,7 +8017,9 @@
       </c>
       <c r="I103" s="55"/>
       <c r="J103" s="32"/>
-      <c r="K103" s="32"/>
+      <c r="K103" s="32" t="s">
+        <v>1348</v>
+      </c>
       <c r="L103" s="29" t="s">
         <v>1327</v>
       </c>
@@ -7911,7 +8054,9 @@
       </c>
       <c r="I104" s="55"/>
       <c r="J104" s="32"/>
-      <c r="K104" s="32"/>
+      <c r="K104" s="32" t="s">
+        <v>1348</v>
+      </c>
       <c r="L104" s="29" t="s">
         <v>1327</v>
       </c>
@@ -7946,7 +8091,9 @@
       </c>
       <c r="I105" s="55"/>
       <c r="J105" s="32"/>
-      <c r="K105" s="32"/>
+      <c r="K105" s="32" t="s">
+        <v>1348</v>
+      </c>
       <c r="L105" s="29" t="s">
         <v>1327</v>
       </c>
@@ -7983,7 +8130,9 @@
         <v>869</v>
       </c>
       <c r="J106" s="32"/>
-      <c r="K106" s="32"/>
+      <c r="K106" s="32" t="s">
+        <v>1348</v>
+      </c>
       <c r="L106" s="29" t="s">
         <v>1327</v>
       </c>
@@ -8020,7 +8169,9 @@
         <v>869</v>
       </c>
       <c r="J107" s="32"/>
-      <c r="K107" s="32"/>
+      <c r="K107" s="32" t="s">
+        <v>1348</v>
+      </c>
       <c r="L107" s="29" t="s">
         <v>1327</v>
       </c>
@@ -8053,7 +8204,9 @@
       </c>
       <c r="I108" s="55"/>
       <c r="J108" s="32"/>
-      <c r="K108" s="32"/>
+      <c r="K108" s="32" t="s">
+        <v>1348</v>
+      </c>
       <c r="L108" s="29" t="s">
         <v>1327</v>
       </c>
@@ -8088,7 +8241,9 @@
       </c>
       <c r="I109" s="55"/>
       <c r="J109" s="32"/>
-      <c r="K109" s="32"/>
+      <c r="K109" s="32" t="s">
+        <v>1348</v>
+      </c>
       <c r="L109" s="29" t="s">
         <v>1327</v>
       </c>
@@ -8123,7 +8278,9 @@
       </c>
       <c r="I110" s="55"/>
       <c r="J110" s="32"/>
-      <c r="K110" s="32"/>
+      <c r="K110" s="32" t="s">
+        <v>1348</v>
+      </c>
       <c r="L110" s="29" t="s">
         <v>1327</v>
       </c>
@@ -8158,7 +8315,9 @@
       </c>
       <c r="I111" s="55"/>
       <c r="J111" s="32"/>
-      <c r="K111" s="32"/>
+      <c r="K111" s="32" t="s">
+        <v>1348</v>
+      </c>
       <c r="L111" s="29" t="s">
         <v>1327</v>
       </c>
@@ -8193,7 +8352,9 @@
       </c>
       <c r="I112" s="55"/>
       <c r="J112" s="29"/>
-      <c r="K112" s="29"/>
+      <c r="K112" s="32" t="s">
+        <v>1348</v>
+      </c>
       <c r="L112" s="29" t="s">
         <v>1327</v>
       </c>
@@ -8228,7 +8389,9 @@
       </c>
       <c r="I113" s="55"/>
       <c r="J113" s="32"/>
-      <c r="K113" s="32"/>
+      <c r="K113" s="32" t="s">
+        <v>1348</v>
+      </c>
       <c r="L113" s="29" t="s">
         <v>1327</v>
       </c>
@@ -8259,7 +8422,9 @@
       </c>
       <c r="I114" s="55"/>
       <c r="J114" s="32"/>
-      <c r="K114" s="32"/>
+      <c r="K114" s="32" t="s">
+        <v>1348</v>
+      </c>
       <c r="L114" s="29" t="s">
         <v>1327</v>
       </c>
@@ -8292,7 +8457,9 @@
       </c>
       <c r="I115" s="55"/>
       <c r="J115" s="32"/>
-      <c r="K115" s="32"/>
+      <c r="K115" s="32" t="s">
+        <v>1348</v>
+      </c>
       <c r="L115" s="29" t="s">
         <v>1327</v>
       </c>
@@ -8325,7 +8492,9 @@
       </c>
       <c r="I116" s="55"/>
       <c r="J116" s="32"/>
-      <c r="K116" s="32"/>
+      <c r="K116" s="32" t="s">
+        <v>1348</v>
+      </c>
       <c r="L116" s="29" t="s">
         <v>1327</v>
       </c>
@@ -8356,7 +8525,9 @@
       </c>
       <c r="I117" s="55"/>
       <c r="J117" s="32"/>
-      <c r="K117" s="32"/>
+      <c r="K117" s="32" t="s">
+        <v>1348</v>
+      </c>
       <c r="L117" s="29" t="s">
         <v>1327</v>
       </c>
@@ -8389,7 +8560,9 @@
       </c>
       <c r="I118" s="55"/>
       <c r="J118" s="32"/>
-      <c r="K118" s="32"/>
+      <c r="K118" s="32" t="s">
+        <v>1348</v>
+      </c>
       <c r="L118" s="29" t="s">
         <v>1327</v>
       </c>
@@ -8424,7 +8597,9 @@
       </c>
       <c r="I119" s="55"/>
       <c r="J119" s="32"/>
-      <c r="K119" s="32"/>
+      <c r="K119" s="32" t="s">
+        <v>1348</v>
+      </c>
       <c r="L119" s="29" t="s">
         <v>1327</v>
       </c>
@@ -8459,7 +8634,9 @@
       </c>
       <c r="I120" s="55"/>
       <c r="J120" s="32"/>
-      <c r="K120" s="32"/>
+      <c r="K120" s="32" t="s">
+        <v>1348</v>
+      </c>
       <c r="L120" s="29" t="s">
         <v>1327</v>
       </c>
@@ -8494,7 +8671,9 @@
       </c>
       <c r="I121" s="55"/>
       <c r="J121" s="32"/>
-      <c r="K121" s="32"/>
+      <c r="K121" s="32" t="s">
+        <v>1348</v>
+      </c>
       <c r="L121" s="29" t="s">
         <v>1327</v>
       </c>
@@ -8529,7 +8708,9 @@
       </c>
       <c r="I122" s="55"/>
       <c r="J122" s="32"/>
-      <c r="K122" s="32"/>
+      <c r="K122" s="32" t="s">
+        <v>1348</v>
+      </c>
       <c r="L122" s="29" t="s">
         <v>1327</v>
       </c>
@@ -8562,7 +8743,9 @@
       </c>
       <c r="I123" s="55"/>
       <c r="J123" s="32"/>
-      <c r="K123" s="32"/>
+      <c r="K123" s="32" t="s">
+        <v>1348</v>
+      </c>
       <c r="L123" s="29" t="s">
         <v>1327</v>
       </c>
@@ -8597,7 +8780,9 @@
       </c>
       <c r="I124" s="55"/>
       <c r="J124" s="32"/>
-      <c r="K124" s="32"/>
+      <c r="K124" s="32" t="s">
+        <v>1348</v>
+      </c>
       <c r="L124" s="29" t="s">
         <v>1327</v>
       </c>
@@ -8632,7 +8817,9 @@
       </c>
       <c r="I125" s="55"/>
       <c r="J125" s="32"/>
-      <c r="K125" s="32"/>
+      <c r="K125" s="32" t="s">
+        <v>1348</v>
+      </c>
       <c r="L125" s="29" t="s">
         <v>1327</v>
       </c>
@@ -8665,7 +8852,9 @@
       </c>
       <c r="I126" s="55"/>
       <c r="J126" s="32"/>
-      <c r="K126" s="32"/>
+      <c r="K126" s="32" t="s">
+        <v>1348</v>
+      </c>
       <c r="L126" s="29" t="s">
         <v>1327</v>
       </c>
@@ -8700,7 +8889,9 @@
       </c>
       <c r="I127" s="55"/>
       <c r="J127" s="32"/>
-      <c r="K127" s="32"/>
+      <c r="K127" s="32" t="s">
+        <v>1348</v>
+      </c>
       <c r="L127" s="29" t="s">
         <v>1327</v>
       </c>
@@ -8737,7 +8928,9 @@
         <v>892</v>
       </c>
       <c r="J128" s="32"/>
-      <c r="K128" s="32"/>
+      <c r="K128" s="32" t="s">
+        <v>1348</v>
+      </c>
       <c r="L128" s="29" t="s">
         <v>1327</v>
       </c>
@@ -8774,7 +8967,9 @@
         <v>892</v>
       </c>
       <c r="J129" s="32"/>
-      <c r="K129" s="32"/>
+      <c r="K129" s="32" t="s">
+        <v>1348</v>
+      </c>
       <c r="L129" s="29" t="s">
         <v>1327</v>
       </c>
@@ -8807,7 +9002,9 @@
       </c>
       <c r="I130" s="55"/>
       <c r="J130" s="32"/>
-      <c r="K130" s="32"/>
+      <c r="K130" s="32" t="s">
+        <v>1348</v>
+      </c>
       <c r="L130" s="29" t="s">
         <v>1327</v>
       </c>
@@ -8840,7 +9037,9 @@
       </c>
       <c r="I131" s="55"/>
       <c r="J131" s="32"/>
-      <c r="K131" s="32"/>
+      <c r="K131" s="32" t="s">
+        <v>1348</v>
+      </c>
       <c r="L131" s="29" t="s">
         <v>1327</v>
       </c>
@@ -8875,7 +9074,9 @@
       </c>
       <c r="I132" s="55"/>
       <c r="J132" s="32"/>
-      <c r="K132" s="32"/>
+      <c r="K132" s="32" t="s">
+        <v>1348</v>
+      </c>
       <c r="L132" s="29" t="s">
         <v>1327</v>
       </c>
@@ -8910,7 +9111,9 @@
       </c>
       <c r="I133" s="55"/>
       <c r="J133" s="32"/>
-      <c r="K133" s="32"/>
+      <c r="K133" s="32" t="s">
+        <v>1348</v>
+      </c>
       <c r="L133" s="29" t="s">
         <v>1327</v>
       </c>
@@ -8943,7 +9146,9 @@
       </c>
       <c r="I134" s="55"/>
       <c r="J134" s="32"/>
-      <c r="K134" s="32"/>
+      <c r="K134" s="32" t="s">
+        <v>1348</v>
+      </c>
       <c r="L134" s="29" t="s">
         <v>1327</v>
       </c>
@@ -8976,7 +9181,9 @@
       </c>
       <c r="I135" s="55"/>
       <c r="J135" s="32"/>
-      <c r="K135" s="32"/>
+      <c r="K135" s="32" t="s">
+        <v>1348</v>
+      </c>
       <c r="L135" s="29" t="s">
         <v>1327</v>
       </c>
@@ -9009,7 +9216,9 @@
       </c>
       <c r="I136" s="55"/>
       <c r="J136" s="32"/>
-      <c r="K136" s="32"/>
+      <c r="K136" s="32" t="s">
+        <v>1348</v>
+      </c>
       <c r="L136" s="29" t="s">
         <v>1327</v>
       </c>
@@ -9042,7 +9251,9 @@
       </c>
       <c r="I137" s="55"/>
       <c r="J137" s="32"/>
-      <c r="K137" s="32"/>
+      <c r="K137" s="32" t="s">
+        <v>1348</v>
+      </c>
       <c r="L137" s="29" t="s">
         <v>1327</v>
       </c>
@@ -9075,7 +9286,9 @@
       </c>
       <c r="I138" s="55"/>
       <c r="J138" s="32"/>
-      <c r="K138" s="32"/>
+      <c r="K138" s="32" t="s">
+        <v>1348</v>
+      </c>
       <c r="L138" s="29" t="s">
         <v>1327</v>
       </c>
@@ -9108,7 +9321,9 @@
       </c>
       <c r="I139" s="55"/>
       <c r="J139" s="32"/>
-      <c r="K139" s="32"/>
+      <c r="K139" s="32" t="s">
+        <v>1348</v>
+      </c>
       <c r="L139" s="29" t="s">
         <v>1327</v>
       </c>
@@ -9143,7 +9358,9 @@
       </c>
       <c r="I140" s="55"/>
       <c r="J140" s="32"/>
-      <c r="K140" s="32"/>
+      <c r="K140" s="32" t="s">
+        <v>1348</v>
+      </c>
       <c r="L140" s="29" t="s">
         <v>1327</v>
       </c>
@@ -9178,7 +9395,9 @@
       </c>
       <c r="I141" s="55"/>
       <c r="J141" s="32"/>
-      <c r="K141" s="32"/>
+      <c r="K141" s="32" t="s">
+        <v>1348</v>
+      </c>
       <c r="L141" s="29" t="s">
         <v>1327</v>
       </c>
@@ -9213,7 +9432,9 @@
       </c>
       <c r="I142" s="55"/>
       <c r="J142" s="32"/>
-      <c r="K142" s="32"/>
+      <c r="K142" s="32" t="s">
+        <v>1348</v>
+      </c>
       <c r="L142" s="29" t="s">
         <v>1327</v>
       </c>
@@ -9248,7 +9469,9 @@
       </c>
       <c r="I143" s="55"/>
       <c r="J143" s="32"/>
-      <c r="K143" s="32"/>
+      <c r="K143" s="32" t="s">
+        <v>1348</v>
+      </c>
       <c r="L143" s="29" t="s">
         <v>1327</v>
       </c>
@@ -9283,7 +9506,9 @@
       </c>
       <c r="I144" s="55"/>
       <c r="J144" s="32"/>
-      <c r="K144" s="32"/>
+      <c r="K144" s="32" t="s">
+        <v>1348</v>
+      </c>
       <c r="L144" s="29" t="s">
         <v>1327</v>
       </c>
@@ -9318,7 +9543,9 @@
       </c>
       <c r="I145" s="55"/>
       <c r="J145" s="32"/>
-      <c r="K145" s="32"/>
+      <c r="K145" s="32" t="s">
+        <v>1348</v>
+      </c>
       <c r="L145" s="29" t="s">
         <v>1327</v>
       </c>
@@ -9353,7 +9580,9 @@
       </c>
       <c r="I146" s="55"/>
       <c r="J146" s="32"/>
-      <c r="K146" s="32"/>
+      <c r="K146" s="32" t="s">
+        <v>1348</v>
+      </c>
       <c r="L146" s="29" t="s">
         <v>1327</v>
       </c>
@@ -9388,7 +9617,9 @@
       </c>
       <c r="I147" s="55"/>
       <c r="J147" s="32"/>
-      <c r="K147" s="32"/>
+      <c r="K147" s="32" t="s">
+        <v>1348</v>
+      </c>
       <c r="L147" s="29" t="s">
         <v>1327</v>
       </c>
@@ -9423,7 +9654,9 @@
       </c>
       <c r="I148" s="55"/>
       <c r="J148" s="32"/>
-      <c r="K148" s="32"/>
+      <c r="K148" s="32" t="s">
+        <v>1348</v>
+      </c>
       <c r="L148" s="29" t="s">
         <v>1327</v>
       </c>
@@ -9458,7 +9691,9 @@
       </c>
       <c r="I149" s="55"/>
       <c r="J149" s="32"/>
-      <c r="K149" s="32"/>
+      <c r="K149" s="32" t="s">
+        <v>1348</v>
+      </c>
       <c r="L149" s="29" t="s">
         <v>1327</v>
       </c>
@@ -9491,7 +9726,9 @@
       </c>
       <c r="I150" s="55"/>
       <c r="J150" s="32"/>
-      <c r="K150" s="32"/>
+      <c r="K150" s="32" t="s">
+        <v>1348</v>
+      </c>
       <c r="L150" s="29" t="s">
         <v>1327</v>
       </c>
@@ -9526,7 +9763,9 @@
       </c>
       <c r="I151" s="55"/>
       <c r="J151" s="32"/>
-      <c r="K151" s="32"/>
+      <c r="K151" s="32" t="s">
+        <v>1348</v>
+      </c>
       <c r="L151" s="29" t="s">
         <v>1327</v>
       </c>
@@ -9561,7 +9800,9 @@
       </c>
       <c r="I152" s="55"/>
       <c r="J152" s="32"/>
-      <c r="K152" s="32"/>
+      <c r="K152" s="32" t="s">
+        <v>1348</v>
+      </c>
       <c r="L152" s="29" t="s">
         <v>1327</v>
       </c>
@@ -9594,7 +9835,9 @@
       </c>
       <c r="I153" s="55"/>
       <c r="J153" s="32"/>
-      <c r="K153" s="32"/>
+      <c r="K153" s="32" t="s">
+        <v>1348</v>
+      </c>
       <c r="L153" s="29" t="s">
         <v>1327</v>
       </c>
@@ -9629,7 +9872,9 @@
       </c>
       <c r="I154" s="55"/>
       <c r="J154" s="32"/>
-      <c r="K154" s="32"/>
+      <c r="K154" s="32" t="s">
+        <v>1348</v>
+      </c>
       <c r="L154" s="29" t="s">
         <v>1327</v>
       </c>
@@ -9664,7 +9909,9 @@
       </c>
       <c r="I155" s="55"/>
       <c r="J155" s="32"/>
-      <c r="K155" s="32"/>
+      <c r="K155" s="32" t="s">
+        <v>1348</v>
+      </c>
       <c r="L155" s="29" t="s">
         <v>1327</v>
       </c>
@@ -9699,7 +9946,9 @@
       </c>
       <c r="I156" s="55"/>
       <c r="J156" s="32"/>
-      <c r="K156" s="32"/>
+      <c r="K156" s="32" t="s">
+        <v>1348</v>
+      </c>
       <c r="L156" s="29" t="s">
         <v>1327</v>
       </c>
@@ -9730,7 +9979,9 @@
       </c>
       <c r="I157" s="56"/>
       <c r="J157" s="32"/>
-      <c r="K157" s="32"/>
+      <c r="K157" s="32" t="s">
+        <v>1348</v>
+      </c>
       <c r="L157" s="29" t="s">
         <v>1327</v>
       </c>
@@ -9763,7 +10014,9 @@
       </c>
       <c r="I158" s="56"/>
       <c r="J158" s="32"/>
-      <c r="K158" s="32"/>
+      <c r="K158" s="32" t="s">
+        <v>1348</v>
+      </c>
       <c r="L158" s="29" t="s">
         <v>1327</v>
       </c>
@@ -9796,7 +10049,9 @@
       </c>
       <c r="I159" s="56"/>
       <c r="J159" s="32"/>
-      <c r="K159" s="32"/>
+      <c r="K159" s="32" t="s">
+        <v>1348</v>
+      </c>
       <c r="L159" s="29" t="s">
         <v>1327</v>
       </c>
@@ -9829,7 +10084,9 @@
       </c>
       <c r="I160" s="56"/>
       <c r="J160" s="32"/>
-      <c r="K160" s="32"/>
+      <c r="K160" s="32" t="s">
+        <v>1348</v>
+      </c>
       <c r="L160" s="29" t="s">
         <v>1327</v>
       </c>
@@ -9864,7 +10121,9 @@
       </c>
       <c r="I161" s="56"/>
       <c r="J161" s="32"/>
-      <c r="K161" s="32"/>
+      <c r="K161" s="32" t="s">
+        <v>1348</v>
+      </c>
       <c r="L161" s="29" t="s">
         <v>1327</v>
       </c>
@@ -9899,7 +10158,9 @@
       </c>
       <c r="I162" s="56"/>
       <c r="J162" s="32"/>
-      <c r="K162" s="32"/>
+      <c r="K162" s="32" t="s">
+        <v>1348</v>
+      </c>
       <c r="L162" s="29" t="s">
         <v>1327</v>
       </c>
@@ -9934,7 +10195,9 @@
       </c>
       <c r="I163" s="56"/>
       <c r="J163" s="32"/>
-      <c r="K163" s="32"/>
+      <c r="K163" s="32" t="s">
+        <v>1348</v>
+      </c>
       <c r="L163" s="29" t="s">
         <v>1327</v>
       </c>
@@ -9969,7 +10232,9 @@
       </c>
       <c r="I164" s="56"/>
       <c r="J164" s="32"/>
-      <c r="K164" s="32"/>
+      <c r="K164" s="32" t="s">
+        <v>1348</v>
+      </c>
       <c r="L164" s="29" t="s">
         <v>1327</v>
       </c>
@@ -10002,7 +10267,9 @@
       </c>
       <c r="I165" s="56"/>
       <c r="J165" s="32"/>
-      <c r="K165" s="32"/>
+      <c r="K165" s="32" t="s">
+        <v>1348</v>
+      </c>
       <c r="L165" s="29" t="s">
         <v>1327</v>
       </c>
@@ -10035,7 +10302,9 @@
       </c>
       <c r="I166" s="56"/>
       <c r="J166" s="32"/>
-      <c r="K166" s="32"/>
+      <c r="K166" s="32" t="s">
+        <v>1348</v>
+      </c>
       <c r="L166" s="29" t="s">
         <v>1327</v>
       </c>
@@ -10066,7 +10335,9 @@
       </c>
       <c r="I167" s="56"/>
       <c r="J167" s="32"/>
-      <c r="K167" s="32"/>
+      <c r="K167" s="32" t="s">
+        <v>1348</v>
+      </c>
       <c r="L167" s="29" t="s">
         <v>1327</v>
       </c>
@@ -10099,7 +10370,9 @@
       </c>
       <c r="I168" s="56"/>
       <c r="J168" s="32"/>
-      <c r="K168" s="32"/>
+      <c r="K168" s="32" t="s">
+        <v>1348</v>
+      </c>
       <c r="L168" s="29" t="s">
         <v>1327</v>
       </c>
@@ -10132,7 +10405,9 @@
       </c>
       <c r="I169" s="56"/>
       <c r="J169" s="32"/>
-      <c r="K169" s="32"/>
+      <c r="K169" s="32" t="s">
+        <v>1348</v>
+      </c>
       <c r="L169" s="29" t="s">
         <v>1327</v>
       </c>
@@ -10163,7 +10438,9 @@
       </c>
       <c r="I170" s="56"/>
       <c r="J170" s="32"/>
-      <c r="K170" s="32"/>
+      <c r="K170" s="32" t="s">
+        <v>1348</v>
+      </c>
       <c r="L170" s="29" t="s">
         <v>1327</v>
       </c>
@@ -10196,7 +10473,9 @@
       </c>
       <c r="I171" s="56"/>
       <c r="J171" s="32"/>
-      <c r="K171" s="32"/>
+      <c r="K171" s="32" t="s">
+        <v>1348</v>
+      </c>
       <c r="L171" s="29" t="s">
         <v>1327</v>
       </c>
@@ -10229,7 +10508,9 @@
       </c>
       <c r="I172" s="57"/>
       <c r="J172" s="12"/>
-      <c r="K172" s="12"/>
+      <c r="K172" s="32" t="s">
+        <v>1348</v>
+      </c>
       <c r="L172" s="29" t="s">
         <v>1327</v>
       </c>
@@ -10262,7 +10543,9 @@
       </c>
       <c r="I173" s="56"/>
       <c r="J173" s="32"/>
-      <c r="K173" s="32"/>
+      <c r="K173" s="32" t="s">
+        <v>1348</v>
+      </c>
       <c r="L173" s="29" t="s">
         <v>1327</v>
       </c>
@@ -10295,7 +10578,9 @@
       </c>
       <c r="I174" s="57"/>
       <c r="J174" s="12"/>
-      <c r="K174" s="12"/>
+      <c r="K174" s="32" t="s">
+        <v>1348</v>
+      </c>
       <c r="L174" s="29" t="s">
         <v>1327</v>
       </c>
@@ -10328,7 +10613,9 @@
       </c>
       <c r="I175" s="56"/>
       <c r="J175" s="32"/>
-      <c r="K175" s="32"/>
+      <c r="K175" s="32" t="s">
+        <v>1348</v>
+      </c>
       <c r="L175" s="29" t="s">
         <v>1327</v>
       </c>
@@ -10361,7 +10648,9 @@
       </c>
       <c r="I176" s="56"/>
       <c r="J176" s="32"/>
-      <c r="K176" s="32"/>
+      <c r="K176" s="32" t="s">
+        <v>1348</v>
+      </c>
       <c r="L176" s="29" t="s">
         <v>1327</v>
       </c>
@@ -10392,7 +10681,9 @@
       </c>
       <c r="I177" s="56"/>
       <c r="J177" s="32"/>
-      <c r="K177" s="32"/>
+      <c r="K177" s="32" t="s">
+        <v>1348</v>
+      </c>
       <c r="L177" s="29" t="s">
         <v>1327</v>
       </c>
@@ -10425,7 +10716,9 @@
       </c>
       <c r="I178" s="56"/>
       <c r="J178" s="32"/>
-      <c r="K178" s="32"/>
+      <c r="K178" s="32" t="s">
+        <v>1348</v>
+      </c>
       <c r="L178" s="29" t="s">
         <v>1327</v>
       </c>
@@ -10458,7 +10751,9 @@
       </c>
       <c r="I179" s="56"/>
       <c r="J179" s="32"/>
-      <c r="K179" s="32"/>
+      <c r="K179" s="32" t="s">
+        <v>1348</v>
+      </c>
       <c r="L179" s="29" t="s">
         <v>1327</v>
       </c>
@@ -10491,7 +10786,9 @@
       </c>
       <c r="I180" s="56"/>
       <c r="J180" s="32"/>
-      <c r="K180" s="32"/>
+      <c r="K180" s="32" t="s">
+        <v>1348</v>
+      </c>
       <c r="L180" s="29" t="s">
         <v>1327</v>
       </c>
@@ -10524,7 +10821,9 @@
       </c>
       <c r="I181" s="56"/>
       <c r="J181" s="32"/>
-      <c r="K181" s="32"/>
+      <c r="K181" s="32" t="s">
+        <v>1348</v>
+      </c>
       <c r="L181" s="29" t="s">
         <v>1327</v>
       </c>
@@ -10559,7 +10858,9 @@
       </c>
       <c r="I182" s="56"/>
       <c r="J182" s="32"/>
-      <c r="K182" s="32"/>
+      <c r="K182" s="32" t="s">
+        <v>1348</v>
+      </c>
       <c r="L182" s="29" t="s">
         <v>1327</v>
       </c>
@@ -10594,7 +10895,9 @@
       </c>
       <c r="I183" s="56"/>
       <c r="J183" s="32"/>
-      <c r="K183" s="32"/>
+      <c r="K183" s="32" t="s">
+        <v>1348</v>
+      </c>
       <c r="L183" s="29" t="s">
         <v>1327</v>
       </c>
@@ -10625,7 +10928,9 @@
       </c>
       <c r="I184" s="56"/>
       <c r="J184" s="32"/>
-      <c r="K184" s="32"/>
+      <c r="K184" s="32" t="s">
+        <v>1348</v>
+      </c>
       <c r="L184" s="29" t="s">
         <v>1327</v>
       </c>
@@ -10658,7 +10963,9 @@
       </c>
       <c r="I185" s="56"/>
       <c r="J185" s="32"/>
-      <c r="K185" s="32"/>
+      <c r="K185" s="32" t="s">
+        <v>1348</v>
+      </c>
       <c r="L185" s="29" t="s">
         <v>1327</v>
       </c>
@@ -10691,7 +10998,9 @@
       </c>
       <c r="I186" s="56"/>
       <c r="J186" s="32"/>
-      <c r="K186" s="32"/>
+      <c r="K186" s="32" t="s">
+        <v>1348</v>
+      </c>
       <c r="L186" s="29" t="s">
         <v>1327</v>
       </c>
@@ -10724,7 +11033,9 @@
       </c>
       <c r="I187" s="56"/>
       <c r="J187" s="32"/>
-      <c r="K187" s="32"/>
+      <c r="K187" s="32" t="s">
+        <v>1348</v>
+      </c>
       <c r="L187" s="29" t="s">
         <v>1327</v>
       </c>
@@ -10757,7 +11068,9 @@
       </c>
       <c r="I188" s="56"/>
       <c r="J188" s="32"/>
-      <c r="K188" s="32"/>
+      <c r="K188" s="32" t="s">
+        <v>1348</v>
+      </c>
       <c r="L188" s="29" t="s">
         <v>1327</v>
       </c>
@@ -10790,7 +11103,9 @@
       </c>
       <c r="I189" s="56"/>
       <c r="J189" s="32"/>
-      <c r="K189" s="32"/>
+      <c r="K189" s="32" t="s">
+        <v>1348</v>
+      </c>
       <c r="L189" s="29" t="s">
         <v>1327</v>
       </c>
@@ -10823,7 +11138,9 @@
       </c>
       <c r="I190" s="56"/>
       <c r="J190" s="32"/>
-      <c r="K190" s="32"/>
+      <c r="K190" s="32" t="s">
+        <v>1348</v>
+      </c>
       <c r="L190" s="29" t="s">
         <v>1327</v>
       </c>
@@ -10856,7 +11173,9 @@
       </c>
       <c r="I191" s="56"/>
       <c r="J191" s="32"/>
-      <c r="K191" s="32"/>
+      <c r="K191" s="32" t="s">
+        <v>1348</v>
+      </c>
       <c r="L191" s="29" t="s">
         <v>1327</v>
       </c>
@@ -10889,7 +11208,9 @@
       </c>
       <c r="I192" s="56"/>
       <c r="J192" s="32"/>
-      <c r="K192" s="32"/>
+      <c r="K192" s="32" t="s">
+        <v>1348</v>
+      </c>
       <c r="L192" s="29" t="s">
         <v>1327</v>
       </c>
@@ -10922,7 +11243,9 @@
       </c>
       <c r="I193" s="56"/>
       <c r="J193" s="32"/>
-      <c r="K193" s="32"/>
+      <c r="K193" s="32" t="s">
+        <v>1348</v>
+      </c>
       <c r="L193" s="29" t="s">
         <v>1327</v>
       </c>
@@ -10959,7 +11282,9 @@
         <v>124</v>
       </c>
       <c r="J194" s="32"/>
-      <c r="K194" s="32"/>
+      <c r="K194" s="32" t="s">
+        <v>1348</v>
+      </c>
       <c r="L194" s="29" t="s">
         <v>1327</v>
       </c>
@@ -10996,7 +11321,9 @@
         <v>124</v>
       </c>
       <c r="J195" s="32"/>
-      <c r="K195" s="32"/>
+      <c r="K195" s="32" t="s">
+        <v>1348</v>
+      </c>
       <c r="L195" s="29" t="s">
         <v>1327</v>
       </c>
@@ -11029,7 +11356,9 @@
       </c>
       <c r="I196" s="56"/>
       <c r="J196" s="32"/>
-      <c r="K196" s="32"/>
+      <c r="K196" s="32" t="s">
+        <v>1348</v>
+      </c>
       <c r="L196" s="29" t="s">
         <v>1327</v>
       </c>
@@ -11062,7 +11391,9 @@
       </c>
       <c r="I197" s="56"/>
       <c r="J197" s="32"/>
-      <c r="K197" s="32"/>
+      <c r="K197" s="32" t="s">
+        <v>1348</v>
+      </c>
       <c r="L197" s="29" t="s">
         <v>1327</v>
       </c>
@@ -11095,7 +11426,9 @@
       </c>
       <c r="I198" s="56"/>
       <c r="J198" s="32"/>
-      <c r="K198" s="32"/>
+      <c r="K198" s="32" t="s">
+        <v>1348</v>
+      </c>
       <c r="L198" s="29" t="s">
         <v>1327</v>
       </c>
@@ -11128,7 +11461,9 @@
       </c>
       <c r="I199" s="56"/>
       <c r="J199" s="32"/>
-      <c r="K199" s="32"/>
+      <c r="K199" s="32" t="s">
+        <v>1348</v>
+      </c>
       <c r="L199" s="29" t="s">
         <v>1327</v>
       </c>
@@ -11161,7 +11496,9 @@
       </c>
       <c r="I200" s="56"/>
       <c r="J200" s="32"/>
-      <c r="K200" s="32"/>
+      <c r="K200" s="32" t="s">
+        <v>1348</v>
+      </c>
       <c r="L200" s="29" t="s">
         <v>1327</v>
       </c>
@@ -11198,7 +11535,9 @@
         <v>148</v>
       </c>
       <c r="J201" s="32"/>
-      <c r="K201" s="32"/>
+      <c r="K201" s="32" t="s">
+        <v>1348</v>
+      </c>
       <c r="L201" s="29" t="s">
         <v>1327</v>
       </c>
@@ -11235,7 +11574,9 @@
         <v>148</v>
       </c>
       <c r="J202" s="32"/>
-      <c r="K202" s="32"/>
+      <c r="K202" s="32" t="s">
+        <v>1348</v>
+      </c>
       <c r="L202" s="29" t="s">
         <v>1327</v>
       </c>
@@ -11268,7 +11609,9 @@
       </c>
       <c r="I203" s="56"/>
       <c r="J203" s="32"/>
-      <c r="K203" s="32"/>
+      <c r="K203" s="32" t="s">
+        <v>1348</v>
+      </c>
       <c r="L203" s="29" t="s">
         <v>1327</v>
       </c>
@@ -11305,7 +11648,9 @@
         <v>160</v>
       </c>
       <c r="J204" s="32"/>
-      <c r="K204" s="32"/>
+      <c r="K204" s="32" t="s">
+        <v>1348</v>
+      </c>
       <c r="L204" s="29" t="s">
         <v>1327</v>
       </c>
@@ -11342,7 +11687,9 @@
         <v>160</v>
       </c>
       <c r="J205" s="32"/>
-      <c r="K205" s="32"/>
+      <c r="K205" s="32" t="s">
+        <v>1348</v>
+      </c>
       <c r="L205" s="29" t="s">
         <v>1327</v>
       </c>
@@ -11375,7 +11722,9 @@
       </c>
       <c r="I206" s="56"/>
       <c r="J206" s="32"/>
-      <c r="K206" s="32"/>
+      <c r="K206" s="32" t="s">
+        <v>1348</v>
+      </c>
       <c r="L206" s="29" t="s">
         <v>1327</v>
       </c>
@@ -11406,7 +11755,9 @@
       </c>
       <c r="I207" s="56"/>
       <c r="J207" s="32"/>
-      <c r="K207" s="32"/>
+      <c r="K207" s="32" t="s">
+        <v>1348</v>
+      </c>
       <c r="L207" s="29" t="s">
         <v>1327</v>
       </c>
@@ -11439,7 +11790,9 @@
       </c>
       <c r="I208" s="56"/>
       <c r="J208" s="32"/>
-      <c r="K208" s="32"/>
+      <c r="K208" s="32" t="s">
+        <v>1348</v>
+      </c>
       <c r="L208" s="29" t="s">
         <v>1327</v>
       </c>
@@ -11472,7 +11825,9 @@
       </c>
       <c r="I209" s="56"/>
       <c r="J209" s="32"/>
-      <c r="K209" s="32"/>
+      <c r="K209" s="32" t="s">
+        <v>1348</v>
+      </c>
       <c r="L209" s="29" t="s">
         <v>1327</v>
       </c>
@@ -11505,7 +11860,9 @@
       </c>
       <c r="I210" s="56"/>
       <c r="J210" s="32"/>
-      <c r="K210" s="32"/>
+      <c r="K210" s="32" t="s">
+        <v>1348</v>
+      </c>
       <c r="L210" s="29" t="s">
         <v>1327</v>
       </c>
@@ -11538,7 +11895,9 @@
       </c>
       <c r="I211" s="56"/>
       <c r="J211" s="32"/>
-      <c r="K211" s="32"/>
+      <c r="K211" s="32" t="s">
+        <v>1348</v>
+      </c>
       <c r="L211" s="29" t="s">
         <v>1327</v>
       </c>
@@ -11571,7 +11930,9 @@
       </c>
       <c r="I212" s="56"/>
       <c r="J212" s="32"/>
-      <c r="K212" s="32"/>
+      <c r="K212" s="32" t="s">
+        <v>1348</v>
+      </c>
       <c r="L212" s="29" t="s">
         <v>1327</v>
       </c>
@@ -11604,7 +11965,9 @@
       </c>
       <c r="I213" s="56"/>
       <c r="J213" s="32"/>
-      <c r="K213" s="32"/>
+      <c r="K213" s="32" t="s">
+        <v>1348</v>
+      </c>
       <c r="L213" s="29" t="s">
         <v>1327</v>
       </c>
@@ -11637,7 +12000,9 @@
       </c>
       <c r="I214" s="56"/>
       <c r="J214" s="32"/>
-      <c r="K214" s="32"/>
+      <c r="K214" s="32" t="s">
+        <v>1348</v>
+      </c>
       <c r="L214" s="29" t="s">
         <v>1327</v>
       </c>
@@ -11670,7 +12035,9 @@
       </c>
       <c r="I215" s="56"/>
       <c r="J215" s="32"/>
-      <c r="K215" s="32"/>
+      <c r="K215" s="32" t="s">
+        <v>1348</v>
+      </c>
       <c r="L215" s="29" t="s">
         <v>1327</v>
       </c>
@@ -11703,7 +12070,9 @@
       </c>
       <c r="I216" s="56"/>
       <c r="J216" s="32"/>
-      <c r="K216" s="32"/>
+      <c r="K216" s="32" t="s">
+        <v>1348</v>
+      </c>
       <c r="L216" s="29" t="s">
         <v>1327</v>
       </c>
@@ -11736,7 +12105,9 @@
       </c>
       <c r="I217" s="56"/>
       <c r="J217" s="32"/>
-      <c r="K217" s="32"/>
+      <c r="K217" s="32" t="s">
+        <v>1348</v>
+      </c>
       <c r="L217" s="29" t="s">
         <v>1327</v>
       </c>
@@ -11769,7 +12140,9 @@
       </c>
       <c r="I218" s="56"/>
       <c r="J218" s="32"/>
-      <c r="K218" s="32"/>
+      <c r="K218" s="32" t="s">
+        <v>1348</v>
+      </c>
       <c r="L218" s="29" t="s">
         <v>1327</v>
       </c>
@@ -11802,7 +12175,9 @@
       </c>
       <c r="I219" s="56"/>
       <c r="J219" s="32"/>
-      <c r="K219" s="32"/>
+      <c r="K219" s="32" t="s">
+        <v>1348</v>
+      </c>
       <c r="L219" s="29" t="s">
         <v>1327</v>
       </c>
@@ -11835,7 +12210,9 @@
       </c>
       <c r="I220" s="56"/>
       <c r="J220" s="32"/>
-      <c r="K220" s="32"/>
+      <c r="K220" s="32" t="s">
+        <v>1348</v>
+      </c>
       <c r="L220" s="29" t="s">
         <v>1327</v>
       </c>
@@ -11868,7 +12245,9 @@
       </c>
       <c r="I221" s="56"/>
       <c r="J221" s="32"/>
-      <c r="K221" s="32"/>
+      <c r="K221" s="32" t="s">
+        <v>1348</v>
+      </c>
       <c r="L221" s="29" t="s">
         <v>1327</v>
       </c>
@@ -11901,7 +12280,9 @@
       </c>
       <c r="I222" s="56"/>
       <c r="J222" s="32"/>
-      <c r="K222" s="32"/>
+      <c r="K222" s="32" t="s">
+        <v>1348</v>
+      </c>
       <c r="L222" s="29" t="s">
         <v>1327</v>
       </c>
@@ -11934,7 +12315,9 @@
       </c>
       <c r="I223" s="56"/>
       <c r="J223" s="32"/>
-      <c r="K223" s="32"/>
+      <c r="K223" s="32" t="s">
+        <v>1348</v>
+      </c>
       <c r="L223" s="29" t="s">
         <v>1327</v>
       </c>
@@ -11967,7 +12350,9 @@
       </c>
       <c r="I224" s="56"/>
       <c r="J224" s="32"/>
-      <c r="K224" s="32"/>
+      <c r="K224" s="32" t="s">
+        <v>1348</v>
+      </c>
       <c r="L224" s="29" t="s">
         <v>1327</v>
       </c>
@@ -12000,7 +12385,9 @@
       </c>
       <c r="I225" s="56"/>
       <c r="J225" s="32"/>
-      <c r="K225" s="32"/>
+      <c r="K225" s="32" t="s">
+        <v>1348</v>
+      </c>
       <c r="L225" s="29" t="s">
         <v>1327</v>
       </c>
@@ -12033,7 +12420,9 @@
       </c>
       <c r="I226" s="56"/>
       <c r="J226" s="32"/>
-      <c r="K226" s="32"/>
+      <c r="K226" s="32" t="s">
+        <v>1348</v>
+      </c>
       <c r="L226" s="29" t="s">
         <v>1327</v>
       </c>
@@ -12066,7 +12455,9 @@
       </c>
       <c r="I227" s="56"/>
       <c r="J227" s="32"/>
-      <c r="K227" s="32"/>
+      <c r="K227" s="32" t="s">
+        <v>1348</v>
+      </c>
       <c r="L227" s="29" t="s">
         <v>1327</v>
       </c>
@@ -12099,7 +12490,9 @@
       </c>
       <c r="I228" s="56"/>
       <c r="J228" s="32"/>
-      <c r="K228" s="32"/>
+      <c r="K228" s="32" t="s">
+        <v>1348</v>
+      </c>
       <c r="L228" s="29" t="s">
         <v>1327</v>
       </c>
@@ -12132,7 +12525,9 @@
       </c>
       <c r="I229" s="56"/>
       <c r="J229" s="32"/>
-      <c r="K229" s="32"/>
+      <c r="K229" s="32" t="s">
+        <v>1348</v>
+      </c>
       <c r="L229" s="29" t="s">
         <v>1327</v>
       </c>
@@ -12165,7 +12560,9 @@
       </c>
       <c r="I230" s="56"/>
       <c r="J230" s="32"/>
-      <c r="K230" s="32"/>
+      <c r="K230" s="32" t="s">
+        <v>1348</v>
+      </c>
       <c r="L230" s="29" t="s">
         <v>1327</v>
       </c>
@@ -12198,7 +12595,9 @@
       </c>
       <c r="I231" s="56"/>
       <c r="J231" s="32"/>
-      <c r="K231" s="32"/>
+      <c r="K231" s="32" t="s">
+        <v>1348</v>
+      </c>
       <c r="L231" s="29" t="s">
         <v>1327</v>
       </c>
@@ -12231,7 +12630,9 @@
       </c>
       <c r="I232" s="56"/>
       <c r="J232" s="32"/>
-      <c r="K232" s="32"/>
+      <c r="K232" s="32" t="s">
+        <v>1348</v>
+      </c>
       <c r="L232" s="29" t="s">
         <v>1327</v>
       </c>
@@ -12264,7 +12665,9 @@
       </c>
       <c r="I233" s="56"/>
       <c r="J233" s="32"/>
-      <c r="K233" s="32"/>
+      <c r="K233" s="32" t="s">
+        <v>1348</v>
+      </c>
       <c r="L233" s="29" t="s">
         <v>1327</v>
       </c>
@@ -12297,7 +12700,9 @@
       </c>
       <c r="I234" s="56"/>
       <c r="J234" s="32"/>
-      <c r="K234" s="32"/>
+      <c r="K234" s="32" t="s">
+        <v>1348</v>
+      </c>
       <c r="L234" s="29" t="s">
         <v>1327</v>
       </c>
@@ -12330,7 +12735,9 @@
       </c>
       <c r="I235" s="56"/>
       <c r="J235" s="32"/>
-      <c r="K235" s="32"/>
+      <c r="K235" s="32" t="s">
+        <v>1348</v>
+      </c>
       <c r="L235" s="29" t="s">
         <v>1327</v>
       </c>
@@ -12363,7 +12770,9 @@
       </c>
       <c r="I236" s="56"/>
       <c r="J236" s="32"/>
-      <c r="K236" s="32"/>
+      <c r="K236" s="32" t="s">
+        <v>1348</v>
+      </c>
       <c r="L236" s="29" t="s">
         <v>1327</v>
       </c>
@@ -12394,7 +12803,9 @@
       </c>
       <c r="I237" s="56"/>
       <c r="J237" s="32"/>
-      <c r="K237" s="32"/>
+      <c r="K237" s="32" t="s">
+        <v>1348</v>
+      </c>
       <c r="L237" s="29" t="s">
         <v>1327</v>
       </c>
@@ -12427,7 +12838,9 @@
       </c>
       <c r="I238" s="56"/>
       <c r="J238" s="32"/>
-      <c r="K238" s="32"/>
+      <c r="K238" s="32" t="s">
+        <v>1348</v>
+      </c>
       <c r="L238" s="29" t="s">
         <v>1327</v>
       </c>
@@ -12460,7 +12873,9 @@
       </c>
       <c r="I239" s="56"/>
       <c r="J239" s="32"/>
-      <c r="K239" s="32"/>
+      <c r="K239" s="32" t="s">
+        <v>1348</v>
+      </c>
       <c r="L239" s="29" t="s">
         <v>1327</v>
       </c>
@@ -12493,7 +12908,9 @@
       </c>
       <c r="I240" s="56"/>
       <c r="J240" s="32"/>
-      <c r="K240" s="32"/>
+      <c r="K240" s="32" t="s">
+        <v>1348</v>
+      </c>
       <c r="L240" s="29" t="s">
         <v>1327</v>
       </c>
@@ -12526,7 +12943,9 @@
       </c>
       <c r="I241" s="56"/>
       <c r="J241" s="32"/>
-      <c r="K241" s="32"/>
+      <c r="K241" s="32" t="s">
+        <v>1348</v>
+      </c>
       <c r="L241" s="29" t="s">
         <v>1327</v>
       </c>
@@ -12557,7 +12976,9 @@
       </c>
       <c r="I242" s="56"/>
       <c r="J242" s="32"/>
-      <c r="K242" s="32"/>
+      <c r="K242" s="32" t="s">
+        <v>1348</v>
+      </c>
       <c r="L242" s="29" t="s">
         <v>1327</v>
       </c>
@@ -12590,7 +13011,9 @@
       </c>
       <c r="I243" s="56"/>
       <c r="J243" s="32"/>
-      <c r="K243" s="32"/>
+      <c r="K243" s="32" t="s">
+        <v>1348</v>
+      </c>
       <c r="L243" s="29" t="s">
         <v>1327</v>
       </c>
@@ -12623,7 +13046,9 @@
       </c>
       <c r="I244" s="56"/>
       <c r="J244" s="32"/>
-      <c r="K244" s="32"/>
+      <c r="K244" s="32" t="s">
+        <v>1348</v>
+      </c>
       <c r="L244" s="29" t="s">
         <v>1327</v>
       </c>
@@ -12656,7 +13081,9 @@
       </c>
       <c r="I245" s="56"/>
       <c r="J245" s="32"/>
-      <c r="K245" s="32"/>
+      <c r="K245" s="32" t="s">
+        <v>1348</v>
+      </c>
       <c r="L245" s="29" t="s">
         <v>1327</v>
       </c>
@@ -12689,7 +13116,9 @@
       </c>
       <c r="I246" s="56"/>
       <c r="J246" s="32"/>
-      <c r="K246" s="32"/>
+      <c r="K246" s="32" t="s">
+        <v>1348</v>
+      </c>
       <c r="L246" s="29" t="s">
         <v>1327</v>
       </c>
@@ -12722,7 +13151,9 @@
       </c>
       <c r="I247" s="56"/>
       <c r="J247" s="32"/>
-      <c r="K247" s="32"/>
+      <c r="K247" s="32" t="s">
+        <v>1348</v>
+      </c>
       <c r="L247" s="29" t="s">
         <v>1327</v>
       </c>
@@ -12753,7 +13184,9 @@
       </c>
       <c r="I248" s="56"/>
       <c r="J248" s="32"/>
-      <c r="K248" s="32"/>
+      <c r="K248" s="32" t="s">
+        <v>1348</v>
+      </c>
       <c r="L248" s="29" t="s">
         <v>1327</v>
       </c>
@@ -12786,7 +13219,9 @@
       </c>
       <c r="I249" s="56"/>
       <c r="J249" s="32"/>
-      <c r="K249" s="32"/>
+      <c r="K249" s="32" t="s">
+        <v>1348</v>
+      </c>
       <c r="L249" s="29" t="s">
         <v>1327</v>
       </c>
@@ -12819,7 +13254,9 @@
       </c>
       <c r="I250" s="56"/>
       <c r="J250" s="32"/>
-      <c r="K250" s="32"/>
+      <c r="K250" s="32" t="s">
+        <v>1348</v>
+      </c>
       <c r="L250" s="29" t="s">
         <v>1327</v>
       </c>
@@ -12852,7 +13289,9 @@
       </c>
       <c r="I251" s="56"/>
       <c r="J251" s="32"/>
-      <c r="K251" s="32"/>
+      <c r="K251" s="32" t="s">
+        <v>1348</v>
+      </c>
       <c r="L251" s="29" t="s">
         <v>1327</v>
       </c>
@@ -12885,7 +13324,9 @@
       </c>
       <c r="I252" s="56"/>
       <c r="J252" s="32"/>
-      <c r="K252" s="32"/>
+      <c r="K252" s="32" t="s">
+        <v>1348</v>
+      </c>
       <c r="L252" s="29" t="s">
         <v>1327</v>
       </c>
@@ -12918,7 +13359,9 @@
       </c>
       <c r="I253" s="56"/>
       <c r="J253" s="32"/>
-      <c r="K253" s="32"/>
+      <c r="K253" s="32" t="s">
+        <v>1348</v>
+      </c>
       <c r="L253" s="29" t="s">
         <v>1327</v>
       </c>
@@ -12951,7 +13394,9 @@
       </c>
       <c r="I254" s="56"/>
       <c r="J254" s="32"/>
-      <c r="K254" s="32"/>
+      <c r="K254" s="32" t="s">
+        <v>1348</v>
+      </c>
       <c r="L254" s="29" t="s">
         <v>1327</v>
       </c>
@@ -12986,7 +13431,9 @@
       </c>
       <c r="I255" s="56"/>
       <c r="J255" s="32"/>
-      <c r="K255" s="32"/>
+      <c r="K255" s="32" t="s">
+        <v>1348</v>
+      </c>
       <c r="L255" s="29" t="s">
         <v>1327</v>
       </c>
@@ -13021,7 +13468,9 @@
       </c>
       <c r="I256" s="56"/>
       <c r="J256" s="32"/>
-      <c r="K256" s="32"/>
+      <c r="K256" s="32" t="s">
+        <v>1348</v>
+      </c>
       <c r="L256" s="29" t="s">
         <v>1327</v>
       </c>
@@ -13054,7 +13503,9 @@
       </c>
       <c r="I257" s="56"/>
       <c r="J257" s="32"/>
-      <c r="K257" s="32"/>
+      <c r="K257" s="32" t="s">
+        <v>1348</v>
+      </c>
       <c r="L257" s="29" t="s">
         <v>1327</v>
       </c>
@@ -13085,7 +13536,9 @@
       </c>
       <c r="I258" s="56"/>
       <c r="J258" s="32"/>
-      <c r="K258" s="32"/>
+      <c r="K258" s="32" t="s">
+        <v>1348</v>
+      </c>
       <c r="L258" s="29" t="s">
         <v>1327</v>
       </c>
@@ -13118,7 +13571,9 @@
       </c>
       <c r="I259" s="56"/>
       <c r="J259" s="32"/>
-      <c r="K259" s="32"/>
+      <c r="K259" s="32" t="s">
+        <v>1348</v>
+      </c>
       <c r="L259" s="29" t="s">
         <v>1327</v>
       </c>
@@ -13151,7 +13606,9 @@
       </c>
       <c r="I260" s="56"/>
       <c r="J260" s="32"/>
-      <c r="K260" s="32"/>
+      <c r="K260" s="32" t="s">
+        <v>1348</v>
+      </c>
       <c r="L260" s="29" t="s">
         <v>1327</v>
       </c>
@@ -13186,7 +13643,9 @@
       </c>
       <c r="I261" s="56"/>
       <c r="J261" s="32"/>
-      <c r="K261" s="32"/>
+      <c r="K261" s="32" t="s">
+        <v>1348</v>
+      </c>
       <c r="L261" s="29" t="s">
         <v>1327</v>
       </c>
@@ -13221,7 +13680,9 @@
       </c>
       <c r="I262" s="56"/>
       <c r="J262" s="32"/>
-      <c r="K262" s="32"/>
+      <c r="K262" s="32" t="s">
+        <v>1348</v>
+      </c>
       <c r="L262" s="29" t="s">
         <v>1327</v>
       </c>
@@ -13254,7 +13715,9 @@
       </c>
       <c r="I263" s="56"/>
       <c r="J263" s="32"/>
-      <c r="K263" s="32"/>
+      <c r="K263" s="32" t="s">
+        <v>1348</v>
+      </c>
       <c r="L263" s="29" t="s">
         <v>1327</v>
       </c>
@@ -13287,7 +13750,9 @@
       </c>
       <c r="I264" s="56"/>
       <c r="J264" s="32"/>
-      <c r="K264" s="32"/>
+      <c r="K264" s="32" t="s">
+        <v>1348</v>
+      </c>
       <c r="L264" s="29" t="s">
         <v>1327</v>
       </c>
@@ -13318,7 +13783,9 @@
       </c>
       <c r="I265" s="56"/>
       <c r="J265" s="32"/>
-      <c r="K265" s="32"/>
+      <c r="K265" s="32" t="s">
+        <v>1348</v>
+      </c>
       <c r="L265" s="29" t="s">
         <v>1327</v>
       </c>
@@ -13351,7 +13818,9 @@
       </c>
       <c r="I266" s="56"/>
       <c r="J266" s="32"/>
-      <c r="K266" s="32"/>
+      <c r="K266" s="32" t="s">
+        <v>1348</v>
+      </c>
       <c r="L266" s="29" t="s">
         <v>1327</v>
       </c>
@@ -13384,7 +13853,9 @@
       </c>
       <c r="I267" s="56"/>
       <c r="J267" s="32"/>
-      <c r="K267" s="32"/>
+      <c r="K267" s="32" t="s">
+        <v>1348</v>
+      </c>
       <c r="L267" s="29" t="s">
         <v>1327</v>
       </c>
@@ -13417,7 +13888,9 @@
       </c>
       <c r="I268" s="56"/>
       <c r="J268" s="32"/>
-      <c r="K268" s="32"/>
+      <c r="K268" s="32" t="s">
+        <v>1348</v>
+      </c>
       <c r="L268" s="29" t="s">
         <v>1327</v>
       </c>
@@ -13450,7 +13923,9 @@
       </c>
       <c r="I269" s="56"/>
       <c r="J269" s="32"/>
-      <c r="K269" s="32"/>
+      <c r="K269" s="32" t="s">
+        <v>1348</v>
+      </c>
       <c r="L269" s="29" t="s">
         <v>1327</v>
       </c>
@@ -13483,7 +13958,9 @@
       </c>
       <c r="I270" s="56"/>
       <c r="J270" s="32"/>
-      <c r="K270" s="32"/>
+      <c r="K270" s="32" t="s">
+        <v>1348</v>
+      </c>
       <c r="L270" s="29" t="s">
         <v>1327</v>
       </c>
@@ -13516,7 +13993,9 @@
       </c>
       <c r="I271" s="56"/>
       <c r="J271" s="32"/>
-      <c r="K271" s="32"/>
+      <c r="K271" s="32" t="s">
+        <v>1348</v>
+      </c>
       <c r="L271" s="29" t="s">
         <v>1327</v>
       </c>
@@ -13549,7 +14028,9 @@
       </c>
       <c r="I272" s="56"/>
       <c r="J272" s="32"/>
-      <c r="K272" s="32"/>
+      <c r="K272" s="32" t="s">
+        <v>1348</v>
+      </c>
       <c r="L272" s="29" t="s">
         <v>1327</v>
       </c>
@@ -13582,7 +14063,9 @@
       </c>
       <c r="I273" s="56"/>
       <c r="J273" s="32"/>
-      <c r="K273" s="32"/>
+      <c r="K273" s="32" t="s">
+        <v>1348</v>
+      </c>
       <c r="L273" s="29" t="s">
         <v>1327</v>
       </c>
@@ -13615,7 +14098,9 @@
       </c>
       <c r="I274" s="56"/>
       <c r="J274" s="32"/>
-      <c r="K274" s="32"/>
+      <c r="K274" s="32" t="s">
+        <v>1348</v>
+      </c>
       <c r="L274" s="29" t="s">
         <v>1327</v>
       </c>
@@ -13648,7 +14133,9 @@
       </c>
       <c r="I275" s="56"/>
       <c r="J275" s="32"/>
-      <c r="K275" s="32"/>
+      <c r="K275" s="32" t="s">
+        <v>1348</v>
+      </c>
       <c r="L275" s="29" t="s">
         <v>1327</v>
       </c>
@@ -13681,7 +14168,9 @@
       </c>
       <c r="I276" s="56"/>
       <c r="J276" s="32"/>
-      <c r="K276" s="32"/>
+      <c r="K276" s="32" t="s">
+        <v>1348</v>
+      </c>
       <c r="L276" s="29" t="s">
         <v>1327</v>
       </c>
@@ -13714,7 +14203,9 @@
       </c>
       <c r="I277" s="56"/>
       <c r="J277" s="32"/>
-      <c r="K277" s="32"/>
+      <c r="K277" s="32" t="s">
+        <v>1348</v>
+      </c>
       <c r="L277" s="29" t="s">
         <v>1327</v>
       </c>
@@ -14283,8 +14774,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4A25E589-C762-47F7-A5B5-46A66BE90C97}">
   <dimension ref="A1:L466"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B12" sqref="B12"/>
+    <sheetView topLeftCell="F22" workbookViewId="0">
+      <selection activeCell="J38" sqref="J38"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
notes and references added to skos:related
</commit_message>
<xml_diff>
--- a/rdf/skosplay-scma-2.xlsx
+++ b/rdf/skosplay-scma-2.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://federationuniversity-my.sharepoint.com/personal/mr_wong_federation_edu_au/Documents/Documents/GitHub/def-au-scma/rdf/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="115" documentId="13_ncr:1_{280EA38A-AAE3-4033-A57D-27CDA991092C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{D711240B-6556-4268-AD2D-63F73FFC9EB8}"/>
+  <xr:revisionPtr revIDLastSave="178" documentId="13_ncr:1_{280EA38A-AAE3-4033-A57D-27CDA991092C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{649CD134-A3DD-4BBF-9B0C-216EC9F0107F}"/>
   <bookViews>
-    <workbookView xWindow="6135" yWindow="-120" windowWidth="18000" windowHeight="9360" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="24240" windowHeight="13140" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="SCMA-2011" sheetId="2" r:id="rId1"/>
@@ -103,7 +103,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4359" uniqueCount="1349">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4359" uniqueCount="1367">
   <si>
     <t>ConceptScheme URI</t>
   </si>
@@ -4196,7 +4196,61 @@
     <t>Australian soil and land survey handbooks ; v. 3.</t>
   </si>
   <si>
-    <t>https://raw.githack.com/ANZSoilData/def-au-scma/master/html/90backmatter/91results01.html, https://raw.githack.com/ANZSoilData/def-au-scma/master/html/90backmatter/92accuracyandprecision02.html, https://raw.githack.com/ANZSoilData/def-au-scma/master/html/90backmatter/93acids03.html, https://raw.githack.com/ANZSoilData/def-au-scma/master/html/90backmatter/94atomicweights04.html, https://raw.githack.com/ANZSoilData/def-au-scma/master/html/90backmatter/95Unitsr05.html</t>
+    <t>https://raw.githack.com/ANZSoilData/def-au-scma/master/html/02/02notes.html, https://raw.githack.com/ANZSoilData/def-au-scma/master/html/02/02refs.html, https://raw.githack.com/ANZSoilData/def-au-scma/master/html/90backmatter/91results01.html, https://raw.githack.com/ANZSoilData/def-au-scma/master/html/90backmatter/92accuracyandprecision02.html, https://raw.githack.com/ANZSoilData/def-au-scma/master/html/90backmatter/93acids03.html, https://raw.githack.com/ANZSoilData/def-au-scma/master/html/90backmatter/94atomicweights04.html, https://raw.githack.com/ANZSoilData/def-au-scma/master/html/90backmatter/95Unitsr05.html</t>
+  </si>
+  <si>
+    <t>https://raw.githack.com/ANZSoilData/def-au-scma/master/html/03/03notes.html, https://raw.githack.com/ANZSoilData/def-au-scma/master/html/03/03refs.html, https://raw.githack.com/ANZSoilData/def-au-scma/master/html/90backmatter/91results01.html, https://raw.githack.com/ANZSoilData/def-au-scma/master/html/90backmatter/92accuracyandprecision02.html, https://raw.githack.com/ANZSoilData/def-au-scma/master/html/90backmatter/93acids03.html, https://raw.githack.com/ANZSoilData/def-au-scma/master/html/90backmatter/94atomicweights04.html, https://raw.githack.com/ANZSoilData/def-au-scma/master/html/90backmatter/95Unitsr05.html</t>
+  </si>
+  <si>
+    <t>https://raw.githack.com/ANZSoilData/def-au-scma/master/html/04-pH/04references.html, https://raw.githack.com/ANZSoilData/def-au-scma/master/html/90backmatter/91results01.html, https://raw.githack.com/ANZSoilData/def-au-scma/master/html/90backmatter/92accuracyandprecision02.html, https://raw.githack.com/ANZSoilData/def-au-scma/master/html/90backmatter/93acids03.html, https://raw.githack.com/ANZSoilData/def-au-scma/master/html/90backmatter/94atomicweights04.html, https://raw.githack.com/ANZSoilData/def-au-scma/master/html/90backmatter/95Unitsr05.html</t>
+  </si>
+  <si>
+    <t>https://raw.githack.com/ANZSoilData/def-au-scma/master/html/05-soluble-Cl/05references.html, https://raw.githack.com/ANZSoilData/def-au-scma/master/html/90backmatter/91results01.html, https://raw.githack.com/ANZSoilData/def-au-scma/master/html/90backmatter/92accuracyandprecision02.html, https://raw.githack.com/ANZSoilData/def-au-scma/master/html/90backmatter/93acids03.html, https://raw.githack.com/ANZSoilData/def-au-scma/master/html/90backmatter/94atomicweights04.html, https://raw.githack.com/ANZSoilData/def-au-scma/master/html/90backmatter/95Unitsr05.html</t>
+  </si>
+  <si>
+    <t>https://raw.githack.com/ANZSoilData/def-au-scma/master/html/06-C/06references.html, https://raw.githack.com/ANZSoilData/def-au-scma/master/html/90backmatter/91results01.html, https://raw.githack.com/ANZSoilData/def-au-scma/master/html/90backmatter/92accuracyandprecision02.html, https://raw.githack.com/ANZSoilData/def-au-scma/master/html/90backmatter/93acids03.html, https://raw.githack.com/ANZSoilData/def-au-scma/master/html/90backmatter/94atomicweights04.html, https://raw.githack.com/ANZSoilData/def-au-scma/master/html/90backmatter/95Unitsr05.html</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> https://raw.githack.com/ANZSoilData/def-au-scma/master/html/07-N/07references.html, https://raw.githack.com/ANZSoilData/def-au-scma/master/html/90backmatter/91results01.html, https://raw.githack.com/ANZSoilData/def-au-scma/master/html/90backmatter/92accuracyandprecision02.html, https://raw.githack.com/ANZSoilData/def-au-scma/master/html/90backmatter/93acids03.html, https://raw.githack.com/ANZSoilData/def-au-scma/master/html/90backmatter/94atomicweights04.html, https://raw.githack.com/ANZSoilData/def-au-scma/master/html/90backmatter/95Unitsr05.html</t>
+  </si>
+  <si>
+    <t>https://raw.githack.com/ANZSoilData/def-au-scma/master/html/08-CN-ratio/08references.html, https://raw.githack.com/ANZSoilData/def-au-scma/master/html/90backmatter/91results01.html, https://raw.githack.com/ANZSoilData/def-au-scma/master/html/90backmatter/92accuracyandprecision02.html, https://raw.githack.com/ANZSoilData/def-au-scma/master/html/90backmatter/93acids03.html, https://raw.githack.com/ANZSoilData/def-au-scma/master/html/90backmatter/94atomicweights04.html, https://raw.githack.com/ANZSoilData/def-au-scma/master/html/90backmatter/95Unitsr05.html</t>
+  </si>
+  <si>
+    <t>https://raw.githack.com/ANZSoilData/def-au-scma/master/html/09-P/09refs.html, https://raw.githack.com/ANZSoilData/def-au-scma/master/html/90backmatter/91results01.html, https://raw.githack.com/ANZSoilData/def-au-scma/master/html/90backmatter/92accuracyandprecision02.html, https://raw.githack.com/ANZSoilData/def-au-scma/master/html/90backmatter/93acids03.html, https://raw.githack.com/ANZSoilData/def-au-scma/master/html/90backmatter/94atomicweights04.html, https://raw.githack.com/ANZSoilData/def-au-scma/master/html/90backmatter/95Unitsr05.html</t>
+  </si>
+  <si>
+    <t>https://raw.githack.com/ANZSoilData/def-au-scma/master/html/10-S/references.html, https://raw.githack.com/ANZSoilData/def-au-scma/master/html/90backmatter/91results01.html, https://raw.githack.com/ANZSoilData/def-au-scma/master/html/90backmatter/92accuracyandprecision02.html, https://raw.githack.com/ANZSoilData/def-au-scma/master/html/90backmatter/93acids03.html, https://raw.githack.com/ANZSoilData/def-au-scma/master/html/90backmatter/94atomicweights04.html, https://raw.githack.com/ANZSoilData/def-au-scma/master/html/90backmatter/95Unitsr05.html</t>
+  </si>
+  <si>
+    <t>https://raw.githack.com/ANZSoilData/def-au-scma/master/html/11-gypsum/references.html, https://raw.githack.com/ANZSoilData/def-au-scma/master/html/90backmatter/91results01.html, https://raw.githack.com/ANZSoilData/def-au-scma/master/html/90backmatter/92accuracyandprecision02.html, https://raw.githack.com/ANZSoilData/def-au-scma/master/html/90backmatter/93acids03.html, https://raw.githack.com/ANZSoilData/def-au-scma/master/html/90backmatter/94atomicweights04.html, https://raw.githack.com/ANZSoilData/def-au-scma/master/html/90backmatter/95Unitsr05.html</t>
+  </si>
+  <si>
+    <t>https://raw.githack.com/ANZSoilData/def-au-scma/master/html/12-micronutrients/references.html, https://raw.githack.com/ANZSoilData/def-au-scma/master/html/90backmatter/91results01.html, https://raw.githack.com/ANZSoilData/def-au-scma/master/html/90backmatter/92accuracyandprecision02.html, https://raw.githack.com/ANZSoilData/def-au-scma/master/html/90backmatter/93acids03.html,  https://raw.githack.com/ANZSoilData/def-au-scma/master/html/90backmatter/91results01.html, https://raw.githack.com/ANZSoilData/def-au-scma/master/html/90backmatter/92accuracyandprecision02.html, https://raw.githack.com/ANZSoilData/def-au-scma/master/html/90backmatter/93acids03.html, https://raw.githack.com/ANZSoilData/def-au-scma/master/html/90backmatter/94atomicweights04.html, https://raw.githack.com/ANZSoilData/def-au-scma/master/html/90backmatter/95Unitsr05.html</t>
+  </si>
+  <si>
+    <t>https://raw.githack.com/ANZSoilData/def-au-scma/master/html/13-extractable-Fe-Al-Si/references.html, https://raw.githack.com/ANZSoilData/def-au-scma/master/html/90backmatter/91results01.html, https://raw.githack.com/ANZSoilData/def-au-scma/master/html/90backmatter/92accuracyandprecision02.html, https://raw.githack.com/ANZSoilData/def-au-scma/master/html/90backmatter/93acids03.html, https://raw.githack.com/ANZSoilData/def-au-scma/master/html/90backmatter/94atomicweights04.html, https://raw.githack.com/ANZSoilData/def-au-scma/master/html/90backmatter/95Unitsr05.html</t>
+  </si>
+  <si>
+    <t>https://raw.githack.com/ANZSoilData/def-au-scma/master/html/14-saturation-extracts/references.html, https://raw.githack.com/ANZSoilData/def-au-scma/master/html/90backmatter/91results01.html, https://raw.githack.com/ANZSoilData/def-au-scma/master/html/90backmatter/92accuracyandprecision02.html, https://raw.githack.com/ANZSoilData/def-au-scma/master/html/90backmatter/93acids03.html, https://raw.githack.com/ANZSoilData/def-au-scma/master/html/90backmatter/94atomicweights04.html, https://raw.githack.com/ANZSoilData/def-au-scma/master/html/90backmatter/95Unitsr05.html</t>
+  </si>
+  <si>
+    <t>https://raw.githack.com/ANZSoilData/def-au-scma/master/html/15-ion-exchange-properties/references.html, https://raw.githack.com/ANZSoilData/def-au-scma/master/html/90backmatter/91results01.html, https://raw.githack.com/ANZSoilData/def-au-scma/master/html/90backmatter/92accuracyandprecision02.html, https://raw.githack.com/ANZSoilData/def-au-scma/master/html/90backmatter/93acids03.html, https://raw.githack.com/ANZSoilData/def-au-scma/master/html/90backmatter/94atomicweights04.html, https://raw.githack.com/ANZSoilData/def-au-scma/master/html/90backmatter/95Unitsr05.html</t>
+  </si>
+  <si>
+    <t>https://raw.githack.com/ANZSoilData/def-au-scma/master/html/16-lime-requirement/references.html, https://raw.githack.com/ANZSoilData/def-au-scma/master/html/90backmatter/91results01.html, https://raw.githack.com/ANZSoilData/def-au-scma/master/html/90backmatter/92accuracyandprecision02.html, https://raw.githack.com/ANZSoilData/def-au-scma/master/html/90backmatter/93acids03.html, https://raw.githack.com/ANZSoilData/def-au-scma/master/html/90backmatter/94atomicweights04.html, https://raw.githack.com/ANZSoilData/def-au-scma/master/html/90backmatter/95Unitsr05.html</t>
+  </si>
+  <si>
+    <t>https://raw.githack.com/ANZSoilData/def-au-scma/master/html/17-total-miscellaneous-elements/references.html, https://raw.githack.com/ANZSoilData/def-au-scma/master/html/90backmatter/91results01.html, https://raw.githack.com/ANZSoilData/def-au-scma/master/html/90backmatter/92accuracyandprecision02.html, https://raw.githack.com/ANZSoilData/def-au-scma/master/html/90backmatter/93acids03.html, https://raw.githack.com/ANZSoilData/def-au-scma/master/html/90backmatter/94atomicweights04.html, https://raw.githack.com/ANZSoilData/def-au-scma/master/html/90backmatter/95Unitsr05.html</t>
+  </si>
+  <si>
+    <t>https://raw.githack.com/ANZSoilData/def-au-scma/master/html/18-miscellaneous-extractable-elements/references.html, https://raw.githack.com/ANZSoilData/def-au-scma/master/html/90backmatter/91results01.html, https://raw.githack.com/ANZSoilData/def-au-scma/master/html/90backmatter/92accuracyandprecision02.html, https://raw.githack.com/ANZSoilData/def-au-scma/master/html/90backmatter/93acids03.html, https://raw.githack.com/ANZSoilData/def-au-scma/master/html/90backmatter/94atomicweights04.html, https://raw.githack.com/ANZSoilData/def-au-scma/master/html/90backmatter/95Unitsr05.html</t>
+  </si>
+  <si>
+    <t>https://raw.githack.com/ANZSoilData/def-au-scma/master/html/19-alkaline-earth-carbonates/references.html, https://raw.githack.com/ANZSoilData/def-au-scma/master/html/90backmatter/91results01.html, https://raw.githack.com/ANZSoilData/def-au-scma/master/html/90backmatter/92accuracyandprecision02.html, https://raw.githack.com/ANZSoilData/def-au-scma/master/html/90backmatter/93acids03.html, https://raw.githack.com/ANZSoilData/def-au-scma/master/html/90backmatter/94atomicweights04.html, https://raw.githack.com/ANZSoilData/def-au-scma/master/html/90backmatter/95Unitsr05.html</t>
+  </si>
+  <si>
+    <t>https://raw.githack.com/ANZSoilData/def-au-scma/master/html/20-acid-sulfate-soils/references.html, https://raw.githack.com/ANZSoilData/def-au-scma/master/html/90backmatter/91results01.html, https://raw.githack.com/ANZSoilData/def-au-scma/master/html/90backmatter/92accuracyandprecision02.html, https://raw.githack.com/ANZSoilData/def-au-scma/master/html/90backmatter/93acids03.html, https://raw.githack.com/ANZSoilData/def-au-scma/master/html/90backmatter/94atomicweights04.html, https://raw.githack.com/ANZSoilData/def-au-scma/master/html/90backmatter/95Unitsr05.html</t>
   </si>
 </sst>
 </file>
@@ -4871,8 +4925,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:M477"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="I24" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="K33" sqref="K33"/>
+    <sheetView tabSelected="1" topLeftCell="F23" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="K27" sqref="K27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5736,7 +5790,7 @@
       <c r="I39" s="55"/>
       <c r="J39" s="32"/>
       <c r="K39" s="32" t="s">
-        <v>1348</v>
+        <v>1349</v>
       </c>
       <c r="L39" s="29" t="s">
         <v>1327</v>
@@ -5771,7 +5825,7 @@
       <c r="I40" s="55"/>
       <c r="J40" s="32"/>
       <c r="K40" s="32" t="s">
-        <v>1348</v>
+        <v>1349</v>
       </c>
       <c r="L40" s="29" t="s">
         <v>1327</v>
@@ -5806,7 +5860,7 @@
       <c r="I41" s="55"/>
       <c r="J41" s="32"/>
       <c r="K41" s="32" t="s">
-        <v>1348</v>
+        <v>1349</v>
       </c>
       <c r="L41" s="29" t="s">
         <v>1327</v>
@@ -5841,7 +5895,7 @@
       <c r="I42" s="55"/>
       <c r="J42" s="32"/>
       <c r="K42" s="32" t="s">
-        <v>1348</v>
+        <v>1349</v>
       </c>
       <c r="L42" s="29" t="s">
         <v>1327</v>
@@ -5876,7 +5930,7 @@
       <c r="I43" s="55"/>
       <c r="J43" s="32"/>
       <c r="K43" s="32" t="s">
-        <v>1348</v>
+        <v>1349</v>
       </c>
       <c r="L43" s="29" t="s">
         <v>1327</v>
@@ -5909,7 +5963,7 @@
       <c r="I44" s="55"/>
       <c r="J44" s="32"/>
       <c r="K44" s="32" t="s">
-        <v>1348</v>
+        <v>1350</v>
       </c>
       <c r="L44" s="29" t="s">
         <v>1327</v>
@@ -5944,7 +5998,7 @@
       <c r="I45" s="55"/>
       <c r="J45" s="32"/>
       <c r="K45" s="32" t="s">
-        <v>1348</v>
+        <v>1350</v>
       </c>
       <c r="L45" s="29" t="s">
         <v>1327</v>
@@ -5979,7 +6033,7 @@
       <c r="I46" s="55"/>
       <c r="J46" s="32"/>
       <c r="K46" s="32" t="s">
-        <v>1348</v>
+        <v>1350</v>
       </c>
       <c r="L46" s="29" t="s">
         <v>1327</v>
@@ -6014,7 +6068,7 @@
       <c r="I47" s="55"/>
       <c r="J47" s="32"/>
       <c r="K47" s="32" t="s">
-        <v>1348</v>
+        <v>1350</v>
       </c>
       <c r="L47" s="29" t="s">
         <v>1327</v>
@@ -6049,7 +6103,7 @@
       <c r="I48" s="55"/>
       <c r="J48" s="32"/>
       <c r="K48" s="32" t="s">
-        <v>1348</v>
+        <v>1350</v>
       </c>
       <c r="L48" s="29" t="s">
         <v>1327</v>
@@ -6084,7 +6138,7 @@
       <c r="I49" s="55"/>
       <c r="J49" s="32"/>
       <c r="K49" s="32" t="s">
-        <v>1348</v>
+        <v>1350</v>
       </c>
       <c r="L49" s="29" t="s">
         <v>1327</v>
@@ -6119,7 +6173,7 @@
       <c r="I50" s="55"/>
       <c r="J50" s="32"/>
       <c r="K50" s="32" t="s">
-        <v>1348</v>
+        <v>1350</v>
       </c>
       <c r="L50" s="29" t="s">
         <v>1327</v>
@@ -6154,7 +6208,7 @@
       <c r="I51" s="55"/>
       <c r="J51" s="32"/>
       <c r="K51" s="32" t="s">
-        <v>1348</v>
+        <v>1350</v>
       </c>
       <c r="L51" s="29" t="s">
         <v>1327</v>
@@ -6189,7 +6243,7 @@
       <c r="I52" s="55"/>
       <c r="J52" s="32"/>
       <c r="K52" s="32" t="s">
-        <v>1348</v>
+        <v>1350</v>
       </c>
       <c r="L52" s="29" t="s">
         <v>1327</v>
@@ -6224,7 +6278,7 @@
       <c r="I53" s="55"/>
       <c r="J53" s="32"/>
       <c r="K53" s="32" t="s">
-        <v>1348</v>
+        <v>1350</v>
       </c>
       <c r="L53" s="29" t="s">
         <v>1327</v>
@@ -6259,7 +6313,7 @@
       <c r="I54" s="55"/>
       <c r="J54" s="32"/>
       <c r="K54" s="32" t="s">
-        <v>1348</v>
+        <v>1350</v>
       </c>
       <c r="L54" s="29" t="s">
         <v>1327</v>
@@ -6294,7 +6348,7 @@
       <c r="I55" s="55"/>
       <c r="J55" s="32"/>
       <c r="K55" s="32" t="s">
-        <v>1348</v>
+        <v>1350</v>
       </c>
       <c r="L55" s="29" t="s">
         <v>1327</v>
@@ -6329,7 +6383,7 @@
       <c r="I56" s="55"/>
       <c r="J56" s="32"/>
       <c r="K56" s="32" t="s">
-        <v>1348</v>
+        <v>1350</v>
       </c>
       <c r="L56" s="29" t="s">
         <v>1327</v>
@@ -6364,7 +6418,7 @@
       <c r="I57" s="55"/>
       <c r="J57" s="32"/>
       <c r="K57" s="32" t="s">
-        <v>1348</v>
+        <v>1350</v>
       </c>
       <c r="L57" s="29" t="s">
         <v>1327</v>
@@ -6399,7 +6453,7 @@
       <c r="I58" s="55"/>
       <c r="J58" s="32"/>
       <c r="K58" s="32" t="s">
-        <v>1348</v>
+        <v>1350</v>
       </c>
       <c r="L58" s="29" t="s">
         <v>1327</v>
@@ -6434,7 +6488,7 @@
       <c r="I59" s="55"/>
       <c r="J59" s="32"/>
       <c r="K59" s="32" t="s">
-        <v>1348</v>
+        <v>1350</v>
       </c>
       <c r="L59" s="29" t="s">
         <v>1327</v>
@@ -6469,7 +6523,7 @@
       <c r="I60" s="55"/>
       <c r="J60" s="32"/>
       <c r="K60" s="32" t="s">
-        <v>1348</v>
+        <v>1350</v>
       </c>
       <c r="L60" s="29" t="s">
         <v>1327</v>
@@ -6502,7 +6556,7 @@
       <c r="I61" s="55"/>
       <c r="J61" s="32"/>
       <c r="K61" s="32" t="s">
-        <v>1348</v>
+        <v>1351</v>
       </c>
       <c r="L61" s="29" t="s">
         <v>1327</v>
@@ -6537,7 +6591,7 @@
       <c r="I62" s="55"/>
       <c r="J62" s="32"/>
       <c r="K62" s="32" t="s">
-        <v>1348</v>
+        <v>1351</v>
       </c>
       <c r="L62" s="29" t="s">
         <v>1327</v>
@@ -6576,7 +6630,7 @@
       </c>
       <c r="J63" s="32"/>
       <c r="K63" s="32" t="s">
-        <v>1348</v>
+        <v>1351</v>
       </c>
       <c r="L63" s="29" t="s">
         <v>1327</v>
@@ -6615,7 +6669,7 @@
       </c>
       <c r="J64" s="32"/>
       <c r="K64" s="32" t="s">
-        <v>1348</v>
+        <v>1351</v>
       </c>
       <c r="L64" s="29" t="s">
         <v>1327</v>
@@ -6650,7 +6704,7 @@
       <c r="I65" s="55"/>
       <c r="J65" s="32"/>
       <c r="K65" s="32" t="s">
-        <v>1348</v>
+        <v>1351</v>
       </c>
       <c r="L65" s="29" t="s">
         <v>1327</v>
@@ -6685,7 +6739,7 @@
       <c r="I66" s="55"/>
       <c r="J66" s="32"/>
       <c r="K66" s="32" t="s">
-        <v>1348</v>
+        <v>1351</v>
       </c>
       <c r="L66" s="29" t="s">
         <v>1327</v>
@@ -6720,7 +6774,7 @@
       <c r="I67" s="55"/>
       <c r="J67" s="32"/>
       <c r="K67" s="32" t="s">
-        <v>1348</v>
+        <v>1351</v>
       </c>
       <c r="L67" s="29" t="s">
         <v>1327</v>
@@ -6753,7 +6807,7 @@
       <c r="I68" s="55"/>
       <c r="J68" s="32"/>
       <c r="K68" s="32" t="s">
-        <v>1348</v>
+        <v>1352</v>
       </c>
       <c r="L68" s="29" t="s">
         <v>1327</v>
@@ -6788,7 +6842,7 @@
       <c r="I69" s="55"/>
       <c r="J69" s="32"/>
       <c r="K69" s="32" t="s">
-        <v>1348</v>
+        <v>1352</v>
       </c>
       <c r="L69" s="29" t="s">
         <v>1327</v>
@@ -6823,7 +6877,7 @@
       <c r="I70" s="55"/>
       <c r="J70" s="32"/>
       <c r="K70" s="32" t="s">
-        <v>1348</v>
+        <v>1352</v>
       </c>
       <c r="L70" s="29" t="s">
         <v>1327</v>
@@ -6858,7 +6912,7 @@
       <c r="I71" s="55"/>
       <c r="J71" s="32"/>
       <c r="K71" s="32" t="s">
-        <v>1348</v>
+        <v>1352</v>
       </c>
       <c r="L71" s="29" t="s">
         <v>1327</v>
@@ -6895,7 +6949,7 @@
       <c r="I72" s="55"/>
       <c r="J72" s="32"/>
       <c r="K72" s="32" t="s">
-        <v>1348</v>
+        <v>1352</v>
       </c>
       <c r="L72" s="29" t="s">
         <v>1327</v>
@@ -6932,7 +6986,7 @@
       <c r="I73" s="55"/>
       <c r="J73" s="32"/>
       <c r="K73" s="32" t="s">
-        <v>1348</v>
+        <v>1352</v>
       </c>
       <c r="L73" s="29" t="s">
         <v>1327</v>
@@ -6967,7 +7021,7 @@
       <c r="I74" s="55"/>
       <c r="J74" s="32"/>
       <c r="K74" s="32" t="s">
-        <v>1348</v>
+        <v>1352</v>
       </c>
       <c r="L74" s="29" t="s">
         <v>1327</v>
@@ -7002,7 +7056,7 @@
       <c r="I75" s="55"/>
       <c r="J75" s="32"/>
       <c r="K75" s="32" t="s">
-        <v>1348</v>
+        <v>1352</v>
       </c>
       <c r="L75" s="29" t="s">
         <v>1327</v>
@@ -7039,7 +7093,7 @@
       <c r="I76" s="55"/>
       <c r="J76" s="32"/>
       <c r="K76" s="32" t="s">
-        <v>1348</v>
+        <v>1352</v>
       </c>
       <c r="L76" s="29" t="s">
         <v>1327</v>
@@ -7076,7 +7130,7 @@
       <c r="I77" s="55"/>
       <c r="J77" s="32"/>
       <c r="K77" s="32" t="s">
-        <v>1348</v>
+        <v>1352</v>
       </c>
       <c r="L77" s="29" t="s">
         <v>1327</v>
@@ -7111,7 +7165,7 @@
       <c r="I78" s="55"/>
       <c r="J78" s="32"/>
       <c r="K78" s="32" t="s">
-        <v>1348</v>
+        <v>1352</v>
       </c>
       <c r="L78" s="29" t="s">
         <v>1327</v>
@@ -7146,7 +7200,7 @@
       <c r="I79" s="55"/>
       <c r="J79" s="32"/>
       <c r="K79" s="32" t="s">
-        <v>1348</v>
+        <v>1352</v>
       </c>
       <c r="L79" s="29" t="s">
         <v>1327</v>
@@ -7181,7 +7235,7 @@
       <c r="I80" s="55"/>
       <c r="J80" s="32"/>
       <c r="K80" s="32" t="s">
-        <v>1348</v>
+        <v>1352</v>
       </c>
       <c r="L80" s="29" t="s">
         <v>1327</v>
@@ -7216,7 +7270,7 @@
       <c r="I81" s="55"/>
       <c r="J81" s="32"/>
       <c r="K81" s="32" t="s">
-        <v>1348</v>
+        <v>1352</v>
       </c>
       <c r="L81" s="29" t="s">
         <v>1327</v>
@@ -7251,7 +7305,7 @@
       <c r="I82" s="55"/>
       <c r="J82" s="32"/>
       <c r="K82" s="32" t="s">
-        <v>1348</v>
+        <v>1352</v>
       </c>
       <c r="L82" s="29" t="s">
         <v>1327</v>
@@ -7284,7 +7338,7 @@
       <c r="I83" s="55"/>
       <c r="J83" s="32"/>
       <c r="K83" s="32" t="s">
-        <v>1348</v>
+        <v>1353</v>
       </c>
       <c r="L83" s="29" t="s">
         <v>1327</v>
@@ -7319,7 +7373,7 @@
       <c r="I84" s="55"/>
       <c r="J84" s="32"/>
       <c r="K84" s="32" t="s">
-        <v>1348</v>
+        <v>1353</v>
       </c>
       <c r="L84" s="29" t="s">
         <v>1327</v>
@@ -7358,7 +7412,7 @@
       </c>
       <c r="J85" s="32"/>
       <c r="K85" s="32" t="s">
-        <v>1348</v>
+        <v>1353</v>
       </c>
       <c r="L85" s="29" t="s">
         <v>1327</v>
@@ -7397,7 +7451,7 @@
       </c>
       <c r="J86" s="32"/>
       <c r="K86" s="32" t="s">
-        <v>1348</v>
+        <v>1353</v>
       </c>
       <c r="L86" s="29" t="s">
         <v>1327</v>
@@ -7432,7 +7486,7 @@
       <c r="I87" s="55"/>
       <c r="J87" s="32"/>
       <c r="K87" s="32" t="s">
-        <v>1348</v>
+        <v>1353</v>
       </c>
       <c r="L87" s="29" t="s">
         <v>1327</v>
@@ -7467,7 +7521,7 @@
       <c r="I88" s="55"/>
       <c r="J88" s="32"/>
       <c r="K88" s="32" t="s">
-        <v>1348</v>
+        <v>1353</v>
       </c>
       <c r="L88" s="29" t="s">
         <v>1327</v>
@@ -7502,7 +7556,7 @@
       <c r="I89" s="55"/>
       <c r="J89" s="32"/>
       <c r="K89" s="32" t="s">
-        <v>1348</v>
+        <v>1353</v>
       </c>
       <c r="L89" s="29" t="s">
         <v>1327</v>
@@ -7537,7 +7591,7 @@
       <c r="I90" s="55"/>
       <c r="J90" s="32"/>
       <c r="K90" s="32" t="s">
-        <v>1348</v>
+        <v>1353</v>
       </c>
       <c r="L90" s="29" t="s">
         <v>1327</v>
@@ -7574,7 +7628,7 @@
       <c r="I91" s="55"/>
       <c r="J91" s="32"/>
       <c r="K91" s="32" t="s">
-        <v>1348</v>
+        <v>1353</v>
       </c>
       <c r="L91" s="29" t="s">
         <v>1327</v>
@@ -7611,7 +7665,7 @@
       <c r="I92" s="55"/>
       <c r="J92" s="32"/>
       <c r="K92" s="32" t="s">
-        <v>1348</v>
+        <v>1353</v>
       </c>
       <c r="L92" s="29" t="s">
         <v>1327</v>
@@ -7646,7 +7700,7 @@
       <c r="I93" s="55"/>
       <c r="J93" s="32"/>
       <c r="K93" s="32" t="s">
-        <v>1348</v>
+        <v>1353</v>
       </c>
       <c r="L93" s="29" t="s">
         <v>1327</v>
@@ -7685,7 +7739,7 @@
       </c>
       <c r="J94" s="32"/>
       <c r="K94" s="32" t="s">
-        <v>1348</v>
+        <v>1353</v>
       </c>
       <c r="L94" s="29" t="s">
         <v>1327</v>
@@ -7724,7 +7778,7 @@
       </c>
       <c r="J95" s="32"/>
       <c r="K95" s="32" t="s">
-        <v>1348</v>
+        <v>1353</v>
       </c>
       <c r="L95" s="29" t="s">
         <v>1327</v>
@@ -7761,7 +7815,7 @@
       <c r="I96" s="55"/>
       <c r="J96" s="32"/>
       <c r="K96" s="32" t="s">
-        <v>1348</v>
+        <v>1353</v>
       </c>
       <c r="L96" s="29" t="s">
         <v>1327</v>
@@ -7796,7 +7850,7 @@
       <c r="I97" s="55"/>
       <c r="J97" s="32"/>
       <c r="K97" s="32" t="s">
-        <v>1348</v>
+        <v>1353</v>
       </c>
       <c r="L97" s="29" t="s">
         <v>1327</v>
@@ -7833,7 +7887,7 @@
       <c r="I98" s="55"/>
       <c r="J98" s="32"/>
       <c r="K98" s="32" t="s">
-        <v>1348</v>
+        <v>1353</v>
       </c>
       <c r="L98" s="29" t="s">
         <v>1327</v>
@@ -7870,7 +7924,7 @@
       <c r="I99" s="55"/>
       <c r="J99" s="32"/>
       <c r="K99" s="32" t="s">
-        <v>1348</v>
+        <v>1353</v>
       </c>
       <c r="L99" s="29" t="s">
         <v>1327</v>
@@ -7907,7 +7961,7 @@
       <c r="I100" s="55"/>
       <c r="J100" s="32"/>
       <c r="K100" s="32" t="s">
-        <v>1348</v>
+        <v>1353</v>
       </c>
       <c r="L100" s="29" t="s">
         <v>1327</v>
@@ -7944,7 +7998,7 @@
       <c r="I101" s="55"/>
       <c r="J101" s="32"/>
       <c r="K101" s="32" t="s">
-        <v>1348</v>
+        <v>1353</v>
       </c>
       <c r="L101" s="29" t="s">
         <v>1327</v>
@@ -7981,7 +8035,7 @@
       <c r="I102" s="55"/>
       <c r="J102" s="32"/>
       <c r="K102" s="32" t="s">
-        <v>1348</v>
+        <v>1353</v>
       </c>
       <c r="L102" s="29" t="s">
         <v>1327</v>
@@ -8018,7 +8072,7 @@
       <c r="I103" s="55"/>
       <c r="J103" s="32"/>
       <c r="K103" s="32" t="s">
-        <v>1348</v>
+        <v>1353</v>
       </c>
       <c r="L103" s="29" t="s">
         <v>1327</v>
@@ -8055,7 +8109,7 @@
       <c r="I104" s="55"/>
       <c r="J104" s="32"/>
       <c r="K104" s="32" t="s">
-        <v>1348</v>
+        <v>1353</v>
       </c>
       <c r="L104" s="29" t="s">
         <v>1327</v>
@@ -8092,7 +8146,7 @@
       <c r="I105" s="55"/>
       <c r="J105" s="32"/>
       <c r="K105" s="32" t="s">
-        <v>1348</v>
+        <v>1353</v>
       </c>
       <c r="L105" s="29" t="s">
         <v>1327</v>
@@ -8131,7 +8185,7 @@
       </c>
       <c r="J106" s="32"/>
       <c r="K106" s="32" t="s">
-        <v>1348</v>
+        <v>1353</v>
       </c>
       <c r="L106" s="29" t="s">
         <v>1327</v>
@@ -8170,7 +8224,7 @@
       </c>
       <c r="J107" s="32"/>
       <c r="K107" s="32" t="s">
-        <v>1348</v>
+        <v>1353</v>
       </c>
       <c r="L107" s="29" t="s">
         <v>1327</v>
@@ -8205,7 +8259,7 @@
       <c r="I108" s="55"/>
       <c r="J108" s="32"/>
       <c r="K108" s="32" t="s">
-        <v>1348</v>
+        <v>1353</v>
       </c>
       <c r="L108" s="29" t="s">
         <v>1327</v>
@@ -8242,7 +8296,7 @@
       <c r="I109" s="55"/>
       <c r="J109" s="32"/>
       <c r="K109" s="32" t="s">
-        <v>1348</v>
+        <v>1353</v>
       </c>
       <c r="L109" s="29" t="s">
         <v>1327</v>
@@ -8279,7 +8333,7 @@
       <c r="I110" s="55"/>
       <c r="J110" s="32"/>
       <c r="K110" s="32" t="s">
-        <v>1348</v>
+        <v>1353</v>
       </c>
       <c r="L110" s="29" t="s">
         <v>1327</v>
@@ -8316,7 +8370,7 @@
       <c r="I111" s="55"/>
       <c r="J111" s="32"/>
       <c r="K111" s="32" t="s">
-        <v>1348</v>
+        <v>1353</v>
       </c>
       <c r="L111" s="29" t="s">
         <v>1327</v>
@@ -8353,7 +8407,7 @@
       <c r="I112" s="55"/>
       <c r="J112" s="29"/>
       <c r="K112" s="32" t="s">
-        <v>1348</v>
+        <v>1353</v>
       </c>
       <c r="L112" s="29" t="s">
         <v>1327</v>
@@ -8390,7 +8444,7 @@
       <c r="I113" s="55"/>
       <c r="J113" s="32"/>
       <c r="K113" s="32" t="s">
-        <v>1348</v>
+        <v>1353</v>
       </c>
       <c r="L113" s="29" t="s">
         <v>1327</v>
@@ -8423,7 +8477,7 @@
       <c r="I114" s="55"/>
       <c r="J114" s="32"/>
       <c r="K114" s="32" t="s">
-        <v>1348</v>
+        <v>1354</v>
       </c>
       <c r="L114" s="29" t="s">
         <v>1327</v>
@@ -8458,7 +8512,7 @@
       <c r="I115" s="55"/>
       <c r="J115" s="32"/>
       <c r="K115" s="32" t="s">
-        <v>1348</v>
+        <v>1354</v>
       </c>
       <c r="L115" s="29" t="s">
         <v>1327</v>
@@ -8493,7 +8547,7 @@
       <c r="I116" s="55"/>
       <c r="J116" s="32"/>
       <c r="K116" s="32" t="s">
-        <v>1348</v>
+        <v>1354</v>
       </c>
       <c r="L116" s="29" t="s">
         <v>1327</v>
@@ -8526,7 +8580,7 @@
       <c r="I117" s="55"/>
       <c r="J117" s="32"/>
       <c r="K117" s="32" t="s">
-        <v>1348</v>
+        <v>1355</v>
       </c>
       <c r="L117" s="29" t="s">
         <v>1327</v>
@@ -8561,7 +8615,7 @@
       <c r="I118" s="55"/>
       <c r="J118" s="32"/>
       <c r="K118" s="32" t="s">
-        <v>1348</v>
+        <v>1355</v>
       </c>
       <c r="L118" s="29" t="s">
         <v>1327</v>
@@ -8598,7 +8652,7 @@
       <c r="I119" s="55"/>
       <c r="J119" s="32"/>
       <c r="K119" s="32" t="s">
-        <v>1348</v>
+        <v>1355</v>
       </c>
       <c r="L119" s="29" t="s">
         <v>1327</v>
@@ -8635,7 +8689,7 @@
       <c r="I120" s="55"/>
       <c r="J120" s="32"/>
       <c r="K120" s="32" t="s">
-        <v>1348</v>
+        <v>1355</v>
       </c>
       <c r="L120" s="29" t="s">
         <v>1327</v>
@@ -8672,7 +8726,7 @@
       <c r="I121" s="55"/>
       <c r="J121" s="32"/>
       <c r="K121" s="32" t="s">
-        <v>1348</v>
+        <v>1355</v>
       </c>
       <c r="L121" s="29" t="s">
         <v>1327</v>
@@ -8709,7 +8763,7 @@
       <c r="I122" s="55"/>
       <c r="J122" s="32"/>
       <c r="K122" s="32" t="s">
-        <v>1348</v>
+        <v>1355</v>
       </c>
       <c r="L122" s="29" t="s">
         <v>1327</v>
@@ -8744,7 +8798,7 @@
       <c r="I123" s="55"/>
       <c r="J123" s="32"/>
       <c r="K123" s="32" t="s">
-        <v>1348</v>
+        <v>1355</v>
       </c>
       <c r="L123" s="29" t="s">
         <v>1327</v>
@@ -8781,7 +8835,7 @@
       <c r="I124" s="55"/>
       <c r="J124" s="32"/>
       <c r="K124" s="32" t="s">
-        <v>1348</v>
+        <v>1355</v>
       </c>
       <c r="L124" s="29" t="s">
         <v>1327</v>
@@ -8818,7 +8872,7 @@
       <c r="I125" s="55"/>
       <c r="J125" s="32"/>
       <c r="K125" s="32" t="s">
-        <v>1348</v>
+        <v>1355</v>
       </c>
       <c r="L125" s="29" t="s">
         <v>1327</v>
@@ -8853,7 +8907,7 @@
       <c r="I126" s="55"/>
       <c r="J126" s="32"/>
       <c r="K126" s="32" t="s">
-        <v>1348</v>
+        <v>1355</v>
       </c>
       <c r="L126" s="29" t="s">
         <v>1327</v>
@@ -8890,7 +8944,7 @@
       <c r="I127" s="55"/>
       <c r="J127" s="32"/>
       <c r="K127" s="32" t="s">
-        <v>1348</v>
+        <v>1355</v>
       </c>
       <c r="L127" s="29" t="s">
         <v>1327</v>
@@ -8929,7 +8983,7 @@
       </c>
       <c r="J128" s="32"/>
       <c r="K128" s="32" t="s">
-        <v>1348</v>
+        <v>1355</v>
       </c>
       <c r="L128" s="29" t="s">
         <v>1327</v>
@@ -8968,7 +9022,7 @@
       </c>
       <c r="J129" s="32"/>
       <c r="K129" s="32" t="s">
-        <v>1348</v>
+        <v>1355</v>
       </c>
       <c r="L129" s="29" t="s">
         <v>1327</v>
@@ -9003,7 +9057,7 @@
       <c r="I130" s="55"/>
       <c r="J130" s="32"/>
       <c r="K130" s="32" t="s">
-        <v>1348</v>
+        <v>1355</v>
       </c>
       <c r="L130" s="29" t="s">
         <v>1327</v>
@@ -9038,7 +9092,7 @@
       <c r="I131" s="55"/>
       <c r="J131" s="32"/>
       <c r="K131" s="32" t="s">
-        <v>1348</v>
+        <v>1355</v>
       </c>
       <c r="L131" s="29" t="s">
         <v>1327</v>
@@ -9075,7 +9129,7 @@
       <c r="I132" s="55"/>
       <c r="J132" s="32"/>
       <c r="K132" s="32" t="s">
-        <v>1348</v>
+        <v>1355</v>
       </c>
       <c r="L132" s="29" t="s">
         <v>1327</v>
@@ -9112,7 +9166,7 @@
       <c r="I133" s="55"/>
       <c r="J133" s="32"/>
       <c r="K133" s="32" t="s">
-        <v>1348</v>
+        <v>1355</v>
       </c>
       <c r="L133" s="29" t="s">
         <v>1327</v>
@@ -9147,7 +9201,7 @@
       <c r="I134" s="55"/>
       <c r="J134" s="32"/>
       <c r="K134" s="32" t="s">
-        <v>1348</v>
+        <v>1355</v>
       </c>
       <c r="L134" s="29" t="s">
         <v>1327</v>
@@ -9182,7 +9236,7 @@
       <c r="I135" s="55"/>
       <c r="J135" s="32"/>
       <c r="K135" s="32" t="s">
-        <v>1348</v>
+        <v>1355</v>
       </c>
       <c r="L135" s="29" t="s">
         <v>1327</v>
@@ -9217,7 +9271,7 @@
       <c r="I136" s="55"/>
       <c r="J136" s="32"/>
       <c r="K136" s="32" t="s">
-        <v>1348</v>
+        <v>1355</v>
       </c>
       <c r="L136" s="29" t="s">
         <v>1327</v>
@@ -9252,7 +9306,7 @@
       <c r="I137" s="55"/>
       <c r="J137" s="32"/>
       <c r="K137" s="32" t="s">
-        <v>1348</v>
+        <v>1355</v>
       </c>
       <c r="L137" s="29" t="s">
         <v>1327</v>
@@ -9287,7 +9341,7 @@
       <c r="I138" s="55"/>
       <c r="J138" s="32"/>
       <c r="K138" s="32" t="s">
-        <v>1348</v>
+        <v>1355</v>
       </c>
       <c r="L138" s="29" t="s">
         <v>1327</v>
@@ -9322,7 +9376,7 @@
       <c r="I139" s="55"/>
       <c r="J139" s="32"/>
       <c r="K139" s="32" t="s">
-        <v>1348</v>
+        <v>1355</v>
       </c>
       <c r="L139" s="29" t="s">
         <v>1327</v>
@@ -9359,7 +9413,7 @@
       <c r="I140" s="55"/>
       <c r="J140" s="32"/>
       <c r="K140" s="32" t="s">
-        <v>1348</v>
+        <v>1355</v>
       </c>
       <c r="L140" s="29" t="s">
         <v>1327</v>
@@ -9396,7 +9450,7 @@
       <c r="I141" s="55"/>
       <c r="J141" s="32"/>
       <c r="K141" s="32" t="s">
-        <v>1348</v>
+        <v>1355</v>
       </c>
       <c r="L141" s="29" t="s">
         <v>1327</v>
@@ -9433,7 +9487,7 @@
       <c r="I142" s="55"/>
       <c r="J142" s="32"/>
       <c r="K142" s="32" t="s">
-        <v>1348</v>
+        <v>1355</v>
       </c>
       <c r="L142" s="29" t="s">
         <v>1327</v>
@@ -9470,7 +9524,7 @@
       <c r="I143" s="55"/>
       <c r="J143" s="32"/>
       <c r="K143" s="32" t="s">
-        <v>1348</v>
+        <v>1355</v>
       </c>
       <c r="L143" s="29" t="s">
         <v>1327</v>
@@ -9507,7 +9561,7 @@
       <c r="I144" s="55"/>
       <c r="J144" s="32"/>
       <c r="K144" s="32" t="s">
-        <v>1348</v>
+        <v>1355</v>
       </c>
       <c r="L144" s="29" t="s">
         <v>1327</v>
@@ -9544,7 +9598,7 @@
       <c r="I145" s="55"/>
       <c r="J145" s="32"/>
       <c r="K145" s="32" t="s">
-        <v>1348</v>
+        <v>1355</v>
       </c>
       <c r="L145" s="29" t="s">
         <v>1327</v>
@@ -9581,7 +9635,7 @@
       <c r="I146" s="55"/>
       <c r="J146" s="32"/>
       <c r="K146" s="32" t="s">
-        <v>1348</v>
+        <v>1355</v>
       </c>
       <c r="L146" s="29" t="s">
         <v>1327</v>
@@ -9618,7 +9672,7 @@
       <c r="I147" s="55"/>
       <c r="J147" s="32"/>
       <c r="K147" s="32" t="s">
-        <v>1348</v>
+        <v>1355</v>
       </c>
       <c r="L147" s="29" t="s">
         <v>1327</v>
@@ -9655,7 +9709,7 @@
       <c r="I148" s="55"/>
       <c r="J148" s="32"/>
       <c r="K148" s="32" t="s">
-        <v>1348</v>
+        <v>1355</v>
       </c>
       <c r="L148" s="29" t="s">
         <v>1327</v>
@@ -9692,7 +9746,7 @@
       <c r="I149" s="55"/>
       <c r="J149" s="32"/>
       <c r="K149" s="32" t="s">
-        <v>1348</v>
+        <v>1355</v>
       </c>
       <c r="L149" s="29" t="s">
         <v>1327</v>
@@ -9727,7 +9781,7 @@
       <c r="I150" s="55"/>
       <c r="J150" s="32"/>
       <c r="K150" s="32" t="s">
-        <v>1348</v>
+        <v>1355</v>
       </c>
       <c r="L150" s="29" t="s">
         <v>1327</v>
@@ -9764,7 +9818,7 @@
       <c r="I151" s="55"/>
       <c r="J151" s="32"/>
       <c r="K151" s="32" t="s">
-        <v>1348</v>
+        <v>1355</v>
       </c>
       <c r="L151" s="29" t="s">
         <v>1327</v>
@@ -9801,7 +9855,7 @@
       <c r="I152" s="55"/>
       <c r="J152" s="32"/>
       <c r="K152" s="32" t="s">
-        <v>1348</v>
+        <v>1355</v>
       </c>
       <c r="L152" s="29" t="s">
         <v>1327</v>
@@ -9836,7 +9890,7 @@
       <c r="I153" s="55"/>
       <c r="J153" s="32"/>
       <c r="K153" s="32" t="s">
-        <v>1348</v>
+        <v>1355</v>
       </c>
       <c r="L153" s="29" t="s">
         <v>1327</v>
@@ -9873,7 +9927,7 @@
       <c r="I154" s="55"/>
       <c r="J154" s="32"/>
       <c r="K154" s="32" t="s">
-        <v>1348</v>
+        <v>1355</v>
       </c>
       <c r="L154" s="29" t="s">
         <v>1327</v>
@@ -9910,7 +9964,7 @@
       <c r="I155" s="55"/>
       <c r="J155" s="32"/>
       <c r="K155" s="32" t="s">
-        <v>1348</v>
+        <v>1355</v>
       </c>
       <c r="L155" s="29" t="s">
         <v>1327</v>
@@ -9947,7 +10001,7 @@
       <c r="I156" s="55"/>
       <c r="J156" s="32"/>
       <c r="K156" s="32" t="s">
-        <v>1348</v>
+        <v>1355</v>
       </c>
       <c r="L156" s="29" t="s">
         <v>1327</v>
@@ -9980,7 +10034,7 @@
       <c r="I157" s="56"/>
       <c r="J157" s="32"/>
       <c r="K157" s="32" t="s">
-        <v>1348</v>
+        <v>1356</v>
       </c>
       <c r="L157" s="29" t="s">
         <v>1327</v>
@@ -10015,7 +10069,7 @@
       <c r="I158" s="56"/>
       <c r="J158" s="32"/>
       <c r="K158" s="32" t="s">
-        <v>1348</v>
+        <v>1356</v>
       </c>
       <c r="L158" s="29" t="s">
         <v>1327</v>
@@ -10050,7 +10104,7 @@
       <c r="I159" s="56"/>
       <c r="J159" s="32"/>
       <c r="K159" s="32" t="s">
-        <v>1348</v>
+        <v>1356</v>
       </c>
       <c r="L159" s="29" t="s">
         <v>1327</v>
@@ -10085,7 +10139,7 @@
       <c r="I160" s="56"/>
       <c r="J160" s="32"/>
       <c r="K160" s="32" t="s">
-        <v>1348</v>
+        <v>1356</v>
       </c>
       <c r="L160" s="29" t="s">
         <v>1327</v>
@@ -10122,7 +10176,7 @@
       <c r="I161" s="56"/>
       <c r="J161" s="32"/>
       <c r="K161" s="32" t="s">
-        <v>1348</v>
+        <v>1356</v>
       </c>
       <c r="L161" s="29" t="s">
         <v>1327</v>
@@ -10159,7 +10213,7 @@
       <c r="I162" s="56"/>
       <c r="J162" s="32"/>
       <c r="K162" s="32" t="s">
-        <v>1348</v>
+        <v>1356</v>
       </c>
       <c r="L162" s="29" t="s">
         <v>1327</v>
@@ -10196,7 +10250,7 @@
       <c r="I163" s="56"/>
       <c r="J163" s="32"/>
       <c r="K163" s="32" t="s">
-        <v>1348</v>
+        <v>1356</v>
       </c>
       <c r="L163" s="29" t="s">
         <v>1327</v>
@@ -10233,7 +10287,7 @@
       <c r="I164" s="56"/>
       <c r="J164" s="32"/>
       <c r="K164" s="32" t="s">
-        <v>1348</v>
+        <v>1356</v>
       </c>
       <c r="L164" s="29" t="s">
         <v>1327</v>
@@ -10268,7 +10322,7 @@
       <c r="I165" s="56"/>
       <c r="J165" s="32"/>
       <c r="K165" s="32" t="s">
-        <v>1348</v>
+        <v>1356</v>
       </c>
       <c r="L165" s="29" t="s">
         <v>1327</v>
@@ -10303,7 +10357,7 @@
       <c r="I166" s="56"/>
       <c r="J166" s="32"/>
       <c r="K166" s="32" t="s">
-        <v>1348</v>
+        <v>1356</v>
       </c>
       <c r="L166" s="29" t="s">
         <v>1327</v>
@@ -10336,7 +10390,7 @@
       <c r="I167" s="56"/>
       <c r="J167" s="32"/>
       <c r="K167" s="32" t="s">
-        <v>1348</v>
+        <v>1357</v>
       </c>
       <c r="L167" s="29" t="s">
         <v>1327</v>
@@ -10371,7 +10425,7 @@
       <c r="I168" s="56"/>
       <c r="J168" s="32"/>
       <c r="K168" s="32" t="s">
-        <v>1348</v>
+        <v>1357</v>
       </c>
       <c r="L168" s="29" t="s">
         <v>1327</v>
@@ -10406,7 +10460,7 @@
       <c r="I169" s="56"/>
       <c r="J169" s="32"/>
       <c r="K169" s="32" t="s">
-        <v>1348</v>
+        <v>1357</v>
       </c>
       <c r="L169" s="29" t="s">
         <v>1327</v>
@@ -10439,7 +10493,7 @@
       <c r="I170" s="56"/>
       <c r="J170" s="32"/>
       <c r="K170" s="32" t="s">
-        <v>1348</v>
+        <v>1358</v>
       </c>
       <c r="L170" s="29" t="s">
         <v>1327</v>
@@ -10474,7 +10528,7 @@
       <c r="I171" s="56"/>
       <c r="J171" s="32"/>
       <c r="K171" s="32" t="s">
-        <v>1348</v>
+        <v>1358</v>
       </c>
       <c r="L171" s="29" t="s">
         <v>1327</v>
@@ -10509,7 +10563,7 @@
       <c r="I172" s="57"/>
       <c r="J172" s="12"/>
       <c r="K172" s="32" t="s">
-        <v>1348</v>
+        <v>1358</v>
       </c>
       <c r="L172" s="29" t="s">
         <v>1327</v>
@@ -10544,7 +10598,7 @@
       <c r="I173" s="56"/>
       <c r="J173" s="32"/>
       <c r="K173" s="32" t="s">
-        <v>1348</v>
+        <v>1358</v>
       </c>
       <c r="L173" s="29" t="s">
         <v>1327</v>
@@ -10579,7 +10633,7 @@
       <c r="I174" s="57"/>
       <c r="J174" s="12"/>
       <c r="K174" s="32" t="s">
-        <v>1348</v>
+        <v>1358</v>
       </c>
       <c r="L174" s="29" t="s">
         <v>1327</v>
@@ -10614,7 +10668,7 @@
       <c r="I175" s="56"/>
       <c r="J175" s="32"/>
       <c r="K175" s="32" t="s">
-        <v>1348</v>
+        <v>1358</v>
       </c>
       <c r="L175" s="29" t="s">
         <v>1327</v>
@@ -10649,7 +10703,7 @@
       <c r="I176" s="56"/>
       <c r="J176" s="32"/>
       <c r="K176" s="32" t="s">
-        <v>1348</v>
+        <v>1358</v>
       </c>
       <c r="L176" s="29" t="s">
         <v>1327</v>
@@ -10682,7 +10736,7 @@
       <c r="I177" s="56"/>
       <c r="J177" s="32"/>
       <c r="K177" s="32" t="s">
-        <v>1348</v>
+        <v>1359</v>
       </c>
       <c r="L177" s="29" t="s">
         <v>1327</v>
@@ -10717,7 +10771,7 @@
       <c r="I178" s="56"/>
       <c r="J178" s="32"/>
       <c r="K178" s="32" t="s">
-        <v>1348</v>
+        <v>1359</v>
       </c>
       <c r="L178" s="29" t="s">
         <v>1327</v>
@@ -10752,7 +10806,7 @@
       <c r="I179" s="56"/>
       <c r="J179" s="32"/>
       <c r="K179" s="32" t="s">
-        <v>1348</v>
+        <v>1359</v>
       </c>
       <c r="L179" s="29" t="s">
         <v>1327</v>
@@ -10787,7 +10841,7 @@
       <c r="I180" s="56"/>
       <c r="J180" s="32"/>
       <c r="K180" s="32" t="s">
-        <v>1348</v>
+        <v>1359</v>
       </c>
       <c r="L180" s="29" t="s">
         <v>1327</v>
@@ -10822,7 +10876,7 @@
       <c r="I181" s="56"/>
       <c r="J181" s="32"/>
       <c r="K181" s="32" t="s">
-        <v>1348</v>
+        <v>1359</v>
       </c>
       <c r="L181" s="29" t="s">
         <v>1327</v>
@@ -10859,7 +10913,7 @@
       <c r="I182" s="56"/>
       <c r="J182" s="32"/>
       <c r="K182" s="32" t="s">
-        <v>1348</v>
+        <v>1359</v>
       </c>
       <c r="L182" s="29" t="s">
         <v>1327</v>
@@ -10896,7 +10950,7 @@
       <c r="I183" s="56"/>
       <c r="J183" s="32"/>
       <c r="K183" s="32" t="s">
-        <v>1348</v>
+        <v>1359</v>
       </c>
       <c r="L183" s="29" t="s">
         <v>1327</v>
@@ -10929,7 +10983,7 @@
       <c r="I184" s="56"/>
       <c r="J184" s="32"/>
       <c r="K184" s="32" t="s">
-        <v>1348</v>
+        <v>1360</v>
       </c>
       <c r="L184" s="29" t="s">
         <v>1327</v>
@@ -10964,7 +11018,7 @@
       <c r="I185" s="56"/>
       <c r="J185" s="32"/>
       <c r="K185" s="32" t="s">
-        <v>1348</v>
+        <v>1360</v>
       </c>
       <c r="L185" s="29" t="s">
         <v>1327</v>
@@ -10999,7 +11053,7 @@
       <c r="I186" s="56"/>
       <c r="J186" s="32"/>
       <c r="K186" s="32" t="s">
-        <v>1348</v>
+        <v>1360</v>
       </c>
       <c r="L186" s="29" t="s">
         <v>1327</v>
@@ -11034,7 +11088,7 @@
       <c r="I187" s="56"/>
       <c r="J187" s="32"/>
       <c r="K187" s="32" t="s">
-        <v>1348</v>
+        <v>1360</v>
       </c>
       <c r="L187" s="29" t="s">
         <v>1327</v>
@@ -11069,7 +11123,7 @@
       <c r="I188" s="56"/>
       <c r="J188" s="32"/>
       <c r="K188" s="32" t="s">
-        <v>1348</v>
+        <v>1360</v>
       </c>
       <c r="L188" s="29" t="s">
         <v>1327</v>
@@ -11104,7 +11158,7 @@
       <c r="I189" s="56"/>
       <c r="J189" s="32"/>
       <c r="K189" s="32" t="s">
-        <v>1348</v>
+        <v>1360</v>
       </c>
       <c r="L189" s="29" t="s">
         <v>1327</v>
@@ -11139,7 +11193,7 @@
       <c r="I190" s="56"/>
       <c r="J190" s="32"/>
       <c r="K190" s="32" t="s">
-        <v>1348</v>
+        <v>1360</v>
       </c>
       <c r="L190" s="29" t="s">
         <v>1327</v>
@@ -11174,7 +11228,7 @@
       <c r="I191" s="56"/>
       <c r="J191" s="32"/>
       <c r="K191" s="32" t="s">
-        <v>1348</v>
+        <v>1360</v>
       </c>
       <c r="L191" s="29" t="s">
         <v>1327</v>
@@ -11209,7 +11263,7 @@
       <c r="I192" s="56"/>
       <c r="J192" s="32"/>
       <c r="K192" s="32" t="s">
-        <v>1348</v>
+        <v>1360</v>
       </c>
       <c r="L192" s="29" t="s">
         <v>1327</v>
@@ -11244,7 +11298,7 @@
       <c r="I193" s="56"/>
       <c r="J193" s="32"/>
       <c r="K193" s="32" t="s">
-        <v>1348</v>
+        <v>1360</v>
       </c>
       <c r="L193" s="29" t="s">
         <v>1327</v>
@@ -11283,7 +11337,7 @@
       </c>
       <c r="J194" s="32"/>
       <c r="K194" s="32" t="s">
-        <v>1348</v>
+        <v>1360</v>
       </c>
       <c r="L194" s="29" t="s">
         <v>1327</v>
@@ -11322,7 +11376,7 @@
       </c>
       <c r="J195" s="32"/>
       <c r="K195" s="32" t="s">
-        <v>1348</v>
+        <v>1360</v>
       </c>
       <c r="L195" s="29" t="s">
         <v>1327</v>
@@ -11357,7 +11411,7 @@
       <c r="I196" s="56"/>
       <c r="J196" s="32"/>
       <c r="K196" s="32" t="s">
-        <v>1348</v>
+        <v>1360</v>
       </c>
       <c r="L196" s="29" t="s">
         <v>1327</v>
@@ -11392,7 +11446,7 @@
       <c r="I197" s="56"/>
       <c r="J197" s="32"/>
       <c r="K197" s="32" t="s">
-        <v>1348</v>
+        <v>1360</v>
       </c>
       <c r="L197" s="29" t="s">
         <v>1327</v>
@@ -11427,7 +11481,7 @@
       <c r="I198" s="56"/>
       <c r="J198" s="32"/>
       <c r="K198" s="32" t="s">
-        <v>1348</v>
+        <v>1360</v>
       </c>
       <c r="L198" s="29" t="s">
         <v>1327</v>
@@ -11462,7 +11516,7 @@
       <c r="I199" s="56"/>
       <c r="J199" s="32"/>
       <c r="K199" s="32" t="s">
-        <v>1348</v>
+        <v>1360</v>
       </c>
       <c r="L199" s="29" t="s">
         <v>1327</v>
@@ -11497,7 +11551,7 @@
       <c r="I200" s="56"/>
       <c r="J200" s="32"/>
       <c r="K200" s="32" t="s">
-        <v>1348</v>
+        <v>1360</v>
       </c>
       <c r="L200" s="29" t="s">
         <v>1327</v>
@@ -11536,7 +11590,7 @@
       </c>
       <c r="J201" s="32"/>
       <c r="K201" s="32" t="s">
-        <v>1348</v>
+        <v>1360</v>
       </c>
       <c r="L201" s="29" t="s">
         <v>1327</v>
@@ -11575,7 +11629,7 @@
       </c>
       <c r="J202" s="32"/>
       <c r="K202" s="32" t="s">
-        <v>1348</v>
+        <v>1360</v>
       </c>
       <c r="L202" s="29" t="s">
         <v>1327</v>
@@ -11610,7 +11664,7 @@
       <c r="I203" s="56"/>
       <c r="J203" s="32"/>
       <c r="K203" s="32" t="s">
-        <v>1348</v>
+        <v>1360</v>
       </c>
       <c r="L203" s="29" t="s">
         <v>1327</v>
@@ -11649,7 +11703,7 @@
       </c>
       <c r="J204" s="32"/>
       <c r="K204" s="32" t="s">
-        <v>1348</v>
+        <v>1360</v>
       </c>
       <c r="L204" s="29" t="s">
         <v>1327</v>
@@ -11688,7 +11742,7 @@
       </c>
       <c r="J205" s="32"/>
       <c r="K205" s="32" t="s">
-        <v>1348</v>
+        <v>1360</v>
       </c>
       <c r="L205" s="29" t="s">
         <v>1327</v>
@@ -11723,7 +11777,7 @@
       <c r="I206" s="56"/>
       <c r="J206" s="32"/>
       <c r="K206" s="32" t="s">
-        <v>1348</v>
+        <v>1360</v>
       </c>
       <c r="L206" s="29" t="s">
         <v>1327</v>
@@ -11756,7 +11810,7 @@
       <c r="I207" s="56"/>
       <c r="J207" s="32"/>
       <c r="K207" s="32" t="s">
-        <v>1348</v>
+        <v>1361</v>
       </c>
       <c r="L207" s="29" t="s">
         <v>1327</v>
@@ -11791,7 +11845,7 @@
       <c r="I208" s="56"/>
       <c r="J208" s="32"/>
       <c r="K208" s="32" t="s">
-        <v>1348</v>
+        <v>1361</v>
       </c>
       <c r="L208" s="29" t="s">
         <v>1327</v>
@@ -11826,7 +11880,7 @@
       <c r="I209" s="56"/>
       <c r="J209" s="32"/>
       <c r="K209" s="32" t="s">
-        <v>1348</v>
+        <v>1361</v>
       </c>
       <c r="L209" s="29" t="s">
         <v>1327</v>
@@ -11861,7 +11915,7 @@
       <c r="I210" s="56"/>
       <c r="J210" s="32"/>
       <c r="K210" s="32" t="s">
-        <v>1348</v>
+        <v>1361</v>
       </c>
       <c r="L210" s="29" t="s">
         <v>1327</v>
@@ -11896,7 +11950,7 @@
       <c r="I211" s="56"/>
       <c r="J211" s="32"/>
       <c r="K211" s="32" t="s">
-        <v>1348</v>
+        <v>1361</v>
       </c>
       <c r="L211" s="29" t="s">
         <v>1327</v>
@@ -11931,7 +11985,7 @@
       <c r="I212" s="56"/>
       <c r="J212" s="32"/>
       <c r="K212" s="32" t="s">
-        <v>1348</v>
+        <v>1361</v>
       </c>
       <c r="L212" s="29" t="s">
         <v>1327</v>
@@ -11966,7 +12020,7 @@
       <c r="I213" s="56"/>
       <c r="J213" s="32"/>
       <c r="K213" s="32" t="s">
-        <v>1348</v>
+        <v>1361</v>
       </c>
       <c r="L213" s="29" t="s">
         <v>1327</v>
@@ -12001,7 +12055,7 @@
       <c r="I214" s="56"/>
       <c r="J214" s="32"/>
       <c r="K214" s="32" t="s">
-        <v>1348</v>
+        <v>1361</v>
       </c>
       <c r="L214" s="29" t="s">
         <v>1327</v>
@@ -12036,7 +12090,7 @@
       <c r="I215" s="56"/>
       <c r="J215" s="32"/>
       <c r="K215" s="32" t="s">
-        <v>1348</v>
+        <v>1361</v>
       </c>
       <c r="L215" s="29" t="s">
         <v>1327</v>
@@ -12071,7 +12125,7 @@
       <c r="I216" s="56"/>
       <c r="J216" s="32"/>
       <c r="K216" s="32" t="s">
-        <v>1348</v>
+        <v>1361</v>
       </c>
       <c r="L216" s="29" t="s">
         <v>1327</v>
@@ -12106,7 +12160,7 @@
       <c r="I217" s="56"/>
       <c r="J217" s="32"/>
       <c r="K217" s="32" t="s">
-        <v>1348</v>
+        <v>1361</v>
       </c>
       <c r="L217" s="29" t="s">
         <v>1327</v>
@@ -12141,7 +12195,7 @@
       <c r="I218" s="56"/>
       <c r="J218" s="32"/>
       <c r="K218" s="32" t="s">
-        <v>1348</v>
+        <v>1361</v>
       </c>
       <c r="L218" s="29" t="s">
         <v>1327</v>
@@ -12176,7 +12230,7 @@
       <c r="I219" s="56"/>
       <c r="J219" s="32"/>
       <c r="K219" s="32" t="s">
-        <v>1348</v>
+        <v>1361</v>
       </c>
       <c r="L219" s="29" t="s">
         <v>1327</v>
@@ -12211,7 +12265,7 @@
       <c r="I220" s="56"/>
       <c r="J220" s="32"/>
       <c r="K220" s="32" t="s">
-        <v>1348</v>
+        <v>1361</v>
       </c>
       <c r="L220" s="29" t="s">
         <v>1327</v>
@@ -12246,7 +12300,7 @@
       <c r="I221" s="56"/>
       <c r="J221" s="32"/>
       <c r="K221" s="32" t="s">
-        <v>1348</v>
+        <v>1361</v>
       </c>
       <c r="L221" s="29" t="s">
         <v>1327</v>
@@ -12281,7 +12335,7 @@
       <c r="I222" s="56"/>
       <c r="J222" s="32"/>
       <c r="K222" s="32" t="s">
-        <v>1348</v>
+        <v>1361</v>
       </c>
       <c r="L222" s="29" t="s">
         <v>1327</v>
@@ -12316,7 +12370,7 @@
       <c r="I223" s="56"/>
       <c r="J223" s="32"/>
       <c r="K223" s="32" t="s">
-        <v>1348</v>
+        <v>1361</v>
       </c>
       <c r="L223" s="29" t="s">
         <v>1327</v>
@@ -12351,7 +12405,7 @@
       <c r="I224" s="56"/>
       <c r="J224" s="32"/>
       <c r="K224" s="32" t="s">
-        <v>1348</v>
+        <v>1361</v>
       </c>
       <c r="L224" s="29" t="s">
         <v>1327</v>
@@ -12386,7 +12440,7 @@
       <c r="I225" s="56"/>
       <c r="J225" s="32"/>
       <c r="K225" s="32" t="s">
-        <v>1348</v>
+        <v>1361</v>
       </c>
       <c r="L225" s="29" t="s">
         <v>1327</v>
@@ -12421,7 +12475,7 @@
       <c r="I226" s="56"/>
       <c r="J226" s="32"/>
       <c r="K226" s="32" t="s">
-        <v>1348</v>
+        <v>1361</v>
       </c>
       <c r="L226" s="29" t="s">
         <v>1327</v>
@@ -12456,7 +12510,7 @@
       <c r="I227" s="56"/>
       <c r="J227" s="32"/>
       <c r="K227" s="32" t="s">
-        <v>1348</v>
+        <v>1361</v>
       </c>
       <c r="L227" s="29" t="s">
         <v>1327</v>
@@ -12491,7 +12545,7 @@
       <c r="I228" s="56"/>
       <c r="J228" s="32"/>
       <c r="K228" s="32" t="s">
-        <v>1348</v>
+        <v>1361</v>
       </c>
       <c r="L228" s="29" t="s">
         <v>1327</v>
@@ -12526,7 +12580,7 @@
       <c r="I229" s="56"/>
       <c r="J229" s="32"/>
       <c r="K229" s="32" t="s">
-        <v>1348</v>
+        <v>1361</v>
       </c>
       <c r="L229" s="29" t="s">
         <v>1327</v>
@@ -12561,7 +12615,7 @@
       <c r="I230" s="56"/>
       <c r="J230" s="32"/>
       <c r="K230" s="32" t="s">
-        <v>1348</v>
+        <v>1361</v>
       </c>
       <c r="L230" s="29" t="s">
         <v>1327</v>
@@ -12596,7 +12650,7 @@
       <c r="I231" s="56"/>
       <c r="J231" s="32"/>
       <c r="K231" s="32" t="s">
-        <v>1348</v>
+        <v>1361</v>
       </c>
       <c r="L231" s="29" t="s">
         <v>1327</v>
@@ -12631,7 +12685,7 @@
       <c r="I232" s="56"/>
       <c r="J232" s="32"/>
       <c r="K232" s="32" t="s">
-        <v>1348</v>
+        <v>1361</v>
       </c>
       <c r="L232" s="29" t="s">
         <v>1327</v>
@@ -12666,7 +12720,7 @@
       <c r="I233" s="56"/>
       <c r="J233" s="32"/>
       <c r="K233" s="32" t="s">
-        <v>1348</v>
+        <v>1361</v>
       </c>
       <c r="L233" s="29" t="s">
         <v>1327</v>
@@ -12701,7 +12755,7 @@
       <c r="I234" s="56"/>
       <c r="J234" s="32"/>
       <c r="K234" s="32" t="s">
-        <v>1348</v>
+        <v>1361</v>
       </c>
       <c r="L234" s="29" t="s">
         <v>1327</v>
@@ -12736,7 +12790,7 @@
       <c r="I235" s="56"/>
       <c r="J235" s="32"/>
       <c r="K235" s="32" t="s">
-        <v>1348</v>
+        <v>1361</v>
       </c>
       <c r="L235" s="29" t="s">
         <v>1327</v>
@@ -12771,7 +12825,7 @@
       <c r="I236" s="56"/>
       <c r="J236" s="32"/>
       <c r="K236" s="32" t="s">
-        <v>1348</v>
+        <v>1361</v>
       </c>
       <c r="L236" s="29" t="s">
         <v>1327</v>
@@ -12804,7 +12858,7 @@
       <c r="I237" s="56"/>
       <c r="J237" s="32"/>
       <c r="K237" s="32" t="s">
-        <v>1348</v>
+        <v>1362</v>
       </c>
       <c r="L237" s="29" t="s">
         <v>1327</v>
@@ -12839,7 +12893,7 @@
       <c r="I238" s="56"/>
       <c r="J238" s="32"/>
       <c r="K238" s="32" t="s">
-        <v>1348</v>
+        <v>1362</v>
       </c>
       <c r="L238" s="29" t="s">
         <v>1327</v>
@@ -12874,7 +12928,7 @@
       <c r="I239" s="56"/>
       <c r="J239" s="32"/>
       <c r="K239" s="32" t="s">
-        <v>1348</v>
+        <v>1362</v>
       </c>
       <c r="L239" s="29" t="s">
         <v>1327</v>
@@ -12909,7 +12963,7 @@
       <c r="I240" s="56"/>
       <c r="J240" s="32"/>
       <c r="K240" s="32" t="s">
-        <v>1348</v>
+        <v>1362</v>
       </c>
       <c r="L240" s="29" t="s">
         <v>1327</v>
@@ -12944,7 +12998,7 @@
       <c r="I241" s="56"/>
       <c r="J241" s="32"/>
       <c r="K241" s="32" t="s">
-        <v>1348</v>
+        <v>1362</v>
       </c>
       <c r="L241" s="29" t="s">
         <v>1327</v>
@@ -12977,7 +13031,7 @@
       <c r="I242" s="56"/>
       <c r="J242" s="32"/>
       <c r="K242" s="32" t="s">
-        <v>1348</v>
+        <v>1363</v>
       </c>
       <c r="L242" s="29" t="s">
         <v>1327</v>
@@ -13012,7 +13066,7 @@
       <c r="I243" s="56"/>
       <c r="J243" s="32"/>
       <c r="K243" s="32" t="s">
-        <v>1348</v>
+        <v>1363</v>
       </c>
       <c r="L243" s="29" t="s">
         <v>1327</v>
@@ -13047,7 +13101,7 @@
       <c r="I244" s="56"/>
       <c r="J244" s="32"/>
       <c r="K244" s="32" t="s">
-        <v>1348</v>
+        <v>1363</v>
       </c>
       <c r="L244" s="29" t="s">
         <v>1327</v>
@@ -13082,7 +13136,7 @@
       <c r="I245" s="56"/>
       <c r="J245" s="32"/>
       <c r="K245" s="32" t="s">
-        <v>1348</v>
+        <v>1363</v>
       </c>
       <c r="L245" s="29" t="s">
         <v>1327</v>
@@ -13117,7 +13171,7 @@
       <c r="I246" s="56"/>
       <c r="J246" s="32"/>
       <c r="K246" s="32" t="s">
-        <v>1348</v>
+        <v>1363</v>
       </c>
       <c r="L246" s="29" t="s">
         <v>1327</v>
@@ -13152,7 +13206,7 @@
       <c r="I247" s="56"/>
       <c r="J247" s="32"/>
       <c r="K247" s="32" t="s">
-        <v>1348</v>
+        <v>1363</v>
       </c>
       <c r="L247" s="29" t="s">
         <v>1327</v>
@@ -13185,7 +13239,7 @@
       <c r="I248" s="56"/>
       <c r="J248" s="32"/>
       <c r="K248" s="32" t="s">
-        <v>1348</v>
+        <v>1364</v>
       </c>
       <c r="L248" s="29" t="s">
         <v>1327</v>
@@ -13220,7 +13274,7 @@
       <c r="I249" s="56"/>
       <c r="J249" s="32"/>
       <c r="K249" s="32" t="s">
-        <v>1348</v>
+        <v>1364</v>
       </c>
       <c r="L249" s="29" t="s">
         <v>1327</v>
@@ -13255,7 +13309,7 @@
       <c r="I250" s="56"/>
       <c r="J250" s="32"/>
       <c r="K250" s="32" t="s">
-        <v>1348</v>
+        <v>1364</v>
       </c>
       <c r="L250" s="29" t="s">
         <v>1327</v>
@@ -13290,7 +13344,7 @@
       <c r="I251" s="56"/>
       <c r="J251" s="32"/>
       <c r="K251" s="32" t="s">
-        <v>1348</v>
+        <v>1364</v>
       </c>
       <c r="L251" s="29" t="s">
         <v>1327</v>
@@ -13325,7 +13379,7 @@
       <c r="I252" s="56"/>
       <c r="J252" s="32"/>
       <c r="K252" s="32" t="s">
-        <v>1348</v>
+        <v>1364</v>
       </c>
       <c r="L252" s="29" t="s">
         <v>1327</v>
@@ -13360,7 +13414,7 @@
       <c r="I253" s="56"/>
       <c r="J253" s="32"/>
       <c r="K253" s="32" t="s">
-        <v>1348</v>
+        <v>1364</v>
       </c>
       <c r="L253" s="29" t="s">
         <v>1327</v>
@@ -13395,7 +13449,7 @@
       <c r="I254" s="56"/>
       <c r="J254" s="32"/>
       <c r="K254" s="32" t="s">
-        <v>1348</v>
+        <v>1364</v>
       </c>
       <c r="L254" s="29" t="s">
         <v>1327</v>
@@ -13432,7 +13486,7 @@
       <c r="I255" s="56"/>
       <c r="J255" s="32"/>
       <c r="K255" s="32" t="s">
-        <v>1348</v>
+        <v>1364</v>
       </c>
       <c r="L255" s="29" t="s">
         <v>1327</v>
@@ -13469,7 +13523,7 @@
       <c r="I256" s="56"/>
       <c r="J256" s="32"/>
       <c r="K256" s="32" t="s">
-        <v>1348</v>
+        <v>1364</v>
       </c>
       <c r="L256" s="29" t="s">
         <v>1327</v>
@@ -13504,7 +13558,7 @@
       <c r="I257" s="56"/>
       <c r="J257" s="32"/>
       <c r="K257" s="32" t="s">
-        <v>1348</v>
+        <v>1364</v>
       </c>
       <c r="L257" s="29" t="s">
         <v>1327</v>
@@ -13537,7 +13591,7 @@
       <c r="I258" s="56"/>
       <c r="J258" s="32"/>
       <c r="K258" s="32" t="s">
-        <v>1348</v>
+        <v>1365</v>
       </c>
       <c r="L258" s="29" t="s">
         <v>1327</v>
@@ -13572,7 +13626,7 @@
       <c r="I259" s="56"/>
       <c r="J259" s="32"/>
       <c r="K259" s="32" t="s">
-        <v>1348</v>
+        <v>1365</v>
       </c>
       <c r="L259" s="29" t="s">
         <v>1327</v>
@@ -13607,7 +13661,7 @@
       <c r="I260" s="56"/>
       <c r="J260" s="32"/>
       <c r="K260" s="32" t="s">
-        <v>1348</v>
+        <v>1365</v>
       </c>
       <c r="L260" s="29" t="s">
         <v>1327</v>
@@ -13644,7 +13698,7 @@
       <c r="I261" s="56"/>
       <c r="J261" s="32"/>
       <c r="K261" s="32" t="s">
-        <v>1348</v>
+        <v>1365</v>
       </c>
       <c r="L261" s="29" t="s">
         <v>1327</v>
@@ -13681,7 +13735,7 @@
       <c r="I262" s="56"/>
       <c r="J262" s="32"/>
       <c r="K262" s="32" t="s">
-        <v>1348</v>
+        <v>1365</v>
       </c>
       <c r="L262" s="29" t="s">
         <v>1327</v>
@@ -13716,7 +13770,7 @@
       <c r="I263" s="56"/>
       <c r="J263" s="32"/>
       <c r="K263" s="32" t="s">
-        <v>1348</v>
+        <v>1365</v>
       </c>
       <c r="L263" s="29" t="s">
         <v>1327</v>
@@ -13751,7 +13805,7 @@
       <c r="I264" s="56"/>
       <c r="J264" s="32"/>
       <c r="K264" s="32" t="s">
-        <v>1348</v>
+        <v>1365</v>
       </c>
       <c r="L264" s="29" t="s">
         <v>1327</v>
@@ -13784,7 +13838,7 @@
       <c r="I265" s="56"/>
       <c r="J265" s="32"/>
       <c r="K265" s="32" t="s">
-        <v>1348</v>
+        <v>1366</v>
       </c>
       <c r="L265" s="29" t="s">
         <v>1327</v>
@@ -13819,7 +13873,7 @@
       <c r="I266" s="56"/>
       <c r="J266" s="32"/>
       <c r="K266" s="32" t="s">
-        <v>1348</v>
+        <v>1366</v>
       </c>
       <c r="L266" s="29" t="s">
         <v>1327</v>
@@ -13854,7 +13908,7 @@
       <c r="I267" s="56"/>
       <c r="J267" s="32"/>
       <c r="K267" s="32" t="s">
-        <v>1348</v>
+        <v>1366</v>
       </c>
       <c r="L267" s="29" t="s">
         <v>1327</v>
@@ -13889,7 +13943,7 @@
       <c r="I268" s="56"/>
       <c r="J268" s="32"/>
       <c r="K268" s="32" t="s">
-        <v>1348</v>
+        <v>1366</v>
       </c>
       <c r="L268" s="29" t="s">
         <v>1327</v>
@@ -13924,7 +13978,7 @@
       <c r="I269" s="56"/>
       <c r="J269" s="32"/>
       <c r="K269" s="32" t="s">
-        <v>1348</v>
+        <v>1366</v>
       </c>
       <c r="L269" s="29" t="s">
         <v>1327</v>
@@ -13959,7 +14013,7 @@
       <c r="I270" s="56"/>
       <c r="J270" s="32"/>
       <c r="K270" s="32" t="s">
-        <v>1348</v>
+        <v>1366</v>
       </c>
       <c r="L270" s="29" t="s">
         <v>1327</v>
@@ -13994,7 +14048,7 @@
       <c r="I271" s="56"/>
       <c r="J271" s="32"/>
       <c r="K271" s="32" t="s">
-        <v>1348</v>
+        <v>1366</v>
       </c>
       <c r="L271" s="29" t="s">
         <v>1327</v>
@@ -14029,7 +14083,7 @@
       <c r="I272" s="56"/>
       <c r="J272" s="32"/>
       <c r="K272" s="32" t="s">
-        <v>1348</v>
+        <v>1366</v>
       </c>
       <c r="L272" s="29" t="s">
         <v>1327</v>
@@ -14064,7 +14118,7 @@
       <c r="I273" s="56"/>
       <c r="J273" s="32"/>
       <c r="K273" s="32" t="s">
-        <v>1348</v>
+        <v>1366</v>
       </c>
       <c r="L273" s="29" t="s">
         <v>1327</v>
@@ -14099,7 +14153,7 @@
       <c r="I274" s="56"/>
       <c r="J274" s="32"/>
       <c r="K274" s="32" t="s">
-        <v>1348</v>
+        <v>1366</v>
       </c>
       <c r="L274" s="29" t="s">
         <v>1327</v>
@@ -14134,7 +14188,7 @@
       <c r="I275" s="56"/>
       <c r="J275" s="32"/>
       <c r="K275" s="32" t="s">
-        <v>1348</v>
+        <v>1366</v>
       </c>
       <c r="L275" s="29" t="s">
         <v>1327</v>
@@ -14169,7 +14223,7 @@
       <c r="I276" s="56"/>
       <c r="J276" s="32"/>
       <c r="K276" s="32" t="s">
-        <v>1348</v>
+        <v>1366</v>
       </c>
       <c r="L276" s="29" t="s">
         <v>1327</v>
@@ -14204,7 +14258,7 @@
       <c r="I277" s="56"/>
       <c r="J277" s="32"/>
       <c r="K277" s="32" t="s">
-        <v>1348</v>
+        <v>1366</v>
       </c>
       <c r="L277" s="29" t="s">
         <v>1327</v>
@@ -22400,9 +22454,12 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
@@ -22617,19 +22674,15 @@
 </file>
 
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{AAE62FC3-7D3B-4886-B53E-C881811D2384}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{008ABE91-8C92-4516-916D-4DC325FB5C89}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
@@ -22654,9 +22707,10 @@
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{008ABE91-8C92-4516-916D-4DC325FB5C89}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{AAE62FC3-7D3B-4886-B53E-C881811D2384}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
Squashed a bunch of namespace prefix bugs; replaced some roles with Schema.org properties; replaced missing definitions with 'TBC'; tidied up metadata
</commit_message>
<xml_diff>
--- a/rdf/skosplay-scma-2.xlsx
+++ b/rdf/skosplay-scma-2.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://federationuniversity-my.sharepoint.com/personal/mr_wong_federation_edu_au/Documents/Documents/GitHub/def-au-scma/rdf/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\cox075\dev\ENV\anzsoil\def-au-scma\rdf\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="178" documentId="13_ncr:1_{280EA38A-AAE3-4033-A57D-27CDA991092C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{649CD134-A3DD-4BBF-9B0C-216EC9F0107F}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0AC01565-73A5-4A6E-AF1D-239FB6028D55}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="24240" windowHeight="13140" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="40065" yWindow="2730" windowWidth="27795" windowHeight="15825" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="SCMA-2011" sheetId="2" r:id="rId1"/>
@@ -103,7 +103,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4359" uniqueCount="1367">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4362" uniqueCount="1368">
   <si>
     <t>ConceptScheme URI</t>
   </si>
@@ -4105,12 +4105,6 @@
     <t>skos:historyNote</t>
   </si>
   <si>
-    <t>NEED SOME TEXT HERE</t>
-  </si>
-  <si>
-    <t xml:space="preserve">NEED SOME TEXT HERE </t>
-  </si>
-  <si>
     <t>dcterms:replaces(separator=",")</t>
   </si>
   <si>
@@ -4135,52 +4129,16 @@
     <t>https://raw.githack.com/ANZSoilData/def-au-scma/master/html/00frontmatter/00WARNING.html, https://raw.githack.com/ANZSoilData/def-au-scma/master/html/00frontmatter/03Abbreviations%20and%20acronyms.html</t>
   </si>
   <si>
-    <t>https://raw.githack.com/ANZSoilData/def-au-scma/master/html/00frontmatter/01Preface%20and%20acknowledgements.html</t>
-  </si>
-  <si>
-    <t>David J. Lyons</t>
-  </si>
-  <si>
-    <t xml:space="preserve">George E.Raymont </t>
-  </si>
-  <si>
-    <t>dcterms:funder</t>
-  </si>
-  <si>
     <t>Queensland Department of Environment and Resource Management</t>
   </si>
   <si>
     <t>https://ror.org/030c92375</t>
   </si>
   <si>
-    <t>Bruce Shelly</t>
-  </si>
-  <si>
-    <t>suppporter</t>
-  </si>
-  <si>
-    <t>Australian Collaborative Land Evaluation Program (ACLEP)</t>
-  </si>
-  <si>
-    <t>Australian Soil and Plant Analysis Council (ASPAC)</t>
-  </si>
-  <si>
-    <t>dcterm:rightsHolder</t>
-  </si>
-  <si>
-    <t>dcterm:publisher</t>
-  </si>
-  <si>
-    <t>dcterms:RightsStatement</t>
-  </si>
-  <si>
     <t>Rayment, G.E.</t>
   </si>
   <si>
     <t>Higginson, F.R. (Francis Ross)</t>
-  </si>
-  <si>
-    <t>dcterm:isPartOf</t>
   </si>
   <si>
     <t>Melbourne : Inkata Press</t>
@@ -4251,6 +4209,85 @@
   </si>
   <si>
     <t>https://raw.githack.com/ANZSoilData/def-au-scma/master/html/20-acid-sulfate-soils/references.html, https://raw.githack.com/ANZSoilData/def-au-scma/master/html/90backmatter/91results01.html, https://raw.githack.com/ANZSoilData/def-au-scma/master/html/90backmatter/92accuracyandprecision02.html, https://raw.githack.com/ANZSoilData/def-au-scma/master/html/90backmatter/93acids03.html, https://raw.githack.com/ANZSoilData/def-au-scma/master/html/90backmatter/94atomicweights04.html, https://raw.githack.com/ANZSoilData/def-au-scma/master/html/90backmatter/95Unitsr05.html</t>
+  </si>
+  <si>
+    <t>skos:editorialNote</t>
+  </si>
+  <si>
+    <r>
+      <t>The data was converted from a HTML</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF7E408A"/>
+        <rFont val="Roboto"/>
+      </rPr>
+      <t xml:space="preserve"> representation</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF4C4C4C"/>
+        <rFont val="Roboto"/>
+      </rPr>
+      <t xml:space="preserve"> to this 'linked-data' format by  Megan Wong and </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF7E408A"/>
+        <rFont val="Roboto"/>
+      </rPr>
+      <t>Simon J D Cox</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF4C4C4C"/>
+        <rFont val="Roboto"/>
+      </rPr>
+      <t>.</t>
+    </r>
+  </si>
+  <si>
+    <t>The data was converted from a HTML representation to this 'linked-data' format by  Megan Wong and Simon J D Cox.</t>
+  </si>
+  <si>
+    <t>TBC</t>
+  </si>
+  <si>
+    <t>https://www.aspac-australasia.com/</t>
+  </si>
+  <si>
+    <t>https://www.clw.csiro.au/aclep/</t>
+  </si>
+  <si>
+    <t>sdo:funder</t>
+  </si>
+  <si>
+    <t>sdo:maintainer</t>
+  </si>
+  <si>
+    <t>dcterms:rightsHolder</t>
+  </si>
+  <si>
+    <t>dcterms:isPartOf</t>
+  </si>
+  <si>
+    <t>dcterms:publisher</t>
+  </si>
+  <si>
+    <t>dcterms:rights</t>
+  </si>
+  <si>
+    <t xml:space="preserve">George E Rayment </t>
+  </si>
+  <si>
+    <t>David J Lyons</t>
+  </si>
+  <si>
+    <t>mailto:bruce.shelley@agriculture.vic.gov.au</t>
   </si>
 </sst>
 </file>
@@ -4260,7 +4297,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="yyyy\-mm\-dd;@"/>
   </numFmts>
-  <fonts count="16" x14ac:knownFonts="1">
+  <fonts count="19" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -4362,6 +4399,20 @@
       <name val="Arial"/>
       <family val="2"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF4C4C4C"/>
+      <name val="Roboto"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF7E408A"/>
+      <name val="Roboto"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <name val="Roboto"/>
+    </font>
   </fonts>
   <fills count="6">
     <fill>
@@ -4418,7 +4469,7 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="65">
+  <cellXfs count="67">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="2" applyBorder="1"/>
@@ -4541,13 +4592,15 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="2" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="2" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="15" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1" indent="1"/>
     </xf>
     <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="2" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Hyperlink" xfId="2" builtinId="8"/>
@@ -4925,8 +4978,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:M477"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="F23" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="K27" sqref="K27"/>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="B17" sqref="B17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4940,7 +4993,8 @@
     <col min="7" max="7" width="24.140625" style="4" customWidth="1"/>
     <col min="8" max="8" width="40.7109375" style="3" customWidth="1"/>
     <col min="9" max="9" width="40.7109375" style="51" customWidth="1"/>
-    <col min="10" max="11" width="24.28515625" style="15" customWidth="1"/>
+    <col min="10" max="10" width="24.28515625" style="15" customWidth="1"/>
+    <col min="11" max="11" width="73.7109375" style="15" customWidth="1"/>
     <col min="12" max="12" width="39.28515625" style="15" customWidth="1"/>
     <col min="13" max="13" width="26.7109375" style="3" bestFit="1" customWidth="1"/>
     <col min="14" max="16384" width="11.42578125" style="3"/>
@@ -5068,12 +5122,12 @@
       <c r="L6" s="15"/>
       <c r="M6" s="3"/>
     </row>
-    <row r="7" spans="1:13" s="16" customFormat="1" ht="135.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:13" s="16" customFormat="1" ht="124.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
         <v>641</v>
       </c>
       <c r="B7" s="23" t="s">
-        <v>1346</v>
+        <v>1332</v>
       </c>
       <c r="C7" s="4"/>
       <c r="D7" s="4"/>
@@ -5087,16 +5141,14 @@
       <c r="L7" s="15"/>
       <c r="M7" s="3"/>
     </row>
-    <row r="8" spans="1:13" s="16" customFormat="1" ht="45" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:13" s="16" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
         <v>638</v>
       </c>
       <c r="B8" s="36" t="s">
         <v>1065</v>
       </c>
-      <c r="C8" s="61" t="s">
-        <v>1328</v>
-      </c>
+      <c r="C8" s="61"/>
       <c r="D8" s="4"/>
       <c r="E8" s="4"/>
       <c r="F8" s="3"/>
@@ -5110,10 +5162,10 @@
     </row>
     <row r="9" spans="1:13" s="16" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
-        <v>1340</v>
-      </c>
-      <c r="B9" s="18" t="s">
-        <v>1321</v>
+        <v>1364</v>
+      </c>
+      <c r="B9" t="s">
+        <v>1319</v>
       </c>
       <c r="C9" s="4"/>
       <c r="D9" s="4"/>
@@ -5129,10 +5181,10 @@
     </row>
     <row r="10" spans="1:13" s="16" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
-        <v>1338</v>
-      </c>
-      <c r="B10" s="62" t="s">
-        <v>1322</v>
+        <v>1361</v>
+      </c>
+      <c r="B10" t="s">
+        <v>1320</v>
       </c>
       <c r="C10" s="4"/>
       <c r="D10" s="4"/>
@@ -5148,10 +5200,10 @@
     </row>
     <row r="11" spans="1:13" s="16" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A11" s="1" t="s">
-        <v>1339</v>
-      </c>
-      <c r="B11" s="62" t="s">
-        <v>1322</v>
+        <v>1363</v>
+      </c>
+      <c r="B11" t="s">
+        <v>1320</v>
       </c>
       <c r="C11" s="4"/>
       <c r="D11" s="4"/>
@@ -5167,10 +5219,10 @@
     </row>
     <row r="12" spans="1:13" s="16" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A12" s="1" t="s">
-        <v>1323</v>
-      </c>
-      <c r="B12" s="18" t="s">
-        <v>1330</v>
+        <v>1321</v>
+      </c>
+      <c r="B12" t="s">
+        <v>1365</v>
       </c>
       <c r="C12" s="4"/>
       <c r="D12" s="4"/>
@@ -5186,10 +5238,10 @@
     </row>
     <row r="13" spans="1:13" s="16" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A13" s="1" t="s">
-        <v>1323</v>
-      </c>
-      <c r="B13" s="18" t="s">
-        <v>1329</v>
+        <v>1321</v>
+      </c>
+      <c r="B13" s="66" t="s">
+        <v>1366</v>
       </c>
       <c r="C13" s="4"/>
       <c r="D13" s="4"/>
@@ -5205,10 +5257,10 @@
     </row>
     <row r="14" spans="1:13" s="16" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A14" s="1" t="s">
-        <v>1323</v>
-      </c>
-      <c r="B14" s="18" t="s">
-        <v>1324</v>
+        <v>1321</v>
+      </c>
+      <c r="B14" t="s">
+        <v>1322</v>
       </c>
       <c r="C14" s="4"/>
       <c r="D14" s="4"/>
@@ -5246,7 +5298,7 @@
         <v>643</v>
       </c>
       <c r="B16" s="41">
-        <v>44629</v>
+        <v>44643</v>
       </c>
       <c r="C16" s="4"/>
       <c r="D16" s="4"/>
@@ -5319,10 +5371,10 @@
     </row>
     <row r="20" spans="1:13" s="16" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A20" s="1" t="s">
-        <v>1331</v>
+        <v>1359</v>
       </c>
       <c r="B20" s="38" t="s">
-        <v>1332</v>
+        <v>1326</v>
       </c>
       <c r="C20" s="4"/>
       <c r="D20" s="4"/>
@@ -5338,10 +5390,10 @@
     </row>
     <row r="21" spans="1:13" s="16" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A21" s="1" t="s">
-        <v>1331</v>
-      </c>
-      <c r="B21" s="18" t="s">
-        <v>1333</v>
+        <v>1359</v>
+      </c>
+      <c r="B21" t="s">
+        <v>1327</v>
       </c>
       <c r="C21" s="4"/>
       <c r="D21" s="4"/>
@@ -5360,7 +5412,7 @@
         <v>644</v>
       </c>
       <c r="B22" s="38" t="s">
-        <v>1334</v>
+        <v>1367</v>
       </c>
       <c r="C22" s="4"/>
       <c r="D22" s="4"/>
@@ -5375,11 +5427,11 @@
       <c r="M22" s="3"/>
     </row>
     <row r="23" spans="1:13" s="16" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A23" s="50" t="s">
-        <v>1335</v>
+      <c r="A23" s="1" t="s">
+        <v>1360</v>
       </c>
       <c r="B23" s="38" t="s">
-        <v>1337</v>
+        <v>1357</v>
       </c>
       <c r="C23" s="4"/>
       <c r="D23" s="4"/>
@@ -5395,10 +5447,10 @@
     </row>
     <row r="24" spans="1:13" s="16" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A24" s="1" t="s">
-        <v>1331</v>
+        <v>1359</v>
       </c>
       <c r="B24" s="38" t="s">
-        <v>1336</v>
+        <v>1358</v>
       </c>
       <c r="C24" s="4"/>
       <c r="D24" s="4"/>
@@ -5416,7 +5468,7 @@
       <c r="A25" s="1" t="s">
         <v>645</v>
       </c>
-      <c r="B25" s="26" t="s">
+      <c r="B25" t="s">
         <v>636</v>
       </c>
       <c r="C25" s="4"/>
@@ -5454,7 +5506,7 @@
       <c r="A27" s="1" t="s">
         <v>1064</v>
       </c>
-      <c r="B27" s="26" t="s">
+      <c r="B27" t="s">
         <v>1066</v>
       </c>
       <c r="C27" s="4"/>
@@ -5489,8 +5541,12 @@
       <c r="M28" s="3"/>
     </row>
     <row r="29" spans="1:13" s="16" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A29" s="3"/>
-      <c r="B29" s="4"/>
+      <c r="A29" s="43" t="s">
+        <v>1353</v>
+      </c>
+      <c r="B29" s="64" t="s">
+        <v>1354</v>
+      </c>
       <c r="C29" s="3"/>
       <c r="D29" s="3"/>
       <c r="E29" s="4"/>
@@ -5578,16 +5634,16 @@
         <v>638</v>
       </c>
       <c r="I33" s="54" t="s">
-        <v>1320</v>
+        <v>1318</v>
       </c>
       <c r="J33" s="48" t="s">
         <v>1315</v>
       </c>
       <c r="K33" s="48" t="s">
-        <v>1326</v>
+        <v>1324</v>
       </c>
       <c r="L33" s="42" t="s">
-        <v>1325</v>
+        <v>1323</v>
       </c>
       <c r="M33" s="21" t="s">
         <v>639</v>
@@ -5617,10 +5673,10 @@
       <c r="I34" s="55"/>
       <c r="J34" s="32"/>
       <c r="K34" s="32" t="s">
-        <v>1348</v>
+        <v>1334</v>
       </c>
       <c r="L34" s="29" t="s">
-        <v>1327</v>
+        <v>1325</v>
       </c>
       <c r="M34" s="32" t="s">
         <v>1062</v>
@@ -5652,10 +5708,10 @@
       <c r="I35" s="55"/>
       <c r="J35" s="32"/>
       <c r="K35" s="32" t="s">
-        <v>1348</v>
+        <v>1334</v>
       </c>
       <c r="L35" s="29" t="s">
-        <v>1327</v>
+        <v>1325</v>
       </c>
       <c r="M35" s="32" t="s">
         <v>1062</v>
@@ -5687,10 +5743,10 @@
       <c r="I36" s="55"/>
       <c r="J36" s="32"/>
       <c r="K36" s="32" t="s">
-        <v>1348</v>
+        <v>1334</v>
       </c>
       <c r="L36" s="29" t="s">
-        <v>1327</v>
+        <v>1325</v>
       </c>
       <c r="M36" s="32" t="s">
         <v>1062</v>
@@ -5722,10 +5778,10 @@
       <c r="I37" s="55"/>
       <c r="J37" s="32"/>
       <c r="K37" s="32" t="s">
-        <v>1348</v>
+        <v>1334</v>
       </c>
       <c r="L37" s="29" t="s">
-        <v>1327</v>
+        <v>1325</v>
       </c>
       <c r="M37" s="32" t="s">
         <v>1062</v>
@@ -5757,10 +5813,10 @@
       <c r="I38" s="55"/>
       <c r="J38" s="32"/>
       <c r="K38" s="32" t="s">
-        <v>1348</v>
+        <v>1334</v>
       </c>
       <c r="L38" s="29" t="s">
-        <v>1327</v>
+        <v>1325</v>
       </c>
       <c r="M38" s="32" t="s">
         <v>1062</v>
@@ -5790,10 +5846,10 @@
       <c r="I39" s="55"/>
       <c r="J39" s="32"/>
       <c r="K39" s="32" t="s">
-        <v>1349</v>
+        <v>1335</v>
       </c>
       <c r="L39" s="29" t="s">
-        <v>1327</v>
+        <v>1325</v>
       </c>
       <c r="M39" s="32" t="s">
         <v>1062</v>
@@ -5825,10 +5881,10 @@
       <c r="I40" s="55"/>
       <c r="J40" s="32"/>
       <c r="K40" s="32" t="s">
-        <v>1349</v>
+        <v>1335</v>
       </c>
       <c r="L40" s="29" t="s">
-        <v>1327</v>
+        <v>1325</v>
       </c>
       <c r="M40" s="32" t="s">
         <v>1062</v>
@@ -5860,10 +5916,10 @@
       <c r="I41" s="55"/>
       <c r="J41" s="32"/>
       <c r="K41" s="32" t="s">
-        <v>1349</v>
+        <v>1335</v>
       </c>
       <c r="L41" s="29" t="s">
-        <v>1327</v>
+        <v>1325</v>
       </c>
       <c r="M41" s="32" t="s">
         <v>1062</v>
@@ -5895,10 +5951,10 @@
       <c r="I42" s="55"/>
       <c r="J42" s="32"/>
       <c r="K42" s="32" t="s">
-        <v>1349</v>
+        <v>1335</v>
       </c>
       <c r="L42" s="29" t="s">
-        <v>1327</v>
+        <v>1325</v>
       </c>
       <c r="M42" s="32" t="s">
         <v>1062</v>
@@ -5930,10 +5986,10 @@
       <c r="I43" s="55"/>
       <c r="J43" s="32"/>
       <c r="K43" s="32" t="s">
-        <v>1349</v>
+        <v>1335</v>
       </c>
       <c r="L43" s="29" t="s">
-        <v>1327</v>
+        <v>1325</v>
       </c>
       <c r="M43" s="32" t="s">
         <v>1062</v>
@@ -5963,10 +6019,10 @@
       <c r="I44" s="55"/>
       <c r="J44" s="32"/>
       <c r="K44" s="32" t="s">
-        <v>1350</v>
+        <v>1336</v>
       </c>
       <c r="L44" s="29" t="s">
-        <v>1327</v>
+        <v>1325</v>
       </c>
       <c r="M44" s="32" t="s">
         <v>1062</v>
@@ -5998,10 +6054,10 @@
       <c r="I45" s="55"/>
       <c r="J45" s="32"/>
       <c r="K45" s="32" t="s">
-        <v>1350</v>
+        <v>1336</v>
       </c>
       <c r="L45" s="29" t="s">
-        <v>1327</v>
+        <v>1325</v>
       </c>
       <c r="M45" s="32" t="s">
         <v>1062</v>
@@ -6033,10 +6089,10 @@
       <c r="I46" s="55"/>
       <c r="J46" s="32"/>
       <c r="K46" s="32" t="s">
-        <v>1350</v>
+        <v>1336</v>
       </c>
       <c r="L46" s="29" t="s">
-        <v>1327</v>
+        <v>1325</v>
       </c>
       <c r="M46" s="32" t="s">
         <v>1062</v>
@@ -6068,10 +6124,10 @@
       <c r="I47" s="55"/>
       <c r="J47" s="32"/>
       <c r="K47" s="32" t="s">
-        <v>1350</v>
+        <v>1336</v>
       </c>
       <c r="L47" s="29" t="s">
-        <v>1327</v>
+        <v>1325</v>
       </c>
       <c r="M47" s="32" t="s">
         <v>1062</v>
@@ -6103,10 +6159,10 @@
       <c r="I48" s="55"/>
       <c r="J48" s="32"/>
       <c r="K48" s="32" t="s">
-        <v>1350</v>
+        <v>1336</v>
       </c>
       <c r="L48" s="29" t="s">
-        <v>1327</v>
+        <v>1325</v>
       </c>
       <c r="M48" s="32" t="s">
         <v>1062</v>
@@ -6138,10 +6194,10 @@
       <c r="I49" s="55"/>
       <c r="J49" s="32"/>
       <c r="K49" s="32" t="s">
-        <v>1350</v>
+        <v>1336</v>
       </c>
       <c r="L49" s="29" t="s">
-        <v>1327</v>
+        <v>1325</v>
       </c>
       <c r="M49" s="32" t="s">
         <v>1062</v>
@@ -6173,10 +6229,10 @@
       <c r="I50" s="55"/>
       <c r="J50" s="32"/>
       <c r="K50" s="32" t="s">
-        <v>1350</v>
+        <v>1336</v>
       </c>
       <c r="L50" s="29" t="s">
-        <v>1327</v>
+        <v>1325</v>
       </c>
       <c r="M50" s="32" t="s">
         <v>1062</v>
@@ -6208,10 +6264,10 @@
       <c r="I51" s="55"/>
       <c r="J51" s="32"/>
       <c r="K51" s="32" t="s">
-        <v>1350</v>
+        <v>1336</v>
       </c>
       <c r="L51" s="29" t="s">
-        <v>1327</v>
+        <v>1325</v>
       </c>
       <c r="M51" s="32" t="s">
         <v>1062</v>
@@ -6243,10 +6299,10 @@
       <c r="I52" s="55"/>
       <c r="J52" s="32"/>
       <c r="K52" s="32" t="s">
-        <v>1350</v>
+        <v>1336</v>
       </c>
       <c r="L52" s="29" t="s">
-        <v>1327</v>
+        <v>1325</v>
       </c>
       <c r="M52" s="32" t="s">
         <v>1062</v>
@@ -6278,10 +6334,10 @@
       <c r="I53" s="55"/>
       <c r="J53" s="32"/>
       <c r="K53" s="32" t="s">
-        <v>1350</v>
+        <v>1336</v>
       </c>
       <c r="L53" s="29" t="s">
-        <v>1327</v>
+        <v>1325</v>
       </c>
       <c r="M53" s="32" t="s">
         <v>1062</v>
@@ -6313,10 +6369,10 @@
       <c r="I54" s="55"/>
       <c r="J54" s="32"/>
       <c r="K54" s="32" t="s">
-        <v>1350</v>
+        <v>1336</v>
       </c>
       <c r="L54" s="29" t="s">
-        <v>1327</v>
+        <v>1325</v>
       </c>
       <c r="M54" s="32" t="s">
         <v>1062</v>
@@ -6348,10 +6404,10 @@
       <c r="I55" s="55"/>
       <c r="J55" s="32"/>
       <c r="K55" s="32" t="s">
-        <v>1350</v>
+        <v>1336</v>
       </c>
       <c r="L55" s="29" t="s">
-        <v>1327</v>
+        <v>1325</v>
       </c>
       <c r="M55" s="32" t="s">
         <v>1062</v>
@@ -6383,10 +6439,10 @@
       <c r="I56" s="55"/>
       <c r="J56" s="32"/>
       <c r="K56" s="32" t="s">
-        <v>1350</v>
+        <v>1336</v>
       </c>
       <c r="L56" s="29" t="s">
-        <v>1327</v>
+        <v>1325</v>
       </c>
       <c r="M56" s="32" t="s">
         <v>1062</v>
@@ -6418,10 +6474,10 @@
       <c r="I57" s="55"/>
       <c r="J57" s="32"/>
       <c r="K57" s="32" t="s">
-        <v>1350</v>
+        <v>1336</v>
       </c>
       <c r="L57" s="29" t="s">
-        <v>1327</v>
+        <v>1325</v>
       </c>
       <c r="M57" s="32" t="s">
         <v>1062</v>
@@ -6453,10 +6509,10 @@
       <c r="I58" s="55"/>
       <c r="J58" s="32"/>
       <c r="K58" s="32" t="s">
-        <v>1350</v>
+        <v>1336</v>
       </c>
       <c r="L58" s="29" t="s">
-        <v>1327</v>
+        <v>1325</v>
       </c>
       <c r="M58" s="32" t="s">
         <v>1062</v>
@@ -6488,10 +6544,10 @@
       <c r="I59" s="55"/>
       <c r="J59" s="32"/>
       <c r="K59" s="32" t="s">
-        <v>1350</v>
+        <v>1336</v>
       </c>
       <c r="L59" s="29" t="s">
-        <v>1327</v>
+        <v>1325</v>
       </c>
       <c r="M59" s="32" t="s">
         <v>1062</v>
@@ -6523,10 +6579,10 @@
       <c r="I60" s="55"/>
       <c r="J60" s="32"/>
       <c r="K60" s="32" t="s">
-        <v>1350</v>
+        <v>1336</v>
       </c>
       <c r="L60" s="29" t="s">
-        <v>1327</v>
+        <v>1325</v>
       </c>
       <c r="M60" s="32" t="s">
         <v>1062</v>
@@ -6556,10 +6612,10 @@
       <c r="I61" s="55"/>
       <c r="J61" s="32"/>
       <c r="K61" s="32" t="s">
-        <v>1351</v>
+        <v>1337</v>
       </c>
       <c r="L61" s="29" t="s">
-        <v>1327</v>
+        <v>1325</v>
       </c>
       <c r="M61" s="32" t="s">
         <v>1062</v>
@@ -6591,10 +6647,10 @@
       <c r="I62" s="55"/>
       <c r="J62" s="32"/>
       <c r="K62" s="32" t="s">
-        <v>1351</v>
+        <v>1337</v>
       </c>
       <c r="L62" s="29" t="s">
-        <v>1327</v>
+        <v>1325</v>
       </c>
       <c r="M62" s="32" t="s">
         <v>1062</v>
@@ -6630,10 +6686,10 @@
       </c>
       <c r="J63" s="32"/>
       <c r="K63" s="32" t="s">
-        <v>1351</v>
+        <v>1337</v>
       </c>
       <c r="L63" s="29" t="s">
-        <v>1327</v>
+        <v>1325</v>
       </c>
       <c r="M63" s="32" t="s">
         <v>1062</v>
@@ -6669,10 +6725,10 @@
       </c>
       <c r="J64" s="32"/>
       <c r="K64" s="32" t="s">
-        <v>1351</v>
+        <v>1337</v>
       </c>
       <c r="L64" s="29" t="s">
-        <v>1327</v>
+        <v>1325</v>
       </c>
       <c r="M64" s="32" t="s">
         <v>1062</v>
@@ -6704,10 +6760,10 @@
       <c r="I65" s="55"/>
       <c r="J65" s="32"/>
       <c r="K65" s="32" t="s">
-        <v>1351</v>
+        <v>1337</v>
       </c>
       <c r="L65" s="29" t="s">
-        <v>1327</v>
+        <v>1325</v>
       </c>
       <c r="M65" s="32" t="s">
         <v>1062</v>
@@ -6739,10 +6795,10 @@
       <c r="I66" s="55"/>
       <c r="J66" s="32"/>
       <c r="K66" s="32" t="s">
-        <v>1351</v>
+        <v>1337</v>
       </c>
       <c r="L66" s="29" t="s">
-        <v>1327</v>
+        <v>1325</v>
       </c>
       <c r="M66" s="32" t="s">
         <v>1062</v>
@@ -6774,10 +6830,10 @@
       <c r="I67" s="55"/>
       <c r="J67" s="32"/>
       <c r="K67" s="32" t="s">
-        <v>1351</v>
+        <v>1337</v>
       </c>
       <c r="L67" s="29" t="s">
-        <v>1327</v>
+        <v>1325</v>
       </c>
       <c r="M67" s="32" t="s">
         <v>1062</v>
@@ -6807,10 +6863,10 @@
       <c r="I68" s="55"/>
       <c r="J68" s="32"/>
       <c r="K68" s="32" t="s">
-        <v>1352</v>
+        <v>1338</v>
       </c>
       <c r="L68" s="29" t="s">
-        <v>1327</v>
+        <v>1325</v>
       </c>
       <c r="M68" s="32" t="s">
         <v>1062</v>
@@ -6842,10 +6898,10 @@
       <c r="I69" s="55"/>
       <c r="J69" s="32"/>
       <c r="K69" s="32" t="s">
-        <v>1352</v>
+        <v>1338</v>
       </c>
       <c r="L69" s="29" t="s">
-        <v>1327</v>
+        <v>1325</v>
       </c>
       <c r="M69" s="32" t="s">
         <v>1062</v>
@@ -6877,10 +6933,10 @@
       <c r="I70" s="55"/>
       <c r="J70" s="32"/>
       <c r="K70" s="32" t="s">
-        <v>1352</v>
+        <v>1338</v>
       </c>
       <c r="L70" s="29" t="s">
-        <v>1327</v>
+        <v>1325</v>
       </c>
       <c r="M70" s="32" t="s">
         <v>1062</v>
@@ -6912,10 +6968,10 @@
       <c r="I71" s="55"/>
       <c r="J71" s="32"/>
       <c r="K71" s="32" t="s">
-        <v>1352</v>
+        <v>1338</v>
       </c>
       <c r="L71" s="29" t="s">
-        <v>1327</v>
+        <v>1325</v>
       </c>
       <c r="M71" s="32" t="s">
         <v>1062</v>
@@ -6949,10 +7005,10 @@
       <c r="I72" s="55"/>
       <c r="J72" s="32"/>
       <c r="K72" s="32" t="s">
-        <v>1352</v>
+        <v>1338</v>
       </c>
       <c r="L72" s="29" t="s">
-        <v>1327</v>
+        <v>1325</v>
       </c>
       <c r="M72" s="32" t="s">
         <v>1062</v>
@@ -6986,10 +7042,10 @@
       <c r="I73" s="55"/>
       <c r="J73" s="32"/>
       <c r="K73" s="32" t="s">
-        <v>1352</v>
+        <v>1338</v>
       </c>
       <c r="L73" s="29" t="s">
-        <v>1327</v>
+        <v>1325</v>
       </c>
       <c r="M73" s="32" t="s">
         <v>1062</v>
@@ -7021,10 +7077,10 @@
       <c r="I74" s="55"/>
       <c r="J74" s="32"/>
       <c r="K74" s="32" t="s">
-        <v>1352</v>
+        <v>1338</v>
       </c>
       <c r="L74" s="29" t="s">
-        <v>1327</v>
+        <v>1325</v>
       </c>
       <c r="M74" s="32" t="s">
         <v>1062</v>
@@ -7056,10 +7112,10 @@
       <c r="I75" s="55"/>
       <c r="J75" s="32"/>
       <c r="K75" s="32" t="s">
-        <v>1352</v>
+        <v>1338</v>
       </c>
       <c r="L75" s="29" t="s">
-        <v>1327</v>
+        <v>1325</v>
       </c>
       <c r="M75" s="32" t="s">
         <v>1062</v>
@@ -7093,10 +7149,10 @@
       <c r="I76" s="55"/>
       <c r="J76" s="32"/>
       <c r="K76" s="32" t="s">
-        <v>1352</v>
+        <v>1338</v>
       </c>
       <c r="L76" s="29" t="s">
-        <v>1327</v>
+        <v>1325</v>
       </c>
       <c r="M76" s="32" t="s">
         <v>1062</v>
@@ -7130,10 +7186,10 @@
       <c r="I77" s="55"/>
       <c r="J77" s="32"/>
       <c r="K77" s="32" t="s">
-        <v>1352</v>
+        <v>1338</v>
       </c>
       <c r="L77" s="29" t="s">
-        <v>1327</v>
+        <v>1325</v>
       </c>
       <c r="M77" s="32" t="s">
         <v>1062</v>
@@ -7165,10 +7221,10 @@
       <c r="I78" s="55"/>
       <c r="J78" s="32"/>
       <c r="K78" s="32" t="s">
-        <v>1352</v>
+        <v>1338</v>
       </c>
       <c r="L78" s="29" t="s">
-        <v>1327</v>
+        <v>1325</v>
       </c>
       <c r="M78" s="32" t="s">
         <v>1062</v>
@@ -7200,10 +7256,10 @@
       <c r="I79" s="55"/>
       <c r="J79" s="32"/>
       <c r="K79" s="32" t="s">
-        <v>1352</v>
+        <v>1338</v>
       </c>
       <c r="L79" s="29" t="s">
-        <v>1327</v>
+        <v>1325</v>
       </c>
       <c r="M79" s="32" t="s">
         <v>1062</v>
@@ -7235,10 +7291,10 @@
       <c r="I80" s="55"/>
       <c r="J80" s="32"/>
       <c r="K80" s="32" t="s">
-        <v>1352</v>
+        <v>1338</v>
       </c>
       <c r="L80" s="29" t="s">
-        <v>1327</v>
+        <v>1325</v>
       </c>
       <c r="M80" s="32" t="s">
         <v>1062</v>
@@ -7270,10 +7326,10 @@
       <c r="I81" s="55"/>
       <c r="J81" s="32"/>
       <c r="K81" s="32" t="s">
-        <v>1352</v>
+        <v>1338</v>
       </c>
       <c r="L81" s="29" t="s">
-        <v>1327</v>
+        <v>1325</v>
       </c>
       <c r="M81" s="32" t="s">
         <v>1062</v>
@@ -7305,10 +7361,10 @@
       <c r="I82" s="55"/>
       <c r="J82" s="32"/>
       <c r="K82" s="32" t="s">
-        <v>1352</v>
+        <v>1338</v>
       </c>
       <c r="L82" s="29" t="s">
-        <v>1327</v>
+        <v>1325</v>
       </c>
       <c r="M82" s="32" t="s">
         <v>1062</v>
@@ -7338,10 +7394,10 @@
       <c r="I83" s="55"/>
       <c r="J83" s="32"/>
       <c r="K83" s="32" t="s">
-        <v>1353</v>
+        <v>1339</v>
       </c>
       <c r="L83" s="29" t="s">
-        <v>1327</v>
+        <v>1325</v>
       </c>
       <c r="M83" s="32" t="s">
         <v>1062</v>
@@ -7373,10 +7429,10 @@
       <c r="I84" s="55"/>
       <c r="J84" s="32"/>
       <c r="K84" s="32" t="s">
-        <v>1353</v>
+        <v>1339</v>
       </c>
       <c r="L84" s="29" t="s">
-        <v>1327</v>
+        <v>1325</v>
       </c>
       <c r="M84" s="32" t="s">
         <v>1062</v>
@@ -7412,10 +7468,10 @@
       </c>
       <c r="J85" s="32"/>
       <c r="K85" s="32" t="s">
-        <v>1353</v>
+        <v>1339</v>
       </c>
       <c r="L85" s="29" t="s">
-        <v>1327</v>
+        <v>1325</v>
       </c>
       <c r="M85" s="32" t="s">
         <v>1062</v>
@@ -7451,10 +7507,10 @@
       </c>
       <c r="J86" s="32"/>
       <c r="K86" s="32" t="s">
-        <v>1353</v>
+        <v>1339</v>
       </c>
       <c r="L86" s="29" t="s">
-        <v>1327</v>
+        <v>1325</v>
       </c>
       <c r="M86" s="32" t="s">
         <v>1062</v>
@@ -7486,10 +7542,10 @@
       <c r="I87" s="55"/>
       <c r="J87" s="32"/>
       <c r="K87" s="32" t="s">
-        <v>1353</v>
+        <v>1339</v>
       </c>
       <c r="L87" s="29" t="s">
-        <v>1327</v>
+        <v>1325</v>
       </c>
       <c r="M87" s="32" t="s">
         <v>1062</v>
@@ -7521,10 +7577,10 @@
       <c r="I88" s="55"/>
       <c r="J88" s="32"/>
       <c r="K88" s="32" t="s">
-        <v>1353</v>
+        <v>1339</v>
       </c>
       <c r="L88" s="29" t="s">
-        <v>1327</v>
+        <v>1325</v>
       </c>
       <c r="M88" s="32" t="s">
         <v>1062</v>
@@ -7556,10 +7612,10 @@
       <c r="I89" s="55"/>
       <c r="J89" s="32"/>
       <c r="K89" s="32" t="s">
-        <v>1353</v>
+        <v>1339</v>
       </c>
       <c r="L89" s="29" t="s">
-        <v>1327</v>
+        <v>1325</v>
       </c>
       <c r="M89" s="32" t="s">
         <v>1062</v>
@@ -7591,10 +7647,10 @@
       <c r="I90" s="55"/>
       <c r="J90" s="32"/>
       <c r="K90" s="32" t="s">
-        <v>1353</v>
+        <v>1339</v>
       </c>
       <c r="L90" s="29" t="s">
-        <v>1327</v>
+        <v>1325</v>
       </c>
       <c r="M90" s="32" t="s">
         <v>1062</v>
@@ -7628,10 +7684,10 @@
       <c r="I91" s="55"/>
       <c r="J91" s="32"/>
       <c r="K91" s="32" t="s">
-        <v>1353</v>
+        <v>1339</v>
       </c>
       <c r="L91" s="29" t="s">
-        <v>1327</v>
+        <v>1325</v>
       </c>
       <c r="M91" s="32" t="s">
         <v>1062</v>
@@ -7665,10 +7721,10 @@
       <c r="I92" s="55"/>
       <c r="J92" s="32"/>
       <c r="K92" s="32" t="s">
-        <v>1353</v>
+        <v>1339</v>
       </c>
       <c r="L92" s="29" t="s">
-        <v>1327</v>
+        <v>1325</v>
       </c>
       <c r="M92" s="32" t="s">
         <v>1062</v>
@@ -7700,10 +7756,10 @@
       <c r="I93" s="55"/>
       <c r="J93" s="32"/>
       <c r="K93" s="32" t="s">
-        <v>1353</v>
+        <v>1339</v>
       </c>
       <c r="L93" s="29" t="s">
-        <v>1327</v>
+        <v>1325</v>
       </c>
       <c r="M93" s="32" t="s">
         <v>1062</v>
@@ -7739,10 +7795,10 @@
       </c>
       <c r="J94" s="32"/>
       <c r="K94" s="32" t="s">
-        <v>1353</v>
+        <v>1339</v>
       </c>
       <c r="L94" s="29" t="s">
-        <v>1327</v>
+        <v>1325</v>
       </c>
       <c r="M94" s="32" t="s">
         <v>1062</v>
@@ -7778,10 +7834,10 @@
       </c>
       <c r="J95" s="32"/>
       <c r="K95" s="32" t="s">
-        <v>1353</v>
+        <v>1339</v>
       </c>
       <c r="L95" s="29" t="s">
-        <v>1327</v>
+        <v>1325</v>
       </c>
       <c r="M95" s="32" t="s">
         <v>1062</v>
@@ -7815,10 +7871,10 @@
       <c r="I96" s="55"/>
       <c r="J96" s="32"/>
       <c r="K96" s="32" t="s">
-        <v>1353</v>
+        <v>1339</v>
       </c>
       <c r="L96" s="29" t="s">
-        <v>1327</v>
+        <v>1325</v>
       </c>
       <c r="M96" s="32" t="s">
         <v>1062</v>
@@ -7850,10 +7906,10 @@
       <c r="I97" s="55"/>
       <c r="J97" s="32"/>
       <c r="K97" s="32" t="s">
-        <v>1353</v>
+        <v>1339</v>
       </c>
       <c r="L97" s="29" t="s">
-        <v>1327</v>
+        <v>1325</v>
       </c>
       <c r="M97" s="32" t="s">
         <v>1062</v>
@@ -7887,10 +7943,10 @@
       <c r="I98" s="55"/>
       <c r="J98" s="32"/>
       <c r="K98" s="32" t="s">
-        <v>1353</v>
+        <v>1339</v>
       </c>
       <c r="L98" s="29" t="s">
-        <v>1327</v>
+        <v>1325</v>
       </c>
       <c r="M98" s="32" t="s">
         <v>1062</v>
@@ -7924,10 +7980,10 @@
       <c r="I99" s="55"/>
       <c r="J99" s="32"/>
       <c r="K99" s="32" t="s">
-        <v>1353</v>
+        <v>1339</v>
       </c>
       <c r="L99" s="29" t="s">
-        <v>1327</v>
+        <v>1325</v>
       </c>
       <c r="M99" s="32" t="s">
         <v>1062</v>
@@ -7961,10 +8017,10 @@
       <c r="I100" s="55"/>
       <c r="J100" s="32"/>
       <c r="K100" s="32" t="s">
-        <v>1353</v>
+        <v>1339</v>
       </c>
       <c r="L100" s="29" t="s">
-        <v>1327</v>
+        <v>1325</v>
       </c>
       <c r="M100" s="32" t="s">
         <v>1062</v>
@@ -7998,10 +8054,10 @@
       <c r="I101" s="55"/>
       <c r="J101" s="32"/>
       <c r="K101" s="32" t="s">
-        <v>1353</v>
+        <v>1339</v>
       </c>
       <c r="L101" s="29" t="s">
-        <v>1327</v>
+        <v>1325</v>
       </c>
       <c r="M101" s="32" t="s">
         <v>1062</v>
@@ -8035,10 +8091,10 @@
       <c r="I102" s="55"/>
       <c r="J102" s="32"/>
       <c r="K102" s="32" t="s">
-        <v>1353</v>
+        <v>1339</v>
       </c>
       <c r="L102" s="29" t="s">
-        <v>1327</v>
+        <v>1325</v>
       </c>
       <c r="M102" s="32" t="s">
         <v>1062</v>
@@ -8072,10 +8128,10 @@
       <c r="I103" s="55"/>
       <c r="J103" s="32"/>
       <c r="K103" s="32" t="s">
-        <v>1353</v>
+        <v>1339</v>
       </c>
       <c r="L103" s="29" t="s">
-        <v>1327</v>
+        <v>1325</v>
       </c>
       <c r="M103" s="32" t="s">
         <v>1062</v>
@@ -8109,10 +8165,10 @@
       <c r="I104" s="55"/>
       <c r="J104" s="32"/>
       <c r="K104" s="32" t="s">
-        <v>1353</v>
+        <v>1339</v>
       </c>
       <c r="L104" s="29" t="s">
-        <v>1327</v>
+        <v>1325</v>
       </c>
       <c r="M104" s="32" t="s">
         <v>1062</v>
@@ -8146,10 +8202,10 @@
       <c r="I105" s="55"/>
       <c r="J105" s="32"/>
       <c r="K105" s="32" t="s">
-        <v>1353</v>
+        <v>1339</v>
       </c>
       <c r="L105" s="29" t="s">
-        <v>1327</v>
+        <v>1325</v>
       </c>
       <c r="M105" s="32" t="s">
         <v>1062</v>
@@ -8185,10 +8241,10 @@
       </c>
       <c r="J106" s="32"/>
       <c r="K106" s="32" t="s">
-        <v>1353</v>
+        <v>1339</v>
       </c>
       <c r="L106" s="29" t="s">
-        <v>1327</v>
+        <v>1325</v>
       </c>
       <c r="M106" s="32" t="s">
         <v>1062</v>
@@ -8224,10 +8280,10 @@
       </c>
       <c r="J107" s="32"/>
       <c r="K107" s="32" t="s">
-        <v>1353</v>
+        <v>1339</v>
       </c>
       <c r="L107" s="29" t="s">
-        <v>1327</v>
+        <v>1325</v>
       </c>
       <c r="M107" s="32" t="s">
         <v>1062</v>
@@ -8259,10 +8315,10 @@
       <c r="I108" s="55"/>
       <c r="J108" s="32"/>
       <c r="K108" s="32" t="s">
-        <v>1353</v>
+        <v>1339</v>
       </c>
       <c r="L108" s="29" t="s">
-        <v>1327</v>
+        <v>1325</v>
       </c>
       <c r="M108" s="32" t="s">
         <v>1062</v>
@@ -8296,10 +8352,10 @@
       <c r="I109" s="55"/>
       <c r="J109" s="32"/>
       <c r="K109" s="32" t="s">
-        <v>1353</v>
+        <v>1339</v>
       </c>
       <c r="L109" s="29" t="s">
-        <v>1327</v>
+        <v>1325</v>
       </c>
       <c r="M109" s="32" t="s">
         <v>1062</v>
@@ -8333,10 +8389,10 @@
       <c r="I110" s="55"/>
       <c r="J110" s="32"/>
       <c r="K110" s="32" t="s">
-        <v>1353</v>
+        <v>1339</v>
       </c>
       <c r="L110" s="29" t="s">
-        <v>1327</v>
+        <v>1325</v>
       </c>
       <c r="M110" s="32" t="s">
         <v>1062</v>
@@ -8370,10 +8426,10 @@
       <c r="I111" s="55"/>
       <c r="J111" s="32"/>
       <c r="K111" s="32" t="s">
-        <v>1353</v>
+        <v>1339</v>
       </c>
       <c r="L111" s="29" t="s">
-        <v>1327</v>
+        <v>1325</v>
       </c>
       <c r="M111" s="32" t="s">
         <v>1062</v>
@@ -8407,10 +8463,10 @@
       <c r="I112" s="55"/>
       <c r="J112" s="29"/>
       <c r="K112" s="32" t="s">
-        <v>1353</v>
+        <v>1339</v>
       </c>
       <c r="L112" s="29" t="s">
-        <v>1327</v>
+        <v>1325</v>
       </c>
       <c r="M112" s="32" t="s">
         <v>1062</v>
@@ -8444,10 +8500,10 @@
       <c r="I113" s="55"/>
       <c r="J113" s="32"/>
       <c r="K113" s="32" t="s">
-        <v>1353</v>
+        <v>1339</v>
       </c>
       <c r="L113" s="29" t="s">
-        <v>1327</v>
+        <v>1325</v>
       </c>
       <c r="M113" s="32" t="s">
         <v>1062</v>
@@ -8477,10 +8533,10 @@
       <c r="I114" s="55"/>
       <c r="J114" s="32"/>
       <c r="K114" s="32" t="s">
-        <v>1354</v>
+        <v>1340</v>
       </c>
       <c r="L114" s="29" t="s">
-        <v>1327</v>
+        <v>1325</v>
       </c>
       <c r="M114" s="32" t="s">
         <v>1062</v>
@@ -8512,10 +8568,10 @@
       <c r="I115" s="55"/>
       <c r="J115" s="32"/>
       <c r="K115" s="32" t="s">
-        <v>1354</v>
+        <v>1340</v>
       </c>
       <c r="L115" s="29" t="s">
-        <v>1327</v>
+        <v>1325</v>
       </c>
       <c r="M115" s="32" t="s">
         <v>1062</v>
@@ -8547,10 +8603,10 @@
       <c r="I116" s="55"/>
       <c r="J116" s="32"/>
       <c r="K116" s="32" t="s">
-        <v>1354</v>
+        <v>1340</v>
       </c>
       <c r="L116" s="29" t="s">
-        <v>1327</v>
+        <v>1325</v>
       </c>
       <c r="M116" s="32" t="s">
         <v>1062</v>
@@ -8580,10 +8636,10 @@
       <c r="I117" s="55"/>
       <c r="J117" s="32"/>
       <c r="K117" s="32" t="s">
-        <v>1355</v>
+        <v>1341</v>
       </c>
       <c r="L117" s="29" t="s">
-        <v>1327</v>
+        <v>1325</v>
       </c>
       <c r="M117" s="32" t="s">
         <v>1062</v>
@@ -8615,10 +8671,10 @@
       <c r="I118" s="55"/>
       <c r="J118" s="32"/>
       <c r="K118" s="32" t="s">
-        <v>1355</v>
+        <v>1341</v>
       </c>
       <c r="L118" s="29" t="s">
-        <v>1327</v>
+        <v>1325</v>
       </c>
       <c r="M118" s="32" t="s">
         <v>1062</v>
@@ -8652,10 +8708,10 @@
       <c r="I119" s="55"/>
       <c r="J119" s="32"/>
       <c r="K119" s="32" t="s">
-        <v>1355</v>
+        <v>1341</v>
       </c>
       <c r="L119" s="29" t="s">
-        <v>1327</v>
+        <v>1325</v>
       </c>
       <c r="M119" s="32" t="s">
         <v>1062</v>
@@ -8689,10 +8745,10 @@
       <c r="I120" s="55"/>
       <c r="J120" s="32"/>
       <c r="K120" s="32" t="s">
-        <v>1355</v>
+        <v>1341</v>
       </c>
       <c r="L120" s="29" t="s">
-        <v>1327</v>
+        <v>1325</v>
       </c>
       <c r="M120" s="32" t="s">
         <v>1062</v>
@@ -8726,10 +8782,10 @@
       <c r="I121" s="55"/>
       <c r="J121" s="32"/>
       <c r="K121" s="32" t="s">
-        <v>1355</v>
+        <v>1341</v>
       </c>
       <c r="L121" s="29" t="s">
-        <v>1327</v>
+        <v>1325</v>
       </c>
       <c r="M121" s="32" t="s">
         <v>1062</v>
@@ -8763,10 +8819,10 @@
       <c r="I122" s="55"/>
       <c r="J122" s="32"/>
       <c r="K122" s="32" t="s">
-        <v>1355</v>
+        <v>1341</v>
       </c>
       <c r="L122" s="29" t="s">
-        <v>1327</v>
+        <v>1325</v>
       </c>
       <c r="M122" s="32" t="s">
         <v>1062</v>
@@ -8798,10 +8854,10 @@
       <c r="I123" s="55"/>
       <c r="J123" s="32"/>
       <c r="K123" s="32" t="s">
-        <v>1355</v>
+        <v>1341</v>
       </c>
       <c r="L123" s="29" t="s">
-        <v>1327</v>
+        <v>1325</v>
       </c>
       <c r="M123" s="32" t="s">
         <v>1062</v>
@@ -8835,10 +8891,10 @@
       <c r="I124" s="55"/>
       <c r="J124" s="32"/>
       <c r="K124" s="32" t="s">
-        <v>1355</v>
+        <v>1341</v>
       </c>
       <c r="L124" s="29" t="s">
-        <v>1327</v>
+        <v>1325</v>
       </c>
       <c r="M124" s="32" t="s">
         <v>1062</v>
@@ -8872,10 +8928,10 @@
       <c r="I125" s="55"/>
       <c r="J125" s="32"/>
       <c r="K125" s="32" t="s">
-        <v>1355</v>
+        <v>1341</v>
       </c>
       <c r="L125" s="29" t="s">
-        <v>1327</v>
+        <v>1325</v>
       </c>
       <c r="M125" s="32" t="s">
         <v>1062</v>
@@ -8907,10 +8963,10 @@
       <c r="I126" s="55"/>
       <c r="J126" s="32"/>
       <c r="K126" s="32" t="s">
-        <v>1355</v>
+        <v>1341</v>
       </c>
       <c r="L126" s="29" t="s">
-        <v>1327</v>
+        <v>1325</v>
       </c>
       <c r="M126" s="32" t="s">
         <v>1062</v>
@@ -8944,10 +9000,10 @@
       <c r="I127" s="55"/>
       <c r="J127" s="32"/>
       <c r="K127" s="32" t="s">
-        <v>1355</v>
+        <v>1341</v>
       </c>
       <c r="L127" s="29" t="s">
-        <v>1327</v>
+        <v>1325</v>
       </c>
       <c r="M127" s="32" t="s">
         <v>1062</v>
@@ -8983,10 +9039,10 @@
       </c>
       <c r="J128" s="32"/>
       <c r="K128" s="32" t="s">
-        <v>1355</v>
+        <v>1341</v>
       </c>
       <c r="L128" s="29" t="s">
-        <v>1327</v>
+        <v>1325</v>
       </c>
       <c r="M128" s="32" t="s">
         <v>1062</v>
@@ -9022,10 +9078,10 @@
       </c>
       <c r="J129" s="32"/>
       <c r="K129" s="32" t="s">
-        <v>1355</v>
+        <v>1341</v>
       </c>
       <c r="L129" s="29" t="s">
-        <v>1327</v>
+        <v>1325</v>
       </c>
       <c r="M129" s="32" t="s">
         <v>1062</v>
@@ -9057,10 +9113,10 @@
       <c r="I130" s="55"/>
       <c r="J130" s="32"/>
       <c r="K130" s="32" t="s">
-        <v>1355</v>
+        <v>1341</v>
       </c>
       <c r="L130" s="29" t="s">
-        <v>1327</v>
+        <v>1325</v>
       </c>
       <c r="M130" s="32" t="s">
         <v>1062</v>
@@ -9092,10 +9148,10 @@
       <c r="I131" s="55"/>
       <c r="J131" s="32"/>
       <c r="K131" s="32" t="s">
-        <v>1355</v>
+        <v>1341</v>
       </c>
       <c r="L131" s="29" t="s">
-        <v>1327</v>
+        <v>1325</v>
       </c>
       <c r="M131" s="32" t="s">
         <v>1062</v>
@@ -9129,10 +9185,10 @@
       <c r="I132" s="55"/>
       <c r="J132" s="32"/>
       <c r="K132" s="32" t="s">
-        <v>1355</v>
+        <v>1341</v>
       </c>
       <c r="L132" s="29" t="s">
-        <v>1327</v>
+        <v>1325</v>
       </c>
       <c r="M132" s="32" t="s">
         <v>1062</v>
@@ -9166,10 +9222,10 @@
       <c r="I133" s="55"/>
       <c r="J133" s="32"/>
       <c r="K133" s="32" t="s">
-        <v>1355</v>
+        <v>1341</v>
       </c>
       <c r="L133" s="29" t="s">
-        <v>1327</v>
+        <v>1325</v>
       </c>
       <c r="M133" s="32" t="s">
         <v>1062</v>
@@ -9201,10 +9257,10 @@
       <c r="I134" s="55"/>
       <c r="J134" s="32"/>
       <c r="K134" s="32" t="s">
-        <v>1355</v>
+        <v>1341</v>
       </c>
       <c r="L134" s="29" t="s">
-        <v>1327</v>
+        <v>1325</v>
       </c>
       <c r="M134" s="32" t="s">
         <v>1062</v>
@@ -9236,10 +9292,10 @@
       <c r="I135" s="55"/>
       <c r="J135" s="32"/>
       <c r="K135" s="32" t="s">
-        <v>1355</v>
+        <v>1341</v>
       </c>
       <c r="L135" s="29" t="s">
-        <v>1327</v>
+        <v>1325</v>
       </c>
       <c r="M135" s="32" t="s">
         <v>1062</v>
@@ -9271,10 +9327,10 @@
       <c r="I136" s="55"/>
       <c r="J136" s="32"/>
       <c r="K136" s="32" t="s">
-        <v>1355</v>
+        <v>1341</v>
       </c>
       <c r="L136" s="29" t="s">
-        <v>1327</v>
+        <v>1325</v>
       </c>
       <c r="M136" s="32" t="s">
         <v>1062</v>
@@ -9306,10 +9362,10 @@
       <c r="I137" s="55"/>
       <c r="J137" s="32"/>
       <c r="K137" s="32" t="s">
-        <v>1355</v>
+        <v>1341</v>
       </c>
       <c r="L137" s="29" t="s">
-        <v>1327</v>
+        <v>1325</v>
       </c>
       <c r="M137" s="32" t="s">
         <v>1062</v>
@@ -9341,10 +9397,10 @@
       <c r="I138" s="55"/>
       <c r="J138" s="32"/>
       <c r="K138" s="32" t="s">
-        <v>1355</v>
+        <v>1341</v>
       </c>
       <c r="L138" s="29" t="s">
-        <v>1327</v>
+        <v>1325</v>
       </c>
       <c r="M138" s="32" t="s">
         <v>1062</v>
@@ -9376,10 +9432,10 @@
       <c r="I139" s="55"/>
       <c r="J139" s="32"/>
       <c r="K139" s="32" t="s">
-        <v>1355</v>
+        <v>1341</v>
       </c>
       <c r="L139" s="29" t="s">
-        <v>1327</v>
+        <v>1325</v>
       </c>
       <c r="M139" s="32" t="s">
         <v>1062</v>
@@ -9413,10 +9469,10 @@
       <c r="I140" s="55"/>
       <c r="J140" s="32"/>
       <c r="K140" s="32" t="s">
-        <v>1355</v>
+        <v>1341</v>
       </c>
       <c r="L140" s="29" t="s">
-        <v>1327</v>
+        <v>1325</v>
       </c>
       <c r="M140" s="32" t="s">
         <v>1062</v>
@@ -9450,10 +9506,10 @@
       <c r="I141" s="55"/>
       <c r="J141" s="32"/>
       <c r="K141" s="32" t="s">
-        <v>1355</v>
+        <v>1341</v>
       </c>
       <c r="L141" s="29" t="s">
-        <v>1327</v>
+        <v>1325</v>
       </c>
       <c r="M141" s="32" t="s">
         <v>1062</v>
@@ -9487,10 +9543,10 @@
       <c r="I142" s="55"/>
       <c r="J142" s="32"/>
       <c r="K142" s="32" t="s">
-        <v>1355</v>
+        <v>1341</v>
       </c>
       <c r="L142" s="29" t="s">
-        <v>1327</v>
+        <v>1325</v>
       </c>
       <c r="M142" s="32" t="s">
         <v>1062</v>
@@ -9524,10 +9580,10 @@
       <c r="I143" s="55"/>
       <c r="J143" s="32"/>
       <c r="K143" s="32" t="s">
-        <v>1355</v>
+        <v>1341</v>
       </c>
       <c r="L143" s="29" t="s">
-        <v>1327</v>
+        <v>1325</v>
       </c>
       <c r="M143" s="32" t="s">
         <v>1062</v>
@@ -9561,10 +9617,10 @@
       <c r="I144" s="55"/>
       <c r="J144" s="32"/>
       <c r="K144" s="32" t="s">
-        <v>1355</v>
+        <v>1341</v>
       </c>
       <c r="L144" s="29" t="s">
-        <v>1327</v>
+        <v>1325</v>
       </c>
       <c r="M144" s="32" t="s">
         <v>1062</v>
@@ -9598,10 +9654,10 @@
       <c r="I145" s="55"/>
       <c r="J145" s="32"/>
       <c r="K145" s="32" t="s">
-        <v>1355</v>
+        <v>1341</v>
       </c>
       <c r="L145" s="29" t="s">
-        <v>1327</v>
+        <v>1325</v>
       </c>
       <c r="M145" s="32" t="s">
         <v>1062</v>
@@ -9635,10 +9691,10 @@
       <c r="I146" s="55"/>
       <c r="J146" s="32"/>
       <c r="K146" s="32" t="s">
-        <v>1355</v>
+        <v>1341</v>
       </c>
       <c r="L146" s="29" t="s">
-        <v>1327</v>
+        <v>1325</v>
       </c>
       <c r="M146" s="32" t="s">
         <v>1062</v>
@@ -9672,10 +9728,10 @@
       <c r="I147" s="55"/>
       <c r="J147" s="32"/>
       <c r="K147" s="32" t="s">
-        <v>1355</v>
+        <v>1341</v>
       </c>
       <c r="L147" s="29" t="s">
-        <v>1327</v>
+        <v>1325</v>
       </c>
       <c r="M147" s="32" t="s">
         <v>1062</v>
@@ -9709,10 +9765,10 @@
       <c r="I148" s="55"/>
       <c r="J148" s="32"/>
       <c r="K148" s="32" t="s">
-        <v>1355</v>
+        <v>1341</v>
       </c>
       <c r="L148" s="29" t="s">
-        <v>1327</v>
+        <v>1325</v>
       </c>
       <c r="M148" s="32" t="s">
         <v>1062</v>
@@ -9746,10 +9802,10 @@
       <c r="I149" s="55"/>
       <c r="J149" s="32"/>
       <c r="K149" s="32" t="s">
-        <v>1355</v>
+        <v>1341</v>
       </c>
       <c r="L149" s="29" t="s">
-        <v>1327</v>
+        <v>1325</v>
       </c>
       <c r="M149" s="32" t="s">
         <v>1062</v>
@@ -9781,10 +9837,10 @@
       <c r="I150" s="55"/>
       <c r="J150" s="32"/>
       <c r="K150" s="32" t="s">
-        <v>1355</v>
+        <v>1341</v>
       </c>
       <c r="L150" s="29" t="s">
-        <v>1327</v>
+        <v>1325</v>
       </c>
       <c r="M150" s="32" t="s">
         <v>1062</v>
@@ -9818,10 +9874,10 @@
       <c r="I151" s="55"/>
       <c r="J151" s="32"/>
       <c r="K151" s="32" t="s">
-        <v>1355</v>
+        <v>1341</v>
       </c>
       <c r="L151" s="29" t="s">
-        <v>1327</v>
+        <v>1325</v>
       </c>
       <c r="M151" s="32" t="s">
         <v>1062</v>
@@ -9855,10 +9911,10 @@
       <c r="I152" s="55"/>
       <c r="J152" s="32"/>
       <c r="K152" s="32" t="s">
-        <v>1355</v>
+        <v>1341</v>
       </c>
       <c r="L152" s="29" t="s">
-        <v>1327</v>
+        <v>1325</v>
       </c>
       <c r="M152" s="32" t="s">
         <v>1062</v>
@@ -9890,10 +9946,10 @@
       <c r="I153" s="55"/>
       <c r="J153" s="32"/>
       <c r="K153" s="32" t="s">
-        <v>1355</v>
+        <v>1341</v>
       </c>
       <c r="L153" s="29" t="s">
-        <v>1327</v>
+        <v>1325</v>
       </c>
       <c r="M153" s="32" t="s">
         <v>1062</v>
@@ -9927,10 +9983,10 @@
       <c r="I154" s="55"/>
       <c r="J154" s="32"/>
       <c r="K154" s="32" t="s">
-        <v>1355</v>
+        <v>1341</v>
       </c>
       <c r="L154" s="29" t="s">
-        <v>1327</v>
+        <v>1325</v>
       </c>
       <c r="M154" s="32" t="s">
         <v>1062</v>
@@ -9964,10 +10020,10 @@
       <c r="I155" s="55"/>
       <c r="J155" s="32"/>
       <c r="K155" s="32" t="s">
-        <v>1355</v>
+        <v>1341</v>
       </c>
       <c r="L155" s="29" t="s">
-        <v>1327</v>
+        <v>1325</v>
       </c>
       <c r="M155" s="32" t="s">
         <v>1062</v>
@@ -10001,10 +10057,10 @@
       <c r="I156" s="55"/>
       <c r="J156" s="32"/>
       <c r="K156" s="32" t="s">
-        <v>1355</v>
+        <v>1341</v>
       </c>
       <c r="L156" s="29" t="s">
-        <v>1327</v>
+        <v>1325</v>
       </c>
       <c r="M156" s="32" t="s">
         <v>1062</v>
@@ -10034,10 +10090,10 @@
       <c r="I157" s="56"/>
       <c r="J157" s="32"/>
       <c r="K157" s="32" t="s">
-        <v>1356</v>
+        <v>1342</v>
       </c>
       <c r="L157" s="29" t="s">
-        <v>1327</v>
+        <v>1325</v>
       </c>
       <c r="M157" s="27" t="s">
         <v>1062</v>
@@ -10069,10 +10125,10 @@
       <c r="I158" s="56"/>
       <c r="J158" s="32"/>
       <c r="K158" s="32" t="s">
-        <v>1356</v>
+        <v>1342</v>
       </c>
       <c r="L158" s="29" t="s">
-        <v>1327</v>
+        <v>1325</v>
       </c>
       <c r="M158" s="27" t="s">
         <v>1062</v>
@@ -10104,10 +10160,10 @@
       <c r="I159" s="56"/>
       <c r="J159" s="32"/>
       <c r="K159" s="32" t="s">
-        <v>1356</v>
+        <v>1342</v>
       </c>
       <c r="L159" s="29" t="s">
-        <v>1327</v>
+        <v>1325</v>
       </c>
       <c r="M159" s="27" t="s">
         <v>1062</v>
@@ -10139,10 +10195,10 @@
       <c r="I160" s="56"/>
       <c r="J160" s="32"/>
       <c r="K160" s="32" t="s">
-        <v>1356</v>
+        <v>1342</v>
       </c>
       <c r="L160" s="29" t="s">
-        <v>1327</v>
+        <v>1325</v>
       </c>
       <c r="M160" s="27" t="s">
         <v>1062</v>
@@ -10176,10 +10232,10 @@
       <c r="I161" s="56"/>
       <c r="J161" s="32"/>
       <c r="K161" s="32" t="s">
-        <v>1356</v>
+        <v>1342</v>
       </c>
       <c r="L161" s="29" t="s">
-        <v>1327</v>
+        <v>1325</v>
       </c>
       <c r="M161" s="27" t="s">
         <v>1062</v>
@@ -10213,10 +10269,10 @@
       <c r="I162" s="56"/>
       <c r="J162" s="32"/>
       <c r="K162" s="32" t="s">
-        <v>1356</v>
+        <v>1342</v>
       </c>
       <c r="L162" s="29" t="s">
-        <v>1327</v>
+        <v>1325</v>
       </c>
       <c r="M162" s="27" t="s">
         <v>1062</v>
@@ -10250,10 +10306,10 @@
       <c r="I163" s="56"/>
       <c r="J163" s="32"/>
       <c r="K163" s="32" t="s">
-        <v>1356</v>
+        <v>1342</v>
       </c>
       <c r="L163" s="29" t="s">
-        <v>1327</v>
+        <v>1325</v>
       </c>
       <c r="M163" s="27" t="s">
         <v>1062</v>
@@ -10287,10 +10343,10 @@
       <c r="I164" s="56"/>
       <c r="J164" s="32"/>
       <c r="K164" s="32" t="s">
-        <v>1356</v>
+        <v>1342</v>
       </c>
       <c r="L164" s="29" t="s">
-        <v>1327</v>
+        <v>1325</v>
       </c>
       <c r="M164" s="27" t="s">
         <v>1062</v>
@@ -10322,10 +10378,10 @@
       <c r="I165" s="56"/>
       <c r="J165" s="32"/>
       <c r="K165" s="32" t="s">
-        <v>1356</v>
+        <v>1342</v>
       </c>
       <c r="L165" s="29" t="s">
-        <v>1327</v>
+        <v>1325</v>
       </c>
       <c r="M165" s="27" t="s">
         <v>1062</v>
@@ -10357,10 +10413,10 @@
       <c r="I166" s="56"/>
       <c r="J166" s="32"/>
       <c r="K166" s="32" t="s">
-        <v>1356</v>
+        <v>1342</v>
       </c>
       <c r="L166" s="29" t="s">
-        <v>1327</v>
+        <v>1325</v>
       </c>
       <c r="M166" s="27" t="s">
         <v>1062</v>
@@ -10390,10 +10446,10 @@
       <c r="I167" s="56"/>
       <c r="J167" s="32"/>
       <c r="K167" s="32" t="s">
-        <v>1357</v>
+        <v>1343</v>
       </c>
       <c r="L167" s="29" t="s">
-        <v>1327</v>
+        <v>1325</v>
       </c>
       <c r="M167" s="27" t="s">
         <v>1062</v>
@@ -10425,10 +10481,10 @@
       <c r="I168" s="56"/>
       <c r="J168" s="32"/>
       <c r="K168" s="32" t="s">
-        <v>1357</v>
+        <v>1343</v>
       </c>
       <c r="L168" s="29" t="s">
-        <v>1327</v>
+        <v>1325</v>
       </c>
       <c r="M168" s="27" t="s">
         <v>1062</v>
@@ -10460,10 +10516,10 @@
       <c r="I169" s="56"/>
       <c r="J169" s="32"/>
       <c r="K169" s="32" t="s">
-        <v>1357</v>
+        <v>1343</v>
       </c>
       <c r="L169" s="29" t="s">
-        <v>1327</v>
+        <v>1325</v>
       </c>
       <c r="M169" s="27" t="s">
         <v>1062</v>
@@ -10493,10 +10549,10 @@
       <c r="I170" s="56"/>
       <c r="J170" s="32"/>
       <c r="K170" s="32" t="s">
-        <v>1358</v>
+        <v>1344</v>
       </c>
       <c r="L170" s="29" t="s">
-        <v>1327</v>
+        <v>1325</v>
       </c>
       <c r="M170" s="27" t="s">
         <v>1062</v>
@@ -10528,10 +10584,10 @@
       <c r="I171" s="56"/>
       <c r="J171" s="32"/>
       <c r="K171" s="32" t="s">
-        <v>1358</v>
+        <v>1344</v>
       </c>
       <c r="L171" s="29" t="s">
-        <v>1327</v>
+        <v>1325</v>
       </c>
       <c r="M171" s="27" t="s">
         <v>1062</v>
@@ -10563,10 +10619,10 @@
       <c r="I172" s="57"/>
       <c r="J172" s="12"/>
       <c r="K172" s="32" t="s">
-        <v>1358</v>
+        <v>1344</v>
       </c>
       <c r="L172" s="29" t="s">
-        <v>1327</v>
+        <v>1325</v>
       </c>
       <c r="M172" s="27" t="s">
         <v>1062</v>
@@ -10598,10 +10654,10 @@
       <c r="I173" s="56"/>
       <c r="J173" s="32"/>
       <c r="K173" s="32" t="s">
-        <v>1358</v>
+        <v>1344</v>
       </c>
       <c r="L173" s="29" t="s">
-        <v>1327</v>
+        <v>1325</v>
       </c>
       <c r="M173" s="27" t="s">
         <v>1062</v>
@@ -10633,10 +10689,10 @@
       <c r="I174" s="57"/>
       <c r="J174" s="12"/>
       <c r="K174" s="32" t="s">
-        <v>1358</v>
+        <v>1344</v>
       </c>
       <c r="L174" s="29" t="s">
-        <v>1327</v>
+        <v>1325</v>
       </c>
       <c r="M174" s="27" t="s">
         <v>1062</v>
@@ -10668,10 +10724,10 @@
       <c r="I175" s="56"/>
       <c r="J175" s="32"/>
       <c r="K175" s="32" t="s">
-        <v>1358</v>
+        <v>1344</v>
       </c>
       <c r="L175" s="29" t="s">
-        <v>1327</v>
+        <v>1325</v>
       </c>
       <c r="M175" s="27" t="s">
         <v>1062</v>
@@ -10703,10 +10759,10 @@
       <c r="I176" s="56"/>
       <c r="J176" s="32"/>
       <c r="K176" s="32" t="s">
-        <v>1358</v>
+        <v>1344</v>
       </c>
       <c r="L176" s="29" t="s">
-        <v>1327</v>
+        <v>1325</v>
       </c>
       <c r="M176" s="27" t="s">
         <v>1062</v>
@@ -10736,10 +10792,10 @@
       <c r="I177" s="56"/>
       <c r="J177" s="32"/>
       <c r="K177" s="32" t="s">
-        <v>1359</v>
+        <v>1345</v>
       </c>
       <c r="L177" s="29" t="s">
-        <v>1327</v>
+        <v>1325</v>
       </c>
       <c r="M177" s="27" t="s">
         <v>1062</v>
@@ -10771,10 +10827,10 @@
       <c r="I178" s="56"/>
       <c r="J178" s="32"/>
       <c r="K178" s="32" t="s">
-        <v>1359</v>
+        <v>1345</v>
       </c>
       <c r="L178" s="29" t="s">
-        <v>1327</v>
+        <v>1325</v>
       </c>
       <c r="M178" s="27" t="s">
         <v>1062</v>
@@ -10806,10 +10862,10 @@
       <c r="I179" s="56"/>
       <c r="J179" s="32"/>
       <c r="K179" s="32" t="s">
-        <v>1359</v>
+        <v>1345</v>
       </c>
       <c r="L179" s="29" t="s">
-        <v>1327</v>
+        <v>1325</v>
       </c>
       <c r="M179" s="27" t="s">
         <v>1062</v>
@@ -10841,10 +10897,10 @@
       <c r="I180" s="56"/>
       <c r="J180" s="32"/>
       <c r="K180" s="32" t="s">
-        <v>1359</v>
+        <v>1345</v>
       </c>
       <c r="L180" s="29" t="s">
-        <v>1327</v>
+        <v>1325</v>
       </c>
       <c r="M180" s="27" t="s">
         <v>1062</v>
@@ -10876,10 +10932,10 @@
       <c r="I181" s="56"/>
       <c r="J181" s="32"/>
       <c r="K181" s="32" t="s">
-        <v>1359</v>
+        <v>1345</v>
       </c>
       <c r="L181" s="29" t="s">
-        <v>1327</v>
+        <v>1325</v>
       </c>
       <c r="M181" s="27" t="s">
         <v>1062</v>
@@ -10913,10 +10969,10 @@
       <c r="I182" s="56"/>
       <c r="J182" s="32"/>
       <c r="K182" s="32" t="s">
-        <v>1359</v>
+        <v>1345</v>
       </c>
       <c r="L182" s="29" t="s">
-        <v>1327</v>
+        <v>1325</v>
       </c>
       <c r="M182" s="27" t="s">
         <v>1062</v>
@@ -10950,10 +11006,10 @@
       <c r="I183" s="56"/>
       <c r="J183" s="32"/>
       <c r="K183" s="32" t="s">
-        <v>1359</v>
+        <v>1345</v>
       </c>
       <c r="L183" s="29" t="s">
-        <v>1327</v>
+        <v>1325</v>
       </c>
       <c r="M183" s="27" t="s">
         <v>1062</v>
@@ -10983,10 +11039,10 @@
       <c r="I184" s="56"/>
       <c r="J184" s="32"/>
       <c r="K184" s="32" t="s">
-        <v>1360</v>
+        <v>1346</v>
       </c>
       <c r="L184" s="29" t="s">
-        <v>1327</v>
+        <v>1325</v>
       </c>
       <c r="M184" s="27" t="s">
         <v>1062</v>
@@ -11018,10 +11074,10 @@
       <c r="I185" s="56"/>
       <c r="J185" s="32"/>
       <c r="K185" s="32" t="s">
-        <v>1360</v>
+        <v>1346</v>
       </c>
       <c r="L185" s="29" t="s">
-        <v>1327</v>
+        <v>1325</v>
       </c>
       <c r="M185" s="27" t="s">
         <v>1062</v>
@@ -11053,10 +11109,10 @@
       <c r="I186" s="56"/>
       <c r="J186" s="32"/>
       <c r="K186" s="32" t="s">
-        <v>1360</v>
+        <v>1346</v>
       </c>
       <c r="L186" s="29" t="s">
-        <v>1327</v>
+        <v>1325</v>
       </c>
       <c r="M186" s="27" t="s">
         <v>1062</v>
@@ -11088,10 +11144,10 @@
       <c r="I187" s="56"/>
       <c r="J187" s="32"/>
       <c r="K187" s="32" t="s">
-        <v>1360</v>
+        <v>1346</v>
       </c>
       <c r="L187" s="29" t="s">
-        <v>1327</v>
+        <v>1325</v>
       </c>
       <c r="M187" s="27" t="s">
         <v>1062</v>
@@ -11123,10 +11179,10 @@
       <c r="I188" s="56"/>
       <c r="J188" s="32"/>
       <c r="K188" s="32" t="s">
-        <v>1360</v>
+        <v>1346</v>
       </c>
       <c r="L188" s="29" t="s">
-        <v>1327</v>
+        <v>1325</v>
       </c>
       <c r="M188" s="27" t="s">
         <v>1062</v>
@@ -11158,10 +11214,10 @@
       <c r="I189" s="56"/>
       <c r="J189" s="32"/>
       <c r="K189" s="32" t="s">
-        <v>1360</v>
+        <v>1346</v>
       </c>
       <c r="L189" s="29" t="s">
-        <v>1327</v>
+        <v>1325</v>
       </c>
       <c r="M189" s="27" t="s">
         <v>1062</v>
@@ -11193,10 +11249,10 @@
       <c r="I190" s="56"/>
       <c r="J190" s="32"/>
       <c r="K190" s="32" t="s">
-        <v>1360</v>
+        <v>1346</v>
       </c>
       <c r="L190" s="29" t="s">
-        <v>1327</v>
+        <v>1325</v>
       </c>
       <c r="M190" s="27" t="s">
         <v>1062</v>
@@ -11228,10 +11284,10 @@
       <c r="I191" s="56"/>
       <c r="J191" s="32"/>
       <c r="K191" s="32" t="s">
-        <v>1360</v>
+        <v>1346</v>
       </c>
       <c r="L191" s="29" t="s">
-        <v>1327</v>
+        <v>1325</v>
       </c>
       <c r="M191" s="27" t="s">
         <v>1062</v>
@@ -11263,10 +11319,10 @@
       <c r="I192" s="56"/>
       <c r="J192" s="32"/>
       <c r="K192" s="32" t="s">
-        <v>1360</v>
+        <v>1346</v>
       </c>
       <c r="L192" s="29" t="s">
-        <v>1327</v>
+        <v>1325</v>
       </c>
       <c r="M192" s="27" t="s">
         <v>1062</v>
@@ -11298,10 +11354,10 @@
       <c r="I193" s="56"/>
       <c r="J193" s="32"/>
       <c r="K193" s="32" t="s">
-        <v>1360</v>
+        <v>1346</v>
       </c>
       <c r="L193" s="29" t="s">
-        <v>1327</v>
+        <v>1325</v>
       </c>
       <c r="M193" s="27" t="s">
         <v>1062</v>
@@ -11337,10 +11393,10 @@
       </c>
       <c r="J194" s="32"/>
       <c r="K194" s="32" t="s">
-        <v>1360</v>
+        <v>1346</v>
       </c>
       <c r="L194" s="29" t="s">
-        <v>1327</v>
+        <v>1325</v>
       </c>
       <c r="M194" s="27" t="s">
         <v>1062</v>
@@ -11376,10 +11432,10 @@
       </c>
       <c r="J195" s="32"/>
       <c r="K195" s="32" t="s">
-        <v>1360</v>
+        <v>1346</v>
       </c>
       <c r="L195" s="29" t="s">
-        <v>1327</v>
+        <v>1325</v>
       </c>
       <c r="M195" s="27" t="s">
         <v>1062</v>
@@ -11411,10 +11467,10 @@
       <c r="I196" s="56"/>
       <c r="J196" s="32"/>
       <c r="K196" s="32" t="s">
-        <v>1360</v>
+        <v>1346</v>
       </c>
       <c r="L196" s="29" t="s">
-        <v>1327</v>
+        <v>1325</v>
       </c>
       <c r="M196" s="27" t="s">
         <v>1062</v>
@@ -11446,10 +11502,10 @@
       <c r="I197" s="56"/>
       <c r="J197" s="32"/>
       <c r="K197" s="32" t="s">
-        <v>1360</v>
+        <v>1346</v>
       </c>
       <c r="L197" s="29" t="s">
-        <v>1327</v>
+        <v>1325</v>
       </c>
       <c r="M197" s="27" t="s">
         <v>1062</v>
@@ -11481,10 +11537,10 @@
       <c r="I198" s="56"/>
       <c r="J198" s="32"/>
       <c r="K198" s="32" t="s">
-        <v>1360</v>
+        <v>1346</v>
       </c>
       <c r="L198" s="29" t="s">
-        <v>1327</v>
+        <v>1325</v>
       </c>
       <c r="M198" s="27" t="s">
         <v>1062</v>
@@ -11516,10 +11572,10 @@
       <c r="I199" s="56"/>
       <c r="J199" s="32"/>
       <c r="K199" s="32" t="s">
-        <v>1360</v>
+        <v>1346</v>
       </c>
       <c r="L199" s="29" t="s">
-        <v>1327</v>
+        <v>1325</v>
       </c>
       <c r="M199" s="27" t="s">
         <v>1062</v>
@@ -11551,10 +11607,10 @@
       <c r="I200" s="56"/>
       <c r="J200" s="32"/>
       <c r="K200" s="32" t="s">
-        <v>1360</v>
+        <v>1346</v>
       </c>
       <c r="L200" s="29" t="s">
-        <v>1327</v>
+        <v>1325</v>
       </c>
       <c r="M200" s="27" t="s">
         <v>1062</v>
@@ -11590,10 +11646,10 @@
       </c>
       <c r="J201" s="32"/>
       <c r="K201" s="32" t="s">
-        <v>1360</v>
+        <v>1346</v>
       </c>
       <c r="L201" s="29" t="s">
-        <v>1327</v>
+        <v>1325</v>
       </c>
       <c r="M201" s="27" t="s">
         <v>1062</v>
@@ -11629,10 +11685,10 @@
       </c>
       <c r="J202" s="32"/>
       <c r="K202" s="32" t="s">
-        <v>1360</v>
+        <v>1346</v>
       </c>
       <c r="L202" s="29" t="s">
-        <v>1327</v>
+        <v>1325</v>
       </c>
       <c r="M202" s="27" t="s">
         <v>1062</v>
@@ -11664,10 +11720,10 @@
       <c r="I203" s="56"/>
       <c r="J203" s="32"/>
       <c r="K203" s="32" t="s">
-        <v>1360</v>
+        <v>1346</v>
       </c>
       <c r="L203" s="29" t="s">
-        <v>1327</v>
+        <v>1325</v>
       </c>
       <c r="M203" s="27" t="s">
         <v>1062</v>
@@ -11703,10 +11759,10 @@
       </c>
       <c r="J204" s="32"/>
       <c r="K204" s="32" t="s">
-        <v>1360</v>
+        <v>1346</v>
       </c>
       <c r="L204" s="29" t="s">
-        <v>1327</v>
+        <v>1325</v>
       </c>
       <c r="M204" s="27" t="s">
         <v>1062</v>
@@ -11742,10 +11798,10 @@
       </c>
       <c r="J205" s="32"/>
       <c r="K205" s="32" t="s">
-        <v>1360</v>
+        <v>1346</v>
       </c>
       <c r="L205" s="29" t="s">
-        <v>1327</v>
+        <v>1325</v>
       </c>
       <c r="M205" s="27" t="s">
         <v>1062</v>
@@ -11777,10 +11833,10 @@
       <c r="I206" s="56"/>
       <c r="J206" s="32"/>
       <c r="K206" s="32" t="s">
-        <v>1360</v>
+        <v>1346</v>
       </c>
       <c r="L206" s="29" t="s">
-        <v>1327</v>
+        <v>1325</v>
       </c>
       <c r="M206" s="27" t="s">
         <v>1062</v>
@@ -11810,10 +11866,10 @@
       <c r="I207" s="56"/>
       <c r="J207" s="32"/>
       <c r="K207" s="32" t="s">
-        <v>1361</v>
+        <v>1347</v>
       </c>
       <c r="L207" s="29" t="s">
-        <v>1327</v>
+        <v>1325</v>
       </c>
       <c r="M207" s="27" t="s">
         <v>1062</v>
@@ -11845,10 +11901,10 @@
       <c r="I208" s="56"/>
       <c r="J208" s="32"/>
       <c r="K208" s="32" t="s">
-        <v>1361</v>
+        <v>1347</v>
       </c>
       <c r="L208" s="29" t="s">
-        <v>1327</v>
+        <v>1325</v>
       </c>
       <c r="M208" s="27" t="s">
         <v>1062</v>
@@ -11880,10 +11936,10 @@
       <c r="I209" s="56"/>
       <c r="J209" s="32"/>
       <c r="K209" s="32" t="s">
-        <v>1361</v>
+        <v>1347</v>
       </c>
       <c r="L209" s="29" t="s">
-        <v>1327</v>
+        <v>1325</v>
       </c>
       <c r="M209" s="27" t="s">
         <v>1062</v>
@@ -11915,10 +11971,10 @@
       <c r="I210" s="56"/>
       <c r="J210" s="32"/>
       <c r="K210" s="32" t="s">
-        <v>1361</v>
+        <v>1347</v>
       </c>
       <c r="L210" s="29" t="s">
-        <v>1327</v>
+        <v>1325</v>
       </c>
       <c r="M210" s="27" t="s">
         <v>1062</v>
@@ -11950,10 +12006,10 @@
       <c r="I211" s="56"/>
       <c r="J211" s="32"/>
       <c r="K211" s="32" t="s">
-        <v>1361</v>
+        <v>1347</v>
       </c>
       <c r="L211" s="29" t="s">
-        <v>1327</v>
+        <v>1325</v>
       </c>
       <c r="M211" s="27" t="s">
         <v>1062</v>
@@ -11985,10 +12041,10 @@
       <c r="I212" s="56"/>
       <c r="J212" s="32"/>
       <c r="K212" s="32" t="s">
-        <v>1361</v>
+        <v>1347</v>
       </c>
       <c r="L212" s="29" t="s">
-        <v>1327</v>
+        <v>1325</v>
       </c>
       <c r="M212" s="27" t="s">
         <v>1062</v>
@@ -12020,10 +12076,10 @@
       <c r="I213" s="56"/>
       <c r="J213" s="32"/>
       <c r="K213" s="32" t="s">
-        <v>1361</v>
+        <v>1347</v>
       </c>
       <c r="L213" s="29" t="s">
-        <v>1327</v>
+        <v>1325</v>
       </c>
       <c r="M213" s="27" t="s">
         <v>1062</v>
@@ -12055,10 +12111,10 @@
       <c r="I214" s="56"/>
       <c r="J214" s="32"/>
       <c r="K214" s="32" t="s">
-        <v>1361</v>
+        <v>1347</v>
       </c>
       <c r="L214" s="29" t="s">
-        <v>1327</v>
+        <v>1325</v>
       </c>
       <c r="M214" s="27" t="s">
         <v>1062</v>
@@ -12090,10 +12146,10 @@
       <c r="I215" s="56"/>
       <c r="J215" s="32"/>
       <c r="K215" s="32" t="s">
-        <v>1361</v>
+        <v>1347</v>
       </c>
       <c r="L215" s="29" t="s">
-        <v>1327</v>
+        <v>1325</v>
       </c>
       <c r="M215" s="27" t="s">
         <v>1062</v>
@@ -12125,10 +12181,10 @@
       <c r="I216" s="56"/>
       <c r="J216" s="32"/>
       <c r="K216" s="32" t="s">
-        <v>1361</v>
+        <v>1347</v>
       </c>
       <c r="L216" s="29" t="s">
-        <v>1327</v>
+        <v>1325</v>
       </c>
       <c r="M216" s="27" t="s">
         <v>1062</v>
@@ -12160,10 +12216,10 @@
       <c r="I217" s="56"/>
       <c r="J217" s="32"/>
       <c r="K217" s="32" t="s">
-        <v>1361</v>
+        <v>1347</v>
       </c>
       <c r="L217" s="29" t="s">
-        <v>1327</v>
+        <v>1325</v>
       </c>
       <c r="M217" s="27" t="s">
         <v>1062</v>
@@ -12195,10 +12251,10 @@
       <c r="I218" s="56"/>
       <c r="J218" s="32"/>
       <c r="K218" s="32" t="s">
-        <v>1361</v>
+        <v>1347</v>
       </c>
       <c r="L218" s="29" t="s">
-        <v>1327</v>
+        <v>1325</v>
       </c>
       <c r="M218" s="27" t="s">
         <v>1062</v>
@@ -12230,10 +12286,10 @@
       <c r="I219" s="56"/>
       <c r="J219" s="32"/>
       <c r="K219" s="32" t="s">
-        <v>1361</v>
+        <v>1347</v>
       </c>
       <c r="L219" s="29" t="s">
-        <v>1327</v>
+        <v>1325</v>
       </c>
       <c r="M219" s="27" t="s">
         <v>1062</v>
@@ -12265,10 +12321,10 @@
       <c r="I220" s="56"/>
       <c r="J220" s="32"/>
       <c r="K220" s="32" t="s">
-        <v>1361</v>
+        <v>1347</v>
       </c>
       <c r="L220" s="29" t="s">
-        <v>1327</v>
+        <v>1325</v>
       </c>
       <c r="M220" s="27" t="s">
         <v>1062</v>
@@ -12300,10 +12356,10 @@
       <c r="I221" s="56"/>
       <c r="J221" s="32"/>
       <c r="K221" s="32" t="s">
-        <v>1361</v>
+        <v>1347</v>
       </c>
       <c r="L221" s="29" t="s">
-        <v>1327</v>
+        <v>1325</v>
       </c>
       <c r="M221" s="27" t="s">
         <v>1062</v>
@@ -12335,10 +12391,10 @@
       <c r="I222" s="56"/>
       <c r="J222" s="32"/>
       <c r="K222" s="32" t="s">
-        <v>1361</v>
+        <v>1347</v>
       </c>
       <c r="L222" s="29" t="s">
-        <v>1327</v>
+        <v>1325</v>
       </c>
       <c r="M222" s="27" t="s">
         <v>1062</v>
@@ -12370,10 +12426,10 @@
       <c r="I223" s="56"/>
       <c r="J223" s="32"/>
       <c r="K223" s="32" t="s">
-        <v>1361</v>
+        <v>1347</v>
       </c>
       <c r="L223" s="29" t="s">
-        <v>1327</v>
+        <v>1325</v>
       </c>
       <c r="M223" s="27" t="s">
         <v>1062</v>
@@ -12405,10 +12461,10 @@
       <c r="I224" s="56"/>
       <c r="J224" s="32"/>
       <c r="K224" s="32" t="s">
-        <v>1361</v>
+        <v>1347</v>
       </c>
       <c r="L224" s="29" t="s">
-        <v>1327</v>
+        <v>1325</v>
       </c>
       <c r="M224" s="27" t="s">
         <v>1062</v>
@@ -12440,10 +12496,10 @@
       <c r="I225" s="56"/>
       <c r="J225" s="32"/>
       <c r="K225" s="32" t="s">
-        <v>1361</v>
+        <v>1347</v>
       </c>
       <c r="L225" s="29" t="s">
-        <v>1327</v>
+        <v>1325</v>
       </c>
       <c r="M225" s="27" t="s">
         <v>1062</v>
@@ -12475,10 +12531,10 @@
       <c r="I226" s="56"/>
       <c r="J226" s="32"/>
       <c r="K226" s="32" t="s">
-        <v>1361</v>
+        <v>1347</v>
       </c>
       <c r="L226" s="29" t="s">
-        <v>1327</v>
+        <v>1325</v>
       </c>
       <c r="M226" s="27" t="s">
         <v>1062</v>
@@ -12510,10 +12566,10 @@
       <c r="I227" s="56"/>
       <c r="J227" s="32"/>
       <c r="K227" s="32" t="s">
-        <v>1361</v>
+        <v>1347</v>
       </c>
       <c r="L227" s="29" t="s">
-        <v>1327</v>
+        <v>1325</v>
       </c>
       <c r="M227" s="27" t="s">
         <v>1062</v>
@@ -12545,10 +12601,10 @@
       <c r="I228" s="56"/>
       <c r="J228" s="32"/>
       <c r="K228" s="32" t="s">
-        <v>1361</v>
+        <v>1347</v>
       </c>
       <c r="L228" s="29" t="s">
-        <v>1327</v>
+        <v>1325</v>
       </c>
       <c r="M228" s="27" t="s">
         <v>1062</v>
@@ -12580,10 +12636,10 @@
       <c r="I229" s="56"/>
       <c r="J229" s="32"/>
       <c r="K229" s="32" t="s">
-        <v>1361</v>
+        <v>1347</v>
       </c>
       <c r="L229" s="29" t="s">
-        <v>1327</v>
+        <v>1325</v>
       </c>
       <c r="M229" s="27" t="s">
         <v>1062</v>
@@ -12615,10 +12671,10 @@
       <c r="I230" s="56"/>
       <c r="J230" s="32"/>
       <c r="K230" s="32" t="s">
-        <v>1361</v>
+        <v>1347</v>
       </c>
       <c r="L230" s="29" t="s">
-        <v>1327</v>
+        <v>1325</v>
       </c>
       <c r="M230" s="27" t="s">
         <v>1062</v>
@@ -12650,10 +12706,10 @@
       <c r="I231" s="56"/>
       <c r="J231" s="32"/>
       <c r="K231" s="32" t="s">
-        <v>1361</v>
+        <v>1347</v>
       </c>
       <c r="L231" s="29" t="s">
-        <v>1327</v>
+        <v>1325</v>
       </c>
       <c r="M231" s="27" t="s">
         <v>1062</v>
@@ -12685,10 +12741,10 @@
       <c r="I232" s="56"/>
       <c r="J232" s="32"/>
       <c r="K232" s="32" t="s">
-        <v>1361</v>
+        <v>1347</v>
       </c>
       <c r="L232" s="29" t="s">
-        <v>1327</v>
+        <v>1325</v>
       </c>
       <c r="M232" s="27" t="s">
         <v>1062</v>
@@ -12720,10 +12776,10 @@
       <c r="I233" s="56"/>
       <c r="J233" s="32"/>
       <c r="K233" s="32" t="s">
-        <v>1361</v>
+        <v>1347</v>
       </c>
       <c r="L233" s="29" t="s">
-        <v>1327</v>
+        <v>1325</v>
       </c>
       <c r="M233" s="27" t="s">
         <v>1062</v>
@@ -12755,10 +12811,10 @@
       <c r="I234" s="56"/>
       <c r="J234" s="32"/>
       <c r="K234" s="32" t="s">
-        <v>1361</v>
+        <v>1347</v>
       </c>
       <c r="L234" s="29" t="s">
-        <v>1327</v>
+        <v>1325</v>
       </c>
       <c r="M234" s="27" t="s">
         <v>1062</v>
@@ -12790,10 +12846,10 @@
       <c r="I235" s="56"/>
       <c r="J235" s="32"/>
       <c r="K235" s="32" t="s">
-        <v>1361</v>
+        <v>1347</v>
       </c>
       <c r="L235" s="29" t="s">
-        <v>1327</v>
+        <v>1325</v>
       </c>
       <c r="M235" s="27" t="s">
         <v>1062</v>
@@ -12825,10 +12881,10 @@
       <c r="I236" s="56"/>
       <c r="J236" s="32"/>
       <c r="K236" s="32" t="s">
-        <v>1361</v>
+        <v>1347</v>
       </c>
       <c r="L236" s="29" t="s">
-        <v>1327</v>
+        <v>1325</v>
       </c>
       <c r="M236" s="27" t="s">
         <v>1062</v>
@@ -12858,10 +12914,10 @@
       <c r="I237" s="56"/>
       <c r="J237" s="32"/>
       <c r="K237" s="32" t="s">
-        <v>1362</v>
+        <v>1348</v>
       </c>
       <c r="L237" s="29" t="s">
-        <v>1327</v>
+        <v>1325</v>
       </c>
       <c r="M237" s="27" t="s">
         <v>1062</v>
@@ -12893,10 +12949,10 @@
       <c r="I238" s="56"/>
       <c r="J238" s="32"/>
       <c r="K238" s="32" t="s">
-        <v>1362</v>
+        <v>1348</v>
       </c>
       <c r="L238" s="29" t="s">
-        <v>1327</v>
+        <v>1325</v>
       </c>
       <c r="M238" s="27" t="s">
         <v>1062</v>
@@ -12928,10 +12984,10 @@
       <c r="I239" s="56"/>
       <c r="J239" s="32"/>
       <c r="K239" s="32" t="s">
-        <v>1362</v>
+        <v>1348</v>
       </c>
       <c r="L239" s="29" t="s">
-        <v>1327</v>
+        <v>1325</v>
       </c>
       <c r="M239" s="27" t="s">
         <v>1062</v>
@@ -12963,10 +13019,10 @@
       <c r="I240" s="56"/>
       <c r="J240" s="32"/>
       <c r="K240" s="32" t="s">
-        <v>1362</v>
+        <v>1348</v>
       </c>
       <c r="L240" s="29" t="s">
-        <v>1327</v>
+        <v>1325</v>
       </c>
       <c r="M240" s="27" t="s">
         <v>1062</v>
@@ -12998,10 +13054,10 @@
       <c r="I241" s="56"/>
       <c r="J241" s="32"/>
       <c r="K241" s="32" t="s">
-        <v>1362</v>
+        <v>1348</v>
       </c>
       <c r="L241" s="29" t="s">
-        <v>1327</v>
+        <v>1325</v>
       </c>
       <c r="M241" s="27" t="s">
         <v>1062</v>
@@ -13031,10 +13087,10 @@
       <c r="I242" s="56"/>
       <c r="J242" s="32"/>
       <c r="K242" s="32" t="s">
-        <v>1363</v>
+        <v>1349</v>
       </c>
       <c r="L242" s="29" t="s">
-        <v>1327</v>
+        <v>1325</v>
       </c>
       <c r="M242" s="27" t="s">
         <v>1062</v>
@@ -13066,10 +13122,10 @@
       <c r="I243" s="56"/>
       <c r="J243" s="32"/>
       <c r="K243" s="32" t="s">
-        <v>1363</v>
+        <v>1349</v>
       </c>
       <c r="L243" s="29" t="s">
-        <v>1327</v>
+        <v>1325</v>
       </c>
       <c r="M243" s="27" t="s">
         <v>1062</v>
@@ -13101,10 +13157,10 @@
       <c r="I244" s="56"/>
       <c r="J244" s="32"/>
       <c r="K244" s="32" t="s">
-        <v>1363</v>
+        <v>1349</v>
       </c>
       <c r="L244" s="29" t="s">
-        <v>1327</v>
+        <v>1325</v>
       </c>
       <c r="M244" s="27" t="s">
         <v>1062</v>
@@ -13136,10 +13192,10 @@
       <c r="I245" s="56"/>
       <c r="J245" s="32"/>
       <c r="K245" s="32" t="s">
-        <v>1363</v>
+        <v>1349</v>
       </c>
       <c r="L245" s="29" t="s">
-        <v>1327</v>
+        <v>1325</v>
       </c>
       <c r="M245" s="32" t="s">
         <v>1062</v>
@@ -13171,10 +13227,10 @@
       <c r="I246" s="56"/>
       <c r="J246" s="32"/>
       <c r="K246" s="32" t="s">
-        <v>1363</v>
+        <v>1349</v>
       </c>
       <c r="L246" s="29" t="s">
-        <v>1327</v>
+        <v>1325</v>
       </c>
       <c r="M246" s="32" t="s">
         <v>1062</v>
@@ -13206,10 +13262,10 @@
       <c r="I247" s="56"/>
       <c r="J247" s="32"/>
       <c r="K247" s="32" t="s">
-        <v>1363</v>
+        <v>1349</v>
       </c>
       <c r="L247" s="29" t="s">
-        <v>1327</v>
+        <v>1325</v>
       </c>
       <c r="M247" s="32" t="s">
         <v>1062</v>
@@ -13239,10 +13295,10 @@
       <c r="I248" s="56"/>
       <c r="J248" s="32"/>
       <c r="K248" s="32" t="s">
-        <v>1364</v>
+        <v>1350</v>
       </c>
       <c r="L248" s="29" t="s">
-        <v>1327</v>
+        <v>1325</v>
       </c>
       <c r="M248" s="32" t="s">
         <v>1062</v>
@@ -13274,10 +13330,10 @@
       <c r="I249" s="56"/>
       <c r="J249" s="32"/>
       <c r="K249" s="32" t="s">
-        <v>1364</v>
+        <v>1350</v>
       </c>
       <c r="L249" s="29" t="s">
-        <v>1327</v>
+        <v>1325</v>
       </c>
       <c r="M249" s="32" t="s">
         <v>1062</v>
@@ -13309,10 +13365,10 @@
       <c r="I250" s="56"/>
       <c r="J250" s="32"/>
       <c r="K250" s="32" t="s">
-        <v>1364</v>
+        <v>1350</v>
       </c>
       <c r="L250" s="29" t="s">
-        <v>1327</v>
+        <v>1325</v>
       </c>
       <c r="M250" s="32" t="s">
         <v>1062</v>
@@ -13344,10 +13400,10 @@
       <c r="I251" s="56"/>
       <c r="J251" s="32"/>
       <c r="K251" s="32" t="s">
-        <v>1364</v>
+        <v>1350</v>
       </c>
       <c r="L251" s="29" t="s">
-        <v>1327</v>
+        <v>1325</v>
       </c>
       <c r="M251" s="32" t="s">
         <v>1062</v>
@@ -13379,10 +13435,10 @@
       <c r="I252" s="56"/>
       <c r="J252" s="32"/>
       <c r="K252" s="32" t="s">
-        <v>1364</v>
+        <v>1350</v>
       </c>
       <c r="L252" s="29" t="s">
-        <v>1327</v>
+        <v>1325</v>
       </c>
       <c r="M252" s="32" t="s">
         <v>1062</v>
@@ -13414,10 +13470,10 @@
       <c r="I253" s="56"/>
       <c r="J253" s="32"/>
       <c r="K253" s="32" t="s">
-        <v>1364</v>
+        <v>1350</v>
       </c>
       <c r="L253" s="29" t="s">
-        <v>1327</v>
+        <v>1325</v>
       </c>
       <c r="M253" s="32" t="s">
         <v>1062</v>
@@ -13449,10 +13505,10 @@
       <c r="I254" s="56"/>
       <c r="J254" s="32"/>
       <c r="K254" s="32" t="s">
-        <v>1364</v>
+        <v>1350</v>
       </c>
       <c r="L254" s="29" t="s">
-        <v>1327</v>
+        <v>1325</v>
       </c>
       <c r="M254" s="32" t="s">
         <v>1062</v>
@@ -13486,10 +13542,10 @@
       <c r="I255" s="56"/>
       <c r="J255" s="32"/>
       <c r="K255" s="32" t="s">
-        <v>1364</v>
+        <v>1350</v>
       </c>
       <c r="L255" s="29" t="s">
-        <v>1327</v>
+        <v>1325</v>
       </c>
       <c r="M255" s="32" t="s">
         <v>1062</v>
@@ -13523,10 +13579,10 @@
       <c r="I256" s="56"/>
       <c r="J256" s="32"/>
       <c r="K256" s="32" t="s">
-        <v>1364</v>
+        <v>1350</v>
       </c>
       <c r="L256" s="29" t="s">
-        <v>1327</v>
+        <v>1325</v>
       </c>
       <c r="M256" s="32" t="s">
         <v>1062</v>
@@ -13558,10 +13614,10 @@
       <c r="I257" s="56"/>
       <c r="J257" s="32"/>
       <c r="K257" s="32" t="s">
-        <v>1364</v>
+        <v>1350</v>
       </c>
       <c r="L257" s="29" t="s">
-        <v>1327</v>
+        <v>1325</v>
       </c>
       <c r="M257" s="32" t="s">
         <v>1062</v>
@@ -13591,10 +13647,10 @@
       <c r="I258" s="56"/>
       <c r="J258" s="32"/>
       <c r="K258" s="32" t="s">
-        <v>1365</v>
+        <v>1351</v>
       </c>
       <c r="L258" s="29" t="s">
-        <v>1327</v>
+        <v>1325</v>
       </c>
       <c r="M258" s="32" t="s">
         <v>1062</v>
@@ -13626,10 +13682,10 @@
       <c r="I259" s="56"/>
       <c r="J259" s="32"/>
       <c r="K259" s="32" t="s">
-        <v>1365</v>
+        <v>1351</v>
       </c>
       <c r="L259" s="29" t="s">
-        <v>1327</v>
+        <v>1325</v>
       </c>
       <c r="M259" s="32" t="s">
         <v>1062</v>
@@ -13661,10 +13717,10 @@
       <c r="I260" s="56"/>
       <c r="J260" s="32"/>
       <c r="K260" s="32" t="s">
-        <v>1365</v>
+        <v>1351</v>
       </c>
       <c r="L260" s="29" t="s">
-        <v>1327</v>
+        <v>1325</v>
       </c>
       <c r="M260" s="32" t="s">
         <v>1062</v>
@@ -13698,10 +13754,10 @@
       <c r="I261" s="56"/>
       <c r="J261" s="32"/>
       <c r="K261" s="32" t="s">
-        <v>1365</v>
+        <v>1351</v>
       </c>
       <c r="L261" s="29" t="s">
-        <v>1327</v>
+        <v>1325</v>
       </c>
       <c r="M261" s="32" t="s">
         <v>1062</v>
@@ -13735,10 +13791,10 @@
       <c r="I262" s="56"/>
       <c r="J262" s="32"/>
       <c r="K262" s="32" t="s">
-        <v>1365</v>
+        <v>1351</v>
       </c>
       <c r="L262" s="29" t="s">
-        <v>1327</v>
+        <v>1325</v>
       </c>
       <c r="M262" s="32" t="s">
         <v>1062</v>
@@ -13770,10 +13826,10 @@
       <c r="I263" s="56"/>
       <c r="J263" s="32"/>
       <c r="K263" s="32" t="s">
-        <v>1365</v>
+        <v>1351</v>
       </c>
       <c r="L263" s="29" t="s">
-        <v>1327</v>
+        <v>1325</v>
       </c>
       <c r="M263" s="32" t="s">
         <v>1062</v>
@@ -13805,10 +13861,10 @@
       <c r="I264" s="56"/>
       <c r="J264" s="32"/>
       <c r="K264" s="32" t="s">
-        <v>1365</v>
+        <v>1351</v>
       </c>
       <c r="L264" s="29" t="s">
-        <v>1327</v>
+        <v>1325</v>
       </c>
       <c r="M264" s="32" t="s">
         <v>1062</v>
@@ -13838,10 +13894,10 @@
       <c r="I265" s="56"/>
       <c r="J265" s="32"/>
       <c r="K265" s="32" t="s">
-        <v>1366</v>
+        <v>1352</v>
       </c>
       <c r="L265" s="29" t="s">
-        <v>1327</v>
+        <v>1325</v>
       </c>
       <c r="M265" s="32" t="s">
         <v>1062</v>
@@ -13873,10 +13929,10 @@
       <c r="I266" s="56"/>
       <c r="J266" s="32"/>
       <c r="K266" s="32" t="s">
-        <v>1366</v>
+        <v>1352</v>
       </c>
       <c r="L266" s="29" t="s">
-        <v>1327</v>
+        <v>1325</v>
       </c>
       <c r="M266" s="32" t="s">
         <v>1062</v>
@@ -13908,10 +13964,10 @@
       <c r="I267" s="56"/>
       <c r="J267" s="32"/>
       <c r="K267" s="32" t="s">
-        <v>1366</v>
+        <v>1352</v>
       </c>
       <c r="L267" s="29" t="s">
-        <v>1327</v>
+        <v>1325</v>
       </c>
       <c r="M267" s="32" t="s">
         <v>1062</v>
@@ -13943,10 +13999,10 @@
       <c r="I268" s="56"/>
       <c r="J268" s="32"/>
       <c r="K268" s="32" t="s">
-        <v>1366</v>
+        <v>1352</v>
       </c>
       <c r="L268" s="29" t="s">
-        <v>1327</v>
+        <v>1325</v>
       </c>
       <c r="M268" s="32" t="s">
         <v>1062</v>
@@ -13978,10 +14034,10 @@
       <c r="I269" s="56"/>
       <c r="J269" s="32"/>
       <c r="K269" s="32" t="s">
-        <v>1366</v>
+        <v>1352</v>
       </c>
       <c r="L269" s="29" t="s">
-        <v>1327</v>
+        <v>1325</v>
       </c>
       <c r="M269" s="32" t="s">
         <v>1062</v>
@@ -14013,10 +14069,10 @@
       <c r="I270" s="56"/>
       <c r="J270" s="32"/>
       <c r="K270" s="32" t="s">
-        <v>1366</v>
+        <v>1352</v>
       </c>
       <c r="L270" s="29" t="s">
-        <v>1327</v>
+        <v>1325</v>
       </c>
       <c r="M270" s="32" t="s">
         <v>1062</v>
@@ -14048,10 +14104,10 @@
       <c r="I271" s="56"/>
       <c r="J271" s="32"/>
       <c r="K271" s="32" t="s">
-        <v>1366</v>
+        <v>1352</v>
       </c>
       <c r="L271" s="29" t="s">
-        <v>1327</v>
+        <v>1325</v>
       </c>
       <c r="M271" s="32" t="s">
         <v>1062</v>
@@ -14083,10 +14139,10 @@
       <c r="I272" s="56"/>
       <c r="J272" s="32"/>
       <c r="K272" s="32" t="s">
-        <v>1366</v>
+        <v>1352</v>
       </c>
       <c r="L272" s="29" t="s">
-        <v>1327</v>
+        <v>1325</v>
       </c>
       <c r="M272" s="32" t="s">
         <v>1062</v>
@@ -14118,10 +14174,10 @@
       <c r="I273" s="56"/>
       <c r="J273" s="32"/>
       <c r="K273" s="32" t="s">
-        <v>1366</v>
+        <v>1352</v>
       </c>
       <c r="L273" s="29" t="s">
-        <v>1327</v>
+        <v>1325</v>
       </c>
       <c r="M273" s="32" t="s">
         <v>1062</v>
@@ -14153,10 +14209,10 @@
       <c r="I274" s="56"/>
       <c r="J274" s="32"/>
       <c r="K274" s="32" t="s">
-        <v>1366</v>
+        <v>1352</v>
       </c>
       <c r="L274" s="29" t="s">
-        <v>1327</v>
+        <v>1325</v>
       </c>
       <c r="M274" s="32" t="s">
         <v>1062</v>
@@ -14188,10 +14244,10 @@
       <c r="I275" s="56"/>
       <c r="J275" s="32"/>
       <c r="K275" s="32" t="s">
-        <v>1366</v>
+        <v>1352</v>
       </c>
       <c r="L275" s="29" t="s">
-        <v>1327</v>
+        <v>1325</v>
       </c>
       <c r="M275" s="32" t="s">
         <v>1062</v>
@@ -14223,10 +14279,10 @@
       <c r="I276" s="56"/>
       <c r="J276" s="32"/>
       <c r="K276" s="32" t="s">
-        <v>1366</v>
+        <v>1352</v>
       </c>
       <c r="L276" s="29" t="s">
-        <v>1327</v>
+        <v>1325</v>
       </c>
       <c r="M276" s="32" t="s">
         <v>1062</v>
@@ -14258,10 +14314,10 @@
       <c r="I277" s="56"/>
       <c r="J277" s="32"/>
       <c r="K277" s="32" t="s">
-        <v>1366</v>
+        <v>1352</v>
       </c>
       <c r="L277" s="29" t="s">
-        <v>1327</v>
+        <v>1325</v>
       </c>
       <c r="M277" s="32" t="s">
         <v>1062</v>
@@ -14562,274 +14618,265 @@
     <hyperlink ref="E34" r:id="rId128" xr:uid="{D8EC1A48-443B-49CD-8D26-7CC2AA23D135}"/>
     <hyperlink ref="E35" r:id="rId129" xr:uid="{91C75FD7-25DF-42C8-AD4B-B2402A824327}"/>
     <hyperlink ref="E36" r:id="rId130" xr:uid="{99A72291-0FF9-459A-85D7-36F2B3051B7B}"/>
-    <hyperlink ref="B27" r:id="rId131" display="http://registry.it.csiro.au/sandbox/soil/scma" xr:uid="{7F51B6B3-1B6F-4778-BCFF-9D0D8B93E835}"/>
-    <hyperlink ref="E63" r:id="rId132" xr:uid="{0B886457-8AB9-4712-BE77-451FB95C6F9F}"/>
-    <hyperlink ref="E39" r:id="rId133" xr:uid="{9B1B8DB9-DF2A-4D3C-8C85-2322F1EA4B4E}"/>
-    <hyperlink ref="B25" r:id="rId134" xr:uid="{0B261E0C-9123-4445-954A-9D8C9B658D44}"/>
-    <hyperlink ref="C8" r:id="rId135" xr:uid="{8DBB0E3C-12E0-4ECD-8E5A-8FF6E1D63DC7}"/>
-    <hyperlink ref="B9" r:id="rId136" xr:uid="{9049C9D3-59FC-4186-9849-EE18D595D102}"/>
-    <hyperlink ref="B10" r:id="rId137" xr:uid="{D03C08EE-FAD9-451A-B164-33EDB0DB69AC}"/>
-    <hyperlink ref="B12" r:id="rId138" display="https://raw.githack.com/ANZSoilData/def-au-scma/master/html/00frontmatter/02About%20the%20authors.html" xr:uid="{9DB91834-4105-4172-ADA0-7AAD7C473A32}"/>
-    <hyperlink ref="L34" r:id="rId139" display="https://raw.githack.com/ANZSoilData/def-au-scma/master/html/00frontmatter/00WARNING.html" xr:uid="{CB3E79BD-6394-47FD-AC9A-691D757C8EEC}"/>
-    <hyperlink ref="L35" r:id="rId140" display="https://raw.githack.com/ANZSoilData/def-au-scma/master/html/00frontmatter/00WARNING.html" xr:uid="{F5F615A3-C1F0-4FEC-916E-AFF4A5EACA64}"/>
-    <hyperlink ref="L36" r:id="rId141" display="https://raw.githack.com/ANZSoilData/def-au-scma/master/html/00frontmatter/00WARNING.html" xr:uid="{278EBF9A-2216-40FB-827E-74BA612AD8BE}"/>
-    <hyperlink ref="L37" r:id="rId142" display="https://raw.githack.com/ANZSoilData/def-au-scma/master/html/00frontmatter/00WARNING.html" xr:uid="{E42C7D67-C252-40CC-93E1-3374C60542A5}"/>
-    <hyperlink ref="L38" r:id="rId143" display="https://raw.githack.com/ANZSoilData/def-au-scma/master/html/00frontmatter/00WARNING.html" xr:uid="{A69D3E3B-ABE6-46AF-9CA2-426AF8E885C7}"/>
-    <hyperlink ref="L42" r:id="rId144" display="https://raw.githack.com/ANZSoilData/def-au-scma/master/html/00frontmatter/00WARNING.html" xr:uid="{C5881908-AD6B-449F-88F5-CC8F544AA5E3}"/>
-    <hyperlink ref="L46" r:id="rId145" display="https://raw.githack.com/ANZSoilData/def-au-scma/master/html/00frontmatter/00WARNING.html" xr:uid="{BB05B484-C5E4-46CF-89B7-98D1661D001D}"/>
-    <hyperlink ref="L50" r:id="rId146" display="https://raw.githack.com/ANZSoilData/def-au-scma/master/html/00frontmatter/00WARNING.html" xr:uid="{C2E65B7B-B331-4507-8D52-5A93FDE8DA79}"/>
-    <hyperlink ref="L54" r:id="rId147" display="https://raw.githack.com/ANZSoilData/def-au-scma/master/html/00frontmatter/00WARNING.html" xr:uid="{384AA51D-A5DC-4119-AF0A-4BD44BC68C19}"/>
-    <hyperlink ref="L58" r:id="rId148" display="https://raw.githack.com/ANZSoilData/def-au-scma/master/html/00frontmatter/00WARNING.html" xr:uid="{A6951591-8A3B-448F-9043-B02DB820C883}"/>
-    <hyperlink ref="L62" r:id="rId149" display="https://raw.githack.com/ANZSoilData/def-au-scma/master/html/00frontmatter/00WARNING.html" xr:uid="{A6B9C716-A31D-49FD-8E69-FEE42AACF1DF}"/>
-    <hyperlink ref="L66" r:id="rId150" display="https://raw.githack.com/ANZSoilData/def-au-scma/master/html/00frontmatter/00WARNING.html" xr:uid="{4B48E133-5738-4DF2-B5CD-0CA87CE52D70}"/>
-    <hyperlink ref="L70" r:id="rId151" display="https://raw.githack.com/ANZSoilData/def-au-scma/master/html/00frontmatter/00WARNING.html" xr:uid="{E9020B38-A1EA-48E4-8340-9B4FCDC63BB6}"/>
-    <hyperlink ref="L74" r:id="rId152" display="https://raw.githack.com/ANZSoilData/def-au-scma/master/html/00frontmatter/00WARNING.html" xr:uid="{B49851C0-0DB5-4DB6-8DFD-C051A230FD34}"/>
-    <hyperlink ref="L78" r:id="rId153" display="https://raw.githack.com/ANZSoilData/def-au-scma/master/html/00frontmatter/00WARNING.html" xr:uid="{271EE2F2-89F0-4999-B130-94B0C0A0B716}"/>
-    <hyperlink ref="L82" r:id="rId154" display="https://raw.githack.com/ANZSoilData/def-au-scma/master/html/00frontmatter/00WARNING.html" xr:uid="{5C525A2B-15E6-4F9A-9183-8DD9535B9618}"/>
-    <hyperlink ref="L86" r:id="rId155" display="https://raw.githack.com/ANZSoilData/def-au-scma/master/html/00frontmatter/00WARNING.html" xr:uid="{6C8F404E-6D7F-4948-9754-DD620C6B6146}"/>
-    <hyperlink ref="L90" r:id="rId156" display="https://raw.githack.com/ANZSoilData/def-au-scma/master/html/00frontmatter/00WARNING.html" xr:uid="{DB279ACA-6062-4BE4-BBCC-40FDEED21C25}"/>
-    <hyperlink ref="L94" r:id="rId157" display="https://raw.githack.com/ANZSoilData/def-au-scma/master/html/00frontmatter/00WARNING.html" xr:uid="{4E90C937-CA16-45AB-99F3-C2AEAC1CB7F8}"/>
-    <hyperlink ref="L98" r:id="rId158" display="https://raw.githack.com/ANZSoilData/def-au-scma/master/html/00frontmatter/00WARNING.html" xr:uid="{04BCE300-1F7C-47F7-9A88-4E6F5A1C60C9}"/>
-    <hyperlink ref="L102" r:id="rId159" display="https://raw.githack.com/ANZSoilData/def-au-scma/master/html/00frontmatter/00WARNING.html" xr:uid="{D0F07E63-373A-436D-AF9B-83E05CAE7CCC}"/>
-    <hyperlink ref="L106" r:id="rId160" display="https://raw.githack.com/ANZSoilData/def-au-scma/master/html/00frontmatter/00WARNING.html" xr:uid="{45D8A7B9-CF8B-425F-8D7D-9A64A370C498}"/>
-    <hyperlink ref="L110" r:id="rId161" display="https://raw.githack.com/ANZSoilData/def-au-scma/master/html/00frontmatter/00WARNING.html" xr:uid="{407BEDCD-8BAB-438A-9F87-53E7F72B8E83}"/>
-    <hyperlink ref="L114" r:id="rId162" display="https://raw.githack.com/ANZSoilData/def-au-scma/master/html/00frontmatter/00WARNING.html" xr:uid="{2B3411EC-5AD3-42DE-A4AA-B892EC4CFF4A}"/>
-    <hyperlink ref="L118" r:id="rId163" display="https://raw.githack.com/ANZSoilData/def-au-scma/master/html/00frontmatter/00WARNING.html" xr:uid="{A933C6C5-ECF5-4273-8C29-D01DC233BB51}"/>
-    <hyperlink ref="L122" r:id="rId164" display="https://raw.githack.com/ANZSoilData/def-au-scma/master/html/00frontmatter/00WARNING.html" xr:uid="{6BFDF12A-9865-48D2-B544-8F2C5034E456}"/>
-    <hyperlink ref="L126" r:id="rId165" display="https://raw.githack.com/ANZSoilData/def-au-scma/master/html/00frontmatter/00WARNING.html" xr:uid="{E0DAF296-E5A7-4CA1-B8E2-1E4DB801A2F3}"/>
-    <hyperlink ref="L130" r:id="rId166" display="https://raw.githack.com/ANZSoilData/def-au-scma/master/html/00frontmatter/00WARNING.html" xr:uid="{88F2EB19-37BA-464D-80A9-F40863778A56}"/>
-    <hyperlink ref="L134" r:id="rId167" display="https://raw.githack.com/ANZSoilData/def-au-scma/master/html/00frontmatter/00WARNING.html" xr:uid="{EE925EA2-0FB1-46EB-B24B-F824122A44E6}"/>
-    <hyperlink ref="L138" r:id="rId168" display="https://raw.githack.com/ANZSoilData/def-au-scma/master/html/00frontmatter/00WARNING.html" xr:uid="{15CD14B3-3B9B-4915-A5B0-3AEBF5B8865A}"/>
-    <hyperlink ref="L142" r:id="rId169" display="https://raw.githack.com/ANZSoilData/def-au-scma/master/html/00frontmatter/00WARNING.html" xr:uid="{000F8552-2647-4F96-8E73-FF190E4B3907}"/>
-    <hyperlink ref="L146" r:id="rId170" display="https://raw.githack.com/ANZSoilData/def-au-scma/master/html/00frontmatter/00WARNING.html" xr:uid="{3DA4F56B-50A1-4981-AD0D-C71A88912DBD}"/>
-    <hyperlink ref="L150" r:id="rId171" display="https://raw.githack.com/ANZSoilData/def-au-scma/master/html/00frontmatter/00WARNING.html" xr:uid="{7FDD363C-A3BB-4CAE-AE96-A7EA6697BE87}"/>
-    <hyperlink ref="L154" r:id="rId172" display="https://raw.githack.com/ANZSoilData/def-au-scma/master/html/00frontmatter/00WARNING.html" xr:uid="{D28C0CC4-2DE7-4AC5-931A-4E92B082AE7B}"/>
-    <hyperlink ref="L158" r:id="rId173" display="https://raw.githack.com/ANZSoilData/def-au-scma/master/html/00frontmatter/00WARNING.html" xr:uid="{2ECA1824-002D-44DA-8AF0-0D43308E8569}"/>
-    <hyperlink ref="L162" r:id="rId174" display="https://raw.githack.com/ANZSoilData/def-au-scma/master/html/00frontmatter/00WARNING.html" xr:uid="{4B19B385-78E8-4DC7-A9B1-941F2EA86EE2}"/>
-    <hyperlink ref="L166" r:id="rId175" display="https://raw.githack.com/ANZSoilData/def-au-scma/master/html/00frontmatter/00WARNING.html" xr:uid="{4CD045CF-019E-4D4F-8F46-7BA1A3F46A2E}"/>
-    <hyperlink ref="L170" r:id="rId176" display="https://raw.githack.com/ANZSoilData/def-au-scma/master/html/00frontmatter/00WARNING.html" xr:uid="{2545A8C8-5423-4375-89F7-EA905B36ADF8}"/>
-    <hyperlink ref="L174" r:id="rId177" display="https://raw.githack.com/ANZSoilData/def-au-scma/master/html/00frontmatter/00WARNING.html" xr:uid="{CB2E050F-4D4E-4FEA-BF7E-21F66502C924}"/>
-    <hyperlink ref="L178" r:id="rId178" display="https://raw.githack.com/ANZSoilData/def-au-scma/master/html/00frontmatter/00WARNING.html" xr:uid="{56F548EA-D6B6-42BA-BB2E-1F2B231D7C3E}"/>
-    <hyperlink ref="L182" r:id="rId179" display="https://raw.githack.com/ANZSoilData/def-au-scma/master/html/00frontmatter/00WARNING.html" xr:uid="{88877C74-6F97-43C4-815E-E177EBE2EF11}"/>
-    <hyperlink ref="L186" r:id="rId180" display="https://raw.githack.com/ANZSoilData/def-au-scma/master/html/00frontmatter/00WARNING.html" xr:uid="{70078424-DD2C-4847-BCB7-F454A3162FC2}"/>
-    <hyperlink ref="L190" r:id="rId181" display="https://raw.githack.com/ANZSoilData/def-au-scma/master/html/00frontmatter/00WARNING.html" xr:uid="{0E6517EB-4855-41DE-987F-143892E2B7C1}"/>
-    <hyperlink ref="L194" r:id="rId182" display="https://raw.githack.com/ANZSoilData/def-au-scma/master/html/00frontmatter/00WARNING.html" xr:uid="{782FDB4D-E6D2-45B9-878C-BE56E11D270A}"/>
-    <hyperlink ref="L198" r:id="rId183" display="https://raw.githack.com/ANZSoilData/def-au-scma/master/html/00frontmatter/00WARNING.html" xr:uid="{86AC3898-4C59-4216-BEF9-29B21713453F}"/>
-    <hyperlink ref="L202" r:id="rId184" display="https://raw.githack.com/ANZSoilData/def-au-scma/master/html/00frontmatter/00WARNING.html" xr:uid="{0BF76340-A769-4B5B-8E2B-0FD8405A7844}"/>
-    <hyperlink ref="L206" r:id="rId185" display="https://raw.githack.com/ANZSoilData/def-au-scma/master/html/00frontmatter/00WARNING.html" xr:uid="{EF1FD8A3-B6C1-4EA6-AE86-65BE742AC40B}"/>
-    <hyperlink ref="L210" r:id="rId186" display="https://raw.githack.com/ANZSoilData/def-au-scma/master/html/00frontmatter/00WARNING.html" xr:uid="{6859DA30-B43E-4C0A-AA9F-2FC8794AFF42}"/>
-    <hyperlink ref="L214" r:id="rId187" display="https://raw.githack.com/ANZSoilData/def-au-scma/master/html/00frontmatter/00WARNING.html" xr:uid="{BE4D8A2D-827D-41E5-8A9E-A5CE9D908B42}"/>
-    <hyperlink ref="L218" r:id="rId188" display="https://raw.githack.com/ANZSoilData/def-au-scma/master/html/00frontmatter/00WARNING.html" xr:uid="{E3CD281C-17A6-4937-9E6D-9D0E74DC683C}"/>
-    <hyperlink ref="L222" r:id="rId189" display="https://raw.githack.com/ANZSoilData/def-au-scma/master/html/00frontmatter/00WARNING.html" xr:uid="{B277ADAB-9569-4012-8E2B-1AE67BF47AE0}"/>
-    <hyperlink ref="L226" r:id="rId190" display="https://raw.githack.com/ANZSoilData/def-au-scma/master/html/00frontmatter/00WARNING.html" xr:uid="{68F9DE8D-DAB9-4472-B057-FC76DB29B45F}"/>
-    <hyperlink ref="L230" r:id="rId191" display="https://raw.githack.com/ANZSoilData/def-au-scma/master/html/00frontmatter/00WARNING.html" xr:uid="{826571F9-51BC-4DDE-A916-A170141BF315}"/>
-    <hyperlink ref="L234" r:id="rId192" display="https://raw.githack.com/ANZSoilData/def-au-scma/master/html/00frontmatter/00WARNING.html" xr:uid="{9C5B3FF8-B36A-4F89-8A77-F8A6E4937D4E}"/>
-    <hyperlink ref="L238" r:id="rId193" display="https://raw.githack.com/ANZSoilData/def-au-scma/master/html/00frontmatter/00WARNING.html" xr:uid="{1193A72D-1EF4-4467-9D1B-6815C2DE1470}"/>
-    <hyperlink ref="L242" r:id="rId194" display="https://raw.githack.com/ANZSoilData/def-au-scma/master/html/00frontmatter/00WARNING.html" xr:uid="{4E0FF932-A770-46BE-B1B1-C3FFBD0CD661}"/>
-    <hyperlink ref="L246" r:id="rId195" display="https://raw.githack.com/ANZSoilData/def-au-scma/master/html/00frontmatter/00WARNING.html" xr:uid="{EB815369-4D6A-4437-A061-E196F51903FA}"/>
-    <hyperlink ref="L250" r:id="rId196" display="https://raw.githack.com/ANZSoilData/def-au-scma/master/html/00frontmatter/00WARNING.html" xr:uid="{318C3648-7B72-4918-B38A-CF1EF4A88545}"/>
-    <hyperlink ref="L254" r:id="rId197" display="https://raw.githack.com/ANZSoilData/def-au-scma/master/html/00frontmatter/00WARNING.html" xr:uid="{0BBD7D6B-1DD3-43D6-8258-B44668713C6F}"/>
-    <hyperlink ref="L258" r:id="rId198" display="https://raw.githack.com/ANZSoilData/def-au-scma/master/html/00frontmatter/00WARNING.html" xr:uid="{93F3205E-2B9E-493C-8403-ECA1835F1C9E}"/>
-    <hyperlink ref="L262" r:id="rId199" display="https://raw.githack.com/ANZSoilData/def-au-scma/master/html/00frontmatter/00WARNING.html" xr:uid="{0508569E-0D73-4B55-B4E6-D07B44434D59}"/>
-    <hyperlink ref="L266" r:id="rId200" display="https://raw.githack.com/ANZSoilData/def-au-scma/master/html/00frontmatter/00WARNING.html" xr:uid="{AE685D0A-D4A5-4F2D-9769-CB5645F2AE8C}"/>
-    <hyperlink ref="L270" r:id="rId201" display="https://raw.githack.com/ANZSoilData/def-au-scma/master/html/00frontmatter/00WARNING.html" xr:uid="{0942CB22-9E70-4BB4-8887-BAF6127F6A93}"/>
-    <hyperlink ref="L274" r:id="rId202" display="https://raw.githack.com/ANZSoilData/def-au-scma/master/html/00frontmatter/00WARNING.html" xr:uid="{5BF9E46E-15C4-4066-B2E6-78BC95C81C6C}"/>
-    <hyperlink ref="L39" r:id="rId203" display="https://raw.githack.com/ANZSoilData/def-au-scma/master/html/00frontmatter/00WARNING.html" xr:uid="{30A42CBA-DD18-467F-9C31-F6FE20395F12}"/>
-    <hyperlink ref="L43" r:id="rId204" display="https://raw.githack.com/ANZSoilData/def-au-scma/master/html/00frontmatter/00WARNING.html" xr:uid="{5A22AFAB-6468-4305-AD73-0CF97A30E89A}"/>
-    <hyperlink ref="L47" r:id="rId205" display="https://raw.githack.com/ANZSoilData/def-au-scma/master/html/00frontmatter/00WARNING.html" xr:uid="{A894C31D-B0B3-40F6-BA59-DCF868A0C957}"/>
-    <hyperlink ref="L51" r:id="rId206" display="https://raw.githack.com/ANZSoilData/def-au-scma/master/html/00frontmatter/00WARNING.html" xr:uid="{D23DA804-39BD-4AEE-8663-7A6F4D17FEFA}"/>
-    <hyperlink ref="L55" r:id="rId207" display="https://raw.githack.com/ANZSoilData/def-au-scma/master/html/00frontmatter/00WARNING.html" xr:uid="{E56FB670-8B05-410B-862D-B206DFE828F1}"/>
-    <hyperlink ref="L59" r:id="rId208" display="https://raw.githack.com/ANZSoilData/def-au-scma/master/html/00frontmatter/00WARNING.html" xr:uid="{8D513C73-0385-4B20-91E6-5018B06FB850}"/>
-    <hyperlink ref="L63" r:id="rId209" display="https://raw.githack.com/ANZSoilData/def-au-scma/master/html/00frontmatter/00WARNING.html" xr:uid="{5BE35CB8-C72D-4045-BA1A-F17E3F258A20}"/>
-    <hyperlink ref="L67" r:id="rId210" display="https://raw.githack.com/ANZSoilData/def-au-scma/master/html/00frontmatter/00WARNING.html" xr:uid="{BB03F070-978E-47EB-BE13-510499AFD277}"/>
-    <hyperlink ref="L71" r:id="rId211" display="https://raw.githack.com/ANZSoilData/def-au-scma/master/html/00frontmatter/00WARNING.html" xr:uid="{73FC3383-83C8-43ED-A91E-628A288D9395}"/>
-    <hyperlink ref="L75" r:id="rId212" display="https://raw.githack.com/ANZSoilData/def-au-scma/master/html/00frontmatter/00WARNING.html" xr:uid="{78E3B867-8170-44BF-827E-6441CA1C2CD0}"/>
-    <hyperlink ref="L79" r:id="rId213" display="https://raw.githack.com/ANZSoilData/def-au-scma/master/html/00frontmatter/00WARNING.html" xr:uid="{CC968019-5D38-4E3D-B76A-490EF3E1AF7A}"/>
-    <hyperlink ref="L83" r:id="rId214" display="https://raw.githack.com/ANZSoilData/def-au-scma/master/html/00frontmatter/00WARNING.html" xr:uid="{709FD2AB-D563-4156-B0D3-CBDCE5FC876F}"/>
-    <hyperlink ref="L87" r:id="rId215" display="https://raw.githack.com/ANZSoilData/def-au-scma/master/html/00frontmatter/00WARNING.html" xr:uid="{8AFE6D1F-27CD-43CC-A3B7-BE202F7ABB64}"/>
-    <hyperlink ref="L91" r:id="rId216" display="https://raw.githack.com/ANZSoilData/def-au-scma/master/html/00frontmatter/00WARNING.html" xr:uid="{A1D6BFA7-BB0A-490A-87DE-3F2989AB6412}"/>
-    <hyperlink ref="L95" r:id="rId217" display="https://raw.githack.com/ANZSoilData/def-au-scma/master/html/00frontmatter/00WARNING.html" xr:uid="{96228920-6203-4418-A1D4-16DFFB530584}"/>
-    <hyperlink ref="L99" r:id="rId218" display="https://raw.githack.com/ANZSoilData/def-au-scma/master/html/00frontmatter/00WARNING.html" xr:uid="{FD3B19A9-F2F6-4A0E-9A24-22FFEE18B162}"/>
-    <hyperlink ref="L103" r:id="rId219" display="https://raw.githack.com/ANZSoilData/def-au-scma/master/html/00frontmatter/00WARNING.html" xr:uid="{A0F35CCF-773B-4A45-980D-174373464D93}"/>
-    <hyperlink ref="L107" r:id="rId220" display="https://raw.githack.com/ANZSoilData/def-au-scma/master/html/00frontmatter/00WARNING.html" xr:uid="{7266C1D8-99A6-4933-AD15-6083CA68C66B}"/>
-    <hyperlink ref="L111" r:id="rId221" display="https://raw.githack.com/ANZSoilData/def-au-scma/master/html/00frontmatter/00WARNING.html" xr:uid="{CB081986-B9B5-4D9A-A30B-41E65BAA2B03}"/>
-    <hyperlink ref="L115" r:id="rId222" display="https://raw.githack.com/ANZSoilData/def-au-scma/master/html/00frontmatter/00WARNING.html" xr:uid="{88E02967-8C20-4A8B-820D-1A9B1D2A239D}"/>
-    <hyperlink ref="L119" r:id="rId223" display="https://raw.githack.com/ANZSoilData/def-au-scma/master/html/00frontmatter/00WARNING.html" xr:uid="{5032FF67-F514-4AC7-9ED9-86936D11C989}"/>
-    <hyperlink ref="L123" r:id="rId224" display="https://raw.githack.com/ANZSoilData/def-au-scma/master/html/00frontmatter/00WARNING.html" xr:uid="{980ECBA1-CE6C-4F9A-BCCA-498D9933620B}"/>
-    <hyperlink ref="L127" r:id="rId225" display="https://raw.githack.com/ANZSoilData/def-au-scma/master/html/00frontmatter/00WARNING.html" xr:uid="{A3D0F967-DB8F-47F4-89BA-4CD45013467C}"/>
-    <hyperlink ref="L131" r:id="rId226" display="https://raw.githack.com/ANZSoilData/def-au-scma/master/html/00frontmatter/00WARNING.html" xr:uid="{F9EAD012-17B1-4863-8FFA-DA7FB15B4704}"/>
-    <hyperlink ref="L135" r:id="rId227" display="https://raw.githack.com/ANZSoilData/def-au-scma/master/html/00frontmatter/00WARNING.html" xr:uid="{CA95C6AF-B27A-42AF-8CB2-B0C8E4EF8232}"/>
-    <hyperlink ref="L139" r:id="rId228" display="https://raw.githack.com/ANZSoilData/def-au-scma/master/html/00frontmatter/00WARNING.html" xr:uid="{4968B8D1-1D97-4C9C-B97D-4334D24C3427}"/>
-    <hyperlink ref="L143" r:id="rId229" display="https://raw.githack.com/ANZSoilData/def-au-scma/master/html/00frontmatter/00WARNING.html" xr:uid="{555B537C-B9B7-4FAD-A13F-DC22ED3EA4FF}"/>
-    <hyperlink ref="L147" r:id="rId230" display="https://raw.githack.com/ANZSoilData/def-au-scma/master/html/00frontmatter/00WARNING.html" xr:uid="{097A3001-1F5F-448D-BE91-B846A20946BF}"/>
-    <hyperlink ref="L151" r:id="rId231" display="https://raw.githack.com/ANZSoilData/def-au-scma/master/html/00frontmatter/00WARNING.html" xr:uid="{6B1D3378-752F-4BAC-8DB4-831C610823E4}"/>
-    <hyperlink ref="L155" r:id="rId232" display="https://raw.githack.com/ANZSoilData/def-au-scma/master/html/00frontmatter/00WARNING.html" xr:uid="{0C853A69-79FF-4051-BB65-8096116EFE05}"/>
-    <hyperlink ref="L159" r:id="rId233" display="https://raw.githack.com/ANZSoilData/def-au-scma/master/html/00frontmatter/00WARNING.html" xr:uid="{BDB03E03-6E05-420B-B6F3-DD509A13AA69}"/>
-    <hyperlink ref="L163" r:id="rId234" display="https://raw.githack.com/ANZSoilData/def-au-scma/master/html/00frontmatter/00WARNING.html" xr:uid="{0E593F0C-E94A-4192-B365-6B1BF3D75FE3}"/>
-    <hyperlink ref="L167" r:id="rId235" display="https://raw.githack.com/ANZSoilData/def-au-scma/master/html/00frontmatter/00WARNING.html" xr:uid="{4C0A014B-F1BC-4D85-892C-5401BB07C8F9}"/>
-    <hyperlink ref="L171" r:id="rId236" display="https://raw.githack.com/ANZSoilData/def-au-scma/master/html/00frontmatter/00WARNING.html" xr:uid="{DACFF655-3EB2-49BA-97BC-7CA8DE3EBAEF}"/>
-    <hyperlink ref="L175" r:id="rId237" display="https://raw.githack.com/ANZSoilData/def-au-scma/master/html/00frontmatter/00WARNING.html" xr:uid="{12E6FF77-73A7-4FB8-A00D-F247483FC12C}"/>
-    <hyperlink ref="L179" r:id="rId238" display="https://raw.githack.com/ANZSoilData/def-au-scma/master/html/00frontmatter/00WARNING.html" xr:uid="{AE645C7B-63D5-4015-A28D-908F7BF75F66}"/>
-    <hyperlink ref="L183" r:id="rId239" display="https://raw.githack.com/ANZSoilData/def-au-scma/master/html/00frontmatter/00WARNING.html" xr:uid="{81FFA0EB-02DD-4EA5-8C05-08CACC157220}"/>
-    <hyperlink ref="L187" r:id="rId240" display="https://raw.githack.com/ANZSoilData/def-au-scma/master/html/00frontmatter/00WARNING.html" xr:uid="{8464762C-F21A-4CDB-8431-52DBE700EF69}"/>
-    <hyperlink ref="L191" r:id="rId241" display="https://raw.githack.com/ANZSoilData/def-au-scma/master/html/00frontmatter/00WARNING.html" xr:uid="{1E6DB17F-AEB3-4A28-958C-C86D718E6D69}"/>
-    <hyperlink ref="L195" r:id="rId242" display="https://raw.githack.com/ANZSoilData/def-au-scma/master/html/00frontmatter/00WARNING.html" xr:uid="{AB2B88FF-BA42-4A3E-8988-89AB43174E5E}"/>
-    <hyperlink ref="L199" r:id="rId243" display="https://raw.githack.com/ANZSoilData/def-au-scma/master/html/00frontmatter/00WARNING.html" xr:uid="{98C388BB-DC1C-4589-9234-F0D03FAB986F}"/>
-    <hyperlink ref="L203" r:id="rId244" display="https://raw.githack.com/ANZSoilData/def-au-scma/master/html/00frontmatter/00WARNING.html" xr:uid="{F2A8149E-C4D1-4E10-8ED8-C1CA95C38F4E}"/>
-    <hyperlink ref="L207" r:id="rId245" display="https://raw.githack.com/ANZSoilData/def-au-scma/master/html/00frontmatter/00WARNING.html" xr:uid="{B27CE42B-FB56-445C-AA4C-CAE253C53384}"/>
-    <hyperlink ref="L211" r:id="rId246" display="https://raw.githack.com/ANZSoilData/def-au-scma/master/html/00frontmatter/00WARNING.html" xr:uid="{2F72E7F4-A004-4AA4-A0BC-373CA95B0FC8}"/>
-    <hyperlink ref="L215" r:id="rId247" display="https://raw.githack.com/ANZSoilData/def-au-scma/master/html/00frontmatter/00WARNING.html" xr:uid="{71D97D79-1841-43F8-8E00-29BB9E4F634D}"/>
-    <hyperlink ref="L219" r:id="rId248" display="https://raw.githack.com/ANZSoilData/def-au-scma/master/html/00frontmatter/00WARNING.html" xr:uid="{C57BE990-59AC-412B-B718-CBD3A5F98AFF}"/>
-    <hyperlink ref="L223" r:id="rId249" display="https://raw.githack.com/ANZSoilData/def-au-scma/master/html/00frontmatter/00WARNING.html" xr:uid="{252723D2-D506-43E4-AA8E-D1AC81C94F2D}"/>
-    <hyperlink ref="L227" r:id="rId250" display="https://raw.githack.com/ANZSoilData/def-au-scma/master/html/00frontmatter/00WARNING.html" xr:uid="{480F6310-1D87-4C3A-860F-86B3FACDD196}"/>
-    <hyperlink ref="L231" r:id="rId251" display="https://raw.githack.com/ANZSoilData/def-au-scma/master/html/00frontmatter/00WARNING.html" xr:uid="{F3793526-865F-4475-9797-A39D3B78171B}"/>
-    <hyperlink ref="L235" r:id="rId252" display="https://raw.githack.com/ANZSoilData/def-au-scma/master/html/00frontmatter/00WARNING.html" xr:uid="{D751496D-50FA-40D6-8093-ADC3D3FF8073}"/>
-    <hyperlink ref="L239" r:id="rId253" display="https://raw.githack.com/ANZSoilData/def-au-scma/master/html/00frontmatter/00WARNING.html" xr:uid="{8AF0ECE2-B8BE-45DA-B1C0-6F647DDD5E3F}"/>
-    <hyperlink ref="L243" r:id="rId254" display="https://raw.githack.com/ANZSoilData/def-au-scma/master/html/00frontmatter/00WARNING.html" xr:uid="{1CC92C21-EC70-434D-8DB7-16DAE06AB483}"/>
-    <hyperlink ref="L247" r:id="rId255" display="https://raw.githack.com/ANZSoilData/def-au-scma/master/html/00frontmatter/00WARNING.html" xr:uid="{A820BB9D-32C7-431C-89F9-BA0A82C0EC5C}"/>
-    <hyperlink ref="L251" r:id="rId256" display="https://raw.githack.com/ANZSoilData/def-au-scma/master/html/00frontmatter/00WARNING.html" xr:uid="{BA3B7869-E9DF-4EAE-9C15-E9EE4533BE99}"/>
-    <hyperlink ref="L255" r:id="rId257" display="https://raw.githack.com/ANZSoilData/def-au-scma/master/html/00frontmatter/00WARNING.html" xr:uid="{236D1A28-656A-468B-9DE9-23E1519F7951}"/>
-    <hyperlink ref="L259" r:id="rId258" display="https://raw.githack.com/ANZSoilData/def-au-scma/master/html/00frontmatter/00WARNING.html" xr:uid="{8EFC5F39-0491-4EB3-9EE0-8D3FD74253A7}"/>
-    <hyperlink ref="L263" r:id="rId259" display="https://raw.githack.com/ANZSoilData/def-au-scma/master/html/00frontmatter/00WARNING.html" xr:uid="{FA3A2069-D9DF-45C6-BDAB-8DF6F1F69E05}"/>
-    <hyperlink ref="L267" r:id="rId260" display="https://raw.githack.com/ANZSoilData/def-au-scma/master/html/00frontmatter/00WARNING.html" xr:uid="{42C16B11-14D3-45E3-87FB-C661497704DA}"/>
-    <hyperlink ref="L271" r:id="rId261" display="https://raw.githack.com/ANZSoilData/def-au-scma/master/html/00frontmatter/00WARNING.html" xr:uid="{B753BF0E-6479-432B-8FD6-14CD1A990CC9}"/>
-    <hyperlink ref="L275" r:id="rId262" display="https://raw.githack.com/ANZSoilData/def-au-scma/master/html/00frontmatter/00WARNING.html" xr:uid="{1B11A110-44A6-4C92-94FC-BF0648BADC68}"/>
-    <hyperlink ref="L40" r:id="rId263" display="https://raw.githack.com/ANZSoilData/def-au-scma/master/html/00frontmatter/00WARNING.html" xr:uid="{5CCA99B3-866E-43B6-A611-4011A70232F3}"/>
-    <hyperlink ref="L44" r:id="rId264" display="https://raw.githack.com/ANZSoilData/def-au-scma/master/html/00frontmatter/00WARNING.html" xr:uid="{60163CA2-837F-43E2-A306-DBAD49073A6A}"/>
-    <hyperlink ref="L48" r:id="rId265" display="https://raw.githack.com/ANZSoilData/def-au-scma/master/html/00frontmatter/00WARNING.html" xr:uid="{7C035D9F-54E0-43B8-BE0D-31005E151DFD}"/>
-    <hyperlink ref="L52" r:id="rId266" display="https://raw.githack.com/ANZSoilData/def-au-scma/master/html/00frontmatter/00WARNING.html" xr:uid="{E5BF080A-7169-457C-9FD9-974AA2A3EA96}"/>
-    <hyperlink ref="L56" r:id="rId267" display="https://raw.githack.com/ANZSoilData/def-au-scma/master/html/00frontmatter/00WARNING.html" xr:uid="{C419F04A-C54F-491B-9CAA-EA6CCE9645F3}"/>
-    <hyperlink ref="L60" r:id="rId268" display="https://raw.githack.com/ANZSoilData/def-au-scma/master/html/00frontmatter/00WARNING.html" xr:uid="{676681FE-C4E1-4AE3-9381-18BF4E9A8C07}"/>
-    <hyperlink ref="L64" r:id="rId269" display="https://raw.githack.com/ANZSoilData/def-au-scma/master/html/00frontmatter/00WARNING.html" xr:uid="{BA256E0C-40BE-4E65-A385-BF6790B75104}"/>
-    <hyperlink ref="L68" r:id="rId270" display="https://raw.githack.com/ANZSoilData/def-au-scma/master/html/00frontmatter/00WARNING.html" xr:uid="{5CE921C2-4E7E-4BC3-AC98-8751264618A2}"/>
-    <hyperlink ref="L72" r:id="rId271" display="https://raw.githack.com/ANZSoilData/def-au-scma/master/html/00frontmatter/00WARNING.html" xr:uid="{68C94CE0-F780-4EFF-A1A8-29A6CD247330}"/>
-    <hyperlink ref="L76" r:id="rId272" display="https://raw.githack.com/ANZSoilData/def-au-scma/master/html/00frontmatter/00WARNING.html" xr:uid="{FC129378-D596-4BC1-85FF-225DA48BE830}"/>
-    <hyperlink ref="L80" r:id="rId273" display="https://raw.githack.com/ANZSoilData/def-au-scma/master/html/00frontmatter/00WARNING.html" xr:uid="{6F208267-F557-49BB-9BF3-DD87EDDC8358}"/>
-    <hyperlink ref="L84" r:id="rId274" display="https://raw.githack.com/ANZSoilData/def-au-scma/master/html/00frontmatter/00WARNING.html" xr:uid="{29FA809A-27F9-4E8B-8D23-5CA7F7981C7E}"/>
-    <hyperlink ref="L88" r:id="rId275" display="https://raw.githack.com/ANZSoilData/def-au-scma/master/html/00frontmatter/00WARNING.html" xr:uid="{5C269D3B-1522-4A46-BC70-FD2C7846FE01}"/>
-    <hyperlink ref="L92" r:id="rId276" display="https://raw.githack.com/ANZSoilData/def-au-scma/master/html/00frontmatter/00WARNING.html" xr:uid="{DDBF9AC4-0578-4EA5-91E5-EF400563AFB8}"/>
-    <hyperlink ref="L96" r:id="rId277" display="https://raw.githack.com/ANZSoilData/def-au-scma/master/html/00frontmatter/00WARNING.html" xr:uid="{BBBAB2BB-66BC-4907-8FF4-F8F983CA027E}"/>
-    <hyperlink ref="L100" r:id="rId278" display="https://raw.githack.com/ANZSoilData/def-au-scma/master/html/00frontmatter/00WARNING.html" xr:uid="{294A4606-458C-441F-8E41-924881F3B04A}"/>
-    <hyperlink ref="L104" r:id="rId279" display="https://raw.githack.com/ANZSoilData/def-au-scma/master/html/00frontmatter/00WARNING.html" xr:uid="{4C91B85F-765B-497E-A795-D052E85F5F55}"/>
-    <hyperlink ref="L108" r:id="rId280" display="https://raw.githack.com/ANZSoilData/def-au-scma/master/html/00frontmatter/00WARNING.html" xr:uid="{FF989142-2B51-4C57-9039-6B44F89F2286}"/>
-    <hyperlink ref="L112" r:id="rId281" display="https://raw.githack.com/ANZSoilData/def-au-scma/master/html/00frontmatter/00WARNING.html" xr:uid="{21ACE121-FF7A-4B33-867E-91F244C80EB4}"/>
-    <hyperlink ref="L116" r:id="rId282" display="https://raw.githack.com/ANZSoilData/def-au-scma/master/html/00frontmatter/00WARNING.html" xr:uid="{1D0130E9-573E-44D8-AD88-388FECD85C16}"/>
-    <hyperlink ref="L120" r:id="rId283" display="https://raw.githack.com/ANZSoilData/def-au-scma/master/html/00frontmatter/00WARNING.html" xr:uid="{774829A9-46DF-4BDE-99C6-1275D3F2E271}"/>
-    <hyperlink ref="L124" r:id="rId284" display="https://raw.githack.com/ANZSoilData/def-au-scma/master/html/00frontmatter/00WARNING.html" xr:uid="{AA566C8D-29BC-4A2C-B261-447942C09FE9}"/>
-    <hyperlink ref="L128" r:id="rId285" display="https://raw.githack.com/ANZSoilData/def-au-scma/master/html/00frontmatter/00WARNING.html" xr:uid="{13B9C285-B467-4AF1-AC33-2F017DA31B03}"/>
-    <hyperlink ref="L132" r:id="rId286" display="https://raw.githack.com/ANZSoilData/def-au-scma/master/html/00frontmatter/00WARNING.html" xr:uid="{70B06375-FA01-4E6D-BD77-6719E0D8DD2A}"/>
-    <hyperlink ref="L136" r:id="rId287" display="https://raw.githack.com/ANZSoilData/def-au-scma/master/html/00frontmatter/00WARNING.html" xr:uid="{A24C20C8-DFF5-4CBF-9ADB-CAC93071C843}"/>
-    <hyperlink ref="L140" r:id="rId288" display="https://raw.githack.com/ANZSoilData/def-au-scma/master/html/00frontmatter/00WARNING.html" xr:uid="{6A175C0E-3DC9-46EA-BBCF-11C27BF0CAB8}"/>
-    <hyperlink ref="L144" r:id="rId289" display="https://raw.githack.com/ANZSoilData/def-au-scma/master/html/00frontmatter/00WARNING.html" xr:uid="{4088B65F-6821-4CC3-95A7-3743BFBA99F7}"/>
-    <hyperlink ref="L148" r:id="rId290" display="https://raw.githack.com/ANZSoilData/def-au-scma/master/html/00frontmatter/00WARNING.html" xr:uid="{7FF78193-6C29-41F2-BC58-2619AA6F81DB}"/>
-    <hyperlink ref="L152" r:id="rId291" display="https://raw.githack.com/ANZSoilData/def-au-scma/master/html/00frontmatter/00WARNING.html" xr:uid="{6A7D753C-BD96-40F8-B028-22A4193AE97D}"/>
-    <hyperlink ref="L156" r:id="rId292" display="https://raw.githack.com/ANZSoilData/def-au-scma/master/html/00frontmatter/00WARNING.html" xr:uid="{DCA6DC69-4135-4519-B98A-FA4E4C9FD6C5}"/>
-    <hyperlink ref="L160" r:id="rId293" display="https://raw.githack.com/ANZSoilData/def-au-scma/master/html/00frontmatter/00WARNING.html" xr:uid="{B343BE67-86D0-4FB5-8434-555231AED175}"/>
-    <hyperlink ref="L164" r:id="rId294" display="https://raw.githack.com/ANZSoilData/def-au-scma/master/html/00frontmatter/00WARNING.html" xr:uid="{31DC2E97-749B-4FB0-AC9C-3AA71EE76372}"/>
-    <hyperlink ref="L168" r:id="rId295" display="https://raw.githack.com/ANZSoilData/def-au-scma/master/html/00frontmatter/00WARNING.html" xr:uid="{4EAAACC7-D31C-4207-83A9-0642D09F4D8D}"/>
-    <hyperlink ref="L172" r:id="rId296" display="https://raw.githack.com/ANZSoilData/def-au-scma/master/html/00frontmatter/00WARNING.html" xr:uid="{13AF4C94-9498-407A-AFB8-BE3F38237FD2}"/>
-    <hyperlink ref="L176" r:id="rId297" display="https://raw.githack.com/ANZSoilData/def-au-scma/master/html/00frontmatter/00WARNING.html" xr:uid="{8F7D3974-22FD-4906-9F5C-5D9EA98DAF04}"/>
-    <hyperlink ref="L180" r:id="rId298" display="https://raw.githack.com/ANZSoilData/def-au-scma/master/html/00frontmatter/00WARNING.html" xr:uid="{8EE35985-963D-4B76-91DA-5142551084B8}"/>
-    <hyperlink ref="L184" r:id="rId299" display="https://raw.githack.com/ANZSoilData/def-au-scma/master/html/00frontmatter/00WARNING.html" xr:uid="{6A81AD3A-73D5-4B78-8C3C-F7473E5C0A9C}"/>
-    <hyperlink ref="L188" r:id="rId300" display="https://raw.githack.com/ANZSoilData/def-au-scma/master/html/00frontmatter/00WARNING.html" xr:uid="{DC984535-9A7B-4AB4-8DA7-CA5DB8609120}"/>
-    <hyperlink ref="L192" r:id="rId301" display="https://raw.githack.com/ANZSoilData/def-au-scma/master/html/00frontmatter/00WARNING.html" xr:uid="{29B6C9A9-646B-430C-8123-3BCE48A33F81}"/>
-    <hyperlink ref="L196" r:id="rId302" display="https://raw.githack.com/ANZSoilData/def-au-scma/master/html/00frontmatter/00WARNING.html" xr:uid="{10D16AE2-36F6-4868-9DB7-C03857B691DB}"/>
-    <hyperlink ref="L200" r:id="rId303" display="https://raw.githack.com/ANZSoilData/def-au-scma/master/html/00frontmatter/00WARNING.html" xr:uid="{E9C6F802-D408-4710-90E8-3CFA4233A1CE}"/>
-    <hyperlink ref="L204" r:id="rId304" display="https://raw.githack.com/ANZSoilData/def-au-scma/master/html/00frontmatter/00WARNING.html" xr:uid="{B4403BD4-6BD6-44F0-9746-17390040B9DB}"/>
-    <hyperlink ref="L208" r:id="rId305" display="https://raw.githack.com/ANZSoilData/def-au-scma/master/html/00frontmatter/00WARNING.html" xr:uid="{050B8865-C8DE-4160-880A-B5D6524E9CB0}"/>
-    <hyperlink ref="L212" r:id="rId306" display="https://raw.githack.com/ANZSoilData/def-au-scma/master/html/00frontmatter/00WARNING.html" xr:uid="{66C262F9-2897-41D2-A86A-D0D64AD22593}"/>
-    <hyperlink ref="L216" r:id="rId307" display="https://raw.githack.com/ANZSoilData/def-au-scma/master/html/00frontmatter/00WARNING.html" xr:uid="{F1B703C3-2898-4AC9-9795-DE7067FC446A}"/>
-    <hyperlink ref="L220" r:id="rId308" display="https://raw.githack.com/ANZSoilData/def-au-scma/master/html/00frontmatter/00WARNING.html" xr:uid="{34AEBBDD-1251-4A9A-AC33-8E55F0780F6A}"/>
-    <hyperlink ref="L224" r:id="rId309" display="https://raw.githack.com/ANZSoilData/def-au-scma/master/html/00frontmatter/00WARNING.html" xr:uid="{CF4F3331-D149-497C-9342-B6502D8EE3A0}"/>
-    <hyperlink ref="L228" r:id="rId310" display="https://raw.githack.com/ANZSoilData/def-au-scma/master/html/00frontmatter/00WARNING.html" xr:uid="{55B893E1-1CDE-4E5C-8319-16A24C45FDB5}"/>
-    <hyperlink ref="L232" r:id="rId311" display="https://raw.githack.com/ANZSoilData/def-au-scma/master/html/00frontmatter/00WARNING.html" xr:uid="{D698468E-B9B5-4A59-AA9C-59D1906B42FC}"/>
-    <hyperlink ref="L236" r:id="rId312" display="https://raw.githack.com/ANZSoilData/def-au-scma/master/html/00frontmatter/00WARNING.html" xr:uid="{6B9A4D10-FD80-4A84-9EE4-4199786D92A6}"/>
-    <hyperlink ref="L240" r:id="rId313" display="https://raw.githack.com/ANZSoilData/def-au-scma/master/html/00frontmatter/00WARNING.html" xr:uid="{16005748-8FFE-42D3-AEDC-33B24C0F45CB}"/>
-    <hyperlink ref="L244" r:id="rId314" display="https://raw.githack.com/ANZSoilData/def-au-scma/master/html/00frontmatter/00WARNING.html" xr:uid="{D8F7454F-9017-418C-B0DE-1D1979473AEF}"/>
-    <hyperlink ref="L248" r:id="rId315" display="https://raw.githack.com/ANZSoilData/def-au-scma/master/html/00frontmatter/00WARNING.html" xr:uid="{F248501B-D943-4136-B872-7C7BAE5EAC28}"/>
-    <hyperlink ref="L252" r:id="rId316" display="https://raw.githack.com/ANZSoilData/def-au-scma/master/html/00frontmatter/00WARNING.html" xr:uid="{890D5642-432C-4F1B-BDEE-2BDEC871BF0B}"/>
-    <hyperlink ref="L256" r:id="rId317" display="https://raw.githack.com/ANZSoilData/def-au-scma/master/html/00frontmatter/00WARNING.html" xr:uid="{D4C728F3-C78C-4F15-8157-2EDE92E30400}"/>
-    <hyperlink ref="L260" r:id="rId318" display="https://raw.githack.com/ANZSoilData/def-au-scma/master/html/00frontmatter/00WARNING.html" xr:uid="{EC6EE0FB-897B-47E1-9E59-EAF768DB0B3F}"/>
-    <hyperlink ref="L264" r:id="rId319" display="https://raw.githack.com/ANZSoilData/def-au-scma/master/html/00frontmatter/00WARNING.html" xr:uid="{8F7614C2-098F-47E8-83F6-DC495F23DE1F}"/>
-    <hyperlink ref="L268" r:id="rId320" display="https://raw.githack.com/ANZSoilData/def-au-scma/master/html/00frontmatter/00WARNING.html" xr:uid="{3C6C3E25-4480-4ADB-B0E0-5C03855D1CAB}"/>
-    <hyperlink ref="L272" r:id="rId321" display="https://raw.githack.com/ANZSoilData/def-au-scma/master/html/00frontmatter/00WARNING.html" xr:uid="{8E6D8811-B7C5-455F-A9EC-71F4128C3FA2}"/>
-    <hyperlink ref="L276" r:id="rId322" display="https://raw.githack.com/ANZSoilData/def-au-scma/master/html/00frontmatter/00WARNING.html" xr:uid="{A12DC7B9-C05B-473D-BA94-403F4B43CFD0}"/>
-    <hyperlink ref="L41" r:id="rId323" display="https://raw.githack.com/ANZSoilData/def-au-scma/master/html/00frontmatter/00WARNING.html" xr:uid="{4C34C87B-EC3C-4277-8F11-99DE8A31B481}"/>
-    <hyperlink ref="L45" r:id="rId324" display="https://raw.githack.com/ANZSoilData/def-au-scma/master/html/00frontmatter/00WARNING.html" xr:uid="{9958797F-909B-410D-9887-AF4CD4052C30}"/>
-    <hyperlink ref="L49" r:id="rId325" display="https://raw.githack.com/ANZSoilData/def-au-scma/master/html/00frontmatter/00WARNING.html" xr:uid="{63A5D804-F181-41C0-A871-76027504D1EF}"/>
-    <hyperlink ref="L53" r:id="rId326" display="https://raw.githack.com/ANZSoilData/def-au-scma/master/html/00frontmatter/00WARNING.html" xr:uid="{1225727E-6B96-4A9E-8DFF-11C981EF3574}"/>
-    <hyperlink ref="L57" r:id="rId327" display="https://raw.githack.com/ANZSoilData/def-au-scma/master/html/00frontmatter/00WARNING.html" xr:uid="{510C5D86-2491-4188-962C-FDCD986F9AC6}"/>
-    <hyperlink ref="L61" r:id="rId328" display="https://raw.githack.com/ANZSoilData/def-au-scma/master/html/00frontmatter/00WARNING.html" xr:uid="{EA88ECA0-6159-4BB3-8941-B58BD8250649}"/>
-    <hyperlink ref="L65" r:id="rId329" display="https://raw.githack.com/ANZSoilData/def-au-scma/master/html/00frontmatter/00WARNING.html" xr:uid="{1BA0B509-C242-47F3-B704-7DD490BB06EA}"/>
-    <hyperlink ref="L69" r:id="rId330" display="https://raw.githack.com/ANZSoilData/def-au-scma/master/html/00frontmatter/00WARNING.html" xr:uid="{13EC7BBE-E50F-4097-839F-0B5F08D73BA2}"/>
-    <hyperlink ref="L73" r:id="rId331" display="https://raw.githack.com/ANZSoilData/def-au-scma/master/html/00frontmatter/00WARNING.html" xr:uid="{92F410AC-9AD7-45D2-89B9-602368303A30}"/>
-    <hyperlink ref="L77" r:id="rId332" display="https://raw.githack.com/ANZSoilData/def-au-scma/master/html/00frontmatter/00WARNING.html" xr:uid="{6ED3F61A-09DB-4BFC-8F86-546CDAC83CEE}"/>
-    <hyperlink ref="L81" r:id="rId333" display="https://raw.githack.com/ANZSoilData/def-au-scma/master/html/00frontmatter/00WARNING.html" xr:uid="{05FB780F-1BB4-47BD-9B6A-45163C6B39C7}"/>
-    <hyperlink ref="L85" r:id="rId334" display="https://raw.githack.com/ANZSoilData/def-au-scma/master/html/00frontmatter/00WARNING.html" xr:uid="{4BE30220-2326-414C-9566-3C5F877C0920}"/>
-    <hyperlink ref="L89" r:id="rId335" display="https://raw.githack.com/ANZSoilData/def-au-scma/master/html/00frontmatter/00WARNING.html" xr:uid="{884E7D29-7BAC-4484-9623-2447EF51A30F}"/>
-    <hyperlink ref="L93" r:id="rId336" display="https://raw.githack.com/ANZSoilData/def-au-scma/master/html/00frontmatter/00WARNING.html" xr:uid="{624E867E-DE71-45EC-921D-C40393BF3F19}"/>
-    <hyperlink ref="L97" r:id="rId337" display="https://raw.githack.com/ANZSoilData/def-au-scma/master/html/00frontmatter/00WARNING.html" xr:uid="{DABCF2DA-EC71-45B8-AF8A-D3AB272C511F}"/>
-    <hyperlink ref="L101" r:id="rId338" display="https://raw.githack.com/ANZSoilData/def-au-scma/master/html/00frontmatter/00WARNING.html" xr:uid="{048BB512-5DAE-45BA-81B2-4D15200F1FFA}"/>
-    <hyperlink ref="L105" r:id="rId339" display="https://raw.githack.com/ANZSoilData/def-au-scma/master/html/00frontmatter/00WARNING.html" xr:uid="{5D137C2A-4433-453E-9AF4-0763C19C93C4}"/>
-    <hyperlink ref="L109" r:id="rId340" display="https://raw.githack.com/ANZSoilData/def-au-scma/master/html/00frontmatter/00WARNING.html" xr:uid="{85E1C986-6C51-472A-8E67-F57C36158757}"/>
-    <hyperlink ref="L113" r:id="rId341" display="https://raw.githack.com/ANZSoilData/def-au-scma/master/html/00frontmatter/00WARNING.html" xr:uid="{F05CCB13-3643-497E-9911-5CA7541FBF16}"/>
-    <hyperlink ref="L117" r:id="rId342" display="https://raw.githack.com/ANZSoilData/def-au-scma/master/html/00frontmatter/00WARNING.html" xr:uid="{EA40CA1F-B034-48FA-887B-DD4E6A3237CF}"/>
-    <hyperlink ref="L121" r:id="rId343" display="https://raw.githack.com/ANZSoilData/def-au-scma/master/html/00frontmatter/00WARNING.html" xr:uid="{6D563724-F769-4141-96DC-4EB7B0325E3A}"/>
-    <hyperlink ref="L125" r:id="rId344" display="https://raw.githack.com/ANZSoilData/def-au-scma/master/html/00frontmatter/00WARNING.html" xr:uid="{7D36677D-9CD8-4FC3-90DF-6A29CF366DCC}"/>
-    <hyperlink ref="L129" r:id="rId345" display="https://raw.githack.com/ANZSoilData/def-au-scma/master/html/00frontmatter/00WARNING.html" xr:uid="{E0E1B35F-5BDB-42A7-8E53-8AE52FF4A345}"/>
-    <hyperlink ref="L133" r:id="rId346" display="https://raw.githack.com/ANZSoilData/def-au-scma/master/html/00frontmatter/00WARNING.html" xr:uid="{DC1FBCE3-81FD-41EA-B586-5F53AC626D35}"/>
-    <hyperlink ref="L137" r:id="rId347" display="https://raw.githack.com/ANZSoilData/def-au-scma/master/html/00frontmatter/00WARNING.html" xr:uid="{8219FFBA-DEEE-431F-8187-F28987EA2AC9}"/>
-    <hyperlink ref="L141" r:id="rId348" display="https://raw.githack.com/ANZSoilData/def-au-scma/master/html/00frontmatter/00WARNING.html" xr:uid="{207F744E-2597-400F-B10C-B7E837C02B4D}"/>
-    <hyperlink ref="L145" r:id="rId349" display="https://raw.githack.com/ANZSoilData/def-au-scma/master/html/00frontmatter/00WARNING.html" xr:uid="{42C1865C-75FA-4D0D-8931-6F7BA8096127}"/>
-    <hyperlink ref="L149" r:id="rId350" display="https://raw.githack.com/ANZSoilData/def-au-scma/master/html/00frontmatter/00WARNING.html" xr:uid="{49A50E75-20AA-4128-BA23-A23115C11C43}"/>
-    <hyperlink ref="L153" r:id="rId351" display="https://raw.githack.com/ANZSoilData/def-au-scma/master/html/00frontmatter/00WARNING.html" xr:uid="{9C2839E9-BED5-4FF6-816F-77B57041A619}"/>
-    <hyperlink ref="L157" r:id="rId352" display="https://raw.githack.com/ANZSoilData/def-au-scma/master/html/00frontmatter/00WARNING.html" xr:uid="{E23A6699-90A5-4856-BF79-2380091F574E}"/>
-    <hyperlink ref="L161" r:id="rId353" display="https://raw.githack.com/ANZSoilData/def-au-scma/master/html/00frontmatter/00WARNING.html" xr:uid="{1A8492DF-94CC-46BC-94FC-8EC8D477843A}"/>
-    <hyperlink ref="L165" r:id="rId354" display="https://raw.githack.com/ANZSoilData/def-au-scma/master/html/00frontmatter/00WARNING.html" xr:uid="{7E9EAA15-2255-4AE8-AE67-0CA5DDA5A347}"/>
-    <hyperlink ref="L169" r:id="rId355" display="https://raw.githack.com/ANZSoilData/def-au-scma/master/html/00frontmatter/00WARNING.html" xr:uid="{7F580A4E-1F87-4BD7-A93B-17D22EC25FD5}"/>
-    <hyperlink ref="L173" r:id="rId356" display="https://raw.githack.com/ANZSoilData/def-au-scma/master/html/00frontmatter/00WARNING.html" xr:uid="{633DE086-4999-4966-A222-4A1181A3581B}"/>
-    <hyperlink ref="L177" r:id="rId357" display="https://raw.githack.com/ANZSoilData/def-au-scma/master/html/00frontmatter/00WARNING.html" xr:uid="{94047688-8533-4E04-94FF-AD5143093431}"/>
-    <hyperlink ref="L181" r:id="rId358" display="https://raw.githack.com/ANZSoilData/def-au-scma/master/html/00frontmatter/00WARNING.html" xr:uid="{41191E41-D130-4834-8125-0F76E602303B}"/>
-    <hyperlink ref="L185" r:id="rId359" display="https://raw.githack.com/ANZSoilData/def-au-scma/master/html/00frontmatter/00WARNING.html" xr:uid="{C4A07BDE-C8E3-40BA-BCCB-DB912E2A1D05}"/>
-    <hyperlink ref="L189" r:id="rId360" display="https://raw.githack.com/ANZSoilData/def-au-scma/master/html/00frontmatter/00WARNING.html" xr:uid="{ACB47CAB-46D8-47F6-A3DF-F8690426B059}"/>
-    <hyperlink ref="L193" r:id="rId361" display="https://raw.githack.com/ANZSoilData/def-au-scma/master/html/00frontmatter/00WARNING.html" xr:uid="{C9BBF2B3-E01C-4EE4-9553-7DFE776F7417}"/>
-    <hyperlink ref="L197" r:id="rId362" display="https://raw.githack.com/ANZSoilData/def-au-scma/master/html/00frontmatter/00WARNING.html" xr:uid="{A05F62DA-B658-4094-A328-4C524EC432B5}"/>
-    <hyperlink ref="L201" r:id="rId363" display="https://raw.githack.com/ANZSoilData/def-au-scma/master/html/00frontmatter/00WARNING.html" xr:uid="{0920E874-3FE7-44A0-8EE0-C1286C5EFC22}"/>
-    <hyperlink ref="L205" r:id="rId364" display="https://raw.githack.com/ANZSoilData/def-au-scma/master/html/00frontmatter/00WARNING.html" xr:uid="{27DFF406-EA84-4411-ADB3-39ABFBC87535}"/>
-    <hyperlink ref="L209" r:id="rId365" display="https://raw.githack.com/ANZSoilData/def-au-scma/master/html/00frontmatter/00WARNING.html" xr:uid="{DDA4DCE9-91E2-4EC0-A178-674FABC561A3}"/>
-    <hyperlink ref="L213" r:id="rId366" display="https://raw.githack.com/ANZSoilData/def-au-scma/master/html/00frontmatter/00WARNING.html" xr:uid="{66A75B59-91E0-4F9C-920C-3DE29142830A}"/>
-    <hyperlink ref="L217" r:id="rId367" display="https://raw.githack.com/ANZSoilData/def-au-scma/master/html/00frontmatter/00WARNING.html" xr:uid="{52D1A870-8B50-4756-919C-35BFD51F3F3F}"/>
-    <hyperlink ref="L221" r:id="rId368" display="https://raw.githack.com/ANZSoilData/def-au-scma/master/html/00frontmatter/00WARNING.html" xr:uid="{3048A8A9-D509-4345-BAC0-96AEB03E4DEA}"/>
-    <hyperlink ref="L225" r:id="rId369" display="https://raw.githack.com/ANZSoilData/def-au-scma/master/html/00frontmatter/00WARNING.html" xr:uid="{EBB126C0-C649-41AD-89E3-162B26844994}"/>
-    <hyperlink ref="L229" r:id="rId370" display="https://raw.githack.com/ANZSoilData/def-au-scma/master/html/00frontmatter/00WARNING.html" xr:uid="{34498225-638F-41B6-8A4E-2CD449DC92E3}"/>
-    <hyperlink ref="L233" r:id="rId371" display="https://raw.githack.com/ANZSoilData/def-au-scma/master/html/00frontmatter/00WARNING.html" xr:uid="{EC1831E6-01E3-4C6F-8864-CB175376670A}"/>
-    <hyperlink ref="L237" r:id="rId372" display="https://raw.githack.com/ANZSoilData/def-au-scma/master/html/00frontmatter/00WARNING.html" xr:uid="{F1779216-B8A7-4361-AF1B-567CE04261A6}"/>
-    <hyperlink ref="L241" r:id="rId373" display="https://raw.githack.com/ANZSoilData/def-au-scma/master/html/00frontmatter/00WARNING.html" xr:uid="{BB66DE9F-2A57-4A53-81A2-006DA68B66F9}"/>
-    <hyperlink ref="L245" r:id="rId374" display="https://raw.githack.com/ANZSoilData/def-au-scma/master/html/00frontmatter/00WARNING.html" xr:uid="{BF202C29-4AF7-41D1-B0AB-B613AA14FBF9}"/>
-    <hyperlink ref="L249" r:id="rId375" display="https://raw.githack.com/ANZSoilData/def-au-scma/master/html/00frontmatter/00WARNING.html" xr:uid="{1413E20E-6508-494F-9E8E-8C7A80E26C89}"/>
-    <hyperlink ref="L253" r:id="rId376" display="https://raw.githack.com/ANZSoilData/def-au-scma/master/html/00frontmatter/00WARNING.html" xr:uid="{693BD0DA-7B63-4EE0-856F-ADFFFFEFA1D6}"/>
-    <hyperlink ref="L257" r:id="rId377" display="https://raw.githack.com/ANZSoilData/def-au-scma/master/html/00frontmatter/00WARNING.html" xr:uid="{E0D95227-4D9D-462A-B990-0F650B304BA3}"/>
-    <hyperlink ref="L261" r:id="rId378" display="https://raw.githack.com/ANZSoilData/def-au-scma/master/html/00frontmatter/00WARNING.html" xr:uid="{F56970D0-CFD9-49B0-AD37-F168BBFA170D}"/>
-    <hyperlink ref="L265" r:id="rId379" display="https://raw.githack.com/ANZSoilData/def-au-scma/master/html/00frontmatter/00WARNING.html" xr:uid="{CD0EDD81-5ABB-4A32-BC15-CAEF04183D54}"/>
-    <hyperlink ref="L269" r:id="rId380" display="https://raw.githack.com/ANZSoilData/def-au-scma/master/html/00frontmatter/00WARNING.html" xr:uid="{24A0523D-5DED-4EAA-9F8F-3CC84B792A73}"/>
-    <hyperlink ref="L273" r:id="rId381" display="https://raw.githack.com/ANZSoilData/def-au-scma/master/html/00frontmatter/00WARNING.html" xr:uid="{397DDA1C-2976-4DA9-91C2-1824D9954851}"/>
-    <hyperlink ref="L277" r:id="rId382" display="https://raw.githack.com/ANZSoilData/def-au-scma/master/html/00frontmatter/00WARNING.html" xr:uid="{00677D20-EC96-4609-AFE2-9D7EE399F72C}"/>
-    <hyperlink ref="B14" r:id="rId383" xr:uid="{80495FFC-B63E-410A-B897-FA453FD8FCE3}"/>
-    <hyperlink ref="B21" r:id="rId384" xr:uid="{1AA2FF53-48CF-4684-8DFB-3406A97FB23C}"/>
-    <hyperlink ref="B11" r:id="rId385" xr:uid="{A2763553-1484-4DCB-942F-C7FEE682C30D}"/>
+    <hyperlink ref="E63" r:id="rId131" xr:uid="{0B886457-8AB9-4712-BE77-451FB95C6F9F}"/>
+    <hyperlink ref="E39" r:id="rId132" xr:uid="{9B1B8DB9-DF2A-4D3C-8C85-2322F1EA4B4E}"/>
+    <hyperlink ref="L34" r:id="rId133" display="https://raw.githack.com/ANZSoilData/def-au-scma/master/html/00frontmatter/00WARNING.html" xr:uid="{CB3E79BD-6394-47FD-AC9A-691D757C8EEC}"/>
+    <hyperlink ref="L35" r:id="rId134" display="https://raw.githack.com/ANZSoilData/def-au-scma/master/html/00frontmatter/00WARNING.html" xr:uid="{F5F615A3-C1F0-4FEC-916E-AFF4A5EACA64}"/>
+    <hyperlink ref="L36" r:id="rId135" display="https://raw.githack.com/ANZSoilData/def-au-scma/master/html/00frontmatter/00WARNING.html" xr:uid="{278EBF9A-2216-40FB-827E-74BA612AD8BE}"/>
+    <hyperlink ref="L37" r:id="rId136" display="https://raw.githack.com/ANZSoilData/def-au-scma/master/html/00frontmatter/00WARNING.html" xr:uid="{E42C7D67-C252-40CC-93E1-3374C60542A5}"/>
+    <hyperlink ref="L38" r:id="rId137" display="https://raw.githack.com/ANZSoilData/def-au-scma/master/html/00frontmatter/00WARNING.html" xr:uid="{A69D3E3B-ABE6-46AF-9CA2-426AF8E885C7}"/>
+    <hyperlink ref="L42" r:id="rId138" display="https://raw.githack.com/ANZSoilData/def-au-scma/master/html/00frontmatter/00WARNING.html" xr:uid="{C5881908-AD6B-449F-88F5-CC8F544AA5E3}"/>
+    <hyperlink ref="L46" r:id="rId139" display="https://raw.githack.com/ANZSoilData/def-au-scma/master/html/00frontmatter/00WARNING.html" xr:uid="{BB05B484-C5E4-46CF-89B7-98D1661D001D}"/>
+    <hyperlink ref="L50" r:id="rId140" display="https://raw.githack.com/ANZSoilData/def-au-scma/master/html/00frontmatter/00WARNING.html" xr:uid="{C2E65B7B-B331-4507-8D52-5A93FDE8DA79}"/>
+    <hyperlink ref="L54" r:id="rId141" display="https://raw.githack.com/ANZSoilData/def-au-scma/master/html/00frontmatter/00WARNING.html" xr:uid="{384AA51D-A5DC-4119-AF0A-4BD44BC68C19}"/>
+    <hyperlink ref="L58" r:id="rId142" display="https://raw.githack.com/ANZSoilData/def-au-scma/master/html/00frontmatter/00WARNING.html" xr:uid="{A6951591-8A3B-448F-9043-B02DB820C883}"/>
+    <hyperlink ref="L62" r:id="rId143" display="https://raw.githack.com/ANZSoilData/def-au-scma/master/html/00frontmatter/00WARNING.html" xr:uid="{A6B9C716-A31D-49FD-8E69-FEE42AACF1DF}"/>
+    <hyperlink ref="L66" r:id="rId144" display="https://raw.githack.com/ANZSoilData/def-au-scma/master/html/00frontmatter/00WARNING.html" xr:uid="{4B48E133-5738-4DF2-B5CD-0CA87CE52D70}"/>
+    <hyperlink ref="L70" r:id="rId145" display="https://raw.githack.com/ANZSoilData/def-au-scma/master/html/00frontmatter/00WARNING.html" xr:uid="{E9020B38-A1EA-48E4-8340-9B4FCDC63BB6}"/>
+    <hyperlink ref="L74" r:id="rId146" display="https://raw.githack.com/ANZSoilData/def-au-scma/master/html/00frontmatter/00WARNING.html" xr:uid="{B49851C0-0DB5-4DB6-8DFD-C051A230FD34}"/>
+    <hyperlink ref="L78" r:id="rId147" display="https://raw.githack.com/ANZSoilData/def-au-scma/master/html/00frontmatter/00WARNING.html" xr:uid="{271EE2F2-89F0-4999-B130-94B0C0A0B716}"/>
+    <hyperlink ref="L82" r:id="rId148" display="https://raw.githack.com/ANZSoilData/def-au-scma/master/html/00frontmatter/00WARNING.html" xr:uid="{5C525A2B-15E6-4F9A-9183-8DD9535B9618}"/>
+    <hyperlink ref="L86" r:id="rId149" display="https://raw.githack.com/ANZSoilData/def-au-scma/master/html/00frontmatter/00WARNING.html" xr:uid="{6C8F404E-6D7F-4948-9754-DD620C6B6146}"/>
+    <hyperlink ref="L90" r:id="rId150" display="https://raw.githack.com/ANZSoilData/def-au-scma/master/html/00frontmatter/00WARNING.html" xr:uid="{DB279ACA-6062-4BE4-BBCC-40FDEED21C25}"/>
+    <hyperlink ref="L94" r:id="rId151" display="https://raw.githack.com/ANZSoilData/def-au-scma/master/html/00frontmatter/00WARNING.html" xr:uid="{4E90C937-CA16-45AB-99F3-C2AEAC1CB7F8}"/>
+    <hyperlink ref="L98" r:id="rId152" display="https://raw.githack.com/ANZSoilData/def-au-scma/master/html/00frontmatter/00WARNING.html" xr:uid="{04BCE300-1F7C-47F7-9A88-4E6F5A1C60C9}"/>
+    <hyperlink ref="L102" r:id="rId153" display="https://raw.githack.com/ANZSoilData/def-au-scma/master/html/00frontmatter/00WARNING.html" xr:uid="{D0F07E63-373A-436D-AF9B-83E05CAE7CCC}"/>
+    <hyperlink ref="L106" r:id="rId154" display="https://raw.githack.com/ANZSoilData/def-au-scma/master/html/00frontmatter/00WARNING.html" xr:uid="{45D8A7B9-CF8B-425F-8D7D-9A64A370C498}"/>
+    <hyperlink ref="L110" r:id="rId155" display="https://raw.githack.com/ANZSoilData/def-au-scma/master/html/00frontmatter/00WARNING.html" xr:uid="{407BEDCD-8BAB-438A-9F87-53E7F72B8E83}"/>
+    <hyperlink ref="L114" r:id="rId156" display="https://raw.githack.com/ANZSoilData/def-au-scma/master/html/00frontmatter/00WARNING.html" xr:uid="{2B3411EC-5AD3-42DE-A4AA-B892EC4CFF4A}"/>
+    <hyperlink ref="L118" r:id="rId157" display="https://raw.githack.com/ANZSoilData/def-au-scma/master/html/00frontmatter/00WARNING.html" xr:uid="{A933C6C5-ECF5-4273-8C29-D01DC233BB51}"/>
+    <hyperlink ref="L122" r:id="rId158" display="https://raw.githack.com/ANZSoilData/def-au-scma/master/html/00frontmatter/00WARNING.html" xr:uid="{6BFDF12A-9865-48D2-B544-8F2C5034E456}"/>
+    <hyperlink ref="L126" r:id="rId159" display="https://raw.githack.com/ANZSoilData/def-au-scma/master/html/00frontmatter/00WARNING.html" xr:uid="{E0DAF296-E5A7-4CA1-B8E2-1E4DB801A2F3}"/>
+    <hyperlink ref="L130" r:id="rId160" display="https://raw.githack.com/ANZSoilData/def-au-scma/master/html/00frontmatter/00WARNING.html" xr:uid="{88F2EB19-37BA-464D-80A9-F40863778A56}"/>
+    <hyperlink ref="L134" r:id="rId161" display="https://raw.githack.com/ANZSoilData/def-au-scma/master/html/00frontmatter/00WARNING.html" xr:uid="{EE925EA2-0FB1-46EB-B24B-F824122A44E6}"/>
+    <hyperlink ref="L138" r:id="rId162" display="https://raw.githack.com/ANZSoilData/def-au-scma/master/html/00frontmatter/00WARNING.html" xr:uid="{15CD14B3-3B9B-4915-A5B0-3AEBF5B8865A}"/>
+    <hyperlink ref="L142" r:id="rId163" display="https://raw.githack.com/ANZSoilData/def-au-scma/master/html/00frontmatter/00WARNING.html" xr:uid="{000F8552-2647-4F96-8E73-FF190E4B3907}"/>
+    <hyperlink ref="L146" r:id="rId164" display="https://raw.githack.com/ANZSoilData/def-au-scma/master/html/00frontmatter/00WARNING.html" xr:uid="{3DA4F56B-50A1-4981-AD0D-C71A88912DBD}"/>
+    <hyperlink ref="L150" r:id="rId165" display="https://raw.githack.com/ANZSoilData/def-au-scma/master/html/00frontmatter/00WARNING.html" xr:uid="{7FDD363C-A3BB-4CAE-AE96-A7EA6697BE87}"/>
+    <hyperlink ref="L154" r:id="rId166" display="https://raw.githack.com/ANZSoilData/def-au-scma/master/html/00frontmatter/00WARNING.html" xr:uid="{D28C0CC4-2DE7-4AC5-931A-4E92B082AE7B}"/>
+    <hyperlink ref="L158" r:id="rId167" display="https://raw.githack.com/ANZSoilData/def-au-scma/master/html/00frontmatter/00WARNING.html" xr:uid="{2ECA1824-002D-44DA-8AF0-0D43308E8569}"/>
+    <hyperlink ref="L162" r:id="rId168" display="https://raw.githack.com/ANZSoilData/def-au-scma/master/html/00frontmatter/00WARNING.html" xr:uid="{4B19B385-78E8-4DC7-A9B1-941F2EA86EE2}"/>
+    <hyperlink ref="L166" r:id="rId169" display="https://raw.githack.com/ANZSoilData/def-au-scma/master/html/00frontmatter/00WARNING.html" xr:uid="{4CD045CF-019E-4D4F-8F46-7BA1A3F46A2E}"/>
+    <hyperlink ref="L170" r:id="rId170" display="https://raw.githack.com/ANZSoilData/def-au-scma/master/html/00frontmatter/00WARNING.html" xr:uid="{2545A8C8-5423-4375-89F7-EA905B36ADF8}"/>
+    <hyperlink ref="L174" r:id="rId171" display="https://raw.githack.com/ANZSoilData/def-au-scma/master/html/00frontmatter/00WARNING.html" xr:uid="{CB2E050F-4D4E-4FEA-BF7E-21F66502C924}"/>
+    <hyperlink ref="L178" r:id="rId172" display="https://raw.githack.com/ANZSoilData/def-au-scma/master/html/00frontmatter/00WARNING.html" xr:uid="{56F548EA-D6B6-42BA-BB2E-1F2B231D7C3E}"/>
+    <hyperlink ref="L182" r:id="rId173" display="https://raw.githack.com/ANZSoilData/def-au-scma/master/html/00frontmatter/00WARNING.html" xr:uid="{88877C74-6F97-43C4-815E-E177EBE2EF11}"/>
+    <hyperlink ref="L186" r:id="rId174" display="https://raw.githack.com/ANZSoilData/def-au-scma/master/html/00frontmatter/00WARNING.html" xr:uid="{70078424-DD2C-4847-BCB7-F454A3162FC2}"/>
+    <hyperlink ref="L190" r:id="rId175" display="https://raw.githack.com/ANZSoilData/def-au-scma/master/html/00frontmatter/00WARNING.html" xr:uid="{0E6517EB-4855-41DE-987F-143892E2B7C1}"/>
+    <hyperlink ref="L194" r:id="rId176" display="https://raw.githack.com/ANZSoilData/def-au-scma/master/html/00frontmatter/00WARNING.html" xr:uid="{782FDB4D-E6D2-45B9-878C-BE56E11D270A}"/>
+    <hyperlink ref="L198" r:id="rId177" display="https://raw.githack.com/ANZSoilData/def-au-scma/master/html/00frontmatter/00WARNING.html" xr:uid="{86AC3898-4C59-4216-BEF9-29B21713453F}"/>
+    <hyperlink ref="L202" r:id="rId178" display="https://raw.githack.com/ANZSoilData/def-au-scma/master/html/00frontmatter/00WARNING.html" xr:uid="{0BF76340-A769-4B5B-8E2B-0FD8405A7844}"/>
+    <hyperlink ref="L206" r:id="rId179" display="https://raw.githack.com/ANZSoilData/def-au-scma/master/html/00frontmatter/00WARNING.html" xr:uid="{EF1FD8A3-B6C1-4EA6-AE86-65BE742AC40B}"/>
+    <hyperlink ref="L210" r:id="rId180" display="https://raw.githack.com/ANZSoilData/def-au-scma/master/html/00frontmatter/00WARNING.html" xr:uid="{6859DA30-B43E-4C0A-AA9F-2FC8794AFF42}"/>
+    <hyperlink ref="L214" r:id="rId181" display="https://raw.githack.com/ANZSoilData/def-au-scma/master/html/00frontmatter/00WARNING.html" xr:uid="{BE4D8A2D-827D-41E5-8A9E-A5CE9D908B42}"/>
+    <hyperlink ref="L218" r:id="rId182" display="https://raw.githack.com/ANZSoilData/def-au-scma/master/html/00frontmatter/00WARNING.html" xr:uid="{E3CD281C-17A6-4937-9E6D-9D0E74DC683C}"/>
+    <hyperlink ref="L222" r:id="rId183" display="https://raw.githack.com/ANZSoilData/def-au-scma/master/html/00frontmatter/00WARNING.html" xr:uid="{B277ADAB-9569-4012-8E2B-1AE67BF47AE0}"/>
+    <hyperlink ref="L226" r:id="rId184" display="https://raw.githack.com/ANZSoilData/def-au-scma/master/html/00frontmatter/00WARNING.html" xr:uid="{68F9DE8D-DAB9-4472-B057-FC76DB29B45F}"/>
+    <hyperlink ref="L230" r:id="rId185" display="https://raw.githack.com/ANZSoilData/def-au-scma/master/html/00frontmatter/00WARNING.html" xr:uid="{826571F9-51BC-4DDE-A916-A170141BF315}"/>
+    <hyperlink ref="L234" r:id="rId186" display="https://raw.githack.com/ANZSoilData/def-au-scma/master/html/00frontmatter/00WARNING.html" xr:uid="{9C5B3FF8-B36A-4F89-8A77-F8A6E4937D4E}"/>
+    <hyperlink ref="L238" r:id="rId187" display="https://raw.githack.com/ANZSoilData/def-au-scma/master/html/00frontmatter/00WARNING.html" xr:uid="{1193A72D-1EF4-4467-9D1B-6815C2DE1470}"/>
+    <hyperlink ref="L242" r:id="rId188" display="https://raw.githack.com/ANZSoilData/def-au-scma/master/html/00frontmatter/00WARNING.html" xr:uid="{4E0FF932-A770-46BE-B1B1-C3FFBD0CD661}"/>
+    <hyperlink ref="L246" r:id="rId189" display="https://raw.githack.com/ANZSoilData/def-au-scma/master/html/00frontmatter/00WARNING.html" xr:uid="{EB815369-4D6A-4437-A061-E196F51903FA}"/>
+    <hyperlink ref="L250" r:id="rId190" display="https://raw.githack.com/ANZSoilData/def-au-scma/master/html/00frontmatter/00WARNING.html" xr:uid="{318C3648-7B72-4918-B38A-CF1EF4A88545}"/>
+    <hyperlink ref="L254" r:id="rId191" display="https://raw.githack.com/ANZSoilData/def-au-scma/master/html/00frontmatter/00WARNING.html" xr:uid="{0BBD7D6B-1DD3-43D6-8258-B44668713C6F}"/>
+    <hyperlink ref="L258" r:id="rId192" display="https://raw.githack.com/ANZSoilData/def-au-scma/master/html/00frontmatter/00WARNING.html" xr:uid="{93F3205E-2B9E-493C-8403-ECA1835F1C9E}"/>
+    <hyperlink ref="L262" r:id="rId193" display="https://raw.githack.com/ANZSoilData/def-au-scma/master/html/00frontmatter/00WARNING.html" xr:uid="{0508569E-0D73-4B55-B4E6-D07B44434D59}"/>
+    <hyperlink ref="L266" r:id="rId194" display="https://raw.githack.com/ANZSoilData/def-au-scma/master/html/00frontmatter/00WARNING.html" xr:uid="{AE685D0A-D4A5-4F2D-9769-CB5645F2AE8C}"/>
+    <hyperlink ref="L270" r:id="rId195" display="https://raw.githack.com/ANZSoilData/def-au-scma/master/html/00frontmatter/00WARNING.html" xr:uid="{0942CB22-9E70-4BB4-8887-BAF6127F6A93}"/>
+    <hyperlink ref="L274" r:id="rId196" display="https://raw.githack.com/ANZSoilData/def-au-scma/master/html/00frontmatter/00WARNING.html" xr:uid="{5BF9E46E-15C4-4066-B2E6-78BC95C81C6C}"/>
+    <hyperlink ref="L39" r:id="rId197" display="https://raw.githack.com/ANZSoilData/def-au-scma/master/html/00frontmatter/00WARNING.html" xr:uid="{30A42CBA-DD18-467F-9C31-F6FE20395F12}"/>
+    <hyperlink ref="L43" r:id="rId198" display="https://raw.githack.com/ANZSoilData/def-au-scma/master/html/00frontmatter/00WARNING.html" xr:uid="{5A22AFAB-6468-4305-AD73-0CF97A30E89A}"/>
+    <hyperlink ref="L47" r:id="rId199" display="https://raw.githack.com/ANZSoilData/def-au-scma/master/html/00frontmatter/00WARNING.html" xr:uid="{A894C31D-B0B3-40F6-BA59-DCF868A0C957}"/>
+    <hyperlink ref="L51" r:id="rId200" display="https://raw.githack.com/ANZSoilData/def-au-scma/master/html/00frontmatter/00WARNING.html" xr:uid="{D23DA804-39BD-4AEE-8663-7A6F4D17FEFA}"/>
+    <hyperlink ref="L55" r:id="rId201" display="https://raw.githack.com/ANZSoilData/def-au-scma/master/html/00frontmatter/00WARNING.html" xr:uid="{E56FB670-8B05-410B-862D-B206DFE828F1}"/>
+    <hyperlink ref="L59" r:id="rId202" display="https://raw.githack.com/ANZSoilData/def-au-scma/master/html/00frontmatter/00WARNING.html" xr:uid="{8D513C73-0385-4B20-91E6-5018B06FB850}"/>
+    <hyperlink ref="L63" r:id="rId203" display="https://raw.githack.com/ANZSoilData/def-au-scma/master/html/00frontmatter/00WARNING.html" xr:uid="{5BE35CB8-C72D-4045-BA1A-F17E3F258A20}"/>
+    <hyperlink ref="L67" r:id="rId204" display="https://raw.githack.com/ANZSoilData/def-au-scma/master/html/00frontmatter/00WARNING.html" xr:uid="{BB03F070-978E-47EB-BE13-510499AFD277}"/>
+    <hyperlink ref="L71" r:id="rId205" display="https://raw.githack.com/ANZSoilData/def-au-scma/master/html/00frontmatter/00WARNING.html" xr:uid="{73FC3383-83C8-43ED-A91E-628A288D9395}"/>
+    <hyperlink ref="L75" r:id="rId206" display="https://raw.githack.com/ANZSoilData/def-au-scma/master/html/00frontmatter/00WARNING.html" xr:uid="{78E3B867-8170-44BF-827E-6441CA1C2CD0}"/>
+    <hyperlink ref="L79" r:id="rId207" display="https://raw.githack.com/ANZSoilData/def-au-scma/master/html/00frontmatter/00WARNING.html" xr:uid="{CC968019-5D38-4E3D-B76A-490EF3E1AF7A}"/>
+    <hyperlink ref="L83" r:id="rId208" display="https://raw.githack.com/ANZSoilData/def-au-scma/master/html/00frontmatter/00WARNING.html" xr:uid="{709FD2AB-D563-4156-B0D3-CBDCE5FC876F}"/>
+    <hyperlink ref="L87" r:id="rId209" display="https://raw.githack.com/ANZSoilData/def-au-scma/master/html/00frontmatter/00WARNING.html" xr:uid="{8AFE6D1F-27CD-43CC-A3B7-BE202F7ABB64}"/>
+    <hyperlink ref="L91" r:id="rId210" display="https://raw.githack.com/ANZSoilData/def-au-scma/master/html/00frontmatter/00WARNING.html" xr:uid="{A1D6BFA7-BB0A-490A-87DE-3F2989AB6412}"/>
+    <hyperlink ref="L95" r:id="rId211" display="https://raw.githack.com/ANZSoilData/def-au-scma/master/html/00frontmatter/00WARNING.html" xr:uid="{96228920-6203-4418-A1D4-16DFFB530584}"/>
+    <hyperlink ref="L99" r:id="rId212" display="https://raw.githack.com/ANZSoilData/def-au-scma/master/html/00frontmatter/00WARNING.html" xr:uid="{FD3B19A9-F2F6-4A0E-9A24-22FFEE18B162}"/>
+    <hyperlink ref="L103" r:id="rId213" display="https://raw.githack.com/ANZSoilData/def-au-scma/master/html/00frontmatter/00WARNING.html" xr:uid="{A0F35CCF-773B-4A45-980D-174373464D93}"/>
+    <hyperlink ref="L107" r:id="rId214" display="https://raw.githack.com/ANZSoilData/def-au-scma/master/html/00frontmatter/00WARNING.html" xr:uid="{7266C1D8-99A6-4933-AD15-6083CA68C66B}"/>
+    <hyperlink ref="L111" r:id="rId215" display="https://raw.githack.com/ANZSoilData/def-au-scma/master/html/00frontmatter/00WARNING.html" xr:uid="{CB081986-B9B5-4D9A-A30B-41E65BAA2B03}"/>
+    <hyperlink ref="L115" r:id="rId216" display="https://raw.githack.com/ANZSoilData/def-au-scma/master/html/00frontmatter/00WARNING.html" xr:uid="{88E02967-8C20-4A8B-820D-1A9B1D2A239D}"/>
+    <hyperlink ref="L119" r:id="rId217" display="https://raw.githack.com/ANZSoilData/def-au-scma/master/html/00frontmatter/00WARNING.html" xr:uid="{5032FF67-F514-4AC7-9ED9-86936D11C989}"/>
+    <hyperlink ref="L123" r:id="rId218" display="https://raw.githack.com/ANZSoilData/def-au-scma/master/html/00frontmatter/00WARNING.html" xr:uid="{980ECBA1-CE6C-4F9A-BCCA-498D9933620B}"/>
+    <hyperlink ref="L127" r:id="rId219" display="https://raw.githack.com/ANZSoilData/def-au-scma/master/html/00frontmatter/00WARNING.html" xr:uid="{A3D0F967-DB8F-47F4-89BA-4CD45013467C}"/>
+    <hyperlink ref="L131" r:id="rId220" display="https://raw.githack.com/ANZSoilData/def-au-scma/master/html/00frontmatter/00WARNING.html" xr:uid="{F9EAD012-17B1-4863-8FFA-DA7FB15B4704}"/>
+    <hyperlink ref="L135" r:id="rId221" display="https://raw.githack.com/ANZSoilData/def-au-scma/master/html/00frontmatter/00WARNING.html" xr:uid="{CA95C6AF-B27A-42AF-8CB2-B0C8E4EF8232}"/>
+    <hyperlink ref="L139" r:id="rId222" display="https://raw.githack.com/ANZSoilData/def-au-scma/master/html/00frontmatter/00WARNING.html" xr:uid="{4968B8D1-1D97-4C9C-B97D-4334D24C3427}"/>
+    <hyperlink ref="L143" r:id="rId223" display="https://raw.githack.com/ANZSoilData/def-au-scma/master/html/00frontmatter/00WARNING.html" xr:uid="{555B537C-B9B7-4FAD-A13F-DC22ED3EA4FF}"/>
+    <hyperlink ref="L147" r:id="rId224" display="https://raw.githack.com/ANZSoilData/def-au-scma/master/html/00frontmatter/00WARNING.html" xr:uid="{097A3001-1F5F-448D-BE91-B846A20946BF}"/>
+    <hyperlink ref="L151" r:id="rId225" display="https://raw.githack.com/ANZSoilData/def-au-scma/master/html/00frontmatter/00WARNING.html" xr:uid="{6B1D3378-752F-4BAC-8DB4-831C610823E4}"/>
+    <hyperlink ref="L155" r:id="rId226" display="https://raw.githack.com/ANZSoilData/def-au-scma/master/html/00frontmatter/00WARNING.html" xr:uid="{0C853A69-79FF-4051-BB65-8096116EFE05}"/>
+    <hyperlink ref="L159" r:id="rId227" display="https://raw.githack.com/ANZSoilData/def-au-scma/master/html/00frontmatter/00WARNING.html" xr:uid="{BDB03E03-6E05-420B-B6F3-DD509A13AA69}"/>
+    <hyperlink ref="L163" r:id="rId228" display="https://raw.githack.com/ANZSoilData/def-au-scma/master/html/00frontmatter/00WARNING.html" xr:uid="{0E593F0C-E94A-4192-B365-6B1BF3D75FE3}"/>
+    <hyperlink ref="L167" r:id="rId229" display="https://raw.githack.com/ANZSoilData/def-au-scma/master/html/00frontmatter/00WARNING.html" xr:uid="{4C0A014B-F1BC-4D85-892C-5401BB07C8F9}"/>
+    <hyperlink ref="L171" r:id="rId230" display="https://raw.githack.com/ANZSoilData/def-au-scma/master/html/00frontmatter/00WARNING.html" xr:uid="{DACFF655-3EB2-49BA-97BC-7CA8DE3EBAEF}"/>
+    <hyperlink ref="L175" r:id="rId231" display="https://raw.githack.com/ANZSoilData/def-au-scma/master/html/00frontmatter/00WARNING.html" xr:uid="{12E6FF77-73A7-4FB8-A00D-F247483FC12C}"/>
+    <hyperlink ref="L179" r:id="rId232" display="https://raw.githack.com/ANZSoilData/def-au-scma/master/html/00frontmatter/00WARNING.html" xr:uid="{AE645C7B-63D5-4015-A28D-908F7BF75F66}"/>
+    <hyperlink ref="L183" r:id="rId233" display="https://raw.githack.com/ANZSoilData/def-au-scma/master/html/00frontmatter/00WARNING.html" xr:uid="{81FFA0EB-02DD-4EA5-8C05-08CACC157220}"/>
+    <hyperlink ref="L187" r:id="rId234" display="https://raw.githack.com/ANZSoilData/def-au-scma/master/html/00frontmatter/00WARNING.html" xr:uid="{8464762C-F21A-4CDB-8431-52DBE700EF69}"/>
+    <hyperlink ref="L191" r:id="rId235" display="https://raw.githack.com/ANZSoilData/def-au-scma/master/html/00frontmatter/00WARNING.html" xr:uid="{1E6DB17F-AEB3-4A28-958C-C86D718E6D69}"/>
+    <hyperlink ref="L195" r:id="rId236" display="https://raw.githack.com/ANZSoilData/def-au-scma/master/html/00frontmatter/00WARNING.html" xr:uid="{AB2B88FF-BA42-4A3E-8988-89AB43174E5E}"/>
+    <hyperlink ref="L199" r:id="rId237" display="https://raw.githack.com/ANZSoilData/def-au-scma/master/html/00frontmatter/00WARNING.html" xr:uid="{98C388BB-DC1C-4589-9234-F0D03FAB986F}"/>
+    <hyperlink ref="L203" r:id="rId238" display="https://raw.githack.com/ANZSoilData/def-au-scma/master/html/00frontmatter/00WARNING.html" xr:uid="{F2A8149E-C4D1-4E10-8ED8-C1CA95C38F4E}"/>
+    <hyperlink ref="L207" r:id="rId239" display="https://raw.githack.com/ANZSoilData/def-au-scma/master/html/00frontmatter/00WARNING.html" xr:uid="{B27CE42B-FB56-445C-AA4C-CAE253C53384}"/>
+    <hyperlink ref="L211" r:id="rId240" display="https://raw.githack.com/ANZSoilData/def-au-scma/master/html/00frontmatter/00WARNING.html" xr:uid="{2F72E7F4-A004-4AA4-A0BC-373CA95B0FC8}"/>
+    <hyperlink ref="L215" r:id="rId241" display="https://raw.githack.com/ANZSoilData/def-au-scma/master/html/00frontmatter/00WARNING.html" xr:uid="{71D97D79-1841-43F8-8E00-29BB9E4F634D}"/>
+    <hyperlink ref="L219" r:id="rId242" display="https://raw.githack.com/ANZSoilData/def-au-scma/master/html/00frontmatter/00WARNING.html" xr:uid="{C57BE990-59AC-412B-B718-CBD3A5F98AFF}"/>
+    <hyperlink ref="L223" r:id="rId243" display="https://raw.githack.com/ANZSoilData/def-au-scma/master/html/00frontmatter/00WARNING.html" xr:uid="{252723D2-D506-43E4-AA8E-D1AC81C94F2D}"/>
+    <hyperlink ref="L227" r:id="rId244" display="https://raw.githack.com/ANZSoilData/def-au-scma/master/html/00frontmatter/00WARNING.html" xr:uid="{480F6310-1D87-4C3A-860F-86B3FACDD196}"/>
+    <hyperlink ref="L231" r:id="rId245" display="https://raw.githack.com/ANZSoilData/def-au-scma/master/html/00frontmatter/00WARNING.html" xr:uid="{F3793526-865F-4475-9797-A39D3B78171B}"/>
+    <hyperlink ref="L235" r:id="rId246" display="https://raw.githack.com/ANZSoilData/def-au-scma/master/html/00frontmatter/00WARNING.html" xr:uid="{D751496D-50FA-40D6-8093-ADC3D3FF8073}"/>
+    <hyperlink ref="L239" r:id="rId247" display="https://raw.githack.com/ANZSoilData/def-au-scma/master/html/00frontmatter/00WARNING.html" xr:uid="{8AF0ECE2-B8BE-45DA-B1C0-6F647DDD5E3F}"/>
+    <hyperlink ref="L243" r:id="rId248" display="https://raw.githack.com/ANZSoilData/def-au-scma/master/html/00frontmatter/00WARNING.html" xr:uid="{1CC92C21-EC70-434D-8DB7-16DAE06AB483}"/>
+    <hyperlink ref="L247" r:id="rId249" display="https://raw.githack.com/ANZSoilData/def-au-scma/master/html/00frontmatter/00WARNING.html" xr:uid="{A820BB9D-32C7-431C-89F9-BA0A82C0EC5C}"/>
+    <hyperlink ref="L251" r:id="rId250" display="https://raw.githack.com/ANZSoilData/def-au-scma/master/html/00frontmatter/00WARNING.html" xr:uid="{BA3B7869-E9DF-4EAE-9C15-E9EE4533BE99}"/>
+    <hyperlink ref="L255" r:id="rId251" display="https://raw.githack.com/ANZSoilData/def-au-scma/master/html/00frontmatter/00WARNING.html" xr:uid="{236D1A28-656A-468B-9DE9-23E1519F7951}"/>
+    <hyperlink ref="L259" r:id="rId252" display="https://raw.githack.com/ANZSoilData/def-au-scma/master/html/00frontmatter/00WARNING.html" xr:uid="{8EFC5F39-0491-4EB3-9EE0-8D3FD74253A7}"/>
+    <hyperlink ref="L263" r:id="rId253" display="https://raw.githack.com/ANZSoilData/def-au-scma/master/html/00frontmatter/00WARNING.html" xr:uid="{FA3A2069-D9DF-45C6-BDAB-8DF6F1F69E05}"/>
+    <hyperlink ref="L267" r:id="rId254" display="https://raw.githack.com/ANZSoilData/def-au-scma/master/html/00frontmatter/00WARNING.html" xr:uid="{42C16B11-14D3-45E3-87FB-C661497704DA}"/>
+    <hyperlink ref="L271" r:id="rId255" display="https://raw.githack.com/ANZSoilData/def-au-scma/master/html/00frontmatter/00WARNING.html" xr:uid="{B753BF0E-6479-432B-8FD6-14CD1A990CC9}"/>
+    <hyperlink ref="L275" r:id="rId256" display="https://raw.githack.com/ANZSoilData/def-au-scma/master/html/00frontmatter/00WARNING.html" xr:uid="{1B11A110-44A6-4C92-94FC-BF0648BADC68}"/>
+    <hyperlink ref="L40" r:id="rId257" display="https://raw.githack.com/ANZSoilData/def-au-scma/master/html/00frontmatter/00WARNING.html" xr:uid="{5CCA99B3-866E-43B6-A611-4011A70232F3}"/>
+    <hyperlink ref="L44" r:id="rId258" display="https://raw.githack.com/ANZSoilData/def-au-scma/master/html/00frontmatter/00WARNING.html" xr:uid="{60163CA2-837F-43E2-A306-DBAD49073A6A}"/>
+    <hyperlink ref="L48" r:id="rId259" display="https://raw.githack.com/ANZSoilData/def-au-scma/master/html/00frontmatter/00WARNING.html" xr:uid="{7C035D9F-54E0-43B8-BE0D-31005E151DFD}"/>
+    <hyperlink ref="L52" r:id="rId260" display="https://raw.githack.com/ANZSoilData/def-au-scma/master/html/00frontmatter/00WARNING.html" xr:uid="{E5BF080A-7169-457C-9FD9-974AA2A3EA96}"/>
+    <hyperlink ref="L56" r:id="rId261" display="https://raw.githack.com/ANZSoilData/def-au-scma/master/html/00frontmatter/00WARNING.html" xr:uid="{C419F04A-C54F-491B-9CAA-EA6CCE9645F3}"/>
+    <hyperlink ref="L60" r:id="rId262" display="https://raw.githack.com/ANZSoilData/def-au-scma/master/html/00frontmatter/00WARNING.html" xr:uid="{676681FE-C4E1-4AE3-9381-18BF4E9A8C07}"/>
+    <hyperlink ref="L64" r:id="rId263" display="https://raw.githack.com/ANZSoilData/def-au-scma/master/html/00frontmatter/00WARNING.html" xr:uid="{BA256E0C-40BE-4E65-A385-BF6790B75104}"/>
+    <hyperlink ref="L68" r:id="rId264" display="https://raw.githack.com/ANZSoilData/def-au-scma/master/html/00frontmatter/00WARNING.html" xr:uid="{5CE921C2-4E7E-4BC3-AC98-8751264618A2}"/>
+    <hyperlink ref="L72" r:id="rId265" display="https://raw.githack.com/ANZSoilData/def-au-scma/master/html/00frontmatter/00WARNING.html" xr:uid="{68C94CE0-F780-4EFF-A1A8-29A6CD247330}"/>
+    <hyperlink ref="L76" r:id="rId266" display="https://raw.githack.com/ANZSoilData/def-au-scma/master/html/00frontmatter/00WARNING.html" xr:uid="{FC129378-D596-4BC1-85FF-225DA48BE830}"/>
+    <hyperlink ref="L80" r:id="rId267" display="https://raw.githack.com/ANZSoilData/def-au-scma/master/html/00frontmatter/00WARNING.html" xr:uid="{6F208267-F557-49BB-9BF3-DD87EDDC8358}"/>
+    <hyperlink ref="L84" r:id="rId268" display="https://raw.githack.com/ANZSoilData/def-au-scma/master/html/00frontmatter/00WARNING.html" xr:uid="{29FA809A-27F9-4E8B-8D23-5CA7F7981C7E}"/>
+    <hyperlink ref="L88" r:id="rId269" display="https://raw.githack.com/ANZSoilData/def-au-scma/master/html/00frontmatter/00WARNING.html" xr:uid="{5C269D3B-1522-4A46-BC70-FD2C7846FE01}"/>
+    <hyperlink ref="L92" r:id="rId270" display="https://raw.githack.com/ANZSoilData/def-au-scma/master/html/00frontmatter/00WARNING.html" xr:uid="{DDBF9AC4-0578-4EA5-91E5-EF400563AFB8}"/>
+    <hyperlink ref="L96" r:id="rId271" display="https://raw.githack.com/ANZSoilData/def-au-scma/master/html/00frontmatter/00WARNING.html" xr:uid="{BBBAB2BB-66BC-4907-8FF4-F8F983CA027E}"/>
+    <hyperlink ref="L100" r:id="rId272" display="https://raw.githack.com/ANZSoilData/def-au-scma/master/html/00frontmatter/00WARNING.html" xr:uid="{294A4606-458C-441F-8E41-924881F3B04A}"/>
+    <hyperlink ref="L104" r:id="rId273" display="https://raw.githack.com/ANZSoilData/def-au-scma/master/html/00frontmatter/00WARNING.html" xr:uid="{4C91B85F-765B-497E-A795-D052E85F5F55}"/>
+    <hyperlink ref="L108" r:id="rId274" display="https://raw.githack.com/ANZSoilData/def-au-scma/master/html/00frontmatter/00WARNING.html" xr:uid="{FF989142-2B51-4C57-9039-6B44F89F2286}"/>
+    <hyperlink ref="L112" r:id="rId275" display="https://raw.githack.com/ANZSoilData/def-au-scma/master/html/00frontmatter/00WARNING.html" xr:uid="{21ACE121-FF7A-4B33-867E-91F244C80EB4}"/>
+    <hyperlink ref="L116" r:id="rId276" display="https://raw.githack.com/ANZSoilData/def-au-scma/master/html/00frontmatter/00WARNING.html" xr:uid="{1D0130E9-573E-44D8-AD88-388FECD85C16}"/>
+    <hyperlink ref="L120" r:id="rId277" display="https://raw.githack.com/ANZSoilData/def-au-scma/master/html/00frontmatter/00WARNING.html" xr:uid="{774829A9-46DF-4BDE-99C6-1275D3F2E271}"/>
+    <hyperlink ref="L124" r:id="rId278" display="https://raw.githack.com/ANZSoilData/def-au-scma/master/html/00frontmatter/00WARNING.html" xr:uid="{AA566C8D-29BC-4A2C-B261-447942C09FE9}"/>
+    <hyperlink ref="L128" r:id="rId279" display="https://raw.githack.com/ANZSoilData/def-au-scma/master/html/00frontmatter/00WARNING.html" xr:uid="{13B9C285-B467-4AF1-AC33-2F017DA31B03}"/>
+    <hyperlink ref="L132" r:id="rId280" display="https://raw.githack.com/ANZSoilData/def-au-scma/master/html/00frontmatter/00WARNING.html" xr:uid="{70B06375-FA01-4E6D-BD77-6719E0D8DD2A}"/>
+    <hyperlink ref="L136" r:id="rId281" display="https://raw.githack.com/ANZSoilData/def-au-scma/master/html/00frontmatter/00WARNING.html" xr:uid="{A24C20C8-DFF5-4CBF-9ADB-CAC93071C843}"/>
+    <hyperlink ref="L140" r:id="rId282" display="https://raw.githack.com/ANZSoilData/def-au-scma/master/html/00frontmatter/00WARNING.html" xr:uid="{6A175C0E-3DC9-46EA-BBCF-11C27BF0CAB8}"/>
+    <hyperlink ref="L144" r:id="rId283" display="https://raw.githack.com/ANZSoilData/def-au-scma/master/html/00frontmatter/00WARNING.html" xr:uid="{4088B65F-6821-4CC3-95A7-3743BFBA99F7}"/>
+    <hyperlink ref="L148" r:id="rId284" display="https://raw.githack.com/ANZSoilData/def-au-scma/master/html/00frontmatter/00WARNING.html" xr:uid="{7FF78193-6C29-41F2-BC58-2619AA6F81DB}"/>
+    <hyperlink ref="L152" r:id="rId285" display="https://raw.githack.com/ANZSoilData/def-au-scma/master/html/00frontmatter/00WARNING.html" xr:uid="{6A7D753C-BD96-40F8-B028-22A4193AE97D}"/>
+    <hyperlink ref="L156" r:id="rId286" display="https://raw.githack.com/ANZSoilData/def-au-scma/master/html/00frontmatter/00WARNING.html" xr:uid="{DCA6DC69-4135-4519-B98A-FA4E4C9FD6C5}"/>
+    <hyperlink ref="L160" r:id="rId287" display="https://raw.githack.com/ANZSoilData/def-au-scma/master/html/00frontmatter/00WARNING.html" xr:uid="{B343BE67-86D0-4FB5-8434-555231AED175}"/>
+    <hyperlink ref="L164" r:id="rId288" display="https://raw.githack.com/ANZSoilData/def-au-scma/master/html/00frontmatter/00WARNING.html" xr:uid="{31DC2E97-749B-4FB0-AC9C-3AA71EE76372}"/>
+    <hyperlink ref="L168" r:id="rId289" display="https://raw.githack.com/ANZSoilData/def-au-scma/master/html/00frontmatter/00WARNING.html" xr:uid="{4EAAACC7-D31C-4207-83A9-0642D09F4D8D}"/>
+    <hyperlink ref="L172" r:id="rId290" display="https://raw.githack.com/ANZSoilData/def-au-scma/master/html/00frontmatter/00WARNING.html" xr:uid="{13AF4C94-9498-407A-AFB8-BE3F38237FD2}"/>
+    <hyperlink ref="L176" r:id="rId291" display="https://raw.githack.com/ANZSoilData/def-au-scma/master/html/00frontmatter/00WARNING.html" xr:uid="{8F7D3974-22FD-4906-9F5C-5D9EA98DAF04}"/>
+    <hyperlink ref="L180" r:id="rId292" display="https://raw.githack.com/ANZSoilData/def-au-scma/master/html/00frontmatter/00WARNING.html" xr:uid="{8EE35985-963D-4B76-91DA-5142551084B8}"/>
+    <hyperlink ref="L184" r:id="rId293" display="https://raw.githack.com/ANZSoilData/def-au-scma/master/html/00frontmatter/00WARNING.html" xr:uid="{6A81AD3A-73D5-4B78-8C3C-F7473E5C0A9C}"/>
+    <hyperlink ref="L188" r:id="rId294" display="https://raw.githack.com/ANZSoilData/def-au-scma/master/html/00frontmatter/00WARNING.html" xr:uid="{DC984535-9A7B-4AB4-8DA7-CA5DB8609120}"/>
+    <hyperlink ref="L192" r:id="rId295" display="https://raw.githack.com/ANZSoilData/def-au-scma/master/html/00frontmatter/00WARNING.html" xr:uid="{29B6C9A9-646B-430C-8123-3BCE48A33F81}"/>
+    <hyperlink ref="L196" r:id="rId296" display="https://raw.githack.com/ANZSoilData/def-au-scma/master/html/00frontmatter/00WARNING.html" xr:uid="{10D16AE2-36F6-4868-9DB7-C03857B691DB}"/>
+    <hyperlink ref="L200" r:id="rId297" display="https://raw.githack.com/ANZSoilData/def-au-scma/master/html/00frontmatter/00WARNING.html" xr:uid="{E9C6F802-D408-4710-90E8-3CFA4233A1CE}"/>
+    <hyperlink ref="L204" r:id="rId298" display="https://raw.githack.com/ANZSoilData/def-au-scma/master/html/00frontmatter/00WARNING.html" xr:uid="{B4403BD4-6BD6-44F0-9746-17390040B9DB}"/>
+    <hyperlink ref="L208" r:id="rId299" display="https://raw.githack.com/ANZSoilData/def-au-scma/master/html/00frontmatter/00WARNING.html" xr:uid="{050B8865-C8DE-4160-880A-B5D6524E9CB0}"/>
+    <hyperlink ref="L212" r:id="rId300" display="https://raw.githack.com/ANZSoilData/def-au-scma/master/html/00frontmatter/00WARNING.html" xr:uid="{66C262F9-2897-41D2-A86A-D0D64AD22593}"/>
+    <hyperlink ref="L216" r:id="rId301" display="https://raw.githack.com/ANZSoilData/def-au-scma/master/html/00frontmatter/00WARNING.html" xr:uid="{F1B703C3-2898-4AC9-9795-DE7067FC446A}"/>
+    <hyperlink ref="L220" r:id="rId302" display="https://raw.githack.com/ANZSoilData/def-au-scma/master/html/00frontmatter/00WARNING.html" xr:uid="{34AEBBDD-1251-4A9A-AC33-8E55F0780F6A}"/>
+    <hyperlink ref="L224" r:id="rId303" display="https://raw.githack.com/ANZSoilData/def-au-scma/master/html/00frontmatter/00WARNING.html" xr:uid="{CF4F3331-D149-497C-9342-B6502D8EE3A0}"/>
+    <hyperlink ref="L228" r:id="rId304" display="https://raw.githack.com/ANZSoilData/def-au-scma/master/html/00frontmatter/00WARNING.html" xr:uid="{55B893E1-1CDE-4E5C-8319-16A24C45FDB5}"/>
+    <hyperlink ref="L232" r:id="rId305" display="https://raw.githack.com/ANZSoilData/def-au-scma/master/html/00frontmatter/00WARNING.html" xr:uid="{D698468E-B9B5-4A59-AA9C-59D1906B42FC}"/>
+    <hyperlink ref="L236" r:id="rId306" display="https://raw.githack.com/ANZSoilData/def-au-scma/master/html/00frontmatter/00WARNING.html" xr:uid="{6B9A4D10-FD80-4A84-9EE4-4199786D92A6}"/>
+    <hyperlink ref="L240" r:id="rId307" display="https://raw.githack.com/ANZSoilData/def-au-scma/master/html/00frontmatter/00WARNING.html" xr:uid="{16005748-8FFE-42D3-AEDC-33B24C0F45CB}"/>
+    <hyperlink ref="L244" r:id="rId308" display="https://raw.githack.com/ANZSoilData/def-au-scma/master/html/00frontmatter/00WARNING.html" xr:uid="{D8F7454F-9017-418C-B0DE-1D1979473AEF}"/>
+    <hyperlink ref="L248" r:id="rId309" display="https://raw.githack.com/ANZSoilData/def-au-scma/master/html/00frontmatter/00WARNING.html" xr:uid="{F248501B-D943-4136-B872-7C7BAE5EAC28}"/>
+    <hyperlink ref="L252" r:id="rId310" display="https://raw.githack.com/ANZSoilData/def-au-scma/master/html/00frontmatter/00WARNING.html" xr:uid="{890D5642-432C-4F1B-BDEE-2BDEC871BF0B}"/>
+    <hyperlink ref="L256" r:id="rId311" display="https://raw.githack.com/ANZSoilData/def-au-scma/master/html/00frontmatter/00WARNING.html" xr:uid="{D4C728F3-C78C-4F15-8157-2EDE92E30400}"/>
+    <hyperlink ref="L260" r:id="rId312" display="https://raw.githack.com/ANZSoilData/def-au-scma/master/html/00frontmatter/00WARNING.html" xr:uid="{EC6EE0FB-897B-47E1-9E59-EAF768DB0B3F}"/>
+    <hyperlink ref="L264" r:id="rId313" display="https://raw.githack.com/ANZSoilData/def-au-scma/master/html/00frontmatter/00WARNING.html" xr:uid="{8F7614C2-098F-47E8-83F6-DC495F23DE1F}"/>
+    <hyperlink ref="L268" r:id="rId314" display="https://raw.githack.com/ANZSoilData/def-au-scma/master/html/00frontmatter/00WARNING.html" xr:uid="{3C6C3E25-4480-4ADB-B0E0-5C03855D1CAB}"/>
+    <hyperlink ref="L272" r:id="rId315" display="https://raw.githack.com/ANZSoilData/def-au-scma/master/html/00frontmatter/00WARNING.html" xr:uid="{8E6D8811-B7C5-455F-A9EC-71F4128C3FA2}"/>
+    <hyperlink ref="L276" r:id="rId316" display="https://raw.githack.com/ANZSoilData/def-au-scma/master/html/00frontmatter/00WARNING.html" xr:uid="{A12DC7B9-C05B-473D-BA94-403F4B43CFD0}"/>
+    <hyperlink ref="L41" r:id="rId317" display="https://raw.githack.com/ANZSoilData/def-au-scma/master/html/00frontmatter/00WARNING.html" xr:uid="{4C34C87B-EC3C-4277-8F11-99DE8A31B481}"/>
+    <hyperlink ref="L45" r:id="rId318" display="https://raw.githack.com/ANZSoilData/def-au-scma/master/html/00frontmatter/00WARNING.html" xr:uid="{9958797F-909B-410D-9887-AF4CD4052C30}"/>
+    <hyperlink ref="L49" r:id="rId319" display="https://raw.githack.com/ANZSoilData/def-au-scma/master/html/00frontmatter/00WARNING.html" xr:uid="{63A5D804-F181-41C0-A871-76027504D1EF}"/>
+    <hyperlink ref="L53" r:id="rId320" display="https://raw.githack.com/ANZSoilData/def-au-scma/master/html/00frontmatter/00WARNING.html" xr:uid="{1225727E-6B96-4A9E-8DFF-11C981EF3574}"/>
+    <hyperlink ref="L57" r:id="rId321" display="https://raw.githack.com/ANZSoilData/def-au-scma/master/html/00frontmatter/00WARNING.html" xr:uid="{510C5D86-2491-4188-962C-FDCD986F9AC6}"/>
+    <hyperlink ref="L61" r:id="rId322" display="https://raw.githack.com/ANZSoilData/def-au-scma/master/html/00frontmatter/00WARNING.html" xr:uid="{EA88ECA0-6159-4BB3-8941-B58BD8250649}"/>
+    <hyperlink ref="L65" r:id="rId323" display="https://raw.githack.com/ANZSoilData/def-au-scma/master/html/00frontmatter/00WARNING.html" xr:uid="{1BA0B509-C242-47F3-B704-7DD490BB06EA}"/>
+    <hyperlink ref="L69" r:id="rId324" display="https://raw.githack.com/ANZSoilData/def-au-scma/master/html/00frontmatter/00WARNING.html" xr:uid="{13EC7BBE-E50F-4097-839F-0B5F08D73BA2}"/>
+    <hyperlink ref="L73" r:id="rId325" display="https://raw.githack.com/ANZSoilData/def-au-scma/master/html/00frontmatter/00WARNING.html" xr:uid="{92F410AC-9AD7-45D2-89B9-602368303A30}"/>
+    <hyperlink ref="L77" r:id="rId326" display="https://raw.githack.com/ANZSoilData/def-au-scma/master/html/00frontmatter/00WARNING.html" xr:uid="{6ED3F61A-09DB-4BFC-8F86-546CDAC83CEE}"/>
+    <hyperlink ref="L81" r:id="rId327" display="https://raw.githack.com/ANZSoilData/def-au-scma/master/html/00frontmatter/00WARNING.html" xr:uid="{05FB780F-1BB4-47BD-9B6A-45163C6B39C7}"/>
+    <hyperlink ref="L85" r:id="rId328" display="https://raw.githack.com/ANZSoilData/def-au-scma/master/html/00frontmatter/00WARNING.html" xr:uid="{4BE30220-2326-414C-9566-3C5F877C0920}"/>
+    <hyperlink ref="L89" r:id="rId329" display="https://raw.githack.com/ANZSoilData/def-au-scma/master/html/00frontmatter/00WARNING.html" xr:uid="{884E7D29-7BAC-4484-9623-2447EF51A30F}"/>
+    <hyperlink ref="L93" r:id="rId330" display="https://raw.githack.com/ANZSoilData/def-au-scma/master/html/00frontmatter/00WARNING.html" xr:uid="{624E867E-DE71-45EC-921D-C40393BF3F19}"/>
+    <hyperlink ref="L97" r:id="rId331" display="https://raw.githack.com/ANZSoilData/def-au-scma/master/html/00frontmatter/00WARNING.html" xr:uid="{DABCF2DA-EC71-45B8-AF8A-D3AB272C511F}"/>
+    <hyperlink ref="L101" r:id="rId332" display="https://raw.githack.com/ANZSoilData/def-au-scma/master/html/00frontmatter/00WARNING.html" xr:uid="{048BB512-5DAE-45BA-81B2-4D15200F1FFA}"/>
+    <hyperlink ref="L105" r:id="rId333" display="https://raw.githack.com/ANZSoilData/def-au-scma/master/html/00frontmatter/00WARNING.html" xr:uid="{5D137C2A-4433-453E-9AF4-0763C19C93C4}"/>
+    <hyperlink ref="L109" r:id="rId334" display="https://raw.githack.com/ANZSoilData/def-au-scma/master/html/00frontmatter/00WARNING.html" xr:uid="{85E1C986-6C51-472A-8E67-F57C36158757}"/>
+    <hyperlink ref="L113" r:id="rId335" display="https://raw.githack.com/ANZSoilData/def-au-scma/master/html/00frontmatter/00WARNING.html" xr:uid="{F05CCB13-3643-497E-9911-5CA7541FBF16}"/>
+    <hyperlink ref="L117" r:id="rId336" display="https://raw.githack.com/ANZSoilData/def-au-scma/master/html/00frontmatter/00WARNING.html" xr:uid="{EA40CA1F-B034-48FA-887B-DD4E6A3237CF}"/>
+    <hyperlink ref="L121" r:id="rId337" display="https://raw.githack.com/ANZSoilData/def-au-scma/master/html/00frontmatter/00WARNING.html" xr:uid="{6D563724-F769-4141-96DC-4EB7B0325E3A}"/>
+    <hyperlink ref="L125" r:id="rId338" display="https://raw.githack.com/ANZSoilData/def-au-scma/master/html/00frontmatter/00WARNING.html" xr:uid="{7D36677D-9CD8-4FC3-90DF-6A29CF366DCC}"/>
+    <hyperlink ref="L129" r:id="rId339" display="https://raw.githack.com/ANZSoilData/def-au-scma/master/html/00frontmatter/00WARNING.html" xr:uid="{E0E1B35F-5BDB-42A7-8E53-8AE52FF4A345}"/>
+    <hyperlink ref="L133" r:id="rId340" display="https://raw.githack.com/ANZSoilData/def-au-scma/master/html/00frontmatter/00WARNING.html" xr:uid="{DC1FBCE3-81FD-41EA-B586-5F53AC626D35}"/>
+    <hyperlink ref="L137" r:id="rId341" display="https://raw.githack.com/ANZSoilData/def-au-scma/master/html/00frontmatter/00WARNING.html" xr:uid="{8219FFBA-DEEE-431F-8187-F28987EA2AC9}"/>
+    <hyperlink ref="L141" r:id="rId342" display="https://raw.githack.com/ANZSoilData/def-au-scma/master/html/00frontmatter/00WARNING.html" xr:uid="{207F744E-2597-400F-B10C-B7E837C02B4D}"/>
+    <hyperlink ref="L145" r:id="rId343" display="https://raw.githack.com/ANZSoilData/def-au-scma/master/html/00frontmatter/00WARNING.html" xr:uid="{42C1865C-75FA-4D0D-8931-6F7BA8096127}"/>
+    <hyperlink ref="L149" r:id="rId344" display="https://raw.githack.com/ANZSoilData/def-au-scma/master/html/00frontmatter/00WARNING.html" xr:uid="{49A50E75-20AA-4128-BA23-A23115C11C43}"/>
+    <hyperlink ref="L153" r:id="rId345" display="https://raw.githack.com/ANZSoilData/def-au-scma/master/html/00frontmatter/00WARNING.html" xr:uid="{9C2839E9-BED5-4FF6-816F-77B57041A619}"/>
+    <hyperlink ref="L157" r:id="rId346" display="https://raw.githack.com/ANZSoilData/def-au-scma/master/html/00frontmatter/00WARNING.html" xr:uid="{E23A6699-90A5-4856-BF79-2380091F574E}"/>
+    <hyperlink ref="L161" r:id="rId347" display="https://raw.githack.com/ANZSoilData/def-au-scma/master/html/00frontmatter/00WARNING.html" xr:uid="{1A8492DF-94CC-46BC-94FC-8EC8D477843A}"/>
+    <hyperlink ref="L165" r:id="rId348" display="https://raw.githack.com/ANZSoilData/def-au-scma/master/html/00frontmatter/00WARNING.html" xr:uid="{7E9EAA15-2255-4AE8-AE67-0CA5DDA5A347}"/>
+    <hyperlink ref="L169" r:id="rId349" display="https://raw.githack.com/ANZSoilData/def-au-scma/master/html/00frontmatter/00WARNING.html" xr:uid="{7F580A4E-1F87-4BD7-A93B-17D22EC25FD5}"/>
+    <hyperlink ref="L173" r:id="rId350" display="https://raw.githack.com/ANZSoilData/def-au-scma/master/html/00frontmatter/00WARNING.html" xr:uid="{633DE086-4999-4966-A222-4A1181A3581B}"/>
+    <hyperlink ref="L177" r:id="rId351" display="https://raw.githack.com/ANZSoilData/def-au-scma/master/html/00frontmatter/00WARNING.html" xr:uid="{94047688-8533-4E04-94FF-AD5143093431}"/>
+    <hyperlink ref="L181" r:id="rId352" display="https://raw.githack.com/ANZSoilData/def-au-scma/master/html/00frontmatter/00WARNING.html" xr:uid="{41191E41-D130-4834-8125-0F76E602303B}"/>
+    <hyperlink ref="L185" r:id="rId353" display="https://raw.githack.com/ANZSoilData/def-au-scma/master/html/00frontmatter/00WARNING.html" xr:uid="{C4A07BDE-C8E3-40BA-BCCB-DB912E2A1D05}"/>
+    <hyperlink ref="L189" r:id="rId354" display="https://raw.githack.com/ANZSoilData/def-au-scma/master/html/00frontmatter/00WARNING.html" xr:uid="{ACB47CAB-46D8-47F6-A3DF-F8690426B059}"/>
+    <hyperlink ref="L193" r:id="rId355" display="https://raw.githack.com/ANZSoilData/def-au-scma/master/html/00frontmatter/00WARNING.html" xr:uid="{C9BBF2B3-E01C-4EE4-9553-7DFE776F7417}"/>
+    <hyperlink ref="L197" r:id="rId356" display="https://raw.githack.com/ANZSoilData/def-au-scma/master/html/00frontmatter/00WARNING.html" xr:uid="{A05F62DA-B658-4094-A328-4C524EC432B5}"/>
+    <hyperlink ref="L201" r:id="rId357" display="https://raw.githack.com/ANZSoilData/def-au-scma/master/html/00frontmatter/00WARNING.html" xr:uid="{0920E874-3FE7-44A0-8EE0-C1286C5EFC22}"/>
+    <hyperlink ref="L205" r:id="rId358" display="https://raw.githack.com/ANZSoilData/def-au-scma/master/html/00frontmatter/00WARNING.html" xr:uid="{27DFF406-EA84-4411-ADB3-39ABFBC87535}"/>
+    <hyperlink ref="L209" r:id="rId359" display="https://raw.githack.com/ANZSoilData/def-au-scma/master/html/00frontmatter/00WARNING.html" xr:uid="{DDA4DCE9-91E2-4EC0-A178-674FABC561A3}"/>
+    <hyperlink ref="L213" r:id="rId360" display="https://raw.githack.com/ANZSoilData/def-au-scma/master/html/00frontmatter/00WARNING.html" xr:uid="{66A75B59-91E0-4F9C-920C-3DE29142830A}"/>
+    <hyperlink ref="L217" r:id="rId361" display="https://raw.githack.com/ANZSoilData/def-au-scma/master/html/00frontmatter/00WARNING.html" xr:uid="{52D1A870-8B50-4756-919C-35BFD51F3F3F}"/>
+    <hyperlink ref="L221" r:id="rId362" display="https://raw.githack.com/ANZSoilData/def-au-scma/master/html/00frontmatter/00WARNING.html" xr:uid="{3048A8A9-D509-4345-BAC0-96AEB03E4DEA}"/>
+    <hyperlink ref="L225" r:id="rId363" display="https://raw.githack.com/ANZSoilData/def-au-scma/master/html/00frontmatter/00WARNING.html" xr:uid="{EBB126C0-C649-41AD-89E3-162B26844994}"/>
+    <hyperlink ref="L229" r:id="rId364" display="https://raw.githack.com/ANZSoilData/def-au-scma/master/html/00frontmatter/00WARNING.html" xr:uid="{34498225-638F-41B6-8A4E-2CD449DC92E3}"/>
+    <hyperlink ref="L233" r:id="rId365" display="https://raw.githack.com/ANZSoilData/def-au-scma/master/html/00frontmatter/00WARNING.html" xr:uid="{EC1831E6-01E3-4C6F-8864-CB175376670A}"/>
+    <hyperlink ref="L237" r:id="rId366" display="https://raw.githack.com/ANZSoilData/def-au-scma/master/html/00frontmatter/00WARNING.html" xr:uid="{F1779216-B8A7-4361-AF1B-567CE04261A6}"/>
+    <hyperlink ref="L241" r:id="rId367" display="https://raw.githack.com/ANZSoilData/def-au-scma/master/html/00frontmatter/00WARNING.html" xr:uid="{BB66DE9F-2A57-4A53-81A2-006DA68B66F9}"/>
+    <hyperlink ref="L245" r:id="rId368" display="https://raw.githack.com/ANZSoilData/def-au-scma/master/html/00frontmatter/00WARNING.html" xr:uid="{BF202C29-4AF7-41D1-B0AB-B613AA14FBF9}"/>
+    <hyperlink ref="L249" r:id="rId369" display="https://raw.githack.com/ANZSoilData/def-au-scma/master/html/00frontmatter/00WARNING.html" xr:uid="{1413E20E-6508-494F-9E8E-8C7A80E26C89}"/>
+    <hyperlink ref="L253" r:id="rId370" display="https://raw.githack.com/ANZSoilData/def-au-scma/master/html/00frontmatter/00WARNING.html" xr:uid="{693BD0DA-7B63-4EE0-856F-ADFFFFEFA1D6}"/>
+    <hyperlink ref="L257" r:id="rId371" display="https://raw.githack.com/ANZSoilData/def-au-scma/master/html/00frontmatter/00WARNING.html" xr:uid="{E0D95227-4D9D-462A-B990-0F650B304BA3}"/>
+    <hyperlink ref="L261" r:id="rId372" display="https://raw.githack.com/ANZSoilData/def-au-scma/master/html/00frontmatter/00WARNING.html" xr:uid="{F56970D0-CFD9-49B0-AD37-F168BBFA170D}"/>
+    <hyperlink ref="L265" r:id="rId373" display="https://raw.githack.com/ANZSoilData/def-au-scma/master/html/00frontmatter/00WARNING.html" xr:uid="{CD0EDD81-5ABB-4A32-BC15-CAEF04183D54}"/>
+    <hyperlink ref="L269" r:id="rId374" display="https://raw.githack.com/ANZSoilData/def-au-scma/master/html/00frontmatter/00WARNING.html" xr:uid="{24A0523D-5DED-4EAA-9F8F-3CC84B792A73}"/>
+    <hyperlink ref="L273" r:id="rId375" display="https://raw.githack.com/ANZSoilData/def-au-scma/master/html/00frontmatter/00WARNING.html" xr:uid="{397DDA1C-2976-4DA9-91C2-1824D9954851}"/>
+    <hyperlink ref="L277" r:id="rId376" display="https://raw.githack.com/ANZSoilData/def-au-scma/master/html/00frontmatter/00WARNING.html" xr:uid="{00677D20-EC96-4609-AFE2-9D7EE399F72C}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId386"/>
-  <legacyDrawing r:id="rId387"/>
+  <pageSetup orientation="portrait" r:id="rId377"/>
+  <legacyDrawing r:id="rId378"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4A25E589-C762-47F7-A5B5-46A66BE90C97}">
-  <dimension ref="A1:L466"/>
+  <dimension ref="A1:M466"/>
   <sheetViews>
-    <sheetView topLeftCell="F22" workbookViewId="0">
-      <selection activeCell="J38" sqref="J38"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A17" sqref="A17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -15038,10 +15085,10 @@
     </row>
     <row r="11" spans="1:12" s="16" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A11" s="1" t="s">
-        <v>1338</v>
+        <v>1361</v>
       </c>
       <c r="B11" s="41" t="s">
-        <v>1345</v>
+        <v>1331</v>
       </c>
       <c r="C11" s="4"/>
       <c r="D11" s="4"/>
@@ -15056,10 +15103,10 @@
     </row>
     <row r="12" spans="1:12" s="16" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A12" s="1" t="s">
-        <v>1343</v>
-      </c>
-      <c r="B12" s="64" t="s">
-        <v>1347</v>
+        <v>1362</v>
+      </c>
+      <c r="B12" s="63" t="s">
+        <v>1333</v>
       </c>
       <c r="C12" s="4"/>
       <c r="D12" s="4"/>
@@ -15074,10 +15121,10 @@
     </row>
     <row r="13" spans="1:12" s="16" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A13" s="1" t="s">
-        <v>1339</v>
-      </c>
-      <c r="B13" s="63" t="s">
-        <v>1344</v>
+        <v>1363</v>
+      </c>
+      <c r="B13" s="62" t="s">
+        <v>1330</v>
       </c>
       <c r="C13" s="4"/>
       <c r="D13" s="4"/>
@@ -15092,10 +15139,10 @@
     </row>
     <row r="14" spans="1:12" s="16" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A14" s="1" t="s">
-        <v>1323</v>
+        <v>1321</v>
       </c>
       <c r="B14" s="41" t="s">
-        <v>1341</v>
+        <v>1328</v>
       </c>
       <c r="C14" s="4"/>
       <c r="D14" s="4"/>
@@ -15110,10 +15157,10 @@
     </row>
     <row r="15" spans="1:12" s="16" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A15" s="1" t="s">
-        <v>1323</v>
+        <v>1321</v>
       </c>
       <c r="B15" s="41" t="s">
-        <v>1342</v>
+        <v>1329</v>
       </c>
       <c r="C15" s="4"/>
       <c r="D15" s="4"/>
@@ -15144,7 +15191,7 @@
       <c r="K16" s="15"/>
       <c r="L16" s="3"/>
     </row>
-    <row r="17" spans="1:12" s="16" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:13" s="16" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A17" s="1" t="s">
         <v>644</v>
       </c>
@@ -15162,7 +15209,7 @@
       <c r="K17" s="15"/>
       <c r="L17" s="3"/>
     </row>
-    <row r="18" spans="1:12" s="16" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:13" s="16" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A18" s="1" t="s">
         <v>645</v>
       </c>
@@ -15180,7 +15227,7 @@
       <c r="K18" s="15"/>
       <c r="L18" s="3"/>
     </row>
-    <row r="19" spans="1:12" s="16" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:13" s="16" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A19" s="1" t="s">
         <v>646</v>
       </c>
@@ -15198,7 +15245,7 @@
       <c r="K19" s="15"/>
       <c r="L19" s="3"/>
     </row>
-    <row r="20" spans="1:12" s="16" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:13" s="16" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A20" s="1" t="s">
         <v>1069</v>
       </c>
@@ -15216,7 +15263,7 @@
       <c r="K20" s="15"/>
       <c r="L20" s="3"/>
     </row>
-    <row r="21" spans="1:12" s="16" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:13" s="16" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A21" s="1" t="s">
         <v>649</v>
       </c>
@@ -15234,21 +15281,26 @@
       <c r="K21" s="15"/>
       <c r="L21" s="3"/>
     </row>
-    <row r="22" spans="1:12" s="16" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A22" s="3"/>
-      <c r="B22" s="4"/>
+    <row r="22" spans="1:13" s="16" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A22" s="43" t="s">
+        <v>1353</v>
+      </c>
+      <c r="B22" s="65" t="s">
+        <v>1355</v>
+      </c>
       <c r="C22" s="3"/>
       <c r="D22" s="3"/>
       <c r="E22" s="4"/>
       <c r="F22" s="3"/>
       <c r="G22" s="4"/>
       <c r="H22" s="3"/>
-      <c r="I22" s="15"/>
+      <c r="I22" s="51"/>
       <c r="J22" s="15"/>
       <c r="K22" s="15"/>
-      <c r="L22" s="3"/>
-    </row>
-    <row r="23" spans="1:12" s="16" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="L22" s="15"/>
+      <c r="M22" s="3"/>
+    </row>
+    <row r="23" spans="1:13" s="16" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A23" s="34"/>
       <c r="B23" s="35"/>
       <c r="C23" s="35"/>
@@ -15262,7 +15314,7 @@
       <c r="K23" s="44"/>
       <c r="L23" s="35"/>
     </row>
-    <row r="24" spans="1:12" s="16" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:13" s="16" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>637</v>
       </c>
@@ -15278,7 +15330,7 @@
       <c r="K24" s="45"/>
       <c r="L24" s="6"/>
     </row>
-    <row r="25" spans="1:12" s="16" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:13" s="16" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A25" s="6" t="s">
         <v>6</v>
       </c>
@@ -15294,7 +15346,7 @@
       <c r="K25" s="45"/>
       <c r="L25" s="6"/>
     </row>
-    <row r="26" spans="1:12" ht="30" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:13" ht="30" x14ac:dyDescent="0.25">
       <c r="A26" s="20" t="s">
         <v>7</v>
       </c>
@@ -15332,7 +15384,7 @@
         <v>639</v>
       </c>
     </row>
-    <row r="27" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A27" s="25" t="s">
         <v>785</v>
       </c>
@@ -15359,7 +15411,7 @@
         <v>1068</v>
       </c>
     </row>
-    <row r="28" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A28" s="30" t="s">
         <v>786</v>
       </c>
@@ -15373,7 +15425,7 @@
         <v>790</v>
       </c>
       <c r="E28" s="60" t="s">
-        <v>1318</v>
+        <v>1356</v>
       </c>
       <c r="F28" s="12"/>
       <c r="G28" s="25" t="s">
@@ -15393,7 +15445,7 @@
         <v>1068</v>
       </c>
     </row>
-    <row r="29" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A29" s="30" t="s">
         <v>787</v>
       </c>
@@ -15407,7 +15459,7 @@
         <v>791</v>
       </c>
       <c r="E29" s="60" t="s">
-        <v>1318</v>
+        <v>1356</v>
       </c>
       <c r="F29" s="12"/>
       <c r="G29" s="25" t="s">
@@ -15427,7 +15479,7 @@
         <v>1068</v>
       </c>
     </row>
-    <row r="30" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A30" s="30" t="s">
         <v>788</v>
       </c>
@@ -15441,7 +15493,7 @@
         <v>792</v>
       </c>
       <c r="E30" s="60" t="s">
-        <v>1318</v>
+        <v>1356</v>
       </c>
       <c r="F30" s="12"/>
       <c r="G30" s="25" t="s">
@@ -15461,7 +15513,7 @@
         <v>1068</v>
       </c>
     </row>
-    <row r="31" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A31" s="30" t="s">
         <v>794</v>
       </c>
@@ -15487,7 +15539,7 @@
         <v>1068</v>
       </c>
     </row>
-    <row r="32" spans="1:12" ht="55.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:13" ht="55.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A32" s="30" t="s">
         <v>795</v>
       </c>
@@ -16279,7 +16331,7 @@
         <v>691</v>
       </c>
       <c r="E60" s="60" t="s">
-        <v>1319</v>
+        <v>1356</v>
       </c>
       <c r="F60" s="12"/>
       <c r="G60" s="30" t="s">
@@ -16875,7 +16927,7 @@
         <v>712</v>
       </c>
       <c r="E81" s="60" t="s">
-        <v>1319</v>
+        <v>1356</v>
       </c>
       <c r="F81" s="12"/>
       <c r="G81" s="30" t="s">
@@ -17107,7 +17159,7 @@
         <v>722</v>
       </c>
       <c r="E89" s="60" t="s">
-        <v>1319</v>
+        <v>1356</v>
       </c>
       <c r="F89" s="12" t="s">
         <v>855</v>
@@ -17439,7 +17491,7 @@
         <v>735</v>
       </c>
       <c r="E100" s="60" t="s">
-        <v>1319</v>
+        <v>1356</v>
       </c>
       <c r="F100" s="12"/>
       <c r="G100" s="30" t="s">
@@ -18051,7 +18103,7 @@
         <v>756</v>
       </c>
       <c r="E121" s="60" t="s">
-        <v>1319</v>
+        <v>1356</v>
       </c>
       <c r="F121" s="12" t="s">
         <v>890</v>
@@ -19913,7 +19965,7 @@
         <v>126</v>
       </c>
       <c r="E186" s="60" t="s">
-        <v>1319</v>
+        <v>1356</v>
       </c>
       <c r="F186"/>
       <c r="G186" s="19" t="s">
@@ -20085,7 +20137,7 @@
         <v>150</v>
       </c>
       <c r="E192" s="60" t="s">
-        <v>1319</v>
+        <v>1356</v>
       </c>
       <c r="F192"/>
       <c r="G192" s="19" t="s">
@@ -20145,7 +20197,7 @@
         <v>162</v>
       </c>
       <c r="E194" s="60" t="s">
-        <v>1319</v>
+        <v>1356</v>
       </c>
       <c r="F194"/>
       <c r="G194" s="19" t="s">
@@ -22454,12 +22506,9 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
@@ -22674,15 +22723,19 @@
 </file>
 
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{008ABE91-8C92-4516-916D-4DC325FB5C89}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{AAE62FC3-7D3B-4886-B53E-C881811D2384}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
@@ -22707,10 +22760,9 @@
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{AAE62FC3-7D3B-4886-B53E-C881811D2384}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{008ABE91-8C92-4516-916D-4DC325FB5C89}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
dcterms:licence to dcterms:isFormatOf for NLA
</commit_message>
<xml_diff>
--- a/rdf/skosplay-scma-2.xlsx
+++ b/rdf/skosplay-scma-2.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\cox075\dev\ENV\anzsoil\def-au-scma\rdf\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://federationuniversity-my.sharepoint.com/personal/mr_wong_federation_edu_au/Documents/Documents/GitHub/def-au-scma/rdf/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1D05314A-5E7A-4C37-8E03-3E88D70CCAEC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="9" documentId="13_ncr:1_{1D05314A-5E7A-4C37-8E03-3E88D70CCAEC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{B8CCFFB0-9A95-4D94-8728-9E86B477AEAB}"/>
   <bookViews>
-    <workbookView xWindow="8490" yWindow="6705" windowWidth="27375" windowHeight="13950" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="24240" windowHeight="13140" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="SCMA-2011" sheetId="2" r:id="rId1"/>
@@ -103,7 +103,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4366" uniqueCount="1370">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4366" uniqueCount="1371">
   <si>
     <t>ConceptScheme URI</t>
   </si>
@@ -4294,6 +4294,9 @@
   </si>
   <si>
     <t>Australian Laboratory Handbook of Soil and Water Chemical Methods (Rayment and Higginson 1992)</t>
+  </si>
+  <si>
+    <t>dcterms:isFormatOf</t>
   </si>
 </sst>
 </file>
@@ -4475,7 +4478,7 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="67">
+  <cellXfs count="68">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="2" applyBorder="1"/>
@@ -4606,6 +4609,9 @@
     <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="2" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="2" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="3">
@@ -4984,8 +4990,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:M478"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="B27" sqref="B27"/>
+    <sheetView tabSelected="1" topLeftCell="A4" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="A27" sqref="A27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5341,7 +5347,7 @@
       <c r="A18" s="1" t="s">
         <v>644</v>
       </c>
-      <c r="B18" s="37" t="s">
+      <c r="B18" s="67" t="s">
         <v>634</v>
       </c>
       <c r="C18" s="4"/>
@@ -5360,7 +5366,7 @@
       <c r="A19" s="1" t="s">
         <v>644</v>
       </c>
-      <c r="B19" s="38" t="s">
+      <c r="B19" s="26" t="s">
         <v>635</v>
       </c>
       <c r="C19" s="4"/>
@@ -14889,10 +14895,12 @@
     <hyperlink ref="L270" r:id="rId374" display="https://raw.githack.com/ANZSoilData/def-au-scma/master/html/00frontmatter/00WARNING.html" xr:uid="{24A0523D-5DED-4EAA-9F8F-3CC84B792A73}"/>
     <hyperlink ref="L274" r:id="rId375" display="https://raw.githack.com/ANZSoilData/def-au-scma/master/html/00frontmatter/00WARNING.html" xr:uid="{397DDA1C-2976-4DA9-91C2-1824D9954851}"/>
     <hyperlink ref="L278" r:id="rId376" display="https://raw.githack.com/ANZSoilData/def-au-scma/master/html/00frontmatter/00WARNING.html" xr:uid="{00677D20-EC96-4609-AFE2-9D7EE399F72C}"/>
+    <hyperlink ref="B18" r:id="rId377" xr:uid="{31571278-A517-460E-AA8B-2538A10AD1BA}"/>
+    <hyperlink ref="B19" r:id="rId378" xr:uid="{386259F1-8A48-45EF-9526-D7EE660E59A8}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId377"/>
-  <legacyDrawing r:id="rId378"/>
+  <pageSetup orientation="portrait" r:id="rId379"/>
+  <legacyDrawing r:id="rId380"/>
 </worksheet>
 </file>
 
@@ -14901,7 +14909,7 @@
   <dimension ref="A1:M467"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B21" sqref="B21"/>
+      <selection activeCell="A20" sqref="A20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -15272,7 +15280,7 @@
     </row>
     <row r="20" spans="1:13" s="16" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A20" s="1" t="s">
-        <v>645</v>
+        <v>1370</v>
       </c>
       <c r="B20" s="26" t="s">
         <v>1067</v>
@@ -22549,12 +22557,9 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
@@ -22769,15 +22774,19 @@
 </file>
 
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{008ABE91-8C92-4516-916D-4DC325FB5C89}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{AAE62FC3-7D3B-4886-B53E-C881811D2384}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
@@ -22802,10 +22811,9 @@
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{AAE62FC3-7D3B-4886-B53E-C881811D2384}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{008ABE91-8C92-4516-916D-4DC325FB5C89}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
1. delete all `skos:inScheme` related to `rdf:type skos:Collection`, metadata updates  skos:editorialNote, owl:VersionInfo, dcterms:modified^^xsd:date
</commit_message>
<xml_diff>
--- a/rdf/skosplay-scma-2.xlsx
+++ b/rdf/skosplay-scma-2.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://federationuniversity-my.sharepoint.com/personal/mr_wong_federation_edu_au/Documents/Documents/GitHub/def-au-scma/rdf/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="9" documentId="13_ncr:1_{1D05314A-5E7A-4C37-8E03-3E88D70CCAEC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{B8CCFFB0-9A95-4D94-8728-9E86B477AEAB}"/>
+  <xr:revisionPtr revIDLastSave="23" documentId="13_ncr:1_{1D05314A-5E7A-4C37-8E03-3E88D70CCAEC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{96FC585B-D19C-4F44-A81F-F32F5A390E57}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="24240" windowHeight="13140" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView minimized="1" xWindow="1875" yWindow="1800" windowWidth="18000" windowHeight="9360" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="SCMA-2011" sheetId="2" r:id="rId1"/>
@@ -35,8 +35,6 @@
   <authors>
     <author>tc={B0E3DF97-B13F-494E-A738-184CA7B7851B}</author>
     <author>tc={67160120-CB63-4486-9227-F88649E9E9C7}</author>
-    <author>tc={0B26873D-FA99-482F-BB2A-F523AECB0A02}</author>
-    <author>tc={D93122F8-B2E7-44D8-B776-19855D9E8B0C}</author>
     <author>tc={18599286-A473-45D7-85E2-C1993234C618}</author>
   </authors>
   <commentList>
@@ -56,23 +54,7 @@
     has split  ROR ID https://ror.org/02wtcj248  https://ror.org/01drzr533</t>
       </text>
     </comment>
-    <comment ref="B21" authorId="2" shapeId="0" xr:uid="{0B26873D-FA99-482F-BB2A-F523AECB0A02}">
-      <text>
-        <t>[Threaded comment]
-Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
-Comment:
-    DAWE is funding this work, include?</t>
-      </text>
-    </comment>
-    <comment ref="B22" authorId="3" shapeId="0" xr:uid="{D93122F8-B2E7-44D8-B776-19855D9E8B0C}">
-      <text>
-        <t>[Threaded comment]
-Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
-Comment:
-    aknowldged in book. Others were aknowledged from ASPAC</t>
-      </text>
-    </comment>
-    <comment ref="F34" authorId="4" shapeId="0" xr:uid="{18599286-A473-45D7-85E2-C1993234C618}">
+    <comment ref="F34" authorId="2" shapeId="0" xr:uid="{18599286-A473-45D7-85E2-C1993234C618}">
       <text>
         <t>[Threaded comment]
 Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
@@ -4478,7 +4460,7 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="68">
+  <cellXfs count="66">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="2" applyBorder="1"/>
@@ -4558,11 +4540,7 @@
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -4966,12 +4944,6 @@
   <threadedComment ref="B20" dT="2022-03-18T02:11:05.88" personId="{858A8595-1E7F-44A0-A29C-57D42A21D7F8}" id="{67160120-CB63-4486-9227-F88649E9E9C7}">
     <text>has split  ROR ID https://ror.org/02wtcj248  https://ror.org/01drzr533</text>
   </threadedComment>
-  <threadedComment ref="B21" dT="2022-03-18T02:11:47.38" personId="{858A8595-1E7F-44A0-A29C-57D42A21D7F8}" id="{0B26873D-FA99-482F-BB2A-F523AECB0A02}">
-    <text>DAWE is funding this work, include?</text>
-  </threadedComment>
-  <threadedComment ref="B22" dT="2022-03-18T02:10:25.54" personId="{858A8595-1E7F-44A0-A29C-57D42A21D7F8}" id="{D93122F8-B2E7-44D8-B776-19855D9E8B0C}">
-    <text>aknowldged in book. Others were aknowledged from ASPAC</text>
-  </threadedComment>
   <threadedComment ref="F34" dT="2021-04-26T01:42:21.46" personId="{74AF7186-62D8-498B-BD29-BBBCF0E53A82}" id="{18599286-A473-45D7-85E2-C1993234C618}">
     <text>don't need both broader and narrower columns - they are generated by SKOS-Play! post-processing - https://skos-play.sparna.fr/play/convert#post-processings</text>
   </threadedComment>
@@ -4990,7 +4962,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:M478"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="A7" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
       <selection activeCell="A27" sqref="A27"/>
     </sheetView>
   </sheetViews>
@@ -5004,7 +4976,7 @@
     <col min="6" max="6" width="16.140625" style="3" customWidth="1"/>
     <col min="7" max="7" width="24.140625" style="4" customWidth="1"/>
     <col min="8" max="8" width="40.7109375" style="3" customWidth="1"/>
-    <col min="9" max="9" width="40.7109375" style="51" customWidth="1"/>
+    <col min="9" max="9" width="40.7109375" style="49" customWidth="1"/>
     <col min="10" max="10" width="24.28515625" style="15" customWidth="1"/>
     <col min="11" max="11" width="73.7109375" style="15" customWidth="1"/>
     <col min="12" max="12" width="39.28515625" style="15" customWidth="1"/>
@@ -5025,9 +4997,9 @@
       <c r="F1" s="3"/>
       <c r="G1" s="4"/>
       <c r="H1" s="1"/>
-      <c r="I1" s="50"/>
-      <c r="J1" s="43"/>
-      <c r="K1" s="43"/>
+      <c r="I1" s="48"/>
+      <c r="J1" s="41"/>
+      <c r="K1" s="41"/>
       <c r="L1" s="15"/>
       <c r="M1" s="3"/>
     </row>
@@ -5046,9 +5018,9 @@
       <c r="F2" s="3"/>
       <c r="G2" s="4"/>
       <c r="H2" s="1"/>
-      <c r="I2" s="50"/>
-      <c r="J2" s="43"/>
-      <c r="K2" s="43"/>
+      <c r="I2" s="48"/>
+      <c r="J2" s="41"/>
+      <c r="K2" s="41"/>
       <c r="L2" s="15"/>
       <c r="M2" s="3"/>
     </row>
@@ -5067,9 +5039,9 @@
       <c r="F3" s="3"/>
       <c r="G3" s="4"/>
       <c r="H3" s="1"/>
-      <c r="I3" s="50"/>
-      <c r="J3" s="43"/>
-      <c r="K3" s="43"/>
+      <c r="I3" s="48"/>
+      <c r="J3" s="41"/>
+      <c r="K3" s="41"/>
       <c r="L3" s="15"/>
       <c r="M3" s="3"/>
     </row>
@@ -5088,9 +5060,9 @@
       <c r="F4" s="3"/>
       <c r="G4" s="4"/>
       <c r="H4" s="1"/>
-      <c r="I4" s="50"/>
-      <c r="J4" s="43"/>
-      <c r="K4" s="43"/>
+      <c r="I4" s="48"/>
+      <c r="J4" s="41"/>
+      <c r="K4" s="41"/>
       <c r="L4" s="15"/>
       <c r="M4" s="3"/>
     </row>
@@ -5109,9 +5081,9 @@
       <c r="F5" s="3"/>
       <c r="G5" s="4"/>
       <c r="H5" s="1"/>
-      <c r="I5" s="50"/>
-      <c r="J5" s="43"/>
-      <c r="K5" s="43"/>
+      <c r="I5" s="48"/>
+      <c r="J5" s="41"/>
+      <c r="K5" s="41"/>
       <c r="L5" s="15"/>
       <c r="M5" s="3"/>
     </row>
@@ -5128,9 +5100,9 @@
       <c r="F6" s="3"/>
       <c r="G6" s="4"/>
       <c r="H6" s="1"/>
-      <c r="I6" s="50"/>
-      <c r="J6" s="43"/>
-      <c r="K6" s="43"/>
+      <c r="I6" s="48"/>
+      <c r="J6" s="41"/>
+      <c r="K6" s="41"/>
       <c r="L6" s="15"/>
       <c r="M6" s="3"/>
     </row>
@@ -5147,9 +5119,9 @@
       <c r="F7" s="3"/>
       <c r="G7" s="4"/>
       <c r="H7" s="1"/>
-      <c r="I7" s="50"/>
-      <c r="J7" s="43"/>
-      <c r="K7" s="43"/>
+      <c r="I7" s="48"/>
+      <c r="J7" s="41"/>
+      <c r="K7" s="41"/>
       <c r="L7" s="15"/>
       <c r="M7" s="3"/>
     </row>
@@ -5160,15 +5132,15 @@
       <c r="B8" s="36" t="s">
         <v>1064</v>
       </c>
-      <c r="C8" s="61"/>
+      <c r="C8" s="59"/>
       <c r="D8" s="4"/>
       <c r="E8" s="4"/>
       <c r="F8" s="3"/>
       <c r="G8" s="4"/>
       <c r="H8" s="1"/>
-      <c r="I8" s="50"/>
-      <c r="J8" s="43"/>
-      <c r="K8" s="43"/>
+      <c r="I8" s="48"/>
+      <c r="J8" s="41"/>
+      <c r="K8" s="41"/>
       <c r="L8" s="15"/>
       <c r="M8" s="3"/>
     </row>
@@ -5185,9 +5157,9 @@
       <c r="F9" s="3"/>
       <c r="G9" s="4"/>
       <c r="H9" s="1"/>
-      <c r="I9" s="50"/>
-      <c r="J9" s="43"/>
-      <c r="K9" s="43"/>
+      <c r="I9" s="48"/>
+      <c r="J9" s="41"/>
+      <c r="K9" s="41"/>
       <c r="L9" s="15"/>
       <c r="M9" s="3"/>
     </row>
@@ -5204,9 +5176,9 @@
       <c r="F10" s="3"/>
       <c r="G10" s="4"/>
       <c r="H10" s="1"/>
-      <c r="I10" s="50"/>
-      <c r="J10" s="43"/>
-      <c r="K10" s="43"/>
+      <c r="I10" s="48"/>
+      <c r="J10" s="41"/>
+      <c r="K10" s="41"/>
       <c r="L10" s="15"/>
       <c r="M10" s="3"/>
     </row>
@@ -5223,9 +5195,9 @@
       <c r="F11" s="3"/>
       <c r="G11" s="4"/>
       <c r="H11" s="1"/>
-      <c r="I11" s="50"/>
-      <c r="J11" s="43"/>
-      <c r="K11" s="43"/>
+      <c r="I11" s="48"/>
+      <c r="J11" s="41"/>
+      <c r="K11" s="41"/>
       <c r="L11" s="15"/>
       <c r="M11" s="3"/>
     </row>
@@ -5242,9 +5214,9 @@
       <c r="F12" s="3"/>
       <c r="G12" s="4"/>
       <c r="H12" s="1"/>
-      <c r="I12" s="50"/>
-      <c r="J12" s="43"/>
-      <c r="K12" s="43"/>
+      <c r="I12" s="48"/>
+      <c r="J12" s="41"/>
+      <c r="K12" s="41"/>
       <c r="L12" s="15"/>
       <c r="M12" s="3"/>
     </row>
@@ -5252,7 +5224,7 @@
       <c r="A13" s="1" t="s">
         <v>1320</v>
       </c>
-      <c r="B13" s="66" t="s">
+      <c r="B13" s="64" t="s">
         <v>1365</v>
       </c>
       <c r="C13" s="4"/>
@@ -5261,9 +5233,9 @@
       <c r="F13" s="3"/>
       <c r="G13" s="4"/>
       <c r="H13" s="1"/>
-      <c r="I13" s="50"/>
-      <c r="J13" s="43"/>
-      <c r="K13" s="43"/>
+      <c r="I13" s="48"/>
+      <c r="J13" s="41"/>
+      <c r="K13" s="41"/>
       <c r="L13" s="15"/>
       <c r="M13" s="3"/>
     </row>
@@ -5280,9 +5252,9 @@
       <c r="F14" s="3"/>
       <c r="G14" s="4"/>
       <c r="H14" s="1"/>
-      <c r="I14" s="50"/>
-      <c r="J14" s="43"/>
-      <c r="K14" s="43"/>
+      <c r="I14" s="48"/>
+      <c r="J14" s="41"/>
+      <c r="K14" s="41"/>
       <c r="L14" s="15"/>
       <c r="M14" s="3"/>
     </row>
@@ -5290,7 +5262,7 @@
       <c r="A15" s="1" t="s">
         <v>642</v>
       </c>
-      <c r="B15" s="41">
+      <c r="B15" s="39">
         <v>44197</v>
       </c>
       <c r="C15" s="4"/>
@@ -5299,9 +5271,9 @@
       <c r="F15" s="3"/>
       <c r="G15" s="4"/>
       <c r="H15" s="1"/>
-      <c r="I15" s="50"/>
-      <c r="J15" s="43"/>
-      <c r="K15" s="43"/>
+      <c r="I15" s="48"/>
+      <c r="J15" s="41"/>
+      <c r="K15" s="41"/>
       <c r="L15" s="15"/>
       <c r="M15" s="3"/>
     </row>
@@ -5309,7 +5281,7 @@
       <c r="A16" s="1" t="s">
         <v>643</v>
       </c>
-      <c r="B16" s="41">
+      <c r="B16" s="39">
         <v>44643</v>
       </c>
       <c r="C16" s="4"/>
@@ -5318,9 +5290,9 @@
       <c r="F16" s="3"/>
       <c r="G16" s="4"/>
       <c r="H16" s="1"/>
-      <c r="I16" s="50"/>
-      <c r="J16" s="43"/>
-      <c r="K16" s="43"/>
+      <c r="I16" s="48"/>
+      <c r="J16" s="41"/>
+      <c r="K16" s="41"/>
       <c r="L16" s="15"/>
       <c r="M16" s="3"/>
     </row>
@@ -5328,7 +5300,7 @@
       <c r="A17" s="1" t="s">
         <v>649</v>
       </c>
-      <c r="B17" s="40" t="s">
+      <c r="B17" s="38" t="s">
         <v>1060</v>
       </c>
       <c r="C17" s="4"/>
@@ -5337,9 +5309,9 @@
       <c r="F17" s="3"/>
       <c r="G17" s="4"/>
       <c r="H17" s="1"/>
-      <c r="I17" s="50"/>
-      <c r="J17" s="43"/>
-      <c r="K17" s="43"/>
+      <c r="I17" s="48"/>
+      <c r="J17" s="41"/>
+      <c r="K17" s="41"/>
       <c r="L17" s="15"/>
       <c r="M17" s="3"/>
     </row>
@@ -5347,7 +5319,7 @@
       <c r="A18" s="1" t="s">
         <v>644</v>
       </c>
-      <c r="B18" s="67" t="s">
+      <c r="B18" s="65" t="s">
         <v>634</v>
       </c>
       <c r="C18" s="4"/>
@@ -5356,9 +5328,9 @@
       <c r="F18" s="3"/>
       <c r="G18" s="4"/>
       <c r="H18" s="1"/>
-      <c r="I18" s="50"/>
-      <c r="J18" s="43"/>
-      <c r="K18" s="43"/>
+      <c r="I18" s="48"/>
+      <c r="J18" s="41"/>
+      <c r="K18" s="41"/>
       <c r="L18" s="15"/>
       <c r="M18" s="3"/>
     </row>
@@ -5375,9 +5347,9 @@
       <c r="F19" s="3"/>
       <c r="G19" s="4"/>
       <c r="H19" s="1"/>
-      <c r="I19" s="50"/>
-      <c r="J19" s="43"/>
-      <c r="K19" s="43"/>
+      <c r="I19" s="48"/>
+      <c r="J19" s="41"/>
+      <c r="K19" s="41"/>
       <c r="L19" s="15"/>
       <c r="M19" s="3"/>
     </row>
@@ -5385,7 +5357,7 @@
       <c r="A20" s="1" t="s">
         <v>1358</v>
       </c>
-      <c r="B20" s="38" t="s">
+      <c r="B20" s="37" t="s">
         <v>1325</v>
       </c>
       <c r="C20" s="4"/>
@@ -5394,9 +5366,9 @@
       <c r="F20" s="3"/>
       <c r="G20" s="4"/>
       <c r="H20" s="1"/>
-      <c r="I20" s="50"/>
-      <c r="J20" s="43"/>
-      <c r="K20" s="43"/>
+      <c r="I20" s="48"/>
+      <c r="J20" s="41"/>
+      <c r="K20" s="41"/>
       <c r="L20" s="15"/>
       <c r="M20" s="3"/>
     </row>
@@ -5404,7 +5376,7 @@
       <c r="A21" s="1" t="s">
         <v>1358</v>
       </c>
-      <c r="B21" t="s">
+      <c r="B21" s="26" t="s">
         <v>1326</v>
       </c>
       <c r="C21" s="4"/>
@@ -5413,9 +5385,9 @@
       <c r="F21" s="3"/>
       <c r="G21" s="4"/>
       <c r="H21" s="1"/>
-      <c r="I21" s="50"/>
-      <c r="J21" s="43"/>
-      <c r="K21" s="43"/>
+      <c r="I21" s="48"/>
+      <c r="J21" s="41"/>
+      <c r="K21" s="41"/>
       <c r="L21" s="15"/>
       <c r="M21" s="3"/>
     </row>
@@ -5423,7 +5395,7 @@
       <c r="A22" s="1" t="s">
         <v>644</v>
       </c>
-      <c r="B22" s="38" t="s">
+      <c r="B22" s="37" t="s">
         <v>1366</v>
       </c>
       <c r="C22" s="4"/>
@@ -5432,9 +5404,9 @@
       <c r="F22" s="3"/>
       <c r="G22" s="4"/>
       <c r="H22" s="1"/>
-      <c r="I22" s="50"/>
-      <c r="J22" s="43"/>
-      <c r="K22" s="43"/>
+      <c r="I22" s="48"/>
+      <c r="J22" s="41"/>
+      <c r="K22" s="41"/>
       <c r="L22" s="15"/>
       <c r="M22" s="3"/>
     </row>
@@ -5442,7 +5414,7 @@
       <c r="A23" s="1" t="s">
         <v>1359</v>
       </c>
-      <c r="B23" s="38" t="s">
+      <c r="B23" s="37" t="s">
         <v>1356</v>
       </c>
       <c r="C23" s="4"/>
@@ -5451,9 +5423,9 @@
       <c r="F23" s="3"/>
       <c r="G23" s="4"/>
       <c r="H23" s="1"/>
-      <c r="I23" s="50"/>
-      <c r="J23" s="43"/>
-      <c r="K23" s="43"/>
+      <c r="I23" s="48"/>
+      <c r="J23" s="41"/>
+      <c r="K23" s="41"/>
       <c r="L23" s="15"/>
       <c r="M23" s="3"/>
     </row>
@@ -5461,7 +5433,7 @@
       <c r="A24" s="1" t="s">
         <v>1358</v>
       </c>
-      <c r="B24" s="38" t="s">
+      <c r="B24" s="37" t="s">
         <v>1357</v>
       </c>
       <c r="C24" s="4"/>
@@ -5470,9 +5442,9 @@
       <c r="F24" s="3"/>
       <c r="G24" s="4"/>
       <c r="H24" s="1"/>
-      <c r="I24" s="50"/>
-      <c r="J24" s="43"/>
-      <c r="K24" s="43"/>
+      <c r="I24" s="48"/>
+      <c r="J24" s="41"/>
+      <c r="K24" s="41"/>
       <c r="L24" s="15"/>
       <c r="M24" s="3"/>
     </row>
@@ -5489,9 +5461,9 @@
       <c r="F25" s="3"/>
       <c r="G25" s="4"/>
       <c r="H25" s="1"/>
-      <c r="I25" s="50"/>
-      <c r="J25" s="43"/>
-      <c r="K25" s="43"/>
+      <c r="I25" s="48"/>
+      <c r="J25" s="41"/>
+      <c r="K25" s="41"/>
       <c r="L25" s="15"/>
       <c r="M25" s="3"/>
     </row>
@@ -5508,9 +5480,9 @@
       <c r="F26" s="3"/>
       <c r="G26" s="4"/>
       <c r="H26" s="1"/>
-      <c r="I26" s="50"/>
-      <c r="J26" s="43"/>
-      <c r="K26" s="43"/>
+      <c r="I26" s="48"/>
+      <c r="J26" s="41"/>
+      <c r="K26" s="41"/>
       <c r="L26" s="15"/>
       <c r="M26" s="3"/>
     </row>
@@ -5518,7 +5490,7 @@
       <c r="A27" s="1" t="s">
         <v>1367</v>
       </c>
-      <c r="B27" s="39" t="s">
+      <c r="B27" s="26" t="s">
         <v>1061</v>
       </c>
       <c r="C27" s="4"/>
@@ -5527,9 +5499,9 @@
       <c r="F27" s="3"/>
       <c r="G27" s="4"/>
       <c r="H27" s="1"/>
-      <c r="I27" s="50"/>
-      <c r="J27" s="43"/>
-      <c r="K27" s="43"/>
+      <c r="I27" s="48"/>
+      <c r="J27" s="41"/>
+      <c r="K27" s="41"/>
       <c r="L27" s="15"/>
       <c r="M27" s="3"/>
     </row>
@@ -5546,9 +5518,9 @@
       <c r="F28" s="3"/>
       <c r="G28" s="4"/>
       <c r="H28" s="1"/>
-      <c r="I28" s="50"/>
-      <c r="J28" s="43"/>
-      <c r="K28" s="43"/>
+      <c r="I28" s="48"/>
+      <c r="J28" s="41"/>
+      <c r="K28" s="41"/>
       <c r="L28" s="15"/>
       <c r="M28" s="3"/>
     </row>
@@ -5565,17 +5537,17 @@
       <c r="F29" s="3"/>
       <c r="G29" s="4"/>
       <c r="H29" s="1"/>
-      <c r="I29" s="50"/>
-      <c r="J29" s="43"/>
-      <c r="K29" s="43"/>
+      <c r="I29" s="48"/>
+      <c r="J29" s="41"/>
+      <c r="K29" s="41"/>
       <c r="L29" s="15"/>
       <c r="M29" s="3"/>
     </row>
     <row r="30" spans="1:13" s="16" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A30" s="43" t="s">
+      <c r="A30" s="41" t="s">
         <v>1352</v>
       </c>
-      <c r="B30" s="64" t="s">
+      <c r="B30" s="62" t="s">
         <v>1353</v>
       </c>
       <c r="C30" s="3"/>
@@ -5584,7 +5556,7 @@
       <c r="F30" s="3"/>
       <c r="G30" s="4"/>
       <c r="H30" s="3"/>
-      <c r="I30" s="51"/>
+      <c r="I30" s="49"/>
       <c r="J30" s="15"/>
       <c r="K30" s="15"/>
       <c r="L30" s="15"/>
@@ -5599,10 +5571,10 @@
       <c r="F31" s="35"/>
       <c r="G31" s="35"/>
       <c r="H31" s="35"/>
-      <c r="I31" s="52"/>
-      <c r="J31" s="44"/>
-      <c r="K31" s="44"/>
-      <c r="L31" s="44"/>
+      <c r="I31" s="50"/>
+      <c r="J31" s="42"/>
+      <c r="K31" s="42"/>
+      <c r="L31" s="42"/>
       <c r="M31" s="35"/>
     </row>
     <row r="32" spans="1:13" s="16" customFormat="1" x14ac:dyDescent="0.25">
@@ -5616,10 +5588,10 @@
       <c r="F32" s="6"/>
       <c r="G32" s="7"/>
       <c r="H32" s="6"/>
-      <c r="I32" s="53"/>
-      <c r="J32" s="45"/>
-      <c r="K32" s="45"/>
-      <c r="L32" s="45"/>
+      <c r="I32" s="51"/>
+      <c r="J32" s="43"/>
+      <c r="K32" s="43"/>
+      <c r="L32" s="43"/>
       <c r="M32" s="6"/>
     </row>
     <row r="33" spans="1:13" s="16" customFormat="1" x14ac:dyDescent="0.25">
@@ -5633,10 +5605,10 @@
       <c r="F33" s="6"/>
       <c r="G33" s="7"/>
       <c r="H33" s="6"/>
-      <c r="I33" s="53"/>
-      <c r="J33" s="45"/>
-      <c r="K33" s="45"/>
-      <c r="L33" s="45"/>
+      <c r="I33" s="51"/>
+      <c r="J33" s="43"/>
+      <c r="K33" s="43"/>
+      <c r="L33" s="43"/>
       <c r="M33" s="6"/>
     </row>
     <row r="34" spans="1:13" ht="30" x14ac:dyDescent="0.25">
@@ -5664,16 +5636,16 @@
       <c r="H34" s="20" t="s">
         <v>638</v>
       </c>
-      <c r="I34" s="54" t="s">
+      <c r="I34" s="52" t="s">
         <v>1317</v>
       </c>
-      <c r="J34" s="48" t="s">
+      <c r="J34" s="46" t="s">
         <v>1314</v>
       </c>
-      <c r="K34" s="48" t="s">
+      <c r="K34" s="46" t="s">
         <v>1323</v>
       </c>
-      <c r="L34" s="42" t="s">
+      <c r="L34" s="40" t="s">
         <v>1322</v>
       </c>
       <c r="M34" s="21" t="s">
@@ -5701,7 +5673,7 @@
       <c r="H35" s="29" t="s">
         <v>921</v>
       </c>
-      <c r="I35" s="55"/>
+      <c r="I35" s="53"/>
       <c r="J35" s="32"/>
       <c r="K35" s="32" t="s">
         <v>1333</v>
@@ -5736,7 +5708,7 @@
       <c r="H36" s="29" t="s">
         <v>922</v>
       </c>
-      <c r="I36" s="55"/>
+      <c r="I36" s="53"/>
       <c r="J36" s="32"/>
       <c r="K36" s="32" t="s">
         <v>1333</v>
@@ -5771,7 +5743,7 @@
       <c r="H37" s="29" t="s">
         <v>923</v>
       </c>
-      <c r="I37" s="55"/>
+      <c r="I37" s="53"/>
       <c r="J37" s="32"/>
       <c r="K37" s="32" t="s">
         <v>1333</v>
@@ -5806,7 +5778,7 @@
       <c r="H38" s="29" t="s">
         <v>924</v>
       </c>
-      <c r="I38" s="55"/>
+      <c r="I38" s="53"/>
       <c r="J38" s="32"/>
       <c r="K38" s="32" t="s">
         <v>1333</v>
@@ -5841,7 +5813,7 @@
       <c r="H39" s="29" t="s">
         <v>925</v>
       </c>
-      <c r="I39" s="55"/>
+      <c r="I39" s="53"/>
       <c r="J39" s="32"/>
       <c r="K39" s="32" t="s">
         <v>1333</v>
@@ -5874,7 +5846,7 @@
       <c r="H40" s="29" t="s">
         <v>926</v>
       </c>
-      <c r="I40" s="55"/>
+      <c r="I40" s="53"/>
       <c r="J40" s="32"/>
       <c r="K40" s="32" t="s">
         <v>1334</v>
@@ -5909,7 +5881,7 @@
       <c r="H41" s="29" t="s">
         <v>927</v>
       </c>
-      <c r="I41" s="55"/>
+      <c r="I41" s="53"/>
       <c r="J41" s="32"/>
       <c r="K41" s="32" t="s">
         <v>1334</v>
@@ -5944,7 +5916,7 @@
       <c r="H42" s="29" t="s">
         <v>928</v>
       </c>
-      <c r="I42" s="55"/>
+      <c r="I42" s="53"/>
       <c r="J42" s="32"/>
       <c r="K42" s="32" t="s">
         <v>1334</v>
@@ -5979,7 +5951,7 @@
       <c r="H43" s="29" t="s">
         <v>929</v>
       </c>
-      <c r="I43" s="55"/>
+      <c r="I43" s="53"/>
       <c r="J43" s="32"/>
       <c r="K43" s="32" t="s">
         <v>1334</v>
@@ -6014,7 +5986,7 @@
       <c r="H44" s="29" t="s">
         <v>930</v>
       </c>
-      <c r="I44" s="55"/>
+      <c r="I44" s="53"/>
       <c r="J44" s="32"/>
       <c r="K44" s="32" t="s">
         <v>1334</v>
@@ -6047,7 +6019,7 @@
       <c r="H45" s="29" t="s">
         <v>931</v>
       </c>
-      <c r="I45" s="55"/>
+      <c r="I45" s="53"/>
       <c r="J45" s="32"/>
       <c r="K45" s="32" t="s">
         <v>1335</v>
@@ -6082,7 +6054,7 @@
       <c r="H46" s="29" t="s">
         <v>932</v>
       </c>
-      <c r="I46" s="55"/>
+      <c r="I46" s="53"/>
       <c r="J46" s="32"/>
       <c r="K46" s="32" t="s">
         <v>1335</v>
@@ -6117,7 +6089,7 @@
       <c r="H47" s="29" t="s">
         <v>933</v>
       </c>
-      <c r="I47" s="55"/>
+      <c r="I47" s="53"/>
       <c r="J47" s="32"/>
       <c r="K47" s="32" t="s">
         <v>1335</v>
@@ -6152,7 +6124,7 @@
       <c r="H48" s="29" t="s">
         <v>934</v>
       </c>
-      <c r="I48" s="55"/>
+      <c r="I48" s="53"/>
       <c r="J48" s="32"/>
       <c r="K48" s="32" t="s">
         <v>1335</v>
@@ -6187,7 +6159,7 @@
       <c r="H49" s="29" t="s">
         <v>935</v>
       </c>
-      <c r="I49" s="55"/>
+      <c r="I49" s="53"/>
       <c r="J49" s="32"/>
       <c r="K49" s="32" t="s">
         <v>1335</v>
@@ -6222,7 +6194,7 @@
       <c r="H50" s="29" t="s">
         <v>936</v>
       </c>
-      <c r="I50" s="55"/>
+      <c r="I50" s="53"/>
       <c r="J50" s="32"/>
       <c r="K50" s="32" t="s">
         <v>1335</v>
@@ -6257,7 +6229,7 @@
       <c r="H51" s="29" t="s">
         <v>937</v>
       </c>
-      <c r="I51" s="55"/>
+      <c r="I51" s="53"/>
       <c r="J51" s="32"/>
       <c r="K51" s="32" t="s">
         <v>1335</v>
@@ -6292,7 +6264,7 @@
       <c r="H52" s="29" t="s">
         <v>938</v>
       </c>
-      <c r="I52" s="55"/>
+      <c r="I52" s="53"/>
       <c r="J52" s="32"/>
       <c r="K52" s="32" t="s">
         <v>1335</v>
@@ -6327,7 +6299,7 @@
       <c r="H53" s="29" t="s">
         <v>939</v>
       </c>
-      <c r="I53" s="55"/>
+      <c r="I53" s="53"/>
       <c r="J53" s="32"/>
       <c r="K53" s="32" t="s">
         <v>1335</v>
@@ -6362,7 +6334,7 @@
       <c r="H54" s="29" t="s">
         <v>940</v>
       </c>
-      <c r="I54" s="55"/>
+      <c r="I54" s="53"/>
       <c r="J54" s="32"/>
       <c r="K54" s="32" t="s">
         <v>1335</v>
@@ -6397,7 +6369,7 @@
       <c r="H55" s="29" t="s">
         <v>941</v>
       </c>
-      <c r="I55" s="55"/>
+      <c r="I55" s="53"/>
       <c r="J55" s="32"/>
       <c r="K55" s="32" t="s">
         <v>1335</v>
@@ -6432,7 +6404,7 @@
       <c r="H56" s="29" t="s">
         <v>942</v>
       </c>
-      <c r="I56" s="55"/>
+      <c r="I56" s="53"/>
       <c r="J56" s="32"/>
       <c r="K56" s="32" t="s">
         <v>1335</v>
@@ -6467,7 +6439,7 @@
       <c r="H57" s="29" t="s">
         <v>943</v>
       </c>
-      <c r="I57" s="55"/>
+      <c r="I57" s="53"/>
       <c r="J57" s="32"/>
       <c r="K57" s="32" t="s">
         <v>1335</v>
@@ -6502,7 +6474,7 @@
       <c r="H58" s="29" t="s">
         <v>944</v>
       </c>
-      <c r="I58" s="55"/>
+      <c r="I58" s="53"/>
       <c r="J58" s="32"/>
       <c r="K58" s="32" t="s">
         <v>1335</v>
@@ -6537,7 +6509,7 @@
       <c r="H59" s="29" t="s">
         <v>945</v>
       </c>
-      <c r="I59" s="55"/>
+      <c r="I59" s="53"/>
       <c r="J59" s="32"/>
       <c r="K59" s="32" t="s">
         <v>1335</v>
@@ -6572,7 +6544,7 @@
       <c r="H60" s="29" t="s">
         <v>946</v>
       </c>
-      <c r="I60" s="55"/>
+      <c r="I60" s="53"/>
       <c r="J60" s="32"/>
       <c r="K60" s="32" t="s">
         <v>1335</v>
@@ -6607,7 +6579,7 @@
       <c r="H61" s="29" t="s">
         <v>947</v>
       </c>
-      <c r="I61" s="55"/>
+      <c r="I61" s="53"/>
       <c r="J61" s="32"/>
       <c r="K61" s="32" t="s">
         <v>1335</v>
@@ -6640,7 +6612,7 @@
       <c r="H62" s="29" t="s">
         <v>948</v>
       </c>
-      <c r="I62" s="55"/>
+      <c r="I62" s="53"/>
       <c r="J62" s="32"/>
       <c r="K62" s="32" t="s">
         <v>1336</v>
@@ -6675,7 +6647,7 @@
       <c r="H63" s="29" t="s">
         <v>949</v>
       </c>
-      <c r="I63" s="55"/>
+      <c r="I63" s="53"/>
       <c r="J63" s="32"/>
       <c r="K63" s="32" t="s">
         <v>1336</v>
@@ -6712,7 +6684,7 @@
       <c r="H64" s="29" t="s">
         <v>951</v>
       </c>
-      <c r="I64" s="55" t="s">
+      <c r="I64" s="53" t="s">
         <v>822</v>
       </c>
       <c r="J64" s="32"/>
@@ -6751,7 +6723,7 @@
       <c r="H65" s="29" t="s">
         <v>952</v>
       </c>
-      <c r="I65" s="55" t="s">
+      <c r="I65" s="53" t="s">
         <v>822</v>
       </c>
       <c r="J65" s="32"/>
@@ -6788,7 +6760,7 @@
       <c r="H66" s="29" t="s">
         <v>953</v>
       </c>
-      <c r="I66" s="55"/>
+      <c r="I66" s="53"/>
       <c r="J66" s="32"/>
       <c r="K66" s="32" t="s">
         <v>1336</v>
@@ -6823,7 +6795,7 @@
       <c r="H67" s="29" t="s">
         <v>954</v>
       </c>
-      <c r="I67" s="55"/>
+      <c r="I67" s="53"/>
       <c r="J67" s="32"/>
       <c r="K67" s="32" t="s">
         <v>1336</v>
@@ -6858,7 +6830,7 @@
       <c r="H68" s="29" t="s">
         <v>955</v>
       </c>
-      <c r="I68" s="55"/>
+      <c r="I68" s="53"/>
       <c r="J68" s="32"/>
       <c r="K68" s="32" t="s">
         <v>1336</v>
@@ -6891,7 +6863,7 @@
       <c r="H69" s="29" t="s">
         <v>956</v>
       </c>
-      <c r="I69" s="55"/>
+      <c r="I69" s="53"/>
       <c r="J69" s="32"/>
       <c r="K69" s="32" t="s">
         <v>1337</v>
@@ -6926,7 +6898,7 @@
       <c r="H70" s="29" t="s">
         <v>957</v>
       </c>
-      <c r="I70" s="55"/>
+      <c r="I70" s="53"/>
       <c r="J70" s="32"/>
       <c r="K70" s="32" t="s">
         <v>1337</v>
@@ -6961,7 +6933,7 @@
       <c r="H71" s="29" t="s">
         <v>958</v>
       </c>
-      <c r="I71" s="55"/>
+      <c r="I71" s="53"/>
       <c r="J71" s="32"/>
       <c r="K71" s="32" t="s">
         <v>1337</v>
@@ -6996,7 +6968,7 @@
       <c r="H72" s="29" t="s">
         <v>959</v>
       </c>
-      <c r="I72" s="55"/>
+      <c r="I72" s="53"/>
       <c r="J72" s="32"/>
       <c r="K72" s="32" t="s">
         <v>1337</v>
@@ -7033,7 +7005,7 @@
       <c r="H73" s="29" t="s">
         <v>960</v>
       </c>
-      <c r="I73" s="55"/>
+      <c r="I73" s="53"/>
       <c r="J73" s="32"/>
       <c r="K73" s="32" t="s">
         <v>1337</v>
@@ -7070,7 +7042,7 @@
       <c r="H74" s="29" t="s">
         <v>961</v>
       </c>
-      <c r="I74" s="55"/>
+      <c r="I74" s="53"/>
       <c r="J74" s="32"/>
       <c r="K74" s="32" t="s">
         <v>1337</v>
@@ -7105,7 +7077,7 @@
       <c r="H75" s="29" t="s">
         <v>962</v>
       </c>
-      <c r="I75" s="55"/>
+      <c r="I75" s="53"/>
       <c r="J75" s="32"/>
       <c r="K75" s="32" t="s">
         <v>1337</v>
@@ -7140,7 +7112,7 @@
       <c r="H76" s="29" t="s">
         <v>963</v>
       </c>
-      <c r="I76" s="55"/>
+      <c r="I76" s="53"/>
       <c r="J76" s="32"/>
       <c r="K76" s="32" t="s">
         <v>1337</v>
@@ -7177,7 +7149,7 @@
       <c r="H77" s="29" t="s">
         <v>964</v>
       </c>
-      <c r="I77" s="55"/>
+      <c r="I77" s="53"/>
       <c r="J77" s="32"/>
       <c r="K77" s="32" t="s">
         <v>1337</v>
@@ -7214,7 +7186,7 @@
       <c r="H78" s="29" t="s">
         <v>965</v>
       </c>
-      <c r="I78" s="55"/>
+      <c r="I78" s="53"/>
       <c r="J78" s="32"/>
       <c r="K78" s="32" t="s">
         <v>1337</v>
@@ -7249,7 +7221,7 @@
       <c r="H79" s="29" t="s">
         <v>966</v>
       </c>
-      <c r="I79" s="55"/>
+      <c r="I79" s="53"/>
       <c r="J79" s="32"/>
       <c r="K79" s="32" t="s">
         <v>1337</v>
@@ -7284,7 +7256,7 @@
       <c r="H80" s="29" t="s">
         <v>967</v>
       </c>
-      <c r="I80" s="55"/>
+      <c r="I80" s="53"/>
       <c r="J80" s="32"/>
       <c r="K80" s="32" t="s">
         <v>1337</v>
@@ -7319,7 +7291,7 @@
       <c r="H81" s="29" t="s">
         <v>968</v>
       </c>
-      <c r="I81" s="55"/>
+      <c r="I81" s="53"/>
       <c r="J81" s="32"/>
       <c r="K81" s="32" t="s">
         <v>1337</v>
@@ -7354,7 +7326,7 @@
       <c r="H82" s="29" t="s">
         <v>969</v>
       </c>
-      <c r="I82" s="55"/>
+      <c r="I82" s="53"/>
       <c r="J82" s="32"/>
       <c r="K82" s="32" t="s">
         <v>1337</v>
@@ -7389,7 +7361,7 @@
       <c r="H83" s="29" t="s">
         <v>970</v>
       </c>
-      <c r="I83" s="55"/>
+      <c r="I83" s="53"/>
       <c r="J83" s="32"/>
       <c r="K83" s="32" t="s">
         <v>1337</v>
@@ -7422,7 +7394,7 @@
       <c r="H84" s="29" t="s">
         <v>971</v>
       </c>
-      <c r="I84" s="55"/>
+      <c r="I84" s="53"/>
       <c r="J84" s="32"/>
       <c r="K84" s="32" t="s">
         <v>1338</v>
@@ -7457,7 +7429,7 @@
       <c r="H85" s="29" t="s">
         <v>972</v>
       </c>
-      <c r="I85" s="55"/>
+      <c r="I85" s="53"/>
       <c r="J85" s="32"/>
       <c r="K85" s="32" t="s">
         <v>1338</v>
@@ -7494,7 +7466,7 @@
       <c r="H86" s="29" t="s">
         <v>974</v>
       </c>
-      <c r="I86" s="55" t="s">
+      <c r="I86" s="53" t="s">
         <v>845</v>
       </c>
       <c r="J86" s="32"/>
@@ -7533,7 +7505,7 @@
       <c r="H87" s="29" t="s">
         <v>975</v>
       </c>
-      <c r="I87" s="55" t="s">
+      <c r="I87" s="53" t="s">
         <v>845</v>
       </c>
       <c r="J87" s="32"/>
@@ -7570,7 +7542,7 @@
       <c r="H88" s="29" t="s">
         <v>976</v>
       </c>
-      <c r="I88" s="55"/>
+      <c r="I88" s="53"/>
       <c r="J88" s="32"/>
       <c r="K88" s="32" t="s">
         <v>1338</v>
@@ -7605,7 +7577,7 @@
       <c r="H89" s="29" t="s">
         <v>977</v>
       </c>
-      <c r="I89" s="55"/>
+      <c r="I89" s="53"/>
       <c r="J89" s="32"/>
       <c r="K89" s="32" t="s">
         <v>1338</v>
@@ -7640,7 +7612,7 @@
       <c r="H90" s="29" t="s">
         <v>978</v>
       </c>
-      <c r="I90" s="55"/>
+      <c r="I90" s="53"/>
       <c r="J90" s="32"/>
       <c r="K90" s="32" t="s">
         <v>1338</v>
@@ -7675,7 +7647,7 @@
       <c r="H91" s="29" t="s">
         <v>979</v>
       </c>
-      <c r="I91" s="55"/>
+      <c r="I91" s="53"/>
       <c r="J91" s="32"/>
       <c r="K91" s="32" t="s">
         <v>1338</v>
@@ -7712,7 +7684,7 @@
       <c r="H92" s="29" t="s">
         <v>980</v>
       </c>
-      <c r="I92" s="55"/>
+      <c r="I92" s="53"/>
       <c r="J92" s="32"/>
       <c r="K92" s="32" t="s">
         <v>1338</v>
@@ -7749,7 +7721,7 @@
       <c r="H93" s="29" t="s">
         <v>981</v>
       </c>
-      <c r="I93" s="55"/>
+      <c r="I93" s="53"/>
       <c r="J93" s="32"/>
       <c r="K93" s="32" t="s">
         <v>1338</v>
@@ -7784,7 +7756,7 @@
       <c r="H94" s="29" t="s">
         <v>982</v>
       </c>
-      <c r="I94" s="55"/>
+      <c r="I94" s="53"/>
       <c r="J94" s="32"/>
       <c r="K94" s="32" t="s">
         <v>1338</v>
@@ -7899,7 +7871,7 @@
       <c r="H97" s="29" t="s">
         <v>986</v>
       </c>
-      <c r="I97" s="55"/>
+      <c r="I97" s="53"/>
       <c r="J97" s="32"/>
       <c r="K97" s="32" t="s">
         <v>1338</v>
@@ -7934,7 +7906,7 @@
       <c r="H98" s="29" t="s">
         <v>987</v>
       </c>
-      <c r="I98" s="55"/>
+      <c r="I98" s="53"/>
       <c r="J98" s="32"/>
       <c r="K98" s="32" t="s">
         <v>1338</v>
@@ -7971,7 +7943,7 @@
       <c r="H99" s="29" t="s">
         <v>988</v>
       </c>
-      <c r="I99" s="55"/>
+      <c r="I99" s="53"/>
       <c r="J99" s="32"/>
       <c r="K99" s="32" t="s">
         <v>1338</v>
@@ -8008,7 +7980,7 @@
       <c r="H100" s="29" t="s">
         <v>989</v>
       </c>
-      <c r="I100" s="55"/>
+      <c r="I100" s="53"/>
       <c r="J100" s="32"/>
       <c r="K100" s="32" t="s">
         <v>1338</v>
@@ -8045,7 +8017,7 @@
       <c r="H101" s="29" t="s">
         <v>990</v>
       </c>
-      <c r="I101" s="55"/>
+      <c r="I101" s="53"/>
       <c r="J101" s="32"/>
       <c r="K101" s="32" t="s">
         <v>1338</v>
@@ -8082,7 +8054,7 @@
       <c r="H102" s="29" t="s">
         <v>991</v>
       </c>
-      <c r="I102" s="55"/>
+      <c r="I102" s="53"/>
       <c r="J102" s="32"/>
       <c r="K102" s="32" t="s">
         <v>1338</v>
@@ -8119,7 +8091,7 @@
       <c r="H103" s="29" t="s">
         <v>992</v>
       </c>
-      <c r="I103" s="55"/>
+      <c r="I103" s="53"/>
       <c r="J103" s="32"/>
       <c r="K103" s="32" t="s">
         <v>1338</v>
@@ -8156,7 +8128,7 @@
       <c r="H104" s="29" t="s">
         <v>993</v>
       </c>
-      <c r="I104" s="55"/>
+      <c r="I104" s="53"/>
       <c r="J104" s="32"/>
       <c r="K104" s="32" t="s">
         <v>1338</v>
@@ -8193,7 +8165,7 @@
       <c r="H105" s="29" t="s">
         <v>994</v>
       </c>
-      <c r="I105" s="55"/>
+      <c r="I105" s="53"/>
       <c r="J105" s="32"/>
       <c r="K105" s="32" t="s">
         <v>1338</v>
@@ -8230,7 +8202,7 @@
       <c r="H106" s="29" t="s">
         <v>995</v>
       </c>
-      <c r="I106" s="55"/>
+      <c r="I106" s="53"/>
       <c r="J106" s="32"/>
       <c r="K106" s="32" t="s">
         <v>1338</v>
@@ -8343,7 +8315,7 @@
       <c r="H109" s="29" t="s">
         <v>999</v>
       </c>
-      <c r="I109" s="55"/>
+      <c r="I109" s="53"/>
       <c r="J109" s="32"/>
       <c r="K109" s="32" t="s">
         <v>1338</v>
@@ -8380,7 +8352,7 @@
       <c r="H110" s="29" t="s">
         <v>1000</v>
       </c>
-      <c r="I110" s="55"/>
+      <c r="I110" s="53"/>
       <c r="J110" s="32"/>
       <c r="K110" s="32" t="s">
         <v>1338</v>
@@ -8417,7 +8389,7 @@
       <c r="H111" s="29" t="s">
         <v>1001</v>
       </c>
-      <c r="I111" s="55"/>
+      <c r="I111" s="53"/>
       <c r="J111" s="32"/>
       <c r="K111" s="32" t="s">
         <v>1338</v>
@@ -8454,7 +8426,7 @@
       <c r="H112" s="29" t="s">
         <v>1002</v>
       </c>
-      <c r="I112" s="55"/>
+      <c r="I112" s="53"/>
       <c r="J112" s="32"/>
       <c r="K112" s="32" t="s">
         <v>1338</v>
@@ -8491,7 +8463,7 @@
       <c r="H113" s="29" t="s">
         <v>1003</v>
       </c>
-      <c r="I113" s="55"/>
+      <c r="I113" s="53"/>
       <c r="J113" s="29"/>
       <c r="K113" s="32" t="s">
         <v>1338</v>
@@ -8528,7 +8500,7 @@
       <c r="H114" s="29" t="s">
         <v>1004</v>
       </c>
-      <c r="I114" s="55"/>
+      <c r="I114" s="53"/>
       <c r="J114" s="32"/>
       <c r="K114" s="32" t="s">
         <v>1338</v>
@@ -8561,7 +8533,7 @@
       <c r="H115" s="29" t="s">
         <v>1005</v>
       </c>
-      <c r="I115" s="55"/>
+      <c r="I115" s="53"/>
       <c r="J115" s="32"/>
       <c r="K115" s="32" t="s">
         <v>1339</v>
@@ -8596,7 +8568,7 @@
       <c r="H116" s="29" t="s">
         <v>1006</v>
       </c>
-      <c r="I116" s="55"/>
+      <c r="I116" s="53"/>
       <c r="J116" s="32"/>
       <c r="K116" s="32" t="s">
         <v>1339</v>
@@ -8631,7 +8603,7 @@
       <c r="H117" s="29" t="s">
         <v>1007</v>
       </c>
-      <c r="I117" s="55"/>
+      <c r="I117" s="53"/>
       <c r="J117" s="32"/>
       <c r="K117" s="32" t="s">
         <v>1339</v>
@@ -8664,7 +8636,7 @@
       <c r="H118" s="29" t="s">
         <v>1008</v>
       </c>
-      <c r="I118" s="55"/>
+      <c r="I118" s="53"/>
       <c r="J118" s="32"/>
       <c r="K118" s="32" t="s">
         <v>1340</v>
@@ -8699,7 +8671,7 @@
       <c r="H119" s="29" t="s">
         <v>1009</v>
       </c>
-      <c r="I119" s="55"/>
+      <c r="I119" s="53"/>
       <c r="J119" s="32"/>
       <c r="K119" s="32" t="s">
         <v>1340</v>
@@ -8736,7 +8708,7 @@
       <c r="H120" s="29" t="s">
         <v>1010</v>
       </c>
-      <c r="I120" s="55"/>
+      <c r="I120" s="53"/>
       <c r="J120" s="32"/>
       <c r="K120" s="32" t="s">
         <v>1340</v>
@@ -8773,7 +8745,7 @@
       <c r="H121" s="29" t="s">
         <v>1011</v>
       </c>
-      <c r="I121" s="55"/>
+      <c r="I121" s="53"/>
       <c r="J121" s="32"/>
       <c r="K121" s="32" t="s">
         <v>1340</v>
@@ -8810,7 +8782,7 @@
       <c r="H122" s="29" t="s">
         <v>1012</v>
       </c>
-      <c r="I122" s="55"/>
+      <c r="I122" s="53"/>
       <c r="J122" s="32"/>
       <c r="K122" s="32" t="s">
         <v>1340</v>
@@ -8847,7 +8819,7 @@
       <c r="H123" s="29" t="s">
         <v>1013</v>
       </c>
-      <c r="I123" s="55"/>
+      <c r="I123" s="53"/>
       <c r="J123" s="32"/>
       <c r="K123" s="32" t="s">
         <v>1340</v>
@@ -8882,7 +8854,7 @@
       <c r="H124" s="29" t="s">
         <v>1014</v>
       </c>
-      <c r="I124" s="55"/>
+      <c r="I124" s="53"/>
       <c r="J124" s="32"/>
       <c r="K124" s="32" t="s">
         <v>1340</v>
@@ -8919,7 +8891,7 @@
       <c r="H125" s="29" t="s">
         <v>1015</v>
       </c>
-      <c r="I125" s="55"/>
+      <c r="I125" s="53"/>
       <c r="J125" s="32"/>
       <c r="K125" s="32" t="s">
         <v>1340</v>
@@ -8956,7 +8928,7 @@
       <c r="H126" s="29" t="s">
         <v>1016</v>
       </c>
-      <c r="I126" s="55"/>
+      <c r="I126" s="53"/>
       <c r="J126" s="32"/>
       <c r="K126" s="32" t="s">
         <v>1340</v>
@@ -8991,7 +8963,7 @@
       <c r="H127" s="29" t="s">
         <v>1017</v>
       </c>
-      <c r="I127" s="55"/>
+      <c r="I127" s="53"/>
       <c r="J127" s="32"/>
       <c r="K127" s="32" t="s">
         <v>1340</v>
@@ -9028,7 +9000,7 @@
       <c r="H128" s="29" t="s">
         <v>1018</v>
       </c>
-      <c r="I128" s="55"/>
+      <c r="I128" s="53"/>
       <c r="J128" s="32"/>
       <c r="K128" s="32" t="s">
         <v>1340</v>
@@ -9141,7 +9113,7 @@
       <c r="H131" s="29" t="s">
         <v>1022</v>
       </c>
-      <c r="I131" s="55"/>
+      <c r="I131" s="53"/>
       <c r="J131" s="32"/>
       <c r="K131" s="32" t="s">
         <v>1340</v>
@@ -9176,7 +9148,7 @@
       <c r="H132" s="29" t="s">
         <v>1023</v>
       </c>
-      <c r="I132" s="55"/>
+      <c r="I132" s="53"/>
       <c r="J132" s="32"/>
       <c r="K132" s="32" t="s">
         <v>1340</v>
@@ -9213,7 +9185,7 @@
       <c r="H133" s="29" t="s">
         <v>1024</v>
       </c>
-      <c r="I133" s="55"/>
+      <c r="I133" s="53"/>
       <c r="J133" s="32"/>
       <c r="K133" s="32" t="s">
         <v>1340</v>
@@ -9250,7 +9222,7 @@
       <c r="H134" s="29" t="s">
         <v>1025</v>
       </c>
-      <c r="I134" s="55"/>
+      <c r="I134" s="53"/>
       <c r="J134" s="32"/>
       <c r="K134" s="32" t="s">
         <v>1340</v>
@@ -9285,7 +9257,7 @@
       <c r="H135" s="29" t="s">
         <v>1026</v>
       </c>
-      <c r="I135" s="55"/>
+      <c r="I135" s="53"/>
       <c r="J135" s="32"/>
       <c r="K135" s="32" t="s">
         <v>1340</v>
@@ -9320,7 +9292,7 @@
       <c r="H136" s="29" t="s">
         <v>1027</v>
       </c>
-      <c r="I136" s="55"/>
+      <c r="I136" s="53"/>
       <c r="J136" s="32"/>
       <c r="K136" s="32" t="s">
         <v>1340</v>
@@ -9355,7 +9327,7 @@
       <c r="H137" s="29" t="s">
         <v>1028</v>
       </c>
-      <c r="I137" s="55"/>
+      <c r="I137" s="53"/>
       <c r="J137" s="32"/>
       <c r="K137" s="32" t="s">
         <v>1340</v>
@@ -9390,7 +9362,7 @@
       <c r="H138" s="29" t="s">
         <v>1029</v>
       </c>
-      <c r="I138" s="55"/>
+      <c r="I138" s="53"/>
       <c r="J138" s="32"/>
       <c r="K138" s="32" t="s">
         <v>1340</v>
@@ -9425,7 +9397,7 @@
       <c r="H139" s="29" t="s">
         <v>1030</v>
       </c>
-      <c r="I139" s="55"/>
+      <c r="I139" s="53"/>
       <c r="J139" s="32"/>
       <c r="K139" s="32" t="s">
         <v>1340</v>
@@ -9460,7 +9432,7 @@
       <c r="H140" s="29" t="s">
         <v>1031</v>
       </c>
-      <c r="I140" s="55"/>
+      <c r="I140" s="53"/>
       <c r="J140" s="32"/>
       <c r="K140" s="32" t="s">
         <v>1340</v>
@@ -9497,7 +9469,7 @@
       <c r="H141" s="29" t="s">
         <v>1032</v>
       </c>
-      <c r="I141" s="55"/>
+      <c r="I141" s="53"/>
       <c r="J141" s="32"/>
       <c r="K141" s="32" t="s">
         <v>1340</v>
@@ -9534,7 +9506,7 @@
       <c r="H142" s="29" t="s">
         <v>1033</v>
       </c>
-      <c r="I142" s="55"/>
+      <c r="I142" s="53"/>
       <c r="J142" s="32"/>
       <c r="K142" s="32" t="s">
         <v>1340</v>
@@ -9571,7 +9543,7 @@
       <c r="H143" s="29" t="s">
         <v>1034</v>
       </c>
-      <c r="I143" s="55"/>
+      <c r="I143" s="53"/>
       <c r="J143" s="32"/>
       <c r="K143" s="32" t="s">
         <v>1340</v>
@@ -9608,7 +9580,7 @@
       <c r="H144" s="29" t="s">
         <v>1035</v>
       </c>
-      <c r="I144" s="55"/>
+      <c r="I144" s="53"/>
       <c r="J144" s="32"/>
       <c r="K144" s="32" t="s">
         <v>1340</v>
@@ -9645,7 +9617,7 @@
       <c r="H145" s="29" t="s">
         <v>1036</v>
       </c>
-      <c r="I145" s="55"/>
+      <c r="I145" s="53"/>
       <c r="J145" s="32"/>
       <c r="K145" s="32" t="s">
         <v>1340</v>
@@ -9682,7 +9654,7 @@
       <c r="H146" s="29" t="s">
         <v>1037</v>
       </c>
-      <c r="I146" s="55"/>
+      <c r="I146" s="53"/>
       <c r="J146" s="32"/>
       <c r="K146" s="32" t="s">
         <v>1340</v>
@@ -9719,7 +9691,7 @@
       <c r="H147" s="29" t="s">
         <v>1038</v>
       </c>
-      <c r="I147" s="55"/>
+      <c r="I147" s="53"/>
       <c r="J147" s="32"/>
       <c r="K147" s="32" t="s">
         <v>1340</v>
@@ -9756,7 +9728,7 @@
       <c r="H148" s="29" t="s">
         <v>1039</v>
       </c>
-      <c r="I148" s="55"/>
+      <c r="I148" s="53"/>
       <c r="J148" s="32"/>
       <c r="K148" s="32" t="s">
         <v>1340</v>
@@ -9793,7 +9765,7 @@
       <c r="H149" s="29" t="s">
         <v>1040</v>
       </c>
-      <c r="I149" s="55"/>
+      <c r="I149" s="53"/>
       <c r="J149" s="32"/>
       <c r="K149" s="32" t="s">
         <v>1340</v>
@@ -9830,7 +9802,7 @@
       <c r="H150" s="29" t="s">
         <v>1041</v>
       </c>
-      <c r="I150" s="55"/>
+      <c r="I150" s="53"/>
       <c r="J150" s="32"/>
       <c r="K150" s="32" t="s">
         <v>1340</v>
@@ -9865,7 +9837,7 @@
       <c r="H151" s="29" t="s">
         <v>1042</v>
       </c>
-      <c r="I151" s="55"/>
+      <c r="I151" s="53"/>
       <c r="J151" s="32"/>
       <c r="K151" s="32" t="s">
         <v>1340</v>
@@ -9902,7 +9874,7 @@
       <c r="H152" s="29" t="s">
         <v>1043</v>
       </c>
-      <c r="I152" s="55"/>
+      <c r="I152" s="53"/>
       <c r="J152" s="32"/>
       <c r="K152" s="32" t="s">
         <v>1340</v>
@@ -9939,7 +9911,7 @@
       <c r="H153" s="29" t="s">
         <v>1044</v>
       </c>
-      <c r="I153" s="55"/>
+      <c r="I153" s="53"/>
       <c r="J153" s="32"/>
       <c r="K153" s="32" t="s">
         <v>1340</v>
@@ -9974,7 +9946,7 @@
       <c r="H154" s="29" t="s">
         <v>1045</v>
       </c>
-      <c r="I154" s="55"/>
+      <c r="I154" s="53"/>
       <c r="J154" s="32"/>
       <c r="K154" s="32" t="s">
         <v>1340</v>
@@ -10011,7 +9983,7 @@
       <c r="H155" s="29" t="s">
         <v>1046</v>
       </c>
-      <c r="I155" s="55"/>
+      <c r="I155" s="53"/>
       <c r="J155" s="32"/>
       <c r="K155" s="32" t="s">
         <v>1340</v>
@@ -10048,7 +10020,7 @@
       <c r="H156" s="29" t="s">
         <v>1047</v>
       </c>
-      <c r="I156" s="55"/>
+      <c r="I156" s="53"/>
       <c r="J156" s="32"/>
       <c r="K156" s="32" t="s">
         <v>1340</v>
@@ -10085,7 +10057,7 @@
       <c r="H157" s="29" t="s">
         <v>1048</v>
       </c>
-      <c r="I157" s="55"/>
+      <c r="I157" s="53"/>
       <c r="J157" s="32"/>
       <c r="K157" s="32" t="s">
         <v>1340</v>
@@ -10118,7 +10090,7 @@
       <c r="H158" s="27" t="s">
         <v>509</v>
       </c>
-      <c r="I158" s="56"/>
+      <c r="I158" s="54"/>
       <c r="J158" s="32"/>
       <c r="K158" s="32" t="s">
         <v>1341</v>
@@ -10153,7 +10125,7 @@
       <c r="H159" s="27" t="s">
         <v>510</v>
       </c>
-      <c r="I159" s="56"/>
+      <c r="I159" s="54"/>
       <c r="J159" s="32"/>
       <c r="K159" s="32" t="s">
         <v>1341</v>
@@ -10188,7 +10160,7 @@
       <c r="H160" s="27" t="s">
         <v>511</v>
       </c>
-      <c r="I160" s="56"/>
+      <c r="I160" s="54"/>
       <c r="J160" s="32"/>
       <c r="K160" s="32" t="s">
         <v>1341</v>
@@ -10223,7 +10195,7 @@
       <c r="H161" s="27" t="s">
         <v>512</v>
       </c>
-      <c r="I161" s="56"/>
+      <c r="I161" s="54"/>
       <c r="J161" s="32"/>
       <c r="K161" s="32" t="s">
         <v>1341</v>
@@ -10260,7 +10232,7 @@
       <c r="H162" s="27" t="s">
         <v>513</v>
       </c>
-      <c r="I162" s="56"/>
+      <c r="I162" s="54"/>
       <c r="J162" s="32"/>
       <c r="K162" s="32" t="s">
         <v>1341</v>
@@ -10297,7 +10269,7 @@
       <c r="H163" s="27" t="s">
         <v>514</v>
       </c>
-      <c r="I163" s="56"/>
+      <c r="I163" s="54"/>
       <c r="J163" s="32"/>
       <c r="K163" s="32" t="s">
         <v>1341</v>
@@ -10334,7 +10306,7 @@
       <c r="H164" s="27" t="s">
         <v>515</v>
       </c>
-      <c r="I164" s="56"/>
+      <c r="I164" s="54"/>
       <c r="J164" s="32"/>
       <c r="K164" s="32" t="s">
         <v>1341</v>
@@ -10371,7 +10343,7 @@
       <c r="H165" s="27" t="s">
         <v>516</v>
       </c>
-      <c r="I165" s="56"/>
+      <c r="I165" s="54"/>
       <c r="J165" s="32"/>
       <c r="K165" s="32" t="s">
         <v>1341</v>
@@ -10406,7 +10378,7 @@
       <c r="H166" s="27" t="s">
         <v>517</v>
       </c>
-      <c r="I166" s="56"/>
+      <c r="I166" s="54"/>
       <c r="J166" s="32"/>
       <c r="K166" s="32" t="s">
         <v>1341</v>
@@ -10441,7 +10413,7 @@
       <c r="H167" s="27" t="s">
         <v>518</v>
       </c>
-      <c r="I167" s="56"/>
+      <c r="I167" s="54"/>
       <c r="J167" s="32"/>
       <c r="K167" s="32" t="s">
         <v>1341</v>
@@ -10474,7 +10446,7 @@
       <c r="H168" s="27" t="s">
         <v>633</v>
       </c>
-      <c r="I168" s="56"/>
+      <c r="I168" s="54"/>
       <c r="J168" s="32"/>
       <c r="K168" s="32" t="s">
         <v>1342</v>
@@ -10509,7 +10481,7 @@
       <c r="H169" s="27" t="s">
         <v>519</v>
       </c>
-      <c r="I169" s="56"/>
+      <c r="I169" s="54"/>
       <c r="J169" s="32"/>
       <c r="K169" s="32" t="s">
         <v>1342</v>
@@ -10544,7 +10516,7 @@
       <c r="H170" s="27" t="s">
         <v>520</v>
       </c>
-      <c r="I170" s="56"/>
+      <c r="I170" s="54"/>
       <c r="J170" s="32"/>
       <c r="K170" s="32" t="s">
         <v>1342</v>
@@ -10577,7 +10549,7 @@
       <c r="H171" s="27" t="s">
         <v>521</v>
       </c>
-      <c r="I171" s="56"/>
+      <c r="I171" s="54"/>
       <c r="J171" s="32"/>
       <c r="K171" s="32" t="s">
         <v>1343</v>
@@ -10612,7 +10584,7 @@
       <c r="H172" s="27" t="s">
         <v>522</v>
       </c>
-      <c r="I172" s="56"/>
+      <c r="I172" s="54"/>
       <c r="J172" s="32"/>
       <c r="K172" s="32" t="s">
         <v>1343</v>
@@ -10647,7 +10619,7 @@
       <c r="H173" t="s">
         <v>523</v>
       </c>
-      <c r="I173" s="57"/>
+      <c r="I173" s="55"/>
       <c r="J173" s="12"/>
       <c r="K173" s="32" t="s">
         <v>1343</v>
@@ -10682,7 +10654,7 @@
       <c r="H174" s="27" t="s">
         <v>524</v>
       </c>
-      <c r="I174" s="56"/>
+      <c r="I174" s="54"/>
       <c r="J174" s="32"/>
       <c r="K174" s="32" t="s">
         <v>1343</v>
@@ -10717,7 +10689,7 @@
       <c r="H175" t="s">
         <v>525</v>
       </c>
-      <c r="I175" s="57"/>
+      <c r="I175" s="55"/>
       <c r="J175" s="12"/>
       <c r="K175" s="32" t="s">
         <v>1343</v>
@@ -10752,7 +10724,7 @@
       <c r="H176" s="27" t="s">
         <v>526</v>
       </c>
-      <c r="I176" s="56"/>
+      <c r="I176" s="54"/>
       <c r="J176" s="32"/>
       <c r="K176" s="32" t="s">
         <v>1343</v>
@@ -10787,7 +10759,7 @@
       <c r="H177" s="27" t="s">
         <v>527</v>
       </c>
-      <c r="I177" s="56"/>
+      <c r="I177" s="54"/>
       <c r="J177" s="32"/>
       <c r="K177" s="32" t="s">
         <v>1343</v>
@@ -10820,7 +10792,7 @@
       <c r="H178" s="27" t="s">
         <v>528</v>
       </c>
-      <c r="I178" s="56"/>
+      <c r="I178" s="54"/>
       <c r="J178" s="32"/>
       <c r="K178" s="32" t="s">
         <v>1344</v>
@@ -10855,7 +10827,7 @@
       <c r="H179" s="27" t="s">
         <v>529</v>
       </c>
-      <c r="I179" s="56"/>
+      <c r="I179" s="54"/>
       <c r="J179" s="32"/>
       <c r="K179" s="32" t="s">
         <v>1344</v>
@@ -10890,7 +10862,7 @@
       <c r="H180" s="27" t="s">
         <v>530</v>
       </c>
-      <c r="I180" s="56"/>
+      <c r="I180" s="54"/>
       <c r="J180" s="32"/>
       <c r="K180" s="32" t="s">
         <v>1344</v>
@@ -10925,7 +10897,7 @@
       <c r="H181" s="27" t="s">
         <v>531</v>
       </c>
-      <c r="I181" s="56"/>
+      <c r="I181" s="54"/>
       <c r="J181" s="32"/>
       <c r="K181" s="32" t="s">
         <v>1344</v>
@@ -10960,7 +10932,7 @@
       <c r="H182" s="27" t="s">
         <v>532</v>
       </c>
-      <c r="I182" s="56"/>
+      <c r="I182" s="54"/>
       <c r="J182" s="32"/>
       <c r="K182" s="32" t="s">
         <v>1344</v>
@@ -10997,7 +10969,7 @@
       <c r="H183" s="27" t="s">
         <v>533</v>
       </c>
-      <c r="I183" s="56"/>
+      <c r="I183" s="54"/>
       <c r="J183" s="32"/>
       <c r="K183" s="32" t="s">
         <v>1344</v>
@@ -11034,7 +11006,7 @@
       <c r="H184" s="27" t="s">
         <v>534</v>
       </c>
-      <c r="I184" s="56"/>
+      <c r="I184" s="54"/>
       <c r="J184" s="32"/>
       <c r="K184" s="32" t="s">
         <v>1344</v>
@@ -11067,7 +11039,7 @@
       <c r="H185" s="27" t="s">
         <v>535</v>
       </c>
-      <c r="I185" s="56"/>
+      <c r="I185" s="54"/>
       <c r="J185" s="32"/>
       <c r="K185" s="32" t="s">
         <v>1345</v>
@@ -11102,7 +11074,7 @@
       <c r="H186" s="27" t="s">
         <v>536</v>
       </c>
-      <c r="I186" s="56"/>
+      <c r="I186" s="54"/>
       <c r="J186" s="32"/>
       <c r="K186" s="32" t="s">
         <v>1345</v>
@@ -11137,7 +11109,7 @@
       <c r="H187" s="27" t="s">
         <v>537</v>
       </c>
-      <c r="I187" s="56"/>
+      <c r="I187" s="54"/>
       <c r="J187" s="32"/>
       <c r="K187" s="32" t="s">
         <v>1345</v>
@@ -11172,7 +11144,7 @@
       <c r="H188" s="27" t="s">
         <v>538</v>
       </c>
-      <c r="I188" s="56"/>
+      <c r="I188" s="54"/>
       <c r="J188" s="32"/>
       <c r="K188" s="32" t="s">
         <v>1345</v>
@@ -11207,7 +11179,7 @@
       <c r="H189" s="27" t="s">
         <v>539</v>
       </c>
-      <c r="I189" s="56"/>
+      <c r="I189" s="54"/>
       <c r="J189" s="32"/>
       <c r="K189" s="32" t="s">
         <v>1345</v>
@@ -11242,7 +11214,7 @@
       <c r="H190" s="27" t="s">
         <v>540</v>
       </c>
-      <c r="I190" s="56"/>
+      <c r="I190" s="54"/>
       <c r="J190" s="32"/>
       <c r="K190" s="32" t="s">
         <v>1345</v>
@@ -11277,7 +11249,7 @@
       <c r="H191" s="27" t="s">
         <v>541</v>
       </c>
-      <c r="I191" s="56"/>
+      <c r="I191" s="54"/>
       <c r="J191" s="32"/>
       <c r="K191" s="32" t="s">
         <v>1345</v>
@@ -11312,7 +11284,7 @@
       <c r="H192" s="27" t="s">
         <v>542</v>
       </c>
-      <c r="I192" s="56"/>
+      <c r="I192" s="54"/>
       <c r="J192" s="32"/>
       <c r="K192" s="32" t="s">
         <v>1345</v>
@@ -11347,7 +11319,7 @@
       <c r="H193" s="27" t="s">
         <v>543</v>
       </c>
-      <c r="I193" s="56"/>
+      <c r="I193" s="54"/>
       <c r="J193" s="32"/>
       <c r="K193" s="32" t="s">
         <v>1345</v>
@@ -11382,7 +11354,7 @@
       <c r="H194" s="27" t="s">
         <v>544</v>
       </c>
-      <c r="I194" s="56"/>
+      <c r="I194" s="54"/>
       <c r="J194" s="32"/>
       <c r="K194" s="32" t="s">
         <v>1345</v>
@@ -11495,7 +11467,7 @@
       <c r="H197" s="27" t="s">
         <v>548</v>
       </c>
-      <c r="I197" s="56"/>
+      <c r="I197" s="54"/>
       <c r="J197" s="32"/>
       <c r="K197" s="32" t="s">
         <v>1345</v>
@@ -11530,7 +11502,7 @@
       <c r="H198" s="27" t="s">
         <v>549</v>
       </c>
-      <c r="I198" s="56"/>
+      <c r="I198" s="54"/>
       <c r="J198" s="32"/>
       <c r="K198" s="32" t="s">
         <v>1345</v>
@@ -11565,7 +11537,7 @@
       <c r="H199" s="27" t="s">
         <v>550</v>
       </c>
-      <c r="I199" s="56"/>
+      <c r="I199" s="54"/>
       <c r="J199" s="32"/>
       <c r="K199" s="32" t="s">
         <v>1345</v>
@@ -11600,7 +11572,7 @@
       <c r="H200" s="27" t="s">
         <v>551</v>
       </c>
-      <c r="I200" s="56"/>
+      <c r="I200" s="54"/>
       <c r="J200" s="32"/>
       <c r="K200" s="32" t="s">
         <v>1345</v>
@@ -11635,7 +11607,7 @@
       <c r="H201" s="27" t="s">
         <v>552</v>
       </c>
-      <c r="I201" s="56"/>
+      <c r="I201" s="54"/>
       <c r="J201" s="32"/>
       <c r="K201" s="32" t="s">
         <v>1345</v>
@@ -11748,7 +11720,7 @@
       <c r="H204" s="27" t="s">
         <v>556</v>
       </c>
-      <c r="I204" s="56"/>
+      <c r="I204" s="54"/>
       <c r="J204" s="32"/>
       <c r="K204" s="32" t="s">
         <v>1345</v>
@@ -11861,7 +11833,7 @@
       <c r="H207" s="27" t="s">
         <v>560</v>
       </c>
-      <c r="I207" s="56"/>
+      <c r="I207" s="54"/>
       <c r="J207" s="32"/>
       <c r="K207" s="32" t="s">
         <v>1345</v>
@@ -11894,7 +11866,7 @@
       <c r="H208" s="27" t="s">
         <v>561</v>
       </c>
-      <c r="I208" s="56"/>
+      <c r="I208" s="54"/>
       <c r="J208" s="32"/>
       <c r="K208" s="32" t="s">
         <v>1346</v>
@@ -11929,7 +11901,7 @@
       <c r="H209" s="27" t="s">
         <v>562</v>
       </c>
-      <c r="I209" s="56"/>
+      <c r="I209" s="54"/>
       <c r="J209" s="32"/>
       <c r="K209" s="32" t="s">
         <v>1346</v>
@@ -11964,7 +11936,7 @@
       <c r="H210" s="27" t="s">
         <v>563</v>
       </c>
-      <c r="I210" s="56"/>
+      <c r="I210" s="54"/>
       <c r="J210" s="32"/>
       <c r="K210" s="32" t="s">
         <v>1346</v>
@@ -11999,7 +11971,7 @@
       <c r="H211" s="27" t="s">
         <v>564</v>
       </c>
-      <c r="I211" s="56"/>
+      <c r="I211" s="54"/>
       <c r="J211" s="32"/>
       <c r="K211" s="32" t="s">
         <v>1346</v>
@@ -12034,7 +12006,7 @@
       <c r="H212" s="27" t="s">
         <v>565</v>
       </c>
-      <c r="I212" s="56"/>
+      <c r="I212" s="54"/>
       <c r="J212" s="32"/>
       <c r="K212" s="32" t="s">
         <v>1346</v>
@@ -12069,7 +12041,7 @@
       <c r="H213" s="27" t="s">
         <v>566</v>
       </c>
-      <c r="I213" s="56"/>
+      <c r="I213" s="54"/>
       <c r="J213" s="32"/>
       <c r="K213" s="32" t="s">
         <v>1346</v>
@@ -12104,7 +12076,7 @@
       <c r="H214" s="27" t="s">
         <v>567</v>
       </c>
-      <c r="I214" s="56"/>
+      <c r="I214" s="54"/>
       <c r="J214" s="32"/>
       <c r="K214" s="32" t="s">
         <v>1346</v>
@@ -12139,7 +12111,7 @@
       <c r="H215" s="27" t="s">
         <v>568</v>
       </c>
-      <c r="I215" s="56"/>
+      <c r="I215" s="54"/>
       <c r="J215" s="32"/>
       <c r="K215" s="32" t="s">
         <v>1346</v>
@@ -12174,7 +12146,7 @@
       <c r="H216" s="27" t="s">
         <v>569</v>
       </c>
-      <c r="I216" s="56"/>
+      <c r="I216" s="54"/>
       <c r="J216" s="32"/>
       <c r="K216" s="32" t="s">
         <v>1346</v>
@@ -12209,7 +12181,7 @@
       <c r="H217" s="27" t="s">
         <v>570</v>
       </c>
-      <c r="I217" s="56"/>
+      <c r="I217" s="54"/>
       <c r="J217" s="32"/>
       <c r="K217" s="32" t="s">
         <v>1346</v>
@@ -12244,7 +12216,7 @@
       <c r="H218" s="27" t="s">
         <v>571</v>
       </c>
-      <c r="I218" s="56"/>
+      <c r="I218" s="54"/>
       <c r="J218" s="32"/>
       <c r="K218" s="32" t="s">
         <v>1346</v>
@@ -12279,7 +12251,7 @@
       <c r="H219" s="27" t="s">
         <v>572</v>
       </c>
-      <c r="I219" s="56"/>
+      <c r="I219" s="54"/>
       <c r="J219" s="32"/>
       <c r="K219" s="32" t="s">
         <v>1346</v>
@@ -12314,7 +12286,7 @@
       <c r="H220" s="27" t="s">
         <v>573</v>
       </c>
-      <c r="I220" s="56"/>
+      <c r="I220" s="54"/>
       <c r="J220" s="32"/>
       <c r="K220" s="32" t="s">
         <v>1346</v>
@@ -12349,7 +12321,7 @@
       <c r="H221" s="27" t="s">
         <v>574</v>
       </c>
-      <c r="I221" s="56"/>
+      <c r="I221" s="54"/>
       <c r="J221" s="32"/>
       <c r="K221" s="32" t="s">
         <v>1346</v>
@@ -12384,7 +12356,7 @@
       <c r="H222" s="27" t="s">
         <v>575</v>
       </c>
-      <c r="I222" s="56"/>
+      <c r="I222" s="54"/>
       <c r="J222" s="32"/>
       <c r="K222" s="32" t="s">
         <v>1346</v>
@@ -12419,7 +12391,7 @@
       <c r="H223" s="27" t="s">
         <v>576</v>
       </c>
-      <c r="I223" s="56"/>
+      <c r="I223" s="54"/>
       <c r="J223" s="32"/>
       <c r="K223" s="32" t="s">
         <v>1346</v>
@@ -12454,7 +12426,7 @@
       <c r="H224" s="27" t="s">
         <v>577</v>
       </c>
-      <c r="I224" s="56"/>
+      <c r="I224" s="54"/>
       <c r="J224" s="32"/>
       <c r="K224" s="32" t="s">
         <v>1346</v>
@@ -12489,7 +12461,7 @@
       <c r="H225" s="27" t="s">
         <v>578</v>
       </c>
-      <c r="I225" s="56"/>
+      <c r="I225" s="54"/>
       <c r="J225" s="32"/>
       <c r="K225" s="32" t="s">
         <v>1346</v>
@@ -12524,7 +12496,7 @@
       <c r="H226" s="27" t="s">
         <v>579</v>
       </c>
-      <c r="I226" s="56"/>
+      <c r="I226" s="54"/>
       <c r="J226" s="32"/>
       <c r="K226" s="32" t="s">
         <v>1346</v>
@@ -12559,7 +12531,7 @@
       <c r="H227" s="27" t="s">
         <v>580</v>
       </c>
-      <c r="I227" s="56"/>
+      <c r="I227" s="54"/>
       <c r="J227" s="32"/>
       <c r="K227" s="32" t="s">
         <v>1346</v>
@@ -12594,7 +12566,7 @@
       <c r="H228" s="27" t="s">
         <v>581</v>
       </c>
-      <c r="I228" s="56"/>
+      <c r="I228" s="54"/>
       <c r="J228" s="32"/>
       <c r="K228" s="32" t="s">
         <v>1346</v>
@@ -12629,7 +12601,7 @@
       <c r="H229" s="27" t="s">
         <v>582</v>
       </c>
-      <c r="I229" s="56"/>
+      <c r="I229" s="54"/>
       <c r="J229" s="32"/>
       <c r="K229" s="32" t="s">
         <v>1346</v>
@@ -12664,7 +12636,7 @@
       <c r="H230" s="27" t="s">
         <v>583</v>
       </c>
-      <c r="I230" s="56"/>
+      <c r="I230" s="54"/>
       <c r="J230" s="32"/>
       <c r="K230" s="32" t="s">
         <v>1346</v>
@@ -12699,7 +12671,7 @@
       <c r="H231" s="27" t="s">
         <v>584</v>
       </c>
-      <c r="I231" s="56"/>
+      <c r="I231" s="54"/>
       <c r="J231" s="32"/>
       <c r="K231" s="32" t="s">
         <v>1346</v>
@@ -12734,7 +12706,7 @@
       <c r="H232" s="27" t="s">
         <v>585</v>
       </c>
-      <c r="I232" s="56"/>
+      <c r="I232" s="54"/>
       <c r="J232" s="32"/>
       <c r="K232" s="32" t="s">
         <v>1346</v>
@@ -12769,7 +12741,7 @@
       <c r="H233" s="27" t="s">
         <v>586</v>
       </c>
-      <c r="I233" s="56"/>
+      <c r="I233" s="54"/>
       <c r="J233" s="32"/>
       <c r="K233" s="32" t="s">
         <v>1346</v>
@@ -12804,7 +12776,7 @@
       <c r="H234" s="27" t="s">
         <v>587</v>
       </c>
-      <c r="I234" s="56"/>
+      <c r="I234" s="54"/>
       <c r="J234" s="32"/>
       <c r="K234" s="32" t="s">
         <v>1346</v>
@@ -12839,7 +12811,7 @@
       <c r="H235" s="27" t="s">
         <v>588</v>
       </c>
-      <c r="I235" s="56"/>
+      <c r="I235" s="54"/>
       <c r="J235" s="32"/>
       <c r="K235" s="32" t="s">
         <v>1346</v>
@@ -12874,7 +12846,7 @@
       <c r="H236" s="27" t="s">
         <v>589</v>
       </c>
-      <c r="I236" s="56"/>
+      <c r="I236" s="54"/>
       <c r="J236" s="32"/>
       <c r="K236" s="32" t="s">
         <v>1346</v>
@@ -12909,7 +12881,7 @@
       <c r="H237" s="27" t="s">
         <v>590</v>
       </c>
-      <c r="I237" s="56"/>
+      <c r="I237" s="54"/>
       <c r="J237" s="32"/>
       <c r="K237" s="32" t="s">
         <v>1346</v>
@@ -12942,7 +12914,7 @@
       <c r="H238" s="27" t="s">
         <v>591</v>
       </c>
-      <c r="I238" s="56"/>
+      <c r="I238" s="54"/>
       <c r="J238" s="32"/>
       <c r="K238" s="32" t="s">
         <v>1347</v>
@@ -12977,7 +12949,7 @@
       <c r="H239" s="27" t="s">
         <v>592</v>
       </c>
-      <c r="I239" s="56"/>
+      <c r="I239" s="54"/>
       <c r="J239" s="32"/>
       <c r="K239" s="32" t="s">
         <v>1347</v>
@@ -13012,7 +12984,7 @@
       <c r="H240" s="27" t="s">
         <v>593</v>
       </c>
-      <c r="I240" s="56"/>
+      <c r="I240" s="54"/>
       <c r="J240" s="32"/>
       <c r="K240" s="32" t="s">
         <v>1347</v>
@@ -13047,7 +13019,7 @@
       <c r="H241" s="27" t="s">
         <v>594</v>
       </c>
-      <c r="I241" s="56"/>
+      <c r="I241" s="54"/>
       <c r="J241" s="32"/>
       <c r="K241" s="32" t="s">
         <v>1347</v>
@@ -13082,7 +13054,7 @@
       <c r="H242" s="27" t="s">
         <v>595</v>
       </c>
-      <c r="I242" s="56"/>
+      <c r="I242" s="54"/>
       <c r="J242" s="32"/>
       <c r="K242" s="32" t="s">
         <v>1347</v>
@@ -13115,7 +13087,7 @@
       <c r="H243" s="27" t="s">
         <v>596</v>
       </c>
-      <c r="I243" s="56"/>
+      <c r="I243" s="54"/>
       <c r="J243" s="32"/>
       <c r="K243" s="32" t="s">
         <v>1348</v>
@@ -13150,7 +13122,7 @@
       <c r="H244" s="27" t="s">
         <v>597</v>
       </c>
-      <c r="I244" s="56"/>
+      <c r="I244" s="54"/>
       <c r="J244" s="32"/>
       <c r="K244" s="32" t="s">
         <v>1348</v>
@@ -13185,7 +13157,7 @@
       <c r="H245" s="27" t="s">
         <v>598</v>
       </c>
-      <c r="I245" s="56"/>
+      <c r="I245" s="54"/>
       <c r="J245" s="32"/>
       <c r="K245" s="32" t="s">
         <v>1348</v>
@@ -13220,7 +13192,7 @@
       <c r="H246" s="32" t="s">
         <v>599</v>
       </c>
-      <c r="I246" s="56"/>
+      <c r="I246" s="54"/>
       <c r="J246" s="32"/>
       <c r="K246" s="32" t="s">
         <v>1348</v>
@@ -13255,7 +13227,7 @@
       <c r="H247" s="32" t="s">
         <v>600</v>
       </c>
-      <c r="I247" s="56"/>
+      <c r="I247" s="54"/>
       <c r="J247" s="32"/>
       <c r="K247" s="32" t="s">
         <v>1348</v>
@@ -13290,7 +13262,7 @@
       <c r="H248" s="32" t="s">
         <v>601</v>
       </c>
-      <c r="I248" s="56"/>
+      <c r="I248" s="54"/>
       <c r="J248" s="32"/>
       <c r="K248" s="32" t="s">
         <v>1348</v>
@@ -13323,7 +13295,7 @@
       <c r="H249" s="32" t="s">
         <v>602</v>
       </c>
-      <c r="I249" s="56"/>
+      <c r="I249" s="54"/>
       <c r="J249" s="32"/>
       <c r="K249" s="32" t="s">
         <v>1349</v>
@@ -13358,7 +13330,7 @@
       <c r="H250" s="32" t="s">
         <v>603</v>
       </c>
-      <c r="I250" s="56"/>
+      <c r="I250" s="54"/>
       <c r="J250" s="32"/>
       <c r="K250" s="32" t="s">
         <v>1349</v>
@@ -13393,7 +13365,7 @@
       <c r="H251" s="32" t="s">
         <v>604</v>
       </c>
-      <c r="I251" s="56"/>
+      <c r="I251" s="54"/>
       <c r="J251" s="32"/>
       <c r="K251" s="32" t="s">
         <v>1349</v>
@@ -13428,7 +13400,7 @@
       <c r="H252" s="32" t="s">
         <v>605</v>
       </c>
-      <c r="I252" s="56"/>
+      <c r="I252" s="54"/>
       <c r="J252" s="32"/>
       <c r="K252" s="32" t="s">
         <v>1349</v>
@@ -13463,7 +13435,7 @@
       <c r="H253" s="32" t="s">
         <v>606</v>
       </c>
-      <c r="I253" s="56"/>
+      <c r="I253" s="54"/>
       <c r="J253" s="32"/>
       <c r="K253" s="32" t="s">
         <v>1349</v>
@@ -13498,7 +13470,7 @@
       <c r="H254" s="32" t="s">
         <v>607</v>
       </c>
-      <c r="I254" s="56"/>
+      <c r="I254" s="54"/>
       <c r="J254" s="32"/>
       <c r="K254" s="32" t="s">
         <v>1349</v>
@@ -13533,7 +13505,7 @@
       <c r="H255" s="32" t="s">
         <v>608</v>
       </c>
-      <c r="I255" s="56"/>
+      <c r="I255" s="54"/>
       <c r="J255" s="32"/>
       <c r="K255" s="32" t="s">
         <v>1349</v>
@@ -13570,7 +13542,7 @@
       <c r="H256" s="32" t="s">
         <v>609</v>
       </c>
-      <c r="I256" s="56"/>
+      <c r="I256" s="54"/>
       <c r="J256" s="32"/>
       <c r="K256" s="32" t="s">
         <v>1349</v>
@@ -13607,7 +13579,7 @@
       <c r="H257" s="32" t="s">
         <v>610</v>
       </c>
-      <c r="I257" s="56"/>
+      <c r="I257" s="54"/>
       <c r="J257" s="32"/>
       <c r="K257" s="32" t="s">
         <v>1349</v>
@@ -13642,7 +13614,7 @@
       <c r="H258" s="32" t="s">
         <v>611</v>
       </c>
-      <c r="I258" s="56"/>
+      <c r="I258" s="54"/>
       <c r="J258" s="32"/>
       <c r="K258" s="32" t="s">
         <v>1349</v>
@@ -13675,7 +13647,7 @@
       <c r="H259" s="32" t="s">
         <v>612</v>
       </c>
-      <c r="I259" s="56"/>
+      <c r="I259" s="54"/>
       <c r="J259" s="32"/>
       <c r="K259" s="32" t="s">
         <v>1350</v>
@@ -13710,7 +13682,7 @@
       <c r="H260" s="32" t="s">
         <v>613</v>
       </c>
-      <c r="I260" s="56"/>
+      <c r="I260" s="54"/>
       <c r="J260" s="32"/>
       <c r="K260" s="32" t="s">
         <v>1350</v>
@@ -13745,7 +13717,7 @@
       <c r="H261" s="32" t="s">
         <v>614</v>
       </c>
-      <c r="I261" s="56"/>
+      <c r="I261" s="54"/>
       <c r="J261" s="32"/>
       <c r="K261" s="32" t="s">
         <v>1350</v>
@@ -13782,7 +13754,7 @@
       <c r="H262" s="32" t="s">
         <v>615</v>
       </c>
-      <c r="I262" s="56"/>
+      <c r="I262" s="54"/>
       <c r="J262" s="32"/>
       <c r="K262" s="32" t="s">
         <v>1350</v>
@@ -13819,7 +13791,7 @@
       <c r="H263" s="32" t="s">
         <v>616</v>
       </c>
-      <c r="I263" s="56"/>
+      <c r="I263" s="54"/>
       <c r="J263" s="32"/>
       <c r="K263" s="32" t="s">
         <v>1350</v>
@@ -13854,7 +13826,7 @@
       <c r="H264" s="32" t="s">
         <v>617</v>
       </c>
-      <c r="I264" s="56"/>
+      <c r="I264" s="54"/>
       <c r="J264" s="32"/>
       <c r="K264" s="32" t="s">
         <v>1350</v>
@@ -13889,7 +13861,7 @@
       <c r="H265" s="32" t="s">
         <v>618</v>
       </c>
-      <c r="I265" s="56"/>
+      <c r="I265" s="54"/>
       <c r="J265" s="32"/>
       <c r="K265" s="32" t="s">
         <v>1350</v>
@@ -13922,7 +13894,7 @@
       <c r="H266" s="32" t="s">
         <v>619</v>
       </c>
-      <c r="I266" s="56"/>
+      <c r="I266" s="54"/>
       <c r="J266" s="32"/>
       <c r="K266" s="32" t="s">
         <v>1351</v>
@@ -13957,7 +13929,7 @@
       <c r="H267" s="32" t="s">
         <v>620</v>
       </c>
-      <c r="I267" s="56"/>
+      <c r="I267" s="54"/>
       <c r="J267" s="32"/>
       <c r="K267" s="32" t="s">
         <v>1351</v>
@@ -13992,7 +13964,7 @@
       <c r="H268" s="32" t="s">
         <v>621</v>
       </c>
-      <c r="I268" s="56"/>
+      <c r="I268" s="54"/>
       <c r="J268" s="32"/>
       <c r="K268" s="32" t="s">
         <v>1351</v>
@@ -14027,7 +13999,7 @@
       <c r="H269" s="32" t="s">
         <v>622</v>
       </c>
-      <c r="I269" s="56"/>
+      <c r="I269" s="54"/>
       <c r="J269" s="32"/>
       <c r="K269" s="32" t="s">
         <v>1351</v>
@@ -14062,7 +14034,7 @@
       <c r="H270" s="32" t="s">
         <v>623</v>
       </c>
-      <c r="I270" s="56"/>
+      <c r="I270" s="54"/>
       <c r="J270" s="32"/>
       <c r="K270" s="32" t="s">
         <v>1351</v>
@@ -14097,7 +14069,7 @@
       <c r="H271" s="32" t="s">
         <v>624</v>
       </c>
-      <c r="I271" s="56"/>
+      <c r="I271" s="54"/>
       <c r="J271" s="32"/>
       <c r="K271" s="32" t="s">
         <v>1351</v>
@@ -14132,7 +14104,7 @@
       <c r="H272" s="32" t="s">
         <v>625</v>
       </c>
-      <c r="I272" s="56"/>
+      <c r="I272" s="54"/>
       <c r="J272" s="32"/>
       <c r="K272" s="32" t="s">
         <v>1351</v>
@@ -14167,7 +14139,7 @@
       <c r="H273" s="32" t="s">
         <v>626</v>
       </c>
-      <c r="I273" s="56"/>
+      <c r="I273" s="54"/>
       <c r="J273" s="32"/>
       <c r="K273" s="32" t="s">
         <v>1351</v>
@@ -14202,7 +14174,7 @@
       <c r="H274" s="32" t="s">
         <v>627</v>
       </c>
-      <c r="I274" s="56"/>
+      <c r="I274" s="54"/>
       <c r="J274" s="32"/>
       <c r="K274" s="32" t="s">
         <v>1351</v>
@@ -14237,7 +14209,7 @@
       <c r="H275" s="32" t="s">
         <v>628</v>
       </c>
-      <c r="I275" s="56"/>
+      <c r="I275" s="54"/>
       <c r="J275" s="32"/>
       <c r="K275" s="32" t="s">
         <v>1351</v>
@@ -14272,7 +14244,7 @@
       <c r="H276" s="32" t="s">
         <v>629</v>
       </c>
-      <c r="I276" s="56"/>
+      <c r="I276" s="54"/>
       <c r="J276" s="32"/>
       <c r="K276" s="32" t="s">
         <v>1351</v>
@@ -14307,7 +14279,7 @@
       <c r="H277" s="32" t="s">
         <v>630</v>
       </c>
-      <c r="I277" s="56"/>
+      <c r="I277" s="54"/>
       <c r="J277" s="32"/>
       <c r="K277" s="32" t="s">
         <v>1351</v>
@@ -14342,7 +14314,7 @@
       <c r="H278" s="32" t="s">
         <v>631</v>
       </c>
-      <c r="I278" s="56"/>
+      <c r="I278" s="54"/>
       <c r="J278" s="32"/>
       <c r="K278" s="32" t="s">
         <v>1351</v>
@@ -14355,109 +14327,109 @@
       </c>
     </row>
     <row r="279" spans="1:13" s="4" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="I279" s="58"/>
+      <c r="I279" s="56"/>
       <c r="J279" s="16"/>
       <c r="K279" s="16"/>
       <c r="L279" s="16"/>
     </row>
     <row r="280" spans="1:13" s="4" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="I280" s="58"/>
+      <c r="I280" s="56"/>
       <c r="J280" s="16"/>
       <c r="K280" s="16"/>
       <c r="L280" s="16"/>
     </row>
     <row r="281" spans="1:13" s="4" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="I281" s="58"/>
+      <c r="I281" s="56"/>
       <c r="J281" s="16"/>
       <c r="K281" s="16"/>
       <c r="L281" s="16"/>
     </row>
     <row r="282" spans="1:13" s="4" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="I282" s="58"/>
+      <c r="I282" s="56"/>
       <c r="J282" s="16"/>
       <c r="K282" s="16"/>
       <c r="L282" s="16"/>
     </row>
     <row r="283" spans="1:13" s="4" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="I283" s="58"/>
+      <c r="I283" s="56"/>
       <c r="J283" s="16"/>
       <c r="K283" s="16"/>
       <c r="L283" s="16"/>
     </row>
     <row r="284" spans="1:13" s="4" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="I284" s="58"/>
+      <c r="I284" s="56"/>
       <c r="J284" s="16"/>
       <c r="K284" s="16"/>
       <c r="L284" s="16"/>
     </row>
     <row r="285" spans="1:13" s="4" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="I285" s="58"/>
+      <c r="I285" s="56"/>
       <c r="J285" s="16"/>
       <c r="K285" s="16"/>
       <c r="L285" s="16"/>
     </row>
     <row r="286" spans="1:13" s="4" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="I286" s="58"/>
+      <c r="I286" s="56"/>
       <c r="J286" s="16"/>
       <c r="K286" s="16"/>
       <c r="L286" s="16"/>
     </row>
     <row r="287" spans="1:13" s="4" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="I287" s="58"/>
+      <c r="I287" s="56"/>
       <c r="J287" s="16"/>
       <c r="K287" s="16"/>
       <c r="L287" s="16"/>
     </row>
     <row r="288" spans="1:13" s="4" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="I288" s="58"/>
+      <c r="I288" s="56"/>
       <c r="J288" s="16"/>
       <c r="K288" s="16"/>
       <c r="L288" s="16"/>
     </row>
     <row r="289" spans="9:12" s="4" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="I289" s="58"/>
+      <c r="I289" s="56"/>
       <c r="J289" s="16"/>
       <c r="K289" s="16"/>
       <c r="L289" s="16"/>
     </row>
     <row r="290" spans="9:12" s="4" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="I290" s="58"/>
+      <c r="I290" s="56"/>
       <c r="J290" s="16"/>
       <c r="K290" s="16"/>
       <c r="L290" s="16"/>
     </row>
     <row r="291" spans="9:12" s="4" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="I291" s="58"/>
+      <c r="I291" s="56"/>
       <c r="J291" s="16"/>
       <c r="K291" s="16"/>
       <c r="L291" s="16"/>
     </row>
     <row r="292" spans="9:12" s="4" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="I292" s="58"/>
+      <c r="I292" s="56"/>
       <c r="J292" s="16"/>
       <c r="K292" s="16"/>
       <c r="L292" s="16"/>
     </row>
     <row r="293" spans="9:12" s="4" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="I293" s="58"/>
+      <c r="I293" s="56"/>
       <c r="J293" s="16"/>
       <c r="K293" s="16"/>
       <c r="L293" s="16"/>
     </row>
     <row r="294" spans="9:12" s="4" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="I294" s="58"/>
+      <c r="I294" s="56"/>
       <c r="J294" s="16"/>
       <c r="K294" s="16"/>
       <c r="L294" s="16"/>
     </row>
     <row r="295" spans="9:12" s="4" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="I295" s="58"/>
+      <c r="I295" s="56"/>
       <c r="J295" s="16"/>
       <c r="K295" s="16"/>
       <c r="L295" s="16"/>
     </row>
     <row r="296" spans="9:12" s="4" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="I296" s="58"/>
+      <c r="I296" s="56"/>
       <c r="J296" s="16"/>
       <c r="K296" s="16"/>
       <c r="L296" s="16"/>
@@ -14466,14 +14438,14 @@
       <c r="B322" s="16"/>
       <c r="E322" s="16"/>
       <c r="G322" s="16"/>
-      <c r="I322" s="51"/>
+      <c r="I322" s="49"/>
     </row>
     <row r="348" spans="5:5" x14ac:dyDescent="0.25">
       <c r="E348" s="11"/>
     </row>
     <row r="444" spans="2:12" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B444" s="4"/>
-      <c r="I444" s="57"/>
+      <c r="I444" s="55"/>
       <c r="J444" s="12"/>
       <c r="K444" s="12"/>
       <c r="L444" s="12"/>
@@ -14484,21 +14456,21 @@
     <row r="450" spans="1:12" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A450" s="12"/>
       <c r="B450" s="4"/>
-      <c r="I450" s="57"/>
+      <c r="I450" s="55"/>
       <c r="J450" s="12"/>
       <c r="K450" s="12"/>
       <c r="L450" s="12"/>
     </row>
     <row r="454" spans="1:12" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B454" s="4"/>
-      <c r="I454" s="57"/>
+      <c r="I454" s="55"/>
       <c r="J454" s="12"/>
       <c r="K454" s="12"/>
       <c r="L454" s="12"/>
     </row>
     <row r="467" spans="1:12" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B467" s="4"/>
-      <c r="I467" s="57"/>
+      <c r="I467" s="55"/>
       <c r="J467" s="12"/>
       <c r="K467" s="12"/>
       <c r="L467" s="12"/>
@@ -14510,9 +14482,9 @@
       <c r="E478" s="5"/>
       <c r="G478" s="10"/>
       <c r="H478" s="2"/>
-      <c r="I478" s="59"/>
-      <c r="J478" s="47"/>
-      <c r="K478" s="47"/>
+      <c r="I478" s="57"/>
+      <c r="J478" s="45"/>
+      <c r="K478" s="45"/>
     </row>
   </sheetData>
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A34:M478">
@@ -14897,10 +14869,12 @@
     <hyperlink ref="L278" r:id="rId376" display="https://raw.githack.com/ANZSoilData/def-au-scma/master/html/00frontmatter/00WARNING.html" xr:uid="{00677D20-EC96-4609-AFE2-9D7EE399F72C}"/>
     <hyperlink ref="B18" r:id="rId377" xr:uid="{31571278-A517-460E-AA8B-2538A10AD1BA}"/>
     <hyperlink ref="B19" r:id="rId378" xr:uid="{386259F1-8A48-45EF-9526-D7EE660E59A8}"/>
+    <hyperlink ref="B21" r:id="rId379" xr:uid="{EE8E9D4B-625A-4996-B8E2-8A7D08DA3A45}"/>
+    <hyperlink ref="B27" r:id="rId380" xr:uid="{5C3E9EEF-EDCD-4317-84C5-348730CA5D31}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId379"/>
-  <legacyDrawing r:id="rId380"/>
+  <pageSetup orientation="portrait" r:id="rId381"/>
+  <legacyDrawing r:id="rId382"/>
 </worksheet>
 </file>
 
@@ -14908,8 +14882,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4A25E589-C762-47F7-A5B5-46A66BE90C97}">
   <dimension ref="A1:M467"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A20" sqref="A20"/>
+    <sheetView topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="B20" sqref="B20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -14941,7 +14915,7 @@
       <c r="F1" s="3"/>
       <c r="G1" s="4"/>
       <c r="H1" s="1"/>
-      <c r="I1" s="43"/>
+      <c r="I1" s="41"/>
       <c r="J1" s="15"/>
       <c r="K1" s="15"/>
       <c r="L1" s="3"/>
@@ -14961,7 +14935,7 @@
       <c r="F2" s="3"/>
       <c r="G2" s="4"/>
       <c r="H2" s="1"/>
-      <c r="I2" s="43"/>
+      <c r="I2" s="41"/>
       <c r="J2" s="15"/>
       <c r="K2" s="15"/>
       <c r="L2" s="3"/>
@@ -14981,7 +14955,7 @@
       <c r="F3" s="3"/>
       <c r="G3" s="4"/>
       <c r="H3" s="1"/>
-      <c r="I3" s="43"/>
+      <c r="I3" s="41"/>
       <c r="J3" s="15"/>
       <c r="K3" s="15"/>
       <c r="L3" s="3"/>
@@ -14993,7 +14967,7 @@
       <c r="B4" s="14" t="s">
         <v>646</v>
       </c>
-      <c r="C4" s="8" t="s">
+      <c r="C4" s="18" t="s">
         <v>647</v>
       </c>
       <c r="D4" s="8"/>
@@ -15001,7 +14975,7 @@
       <c r="F4" s="3"/>
       <c r="G4" s="4"/>
       <c r="H4" s="1"/>
-      <c r="I4" s="43"/>
+      <c r="I4" s="41"/>
       <c r="J4" s="15"/>
       <c r="K4" s="15"/>
       <c r="L4" s="3"/>
@@ -15021,7 +14995,7 @@
       <c r="F5" s="3"/>
       <c r="G5" s="4"/>
       <c r="H5" s="1"/>
-      <c r="I5" s="43"/>
+      <c r="I5" s="41"/>
       <c r="J5" s="15"/>
       <c r="K5" s="15"/>
       <c r="L5" s="3"/>
@@ -15030,7 +15004,7 @@
       <c r="A6" s="1" t="s">
         <v>640</v>
       </c>
-      <c r="B6" s="49" t="s">
+      <c r="B6" s="47" t="s">
         <v>1062</v>
       </c>
       <c r="C6" s="4"/>
@@ -15039,7 +15013,7 @@
       <c r="F6" s="3"/>
       <c r="G6" s="4"/>
       <c r="H6" s="1"/>
-      <c r="I6" s="43"/>
+      <c r="I6" s="41"/>
       <c r="J6" s="15"/>
       <c r="K6" s="15"/>
       <c r="L6" s="3"/>
@@ -15057,7 +15031,7 @@
       <c r="F7" s="3"/>
       <c r="G7" s="4"/>
       <c r="H7" s="1"/>
-      <c r="I7" s="43"/>
+      <c r="I7" s="41"/>
       <c r="J7" s="15"/>
       <c r="K7" s="15"/>
       <c r="L7" s="3"/>
@@ -15075,7 +15049,7 @@
       <c r="F8" s="3"/>
       <c r="G8" s="4"/>
       <c r="H8" s="1"/>
-      <c r="I8" s="43"/>
+      <c r="I8" s="41"/>
       <c r="J8" s="15"/>
       <c r="K8" s="15"/>
       <c r="L8" s="3"/>
@@ -15084,7 +15058,7 @@
       <c r="A9" s="1" t="s">
         <v>642</v>
       </c>
-      <c r="B9" s="41">
+      <c r="B9" s="39">
         <v>44624</v>
       </c>
       <c r="C9" s="4"/>
@@ -15093,7 +15067,7 @@
       <c r="F9" s="3"/>
       <c r="G9" s="4"/>
       <c r="H9" s="1"/>
-      <c r="I9" s="43"/>
+      <c r="I9" s="41"/>
       <c r="J9" s="15"/>
       <c r="K9" s="15"/>
       <c r="L9" s="3"/>
@@ -15102,7 +15076,7 @@
       <c r="A10" s="1" t="s">
         <v>643</v>
       </c>
-      <c r="B10" s="41">
+      <c r="B10" s="39">
         <v>44629</v>
       </c>
       <c r="C10" s="4"/>
@@ -15111,7 +15085,7 @@
       <c r="F10" s="3"/>
       <c r="G10" s="4"/>
       <c r="H10" s="1"/>
-      <c r="I10" s="43"/>
+      <c r="I10" s="41"/>
       <c r="J10" s="15"/>
       <c r="K10" s="15"/>
       <c r="L10" s="3"/>
@@ -15120,7 +15094,7 @@
       <c r="A11" s="1" t="s">
         <v>1360</v>
       </c>
-      <c r="B11" s="41" t="s">
+      <c r="B11" s="39" t="s">
         <v>1330</v>
       </c>
       <c r="C11" s="4"/>
@@ -15129,7 +15103,7 @@
       <c r="F11" s="3"/>
       <c r="G11" s="4"/>
       <c r="H11" s="1"/>
-      <c r="I11" s="43"/>
+      <c r="I11" s="41"/>
       <c r="J11" s="15"/>
       <c r="K11" s="15"/>
       <c r="L11" s="3"/>
@@ -15138,7 +15112,7 @@
       <c r="A12" s="1" t="s">
         <v>1361</v>
       </c>
-      <c r="B12" s="63" t="s">
+      <c r="B12" s="61" t="s">
         <v>1332</v>
       </c>
       <c r="C12" s="4"/>
@@ -15147,7 +15121,7 @@
       <c r="F12" s="3"/>
       <c r="G12" s="4"/>
       <c r="H12" s="1"/>
-      <c r="I12" s="43"/>
+      <c r="I12" s="41"/>
       <c r="J12" s="15"/>
       <c r="K12" s="15"/>
       <c r="L12" s="3"/>
@@ -15156,7 +15130,7 @@
       <c r="A13" s="1" t="s">
         <v>1362</v>
       </c>
-      <c r="B13" s="62" t="s">
+      <c r="B13" s="60" t="s">
         <v>1329</v>
       </c>
       <c r="C13" s="4"/>
@@ -15165,7 +15139,7 @@
       <c r="F13" s="3"/>
       <c r="G13" s="4"/>
       <c r="H13" s="1"/>
-      <c r="I13" s="43"/>
+      <c r="I13" s="41"/>
       <c r="J13" s="15"/>
       <c r="K13" s="15"/>
       <c r="L13" s="3"/>
@@ -15174,7 +15148,7 @@
       <c r="A14" s="1" t="s">
         <v>1320</v>
       </c>
-      <c r="B14" s="41" t="s">
+      <c r="B14" s="39" t="s">
         <v>1327</v>
       </c>
       <c r="C14" s="4"/>
@@ -15183,7 +15157,7 @@
       <c r="F14" s="3"/>
       <c r="G14" s="4"/>
       <c r="H14" s="1"/>
-      <c r="I14" s="43"/>
+      <c r="I14" s="41"/>
       <c r="J14" s="15"/>
       <c r="K14" s="15"/>
       <c r="L14" s="3"/>
@@ -15192,7 +15166,7 @@
       <c r="A15" s="1" t="s">
         <v>1320</v>
       </c>
-      <c r="B15" s="41" t="s">
+      <c r="B15" s="39" t="s">
         <v>1328</v>
       </c>
       <c r="C15" s="4"/>
@@ -15201,7 +15175,7 @@
       <c r="F15" s="3"/>
       <c r="G15" s="4"/>
       <c r="H15" s="1"/>
-      <c r="I15" s="43"/>
+      <c r="I15" s="41"/>
       <c r="J15" s="15"/>
       <c r="K15" s="15"/>
       <c r="L15" s="3"/>
@@ -15210,7 +15184,7 @@
       <c r="A16" s="1" t="s">
         <v>644</v>
       </c>
-      <c r="B16" s="37" t="s">
+      <c r="B16" s="65" t="s">
         <v>634</v>
       </c>
       <c r="C16" s="4"/>
@@ -15219,7 +15193,7 @@
       <c r="F16" s="3"/>
       <c r="G16" s="4"/>
       <c r="H16" s="1"/>
-      <c r="I16" s="43"/>
+      <c r="I16" s="41"/>
       <c r="J16" s="15"/>
       <c r="K16" s="15"/>
       <c r="L16" s="3"/>
@@ -15228,7 +15202,7 @@
       <c r="A17" s="1" t="s">
         <v>644</v>
       </c>
-      <c r="B17" s="38" t="s">
+      <c r="B17" s="37" t="s">
         <v>635</v>
       </c>
       <c r="C17" s="4"/>
@@ -15237,7 +15211,7 @@
       <c r="F17" s="3"/>
       <c r="G17" s="4"/>
       <c r="H17" s="1"/>
-      <c r="I17" s="43"/>
+      <c r="I17" s="41"/>
       <c r="J17" s="15"/>
       <c r="K17" s="15"/>
       <c r="L17" s="3"/>
@@ -15246,7 +15220,7 @@
       <c r="A18" s="1" t="s">
         <v>645</v>
       </c>
-      <c r="B18" s="38" t="s">
+      <c r="B18" s="37" t="s">
         <v>636</v>
       </c>
       <c r="C18" s="4"/>
@@ -15255,7 +15229,7 @@
       <c r="F18" s="3"/>
       <c r="G18" s="4"/>
       <c r="H18" s="1"/>
-      <c r="I18" s="43"/>
+      <c r="I18" s="41"/>
       <c r="J18" s="15"/>
       <c r="K18" s="15"/>
       <c r="L18" s="3"/>
@@ -15264,7 +15238,7 @@
       <c r="A19" s="1" t="s">
         <v>639</v>
       </c>
-      <c r="B19" s="38" t="s">
+      <c r="B19" s="37" t="s">
         <v>1369</v>
       </c>
       <c r="C19" s="4"/>
@@ -15273,7 +15247,7 @@
       <c r="F19" s="3"/>
       <c r="G19" s="4"/>
       <c r="H19" s="1"/>
-      <c r="I19" s="43"/>
+      <c r="I19" s="41"/>
       <c r="J19" s="15"/>
       <c r="K19" s="15"/>
       <c r="L19" s="3"/>
@@ -15291,7 +15265,7 @@
       <c r="F20" s="3"/>
       <c r="G20" s="4"/>
       <c r="H20" s="1"/>
-      <c r="I20" s="43"/>
+      <c r="I20" s="41"/>
       <c r="J20" s="15"/>
       <c r="K20" s="15"/>
       <c r="L20" s="3"/>
@@ -15309,7 +15283,7 @@
       <c r="F21" s="3"/>
       <c r="G21" s="4"/>
       <c r="H21" s="1"/>
-      <c r="I21" s="43"/>
+      <c r="I21" s="41"/>
       <c r="J21" s="15"/>
       <c r="K21" s="15"/>
       <c r="L21" s="3"/>
@@ -15327,16 +15301,16 @@
       <c r="F22" s="3"/>
       <c r="G22" s="4"/>
       <c r="H22" s="1"/>
-      <c r="I22" s="43"/>
+      <c r="I22" s="41"/>
       <c r="J22" s="15"/>
       <c r="K22" s="15"/>
       <c r="L22" s="3"/>
     </row>
     <row r="23" spans="1:13" s="16" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A23" s="43" t="s">
+      <c r="A23" s="41" t="s">
         <v>1352</v>
       </c>
-      <c r="B23" s="65" t="s">
+      <c r="B23" s="63" t="s">
         <v>1354</v>
       </c>
       <c r="C23" s="3"/>
@@ -15345,7 +15319,7 @@
       <c r="F23" s="3"/>
       <c r="G23" s="4"/>
       <c r="H23" s="3"/>
-      <c r="I23" s="51"/>
+      <c r="I23" s="49"/>
       <c r="J23" s="15"/>
       <c r="K23" s="15"/>
       <c r="L23" s="15"/>
@@ -15360,9 +15334,9 @@
       <c r="F24" s="35"/>
       <c r="G24" s="35"/>
       <c r="H24" s="35"/>
-      <c r="I24" s="44"/>
-      <c r="J24" s="44"/>
-      <c r="K24" s="44"/>
+      <c r="I24" s="42"/>
+      <c r="J24" s="42"/>
+      <c r="K24" s="42"/>
       <c r="L24" s="35"/>
     </row>
     <row r="25" spans="1:13" s="16" customFormat="1" x14ac:dyDescent="0.25">
@@ -15376,9 +15350,9 @@
       <c r="F25" s="6"/>
       <c r="G25" s="7"/>
       <c r="H25" s="6"/>
-      <c r="I25" s="45"/>
-      <c r="J25" s="45"/>
-      <c r="K25" s="45"/>
+      <c r="I25" s="43"/>
+      <c r="J25" s="43"/>
+      <c r="K25" s="43"/>
       <c r="L25" s="6"/>
     </row>
     <row r="26" spans="1:13" s="16" customFormat="1" x14ac:dyDescent="0.25">
@@ -15392,9 +15366,9 @@
       <c r="F26" s="6"/>
       <c r="G26" s="7"/>
       <c r="H26" s="6"/>
-      <c r="I26" s="45"/>
-      <c r="J26" s="45"/>
-      <c r="K26" s="45"/>
+      <c r="I26" s="43"/>
+      <c r="J26" s="43"/>
+      <c r="K26" s="43"/>
       <c r="L26" s="6"/>
     </row>
     <row r="27" spans="1:13" ht="30" x14ac:dyDescent="0.25">
@@ -15422,13 +15396,13 @@
       <c r="H27" s="20" t="s">
         <v>638</v>
       </c>
-      <c r="I27" s="48" t="s">
+      <c r="I27" s="46" t="s">
         <v>1314</v>
       </c>
-      <c r="J27" s="42" t="s">
+      <c r="J27" s="40" t="s">
         <v>14</v>
       </c>
-      <c r="K27" s="42" t="s">
+      <c r="K27" s="40" t="s">
         <v>1316</v>
       </c>
       <c r="L27" s="21" t="s">
@@ -15475,7 +15449,7 @@
       <c r="D29" s="31" t="s">
         <v>789</v>
       </c>
-      <c r="E29" s="60" t="s">
+      <c r="E29" s="58" t="s">
         <v>1355</v>
       </c>
       <c r="F29" s="12"/>
@@ -15509,7 +15483,7 @@
       <c r="D30" s="31" t="s">
         <v>790</v>
       </c>
-      <c r="E30" s="60" t="s">
+      <c r="E30" s="58" t="s">
         <v>1355</v>
       </c>
       <c r="F30" s="12"/>
@@ -15543,7 +15517,7 @@
       <c r="D31" s="31" t="s">
         <v>791</v>
       </c>
-      <c r="E31" s="60" t="s">
+      <c r="E31" s="58" t="s">
         <v>1355</v>
       </c>
       <c r="F31" s="12"/>
@@ -16381,7 +16355,7 @@
       <c r="D61" s="31" t="s">
         <v>690</v>
       </c>
-      <c r="E61" s="60" t="s">
+      <c r="E61" s="58" t="s">
         <v>1355</v>
       </c>
       <c r="F61" s="12"/>
@@ -16394,8 +16368,8 @@
       <c r="I61" s="32" t="s">
         <v>1049</v>
       </c>
-      <c r="J61" s="46"/>
-      <c r="K61" s="46"/>
+      <c r="J61" s="44"/>
+      <c r="K61" s="44"/>
       <c r="L61" s="27" t="s">
         <v>1067</v>
       </c>
@@ -16977,7 +16951,7 @@
       <c r="D82" s="31" t="s">
         <v>711</v>
       </c>
-      <c r="E82" s="60" t="s">
+      <c r="E82" s="58" t="s">
         <v>1355</v>
       </c>
       <c r="F82" s="12"/>
@@ -17209,7 +17183,7 @@
       <c r="D90" s="31" t="s">
         <v>721</v>
       </c>
-      <c r="E90" s="60" t="s">
+      <c r="E90" s="58" t="s">
         <v>1355</v>
       </c>
       <c r="F90" s="12" t="s">
@@ -17541,7 +17515,7 @@
       <c r="D101" s="31" t="s">
         <v>734</v>
       </c>
-      <c r="E101" s="60" t="s">
+      <c r="E101" s="58" t="s">
         <v>1355</v>
       </c>
       <c r="F101" s="12"/>
@@ -18153,7 +18127,7 @@
       <c r="D122" s="31" t="s">
         <v>755</v>
       </c>
-      <c r="E122" s="60" t="s">
+      <c r="E122" s="58" t="s">
         <v>1355</v>
       </c>
       <c r="F122" s="12" t="s">
@@ -20015,7 +19989,7 @@
       <c r="D187" s="23" t="s">
         <v>126</v>
       </c>
-      <c r="E187" s="60" t="s">
+      <c r="E187" s="58" t="s">
         <v>1355</v>
       </c>
       <c r="F187"/>
@@ -20187,7 +20161,7 @@
       <c r="D193" s="23" t="s">
         <v>150</v>
       </c>
-      <c r="E193" s="60" t="s">
+      <c r="E193" s="58" t="s">
         <v>1355</v>
       </c>
       <c r="F193"/>
@@ -20247,7 +20221,7 @@
       <c r="D195" s="23" t="s">
         <v>162</v>
       </c>
-      <c r="E195" s="60" t="s">
+      <c r="E195" s="58" t="s">
         <v>1355</v>
       </c>
       <c r="F195"/>
@@ -22411,14 +22385,14 @@
       <c r="E467" s="5"/>
       <c r="G467" s="10"/>
       <c r="H467" s="2"/>
-      <c r="I467" s="47"/>
+      <c r="I467" s="45"/>
     </row>
   </sheetData>
   <phoneticPr fontId="14" type="noConversion"/>
   <hyperlinks>
     <hyperlink ref="C2" r:id="rId1" xr:uid="{DDFBFA4A-1B14-4D4E-A2BD-12DE76DDF6D0}"/>
     <hyperlink ref="C3" r:id="rId2" display="http://registry.it.csiro.au/sandbox/soil/scma/" xr:uid="{EDF8FFA1-F2F3-4BB1-BF34-39358F567457}"/>
-    <hyperlink ref="B1" r:id="rId3" display="http://registry.it.csiro.au/sandbox/soil/scma" xr:uid="{06CEEB57-C964-4417-9D98-8525EB7C1644}"/>
+    <hyperlink ref="B1" r:id="rId3" xr:uid="{06CEEB57-C964-4417-9D98-8525EB7C1644}"/>
     <hyperlink ref="H106" r:id="rId4" xr:uid="{04389B99-8122-4DEE-9A4E-3C7BCF22DF7B}"/>
     <hyperlink ref="C5" r:id="rId5" xr:uid="{51359A00-70F8-41BF-ABD9-33E2124068E2}"/>
     <hyperlink ref="H28" r:id="rId6" xr:uid="{7C9D502A-B7C9-4C78-8562-107BC8C370C9}"/>
@@ -22549,10 +22523,12 @@
     <hyperlink ref="H193" r:id="rId131" xr:uid="{56A43D80-5339-4B76-9391-49A025D9212B}"/>
     <hyperlink ref="H195" r:id="rId132" xr:uid="{6315BB13-4B74-464B-9553-A415FD28F07F}"/>
     <hyperlink ref="B20" r:id="rId133" xr:uid="{5A650F16-2CB3-4CB1-820F-ED911B41CBB5}"/>
+    <hyperlink ref="C4" r:id="rId134" xr:uid="{9987F963-EAA1-40E1-9475-0DCBA757DE31}"/>
+    <hyperlink ref="B16" r:id="rId135" xr:uid="{299DA605-8C9B-4B33-9722-CA5BB6F69A14}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId134"/>
-  <legacyDrawing r:id="rId135"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId136"/>
+  <legacyDrawing r:id="rId137"/>
 </worksheet>
 </file>
 

</xml_diff>